<commit_message>
NSMB - a bit of progress on 1-1.  1.5 frames faster compared to the published movie.  It was from the hill sliding trick I used in my previous WIPs but it wasn't utilized in the published movie.  In reality I am 473 frames ahead at this point but all of that is due to 9.6 handling lag better.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="16080" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="V3" sheetId="2" r:id="rId1"/>
-    <sheet name="V1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="V4" sheetId="4" r:id="rId1"/>
+    <sheet name="V3" sheetId="2" r:id="rId2"/>
+    <sheet name="V1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t>1-1</t>
   </si>
@@ -313,6 +314,21 @@
   </si>
   <si>
     <t>Tried: 97780 coin = 97</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>terrot</t>
+  </si>
+  <si>
+    <t>Checkpoint 759</t>
+  </si>
+  <si>
+    <t>Checkpoint 936</t>
   </si>
 </sst>
 </file>
@@ -767,10 +783,1118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="16"/>
+    <col min="6" max="6" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="A2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="16">
+        <v>355</v>
+      </c>
+      <c r="D3" s="16">
+        <f>IF(B3 &gt;  0,C3-B3, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="16">
+        <v>476</v>
+      </c>
+      <c r="C4" s="16">
+        <v>517</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" ref="D4:D6" si="0">IF(B4 &gt;  0,C4-B4, 0)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2937</v>
+      </c>
+      <c r="C5" s="16">
+        <v>2937</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="16">
+        <v>2579</v>
+      </c>
+      <c r="C6" s="16">
+        <v>3038</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
+      <c r="A7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="16">
+        <v>2813</v>
+      </c>
+      <c r="C9" s="16">
+        <v>3285</v>
+      </c>
+      <c r="D9" s="16">
+        <f>IF(B9 &gt;  0,C9-B9, 0)</f>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="16">
+        <v>3099</v>
+      </c>
+      <c r="C10" s="16">
+        <v>3571</v>
+      </c>
+      <c r="D10" s="16">
+        <f>IF(B10 &gt;  0,C10-B10, 0)</f>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="16">
+        <v>3157</v>
+      </c>
+      <c r="C11" s="16">
+        <v>3630</v>
+      </c>
+      <c r="D11" s="16">
+        <f>IF(B11 &gt;  0,C11-B11, 0)</f>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="16">
+        <f t="shared" ref="D12:D38" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="16">
+        <v>6019</v>
+      </c>
+      <c r="C16" s="16">
+        <v>6028</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="16">
+        <v>8849</v>
+      </c>
+      <c r="C17" s="16">
+        <v>8859</v>
+      </c>
+      <c r="D17" s="16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="16">
+        <v>9865</v>
+      </c>
+      <c r="C19" s="16">
+        <v>9903</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="E19">
+        <v>9880</v>
+      </c>
+      <c r="F19" s="16">
+        <f>IF(B19 &gt;  0,E19-B19, 0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="16">
+        <v>10110</v>
+      </c>
+      <c r="C20" s="16">
+        <v>10150</v>
+      </c>
+      <c r="D20" s="16">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>10128</v>
+      </c>
+      <c r="F20" s="16">
+        <f>IF(B20 &gt;  0,E20-B20, 0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="16">
+        <v>10165</v>
+      </c>
+      <c r="C21" s="16">
+        <v>10208</v>
+      </c>
+      <c r="D21" s="16">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="E21">
+        <v>10186</v>
+      </c>
+      <c r="F21" s="16">
+        <f>IF(B21 &gt;  0,E21-B21, 0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22">
+        <v>10254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="16">
+        <v>10733</v>
+      </c>
+      <c r="C23" s="16">
+        <v>10777</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="E23">
+        <v>10746</v>
+      </c>
+      <c r="F23" s="16">
+        <f>IF(B23 &gt;  0,E23-B23, 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24">
+        <v>10769</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="16">
+        <v>11117</v>
+      </c>
+      <c r="C25" s="16">
+        <v>11169</v>
+      </c>
+      <c r="D25" s="16">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E25">
+        <v>11144</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" ref="F25:F30" si="2">IF(B25 &gt;  0,E25-B25, 0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="16">
+        <v>11298</v>
+      </c>
+      <c r="C26" s="16">
+        <v>11349</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E26">
+        <v>11325</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="16">
+        <v>11439</v>
+      </c>
+      <c r="C27" s="16">
+        <v>11490</v>
+      </c>
+      <c r="D27" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E27">
+        <v>11466</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="16">
+        <v>11491</v>
+      </c>
+      <c r="C28" s="16">
+        <v>11542</v>
+      </c>
+      <c r="D28" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E28">
+        <v>11517</v>
+      </c>
+      <c r="F28" s="16">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="16">
+        <v>11552</v>
+      </c>
+      <c r="C29" s="16">
+        <v>11606</v>
+      </c>
+      <c r="D29" s="16">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="E29">
+        <v>11577</v>
+      </c>
+      <c r="F29" s="16">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="16">
+        <v>11616</v>
+      </c>
+      <c r="C30" s="16">
+        <v>11672</v>
+      </c>
+      <c r="D30" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E30">
+        <v>11644</v>
+      </c>
+      <c r="F30" s="16">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="16">
+        <v>11626</v>
+      </c>
+      <c r="C31" s="16">
+        <v>11682</v>
+      </c>
+      <c r="D31" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="16">
+        <v>11652</v>
+      </c>
+      <c r="C32" s="16">
+        <v>11708</v>
+      </c>
+      <c r="D32" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E32">
+        <v>11680</v>
+      </c>
+      <c r="F32" s="16">
+        <f t="shared" ref="F32:F38" si="3">IF(B32 &gt;  0,E32-B32, 0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="16">
+        <v>11810</v>
+      </c>
+      <c r="C33" s="16">
+        <v>11870</v>
+      </c>
+      <c r="D33" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <v>11839</v>
+      </c>
+      <c r="F33" s="16">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="16">
+        <v>12121</v>
+      </c>
+      <c r="C34" s="16">
+        <v>12181</v>
+      </c>
+      <c r="D34" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E34">
+        <v>12150</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="16">
+        <v>12635</v>
+      </c>
+      <c r="C35" s="16">
+        <v>12695</v>
+      </c>
+      <c r="D35" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E35">
+        <v>12664</v>
+      </c>
+      <c r="F35" s="16">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="16">
+        <v>13099</v>
+      </c>
+      <c r="C36" s="16">
+        <v>13187</v>
+      </c>
+      <c r="D36" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E36">
+        <v>13117</v>
+      </c>
+      <c r="F36" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="16">
+        <v>13343</v>
+      </c>
+      <c r="C37" s="16">
+        <v>13431</v>
+      </c>
+      <c r="D37" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E37">
+        <v>13361</v>
+      </c>
+      <c r="F37" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="16">
+        <v>14307</v>
+      </c>
+      <c r="C38" s="16">
+        <v>14395</v>
+      </c>
+      <c r="D38" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E38">
+        <v>14325</v>
+      </c>
+      <c r="F38" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="18.75">
+      <c r="A39" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="16">
+        <v>15202</v>
+      </c>
+      <c r="C41" s="16">
+        <v>15292</v>
+      </c>
+      <c r="D41" s="16">
+        <f t="shared" ref="D41:D62" si="4">IF(B41 &gt;  0,C41-B41, 0)</f>
+        <v>90</v>
+      </c>
+      <c r="E41">
+        <v>15220</v>
+      </c>
+      <c r="F41" s="16">
+        <f t="shared" ref="F41:F52" si="5">IF(B41 &gt;  0,E41-B41, 0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="16">
+        <v>16484</v>
+      </c>
+      <c r="C42" s="16">
+        <v>16574</v>
+      </c>
+      <c r="D42" s="16">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="16">
+        <v>17011</v>
+      </c>
+      <c r="C43" s="16">
+        <v>17101</v>
+      </c>
+      <c r="D43" s="16">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="E43">
+        <v>17027</v>
+      </c>
+      <c r="F43" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="16">
+        <v>17525</v>
+      </c>
+      <c r="C44" s="16">
+        <v>17615</v>
+      </c>
+      <c r="D44" s="16">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="E44">
+        <v>17541</v>
+      </c>
+      <c r="F44" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="16">
+        <v>18058</v>
+      </c>
+      <c r="C45" s="16">
+        <v>18298</v>
+      </c>
+      <c r="D45" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E45">
+        <v>18074</v>
+      </c>
+      <c r="F45" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="16">
+        <v>18356</v>
+      </c>
+      <c r="C47" s="16">
+        <v>18596</v>
+      </c>
+      <c r="D47" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E47">
+        <v>18372</v>
+      </c>
+      <c r="F47" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="16">
+        <v>18742</v>
+      </c>
+      <c r="C48" s="16">
+        <v>18982</v>
+      </c>
+      <c r="D48" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E48">
+        <v>18758</v>
+      </c>
+      <c r="F48" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="16">
+        <v>18974</v>
+      </c>
+      <c r="C49" s="16">
+        <v>19214</v>
+      </c>
+      <c r="D49" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E49">
+        <v>18990</v>
+      </c>
+      <c r="F49" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="16">
+        <v>19152</v>
+      </c>
+      <c r="C50" s="16">
+        <v>19392</v>
+      </c>
+      <c r="D50" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E50">
+        <v>19168</v>
+      </c>
+      <c r="F50" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="16">
+        <v>19206</v>
+      </c>
+      <c r="C51" s="16">
+        <v>19447</v>
+      </c>
+      <c r="D51" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+      <c r="E51">
+        <v>19223</v>
+      </c>
+      <c r="F51" s="16">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="16">
+        <v>19281</v>
+      </c>
+      <c r="C52" s="16">
+        <v>19522</v>
+      </c>
+      <c r="D52" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+      <c r="E52">
+        <v>19299</v>
+      </c>
+      <c r="F52" s="16">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="16">
+        <v>19350</v>
+      </c>
+      <c r="C53" s="16">
+        <v>19591</v>
+      </c>
+      <c r="D53" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="16">
+        <v>19374</v>
+      </c>
+      <c r="C54" s="16">
+        <v>19615</v>
+      </c>
+      <c r="D54" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="16">
+        <v>19461</v>
+      </c>
+      <c r="C55" s="16">
+        <v>19703</v>
+      </c>
+      <c r="D55" s="16">
+        <f t="shared" si="4"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="16">
+        <v>19706</v>
+      </c>
+      <c r="C56" s="16">
+        <v>19949</v>
+      </c>
+      <c r="D56" s="16">
+        <f t="shared" si="4"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="16">
+        <v>20114</v>
+      </c>
+      <c r="C57" s="16">
+        <v>20359</v>
+      </c>
+      <c r="D57" s="16">
+        <f t="shared" si="4"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="16">
+        <v>20117</v>
+      </c>
+      <c r="C58" s="16">
+        <v>20363</v>
+      </c>
+      <c r="D58" s="16">
+        <f t="shared" si="4"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="16">
+        <v>20257</v>
+      </c>
+      <c r="C59" s="16">
+        <v>20512</v>
+      </c>
+      <c r="D59" s="16">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="16">
+        <v>20537</v>
+      </c>
+      <c r="C60" s="16">
+        <v>20832</v>
+      </c>
+      <c r="D60" s="16">
+        <f t="shared" si="4"/>
+        <v>295</v>
+      </c>
+      <c r="E60">
+        <v>20600</v>
+      </c>
+      <c r="F60" s="16">
+        <f t="shared" ref="F60:F62" si="6">IF(B60 &gt;  0,E60-B60, 0)</f>
+        <v>63</v>
+      </c>
+      <c r="G60" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="16">
+        <v>21051</v>
+      </c>
+      <c r="C61" s="16">
+        <v>21346</v>
+      </c>
+      <c r="D61" s="16">
+        <f t="shared" si="4"/>
+        <v>295</v>
+      </c>
+      <c r="E61">
+        <v>21114</v>
+      </c>
+      <c r="F61" s="16">
+        <f t="shared" si="6"/>
+        <v>63</v>
+      </c>
+      <c r="G61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="16">
+        <v>21617</v>
+      </c>
+      <c r="C62" s="16">
+        <v>22007</v>
+      </c>
+      <c r="D62" s="16">
+        <f t="shared" si="4"/>
+        <v>390</v>
+      </c>
+      <c r="E62">
+        <v>21615</v>
+      </c>
+      <c r="F62" s="16">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="G62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A39:F39"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
@@ -1857,7 +2981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C45"/>
   <sheetViews>
@@ -2363,7 +3487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
NSMB - Up to the end of 1-1, stuck trying to manipulate the blue shell.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
   <si>
     <t>1-1</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>Checkpoint 936</t>
+  </si>
+  <si>
+    <t>Checkpoint 2626</t>
   </si>
 </sst>
 </file>
@@ -783,11 +786,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -951,247 +954,245 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="16" t="s">
-        <v>45</v>
+        <v>104</v>
+      </c>
+      <c r="B12" s="16">
+        <v>3718</v>
+      </c>
+      <c r="C12" s="16">
+        <v>4192</v>
       </c>
       <c r="D12" s="16">
-        <f t="shared" ref="D12:D38" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
-        <v>0</v>
+        <f>IF(B12 &gt;  0,C12-B12, 0)</f>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="16">
+        <v>4153</v>
+      </c>
+      <c r="C13" s="16">
+        <v>4627</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" ref="D13:D39" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="16">
+      <c r="B14" s="16">
+        <v>4671</v>
+      </c>
+      <c r="C14" s="16">
+        <v>5145</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="1"/>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17">
+        <v>5738</v>
+      </c>
+      <c r="D15" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="20" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="16">
-        <v>6019</v>
-      </c>
-      <c r="C16" s="16">
-        <v>6028</v>
-      </c>
-      <c r="D16" s="16">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="16">
+        <v>5937</v>
+      </c>
+      <c r="D17" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="16">
-        <v>8849</v>
-      </c>
-      <c r="C17" s="16">
-        <v>8859</v>
-      </c>
-      <c r="D17" s="16">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="20" t="s">
+      <c r="D18" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="20"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="16">
-        <v>9865</v>
-      </c>
-      <c r="C19" s="16">
-        <v>9903</v>
-      </c>
-      <c r="D19" s="16">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="E19">
-        <v>9880</v>
-      </c>
-      <c r="F19" s="16">
-        <f>IF(B19 &gt;  0,E19-B19, 0)</f>
-        <v>15</v>
-      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="16" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B20" s="16">
-        <v>10110</v>
+        <v>9865</v>
       </c>
       <c r="C20" s="16">
-        <v>10150</v>
+        <v>9903</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20">
-        <v>10128</v>
+        <v>9880</v>
       </c>
       <c r="F20" s="16">
         <f>IF(B20 &gt;  0,E20-B20, 0)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="16">
-        <v>10165</v>
+        <v>10110</v>
       </c>
       <c r="C21" s="16">
-        <v>10208</v>
+        <v>10150</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21">
-        <v>10186</v>
+        <v>10128</v>
       </c>
       <c r="F21" s="16">
         <f>IF(B21 &gt;  0,E21-B21, 0)</f>
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="B22" s="16">
+        <v>10165</v>
+      </c>
+      <c r="C22" s="16">
+        <v>10208</v>
+      </c>
+      <c r="D22" s="16">
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="E22">
-        <v>10254</v>
+        <v>10186</v>
+      </c>
+      <c r="F22" s="16">
+        <f>IF(B22 &gt;  0,E22-B22, 0)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="16">
-        <v>10733</v>
-      </c>
-      <c r="C23" s="16">
-        <v>10777</v>
-      </c>
-      <c r="D23" s="16">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="E23">
-        <v>10746</v>
-      </c>
-      <c r="F23" s="16">
-        <f>IF(B23 &gt;  0,E23-B23, 0)</f>
-        <v>13</v>
+        <v>10254</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="B24" s="16">
+        <v>10733</v>
+      </c>
+      <c r="C24" s="16">
+        <v>10777</v>
+      </c>
+      <c r="D24" s="16">
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="E24">
-        <v>10769</v>
+        <v>10746</v>
+      </c>
+      <c r="F24" s="16">
+        <f>IF(B24 &gt;  0,E24-B24, 0)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="16">
-        <v>11117</v>
-      </c>
-      <c r="C25" s="16">
-        <v>11169</v>
-      </c>
-      <c r="D25" s="16">
-        <f t="shared" si="1"/>
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E25">
-        <v>11144</v>
-      </c>
-      <c r="F25" s="16">
-        <f t="shared" ref="F25:F30" si="2">IF(B25 &gt;  0,E25-B25, 0)</f>
-        <v>27</v>
+        <v>10769</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="16">
-        <v>11298</v>
+        <v>11117</v>
       </c>
       <c r="C26" s="16">
-        <v>11349</v>
+        <v>11169</v>
       </c>
       <c r="D26" s="16">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E26">
-        <v>11325</v>
+        <v>11144</v>
       </c>
       <c r="F26" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F26:F31" si="2">IF(B26 &gt;  0,E26-B26, 0)</f>
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="16">
-        <v>11439</v>
+        <v>11298</v>
       </c>
       <c r="C27" s="16">
-        <v>11490</v>
+        <v>11349</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="E27">
-        <v>11466</v>
+        <v>11325</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="2"/>
@@ -1199,146 +1200,146 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="18" t="s">
-        <v>67</v>
+      <c r="A28" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B28" s="16">
-        <v>11491</v>
+        <v>11439</v>
       </c>
       <c r="C28" s="16">
-        <v>11542</v>
+        <v>11490</v>
       </c>
       <c r="D28" s="16">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="E28">
-        <v>11517</v>
+        <v>11466</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="16" t="s">
-        <v>68</v>
+      <c r="A29" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="B29" s="16">
-        <v>11552</v>
+        <v>11491</v>
       </c>
       <c r="C29" s="16">
-        <v>11606</v>
+        <v>11542</v>
       </c>
       <c r="D29" s="16">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E29">
-        <v>11577</v>
+        <v>11517</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="16">
-        <v>11616</v>
+        <v>11552</v>
       </c>
       <c r="C30" s="16">
-        <v>11672</v>
+        <v>11606</v>
       </c>
       <c r="D30" s="16">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30">
-        <v>11644</v>
+        <v>11577</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="16">
-        <v>11626</v>
+        <v>11616</v>
       </c>
       <c r="C31" s="16">
-        <v>11682</v>
+        <v>11672</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="1"/>
         <v>56</v>
+      </c>
+      <c r="E31">
+        <v>11644</v>
+      </c>
+      <c r="F31" s="16">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="16">
-        <v>11652</v>
+        <v>11626</v>
       </c>
       <c r="C32" s="16">
-        <v>11708</v>
+        <v>11682</v>
       </c>
       <c r="D32" s="16">
         <f t="shared" si="1"/>
         <v>56</v>
-      </c>
-      <c r="E32">
-        <v>11680</v>
-      </c>
-      <c r="F32" s="16">
-        <f t="shared" ref="F32:F38" si="3">IF(B32 &gt;  0,E32-B32, 0)</f>
-        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="16">
+        <v>11652</v>
+      </c>
+      <c r="C33" s="16">
+        <v>11708</v>
+      </c>
+      <c r="D33" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E33">
+        <v>11680</v>
+      </c>
+      <c r="F33" s="16">
+        <f t="shared" ref="F33:F39" si="3">IF(B33 &gt;  0,E33-B33, 0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B34" s="16">
         <v>11810</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C34" s="16">
         <v>11870</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D34" s="16">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>11839</v>
-      </c>
-      <c r="F33" s="16">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="16">
-        <v>12121</v>
-      </c>
-      <c r="C34" s="16">
-        <v>12181</v>
-      </c>
-      <c r="D34" s="16">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="E34">
-        <v>12150</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="3"/>
@@ -1346,21 +1347,21 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="16" t="s">
-        <v>73</v>
+      <c r="A35" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B35" s="16">
-        <v>12635</v>
+        <v>12121</v>
       </c>
       <c r="C35" s="16">
-        <v>12695</v>
+        <v>12181</v>
       </c>
       <c r="D35" s="16">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="E35">
-        <v>12664</v>
+        <v>12150</v>
       </c>
       <c r="F35" s="16">
         <f t="shared" si="3"/>
@@ -1369,42 +1370,42 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36" s="16">
-        <v>13099</v>
+        <v>12635</v>
       </c>
       <c r="C36" s="16">
-        <v>13187</v>
+        <v>12695</v>
       </c>
       <c r="D36" s="16">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E36">
-        <v>13117</v>
+        <v>12664</v>
       </c>
       <c r="F36" s="16">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="16" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B37" s="16">
-        <v>13343</v>
+        <v>13099</v>
       </c>
       <c r="C37" s="16">
-        <v>13431</v>
+        <v>13187</v>
       </c>
       <c r="D37" s="16">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="E37">
-        <v>13361</v>
+        <v>13117</v>
       </c>
       <c r="F37" s="16">
         <f t="shared" si="3"/>
@@ -1413,121 +1414,121 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="16" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B38" s="16">
-        <v>14307</v>
+        <v>13343</v>
       </c>
       <c r="C38" s="16">
-        <v>14395</v>
+        <v>13431</v>
       </c>
       <c r="D38" s="16">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="E38">
-        <v>14325</v>
+        <v>13361</v>
       </c>
       <c r="F38" s="16">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75">
-      <c r="A39" s="28" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="16">
+        <v>14307</v>
+      </c>
+      <c r="C39" s="16">
+        <v>14395</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E39">
+        <v>14325</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="18.75">
+      <c r="A40" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="24" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="16">
-        <v>15202</v>
-      </c>
-      <c r="C41" s="16">
-        <v>15292</v>
-      </c>
-      <c r="D41" s="16">
-        <f t="shared" ref="D41:D62" si="4">IF(B41 &gt;  0,C41-B41, 0)</f>
-        <v>90</v>
-      </c>
-      <c r="E41">
-        <v>15220</v>
-      </c>
-      <c r="F41" s="16">
-        <f t="shared" ref="F41:F52" si="5">IF(B41 &gt;  0,E41-B41, 0)</f>
-        <v>18</v>
-      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B42" s="16">
-        <v>16484</v>
+        <v>15202</v>
       </c>
       <c r="C42" s="16">
-        <v>16574</v>
+        <v>15292</v>
       </c>
       <c r="D42" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D42:D63" si="4">IF(B42 &gt;  0,C42-B42, 0)</f>
         <v>90</v>
+      </c>
+      <c r="E42">
+        <v>15220</v>
+      </c>
+      <c r="F42" s="16">
+        <f t="shared" ref="F42:F53" si="5">IF(B42 &gt;  0,E42-B42, 0)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="16" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B43" s="16">
-        <v>17011</v>
+        <v>16484</v>
       </c>
       <c r="C43" s="16">
-        <v>17101</v>
+        <v>16574</v>
       </c>
       <c r="D43" s="16">
         <f t="shared" si="4"/>
         <v>90</v>
-      </c>
-      <c r="E43">
-        <v>17027</v>
-      </c>
-      <c r="F43" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="16" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="B44" s="16">
-        <v>17525</v>
+        <v>17011</v>
       </c>
       <c r="C44" s="16">
-        <v>17615</v>
+        <v>17101</v>
       </c>
       <c r="D44" s="16">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="E44">
-        <v>17541</v>
+        <v>17027</v>
       </c>
       <c r="F44" s="16">
         <f t="shared" si="5"/>
@@ -1536,20 +1537,20 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="16" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B45" s="16">
-        <v>18058</v>
+        <v>17525</v>
       </c>
       <c r="C45" s="16">
-        <v>18298</v>
+        <v>17615</v>
       </c>
       <c r="D45" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="E45">
-        <v>18074</v>
+        <v>17541</v>
       </c>
       <c r="F45" s="16">
         <f t="shared" si="5"/>
@@ -1557,53 +1558,53 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="16">
-        <v>18356</v>
-      </c>
-      <c r="C47" s="16">
-        <v>18596</v>
-      </c>
-      <c r="D47" s="16">
+      <c r="A46" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="16">
+        <v>18058</v>
+      </c>
+      <c r="C46" s="16">
+        <v>18298</v>
+      </c>
+      <c r="D46" s="16">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="E47">
-        <v>18372</v>
-      </c>
-      <c r="F47" s="16">
+      <c r="E46">
+        <v>18074</v>
+      </c>
+      <c r="F46" s="16">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
     </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="22"/>
+    </row>
     <row r="48" spans="1:6">
       <c r="A48" s="16" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B48" s="16">
-        <v>18742</v>
+        <v>18356</v>
       </c>
       <c r="C48" s="16">
-        <v>18982</v>
+        <v>18596</v>
       </c>
       <c r="D48" s="16">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="E48">
-        <v>18758</v>
+        <v>18372</v>
       </c>
       <c r="F48" s="16">
         <f t="shared" si="5"/>
@@ -1612,20 +1613,20 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="16" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B49" s="16">
-        <v>18974</v>
+        <v>18742</v>
       </c>
       <c r="C49" s="16">
-        <v>19214</v>
+        <v>18982</v>
       </c>
       <c r="D49" s="16">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="E49">
-        <v>18990</v>
+        <v>18758</v>
       </c>
       <c r="F49" s="16">
         <f t="shared" si="5"/>
@@ -1634,20 +1635,20 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="16">
-        <v>19152</v>
+        <v>18974</v>
       </c>
       <c r="C50" s="16">
-        <v>19392</v>
+        <v>19214</v>
       </c>
       <c r="D50" s="16">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="E50">
-        <v>19168</v>
+        <v>18990</v>
       </c>
       <c r="F50" s="16">
         <f t="shared" si="5"/>
@@ -1656,72 +1657,79 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51" s="16">
-        <v>19206</v>
+        <v>19152</v>
       </c>
       <c r="C51" s="16">
-        <v>19447</v>
+        <v>19392</v>
       </c>
       <c r="D51" s="16">
         <f t="shared" si="4"/>
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E51">
-        <v>19223</v>
+        <v>19168</v>
       </c>
       <c r="F51" s="16">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" s="16">
-        <v>19281</v>
+        <v>19206</v>
       </c>
       <c r="C52" s="16">
-        <v>19522</v>
+        <v>19447</v>
       </c>
       <c r="D52" s="16">
         <f t="shared" si="4"/>
         <v>241</v>
       </c>
       <c r="E52">
-        <v>19299</v>
+        <v>19223</v>
       </c>
       <c r="F52" s="16">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" s="16">
-        <v>19350</v>
+        <v>19281</v>
       </c>
       <c r="C53" s="16">
-        <v>19591</v>
+        <v>19522</v>
       </c>
       <c r="D53" s="16">
         <f t="shared" si="4"/>
         <v>241</v>
+      </c>
+      <c r="E53">
+        <v>19299</v>
+      </c>
+      <c r="F53" s="16">
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" s="16">
-        <v>19374</v>
+        <v>19350</v>
       </c>
       <c r="C54" s="16">
-        <v>19615</v>
+        <v>19591</v>
       </c>
       <c r="D54" s="16">
         <f t="shared" si="4"/>
@@ -1730,151 +1738,166 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="16">
-        <v>19461</v>
+        <v>19374</v>
       </c>
       <c r="C55" s="16">
-        <v>19703</v>
+        <v>19615</v>
       </c>
       <c r="D55" s="16">
         <f t="shared" si="4"/>
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="16">
-        <v>19706</v>
+        <v>19461</v>
       </c>
       <c r="C56" s="16">
-        <v>19949</v>
+        <v>19703</v>
       </c>
       <c r="D56" s="16">
         <f t="shared" si="4"/>
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B57" s="16">
-        <v>20114</v>
+        <v>19706</v>
       </c>
       <c r="C57" s="16">
-        <v>20359</v>
+        <v>19949</v>
       </c>
       <c r="D57" s="16">
         <f t="shared" si="4"/>
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="16">
-        <v>20117</v>
+        <v>20114</v>
       </c>
       <c r="C58" s="16">
-        <v>20363</v>
+        <v>20359</v>
       </c>
       <c r="D58" s="16">
         <f t="shared" si="4"/>
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="16" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="B59" s="16">
-        <v>20257</v>
+        <v>20117</v>
       </c>
       <c r="C59" s="16">
-        <v>20512</v>
+        <v>20363</v>
       </c>
       <c r="D59" s="16">
         <f t="shared" si="4"/>
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="16" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B60" s="16">
-        <v>20537</v>
+        <v>20257</v>
       </c>
       <c r="C60" s="16">
-        <v>20832</v>
+        <v>20512</v>
       </c>
       <c r="D60" s="16">
         <f t="shared" si="4"/>
-        <v>295</v>
-      </c>
-      <c r="E60">
-        <v>20600</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" ref="F60:F62" si="6">IF(B60 &gt;  0,E60-B60, 0)</f>
-        <v>63</v>
-      </c>
-      <c r="G60" t="s">
-        <v>96</v>
+        <v>255</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="16">
+        <v>20537</v>
+      </c>
+      <c r="C61" s="16">
+        <v>20832</v>
+      </c>
+      <c r="D61" s="16">
+        <f t="shared" si="4"/>
+        <v>295</v>
+      </c>
+      <c r="E61">
+        <v>20600</v>
+      </c>
+      <c r="F61" s="16">
+        <f t="shared" ref="F61:F63" si="6">IF(B61 &gt;  0,E61-B61, 0)</f>
+        <v>63</v>
+      </c>
+      <c r="G61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B62" s="16">
         <v>21051</v>
       </c>
-      <c r="C61" s="16">
+      <c r="C62" s="16">
         <v>21346</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D62" s="16">
         <f t="shared" si="4"/>
         <v>295</v>
       </c>
-      <c r="E61">
+      <c r="E62">
         <v>21114</v>
       </c>
-      <c r="F61" s="16">
+      <c r="F62" s="16">
         <f t="shared" si="6"/>
         <v>63</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="16" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B62" s="16">
+      <c r="B63" s="16">
         <v>21617</v>
       </c>
-      <c r="C62" s="16">
+      <c r="C63" s="16">
         <v>22007</v>
       </c>
-      <c r="D62" s="16">
+      <c r="D63" s="16">
         <f t="shared" si="4"/>
         <v>390</v>
       </c>
-      <c r="E62">
+      <c r="E63">
         <v>21615</v>
       </c>
-      <c r="F62" s="16">
+      <c r="F63" s="16">
         <f t="shared" si="6"/>
         <v>-2</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G63" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1882,7 +1905,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
NSMB - no real progress, more failing to get a blue shell.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
   <si>
     <t>1-1</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>Checkpoint 2626</t>
+  </si>
+  <si>
+    <t>Flower</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>iup</t>
   </si>
 </sst>
 </file>
@@ -786,11 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -800,7 +809,7 @@
     <col min="6" max="6" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
@@ -819,8 +828,14 @@
       <c r="F1" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="G1">
+        <v>4671</v>
+      </c>
+      <c r="I1">
+        <v>4672</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="13" customFormat="1" ht="19.5" thickTop="1">
       <c r="A2" s="25" t="s">
         <v>44</v>
       </c>
@@ -830,7 +845,7 @@
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:10">
       <c r="A3" s="15" t="s">
         <v>47</v>
       </c>
@@ -841,8 +856,14 @@
         <f>IF(B3 &gt;  0,C3-B3, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>22200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="16" t="s">
         <v>48</v>
       </c>
@@ -856,8 +877,14 @@
         <f t="shared" ref="D4:D6" si="0">IF(B4 &gt;  0,C4-B4, 0)</f>
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>22300</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
@@ -871,8 +898,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>22500</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5">
+        <v>22700</v>
+      </c>
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
@@ -886,8 +925,20 @@
         <f t="shared" si="0"/>
         <v>459</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
+      <c r="G6">
+        <v>22900</v>
+      </c>
+      <c r="H6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6">
+        <v>22900</v>
+      </c>
+      <c r="J6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="13" customFormat="1" ht="18.75">
       <c r="A7" s="27" t="s">
         <v>42</v>
       </c>
@@ -896,8 +947,14 @@
       <c r="D7" s="27"/>
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>23100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="20" t="s">
         <v>43</v>
       </c>
@@ -907,7 +964,7 @@
       <c r="E8" s="21"/>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:10">
       <c r="A9" s="16" t="s">
         <v>51</v>
       </c>
@@ -922,7 +979,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:10">
       <c r="A10" s="16" t="s">
         <v>102</v>
       </c>
@@ -937,7 +994,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:10">
       <c r="A11" s="16" t="s">
         <v>103</v>
       </c>
@@ -951,8 +1008,14 @@
         <f>IF(B11 &gt;  0,C11-B11, 0)</f>
         <v>473</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>23500</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="16" t="s">
         <v>104</v>
       </c>
@@ -966,8 +1029,14 @@
         <f>IF(B12 &gt;  0,C12-B12, 0)</f>
         <v>474</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>23600</v>
+      </c>
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="16" t="s">
         <v>45</v>
       </c>
@@ -981,8 +1050,14 @@
         <f t="shared" ref="D13:D39" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
         <v>474</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>23800</v>
+      </c>
+      <c r="H13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="16" t="s">
         <v>46</v>
       </c>
@@ -996,8 +1071,14 @@
         <f t="shared" si="1"/>
         <v>474</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>24200</v>
+      </c>
+      <c r="H14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="17" t="s">
         <v>52</v>
       </c>
@@ -1009,8 +1090,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>24400</v>
+      </c>
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="20" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
NSMB - pasted my old 1-1 because I like it better, same frame count.  Fails on blue shell manipulation too (still haven't got one on any circumstance).
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -795,11 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,7 +809,7 @@
     <col min="6" max="6" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickBot="1">
+    <row r="1" spans="1:13" ht="16.5" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
@@ -835,7 +835,7 @@
         <v>4672</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="13" customFormat="1" ht="19.5" thickTop="1">
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="19.5" thickTop="1">
       <c r="A2" s="25" t="s">
         <v>44</v>
       </c>
@@ -844,8 +844,14 @@
       <c r="D2" s="25"/>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" s="13">
+        <v>2813</v>
+      </c>
+      <c r="M2" s="13">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="15" t="s">
         <v>47</v>
       </c>
@@ -862,8 +868,14 @@
       <c r="H3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3">
+        <v>17</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="16" t="s">
         <v>48</v>
       </c>
@@ -883,8 +895,16 @@
       <c r="H4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4">
+        <f>SUM(L2:L3)</f>
+        <v>2830</v>
+      </c>
+      <c r="M4">
+        <f>SUM(M2:M3)</f>
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
@@ -911,7 +931,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13">
       <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
@@ -938,7 +958,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="13" customFormat="1" ht="18.75">
+    <row r="7" spans="1:13" s="13" customFormat="1" ht="18.75">
       <c r="A7" s="27" t="s">
         <v>42</v>
       </c>
@@ -954,7 +974,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:13">
       <c r="A8" s="20" t="s">
         <v>43</v>
       </c>
@@ -964,7 +984,7 @@
       <c r="E8" s="21"/>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:13">
       <c r="A9" s="16" t="s">
         <v>51</v>
       </c>
@@ -979,7 +999,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:13">
       <c r="A10" s="16" t="s">
         <v>102</v>
       </c>
@@ -994,7 +1014,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:13">
       <c r="A11" s="16" t="s">
         <v>103</v>
       </c>
@@ -1015,7 +1035,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:13">
       <c r="A12" s="16" t="s">
         <v>104</v>
       </c>
@@ -1036,7 +1056,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:13">
       <c r="A13" s="16" t="s">
         <v>45</v>
       </c>
@@ -1057,7 +1077,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:13">
       <c r="A14" s="16" t="s">
         <v>46</v>
       </c>
@@ -1078,7 +1098,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:13">
       <c r="A15" s="17" t="s">
         <v>52</v>
       </c>
@@ -1097,7 +1117,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:13">
       <c r="A16" s="20" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
NSMB - we have blue shell!!!! Note to anyone attempting to watch it: You need desmume 9.6 with Bus level timing disabled (in emulator settings).
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="110">
   <si>
     <t>1-1</t>
   </si>
@@ -341,6 +341,12 @@
   </si>
   <si>
     <t>iup</t>
+  </si>
+  <si>
+    <t>No bus</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -799,7 +805,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -834,6 +840,9 @@
       <c r="I1">
         <v>4672</v>
       </c>
+      <c r="K1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="19.5" thickTop="1">
       <c r="A2" s="25" t="s">
@@ -844,6 +853,9 @@
       <c r="D2" s="25"/>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
+      <c r="K2" s="13">
+        <v>2806</v>
+      </c>
       <c r="L2" s="13">
         <v>2813</v>
       </c>
@@ -868,6 +880,9 @@
       <c r="H3" t="s">
         <v>106</v>
       </c>
+      <c r="K3">
+        <v>17</v>
+      </c>
       <c r="L3">
         <v>17</v>
       </c>
@@ -895,6 +910,10 @@
       <c r="H4" t="s">
         <v>106</v>
       </c>
+      <c r="K4">
+        <f>SUM(K2:K3)</f>
+        <v>2823</v>
+      </c>
       <c r="L4">
         <f>SUM(L2:L3)</f>
         <v>2830</v>
@@ -929,6 +948,9 @@
       </c>
       <c r="J5" t="s">
         <v>107</v>
+      </c>
+      <c r="K5">
+        <v>4146</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -983,35 +1005,43 @@
       <c r="D8" s="20"/>
       <c r="E8" s="21"/>
       <c r="F8" s="20"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B9" s="16">
-        <v>2813</v>
+        <v>2806</v>
       </c>
       <c r="C9" s="16">
         <v>3285</v>
       </c>
       <c r="D9" s="16">
         <f>IF(B9 &gt;  0,C9-B9, 0)</f>
-        <v>472</v>
-      </c>
+        <v>479</v>
+      </c>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="16" t="s">
         <v>102</v>
       </c>
       <c r="B10" s="16">
-        <v>3099</v>
+        <v>3093</v>
       </c>
       <c r="C10" s="16">
         <v>3571</v>
       </c>
       <c r="D10" s="16">
         <f>IF(B10 &gt;  0,C10-B10, 0)</f>
-        <v>472</v>
+        <v>478</v>
+      </c>
+      <c r="K10">
+        <v>22200</v>
+      </c>
+      <c r="L10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1019,20 +1049,26 @@
         <v>103</v>
       </c>
       <c r="B11" s="16">
-        <v>3157</v>
+        <v>3151</v>
       </c>
       <c r="C11" s="16">
         <v>3630</v>
       </c>
       <c r="D11" s="16">
         <f>IF(B11 &gt;  0,C11-B11, 0)</f>
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="G11">
         <v>23500</v>
       </c>
       <c r="H11" t="s">
         <v>105</v>
+      </c>
+      <c r="K11">
+        <v>22300</v>
+      </c>
+      <c r="L11" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1040,20 +1076,26 @@
         <v>104</v>
       </c>
       <c r="B12" s="16">
-        <v>3718</v>
+        <v>3712</v>
       </c>
       <c r="C12" s="16">
         <v>4192</v>
       </c>
       <c r="D12" s="16">
         <f>IF(B12 &gt;  0,C12-B12, 0)</f>
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="G12">
         <v>23600</v>
       </c>
       <c r="H12" t="s">
         <v>105</v>
+      </c>
+      <c r="K12" s="13">
+        <v>22600</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1061,20 +1103,26 @@
         <v>45</v>
       </c>
       <c r="B13" s="16">
-        <v>4153</v>
+        <v>4146</v>
       </c>
       <c r="C13" s="16">
         <v>4627</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" ref="D13:D39" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="G13">
         <v>23800</v>
       </c>
       <c r="H13" t="s">
         <v>105</v>
+      </c>
+      <c r="K13" s="13">
+        <v>22900</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1082,20 +1130,26 @@
         <v>46</v>
       </c>
       <c r="B14" s="16">
-        <v>4671</v>
+        <v>4664</v>
       </c>
       <c r="C14" s="16">
         <v>5145</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="1"/>
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="G14">
         <v>24200</v>
       </c>
       <c r="H14" t="s">
         <v>105</v>
+      </c>
+      <c r="K14" s="13">
+        <v>23100</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1115,6 +1169,12 @@
       </c>
       <c r="H15" t="s">
         <v>105</v>
+      </c>
+      <c r="K15" s="13">
+        <v>22800</v>
+      </c>
+      <c r="L15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1126,20 +1186,32 @@
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
       <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="K16" s="13">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="16" t="s">
         <v>53</v>
       </c>
+      <c r="B17" s="16">
+        <v>5057</v>
+      </c>
       <c r="C17" s="16">
         <v>5937</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>880</v>
+      </c>
+      <c r="K17">
+        <v>23600</v>
+      </c>
+      <c r="L17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="16" t="s">
         <v>55</v>
       </c>
@@ -1148,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:12">
       <c r="A19" s="20" t="s">
         <v>81</v>
       </c>
@@ -1158,7 +1230,7 @@
       <c r="E19" s="21"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:12">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
@@ -1180,7 +1252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:12">
       <c r="A21" s="16" t="s">
         <v>57</v>
       </c>
@@ -1202,7 +1274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:12">
       <c r="A22" s="16" t="s">
         <v>60</v>
       </c>
@@ -1224,7 +1296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:12">
       <c r="A23" s="16" t="s">
         <v>61</v>
       </c>
@@ -1232,7 +1304,7 @@
         <v>10254</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:12">
       <c r="A24" s="16" t="s">
         <v>62</v>
       </c>
@@ -1254,7 +1326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:12">
       <c r="A25" s="16" t="s">
         <v>63</v>
       </c>
@@ -1262,7 +1334,7 @@
         <v>10769</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:12">
       <c r="A26" s="16" t="s">
         <v>64</v>
       </c>
@@ -1284,7 +1356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:12">
       <c r="A27" s="16" t="s">
         <v>65</v>
       </c>
@@ -1306,7 +1378,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:12">
       <c r="A28" s="16" t="s">
         <v>66</v>
       </c>
@@ -1328,7 +1400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:12">
       <c r="A29" s="18" t="s">
         <v>67</v>
       </c>
@@ -1350,7 +1422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:12">
       <c r="A30" s="16" t="s">
         <v>68</v>
       </c>
@@ -1372,7 +1444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:12">
       <c r="A31" s="16" t="s">
         <v>69</v>
       </c>
@@ -1394,7 +1466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:12">
       <c r="A32" s="16" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
NSMB - 1-F done unless better map manipulation is possible.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
   <si>
     <t>1-1</t>
   </si>
@@ -795,11 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,14 +848,14 @@
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
       <c r="I2" s="13">
-        <v>5296</v>
+        <v>9674</v>
       </c>
       <c r="J2" s="13">
-        <v>6281</v>
+        <v>11156</v>
       </c>
       <c r="K2" s="13">
         <f>J2-I2</f>
-        <v>985</v>
+        <v>1482</v>
       </c>
       <c r="L2" s="13">
         <v>5057</v>
@@ -908,11 +908,11 @@
       </c>
       <c r="I4">
         <f>SUM(I2:I3)</f>
-        <v>5313</v>
+        <v>9691</v>
       </c>
       <c r="J4">
         <f>SUM(J2:J3)</f>
-        <v>6290</v>
+        <v>11165</v>
       </c>
       <c r="L4">
         <f>SUM(L2:L3)</f>
@@ -1050,7 +1050,7 @@
         <v>4627</v>
       </c>
       <c r="D13" s="16">
-        <f t="shared" ref="D13:D42" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
+        <f t="shared" ref="D13:D33" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
         <v>481</v>
       </c>
       <c r="K13" s="13"/>
@@ -1098,7 +1098,7 @@
       <c r="F16" s="20"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:14">
       <c r="A17" s="16" t="s">
         <v>53</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:14">
       <c r="A18" s="16" t="s">
         <v>106</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:14">
       <c r="A19" s="16" t="s">
         <v>107</v>
       </c>
@@ -1143,15 +1143,19 @@
         <v>919</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:14">
       <c r="A20" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="16">
         <v>7351</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="D20" s="16">
+        <f t="shared" si="1"/>
+        <v>-7351</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="16" t="s">
         <v>55</v>
       </c>
@@ -1160,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:14">
       <c r="A22" s="20" t="s">
         <v>81</v>
       </c>
@@ -1169,854 +1173,698 @@
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
       <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="I22" s="13">
+        <v>9852</v>
+      </c>
+      <c r="J22" s="13">
+        <v>11335</v>
+      </c>
+      <c r="K22" s="13">
+        <f>J22-I22</f>
+        <v>1483</v>
+      </c>
+      <c r="L22" s="13">
+        <v>5057</v>
+      </c>
+      <c r="M22" s="13">
+        <v>6019</v>
+      </c>
+      <c r="N22" s="13">
+        <f>M22-L22</f>
+        <v>962</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="16" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="16">
-        <v>9865</v>
+        <v>8406</v>
       </c>
       <c r="C23" s="16">
-        <v>9903</v>
+        <v>9830</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>1424</v>
       </c>
       <c r="E23">
         <v>9880</v>
       </c>
       <c r="F23" s="16">
         <f>IF(B23 &gt;  0,E23-B23, 0)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>1474</v>
+      </c>
+      <c r="I23">
+        <v>17</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="L23">
+        <v>17</v>
+      </c>
+      <c r="M23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="16">
-        <v>10110</v>
+        <v>8632</v>
       </c>
       <c r="C24" s="16">
-        <v>10150</v>
+        <v>10077</v>
       </c>
       <c r="D24" s="16">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>1445</v>
       </c>
       <c r="E24">
         <v>10128</v>
       </c>
       <c r="F24" s="16">
         <f>IF(B24 &gt;  0,E24-B24, 0)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>1496</v>
+      </c>
+      <c r="I24">
+        <f>SUM(I22:I23)</f>
+        <v>9869</v>
+      </c>
+      <c r="J24">
+        <f>SUM(J22:J23)</f>
+        <v>11344</v>
+      </c>
+      <c r="L24">
+        <f>SUM(L22:L23)</f>
+        <v>5074</v>
+      </c>
+      <c r="M24">
+        <f>SUM(M22:M23)</f>
+        <v>6028</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="16" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B25" s="16">
-        <v>10165</v>
+        <v>9637</v>
       </c>
       <c r="C25" s="16">
-        <v>10208</v>
+        <v>11112</v>
       </c>
       <c r="D25" s="16">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>1475</v>
       </c>
       <c r="E25">
-        <v>10186</v>
+        <v>11144</v>
       </c>
       <c r="F25" s="16">
-        <f>IF(B25 &gt;  0,E25-B25, 0)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <f t="shared" ref="F25:F27" si="2">IF(B25 &gt;  0,E25-B25, 0)</f>
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26">
-        <v>10254</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>95</v>
+      </c>
+      <c r="B26" s="16">
+        <v>9674</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="1"/>
+        <v>-9674</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B27" s="16">
-        <v>10733</v>
+        <v>9816</v>
       </c>
       <c r="C27" s="16">
-        <v>10777</v>
+        <v>11292</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>1476</v>
       </c>
       <c r="E27">
-        <v>10746</v>
+        <v>11325</v>
       </c>
       <c r="F27" s="16">
-        <f>IF(B27 &gt;  0,E27-B27, 0)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <f t="shared" si="2"/>
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28">
-        <v>10769</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="16" t="s">
-        <v>64</v>
+        <v>20</v>
+      </c>
+      <c r="B28" s="16">
+        <v>10327</v>
+      </c>
+      <c r="C28" s="16">
+        <v>11807</v>
+      </c>
+      <c r="D28" s="16">
+        <f t="shared" si="1"/>
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B29" s="16">
-        <v>11117</v>
+        <v>10626</v>
       </c>
       <c r="C29" s="16">
-        <v>11169</v>
+        <v>12118</v>
       </c>
       <c r="D29" s="16">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>1492</v>
       </c>
       <c r="E29">
-        <v>11144</v>
+        <v>12150</v>
       </c>
       <c r="F29" s="16">
-        <f t="shared" ref="F29:F34" si="2">IF(B29 &gt;  0,E29-B29, 0)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <f t="shared" ref="F29:F33" si="3">IF(B29 &gt;  0,E29-B29, 0)</f>
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="16">
-        <v>11298</v>
-      </c>
-      <c r="C30" s="16">
-        <v>11349</v>
+        <v>73</v>
       </c>
       <c r="D30" s="16">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>11325</v>
+        <v>12664</v>
       </c>
       <c r="F30" s="16">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="16">
-        <v>11439</v>
-      </c>
-      <c r="C31" s="16">
-        <v>11490</v>
+        <v>74</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>11466</v>
+        <v>13117</v>
       </c>
       <c r="F31" s="16">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="16">
-        <v>11491</v>
-      </c>
-      <c r="C32" s="16">
-        <v>11542</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="D32" s="16">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>11517</v>
+        <v>13361</v>
       </c>
       <c r="F32" s="16">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="16">
-        <v>11552</v>
-      </c>
-      <c r="C33" s="16">
-        <v>11606</v>
+        <v>76</v>
       </c>
       <c r="D33" s="16">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>11577</v>
+        <v>14325</v>
       </c>
       <c r="F33" s="16">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="16">
-        <v>11616</v>
-      </c>
-      <c r="C34" s="16">
-        <v>11672</v>
-      </c>
-      <c r="D34" s="16">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="E34">
-        <v>11644</v>
-      </c>
-      <c r="F34" s="16">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18.75">
+      <c r="A34" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="16">
-        <v>11626</v>
-      </c>
-      <c r="C35" s="16">
-        <v>11682</v>
-      </c>
-      <c r="D35" s="16">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
+      <c r="A35" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="16" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B36" s="16">
-        <v>11652</v>
+        <v>15202</v>
       </c>
       <c r="C36" s="16">
-        <v>11708</v>
+        <v>15292</v>
       </c>
       <c r="D36" s="16">
-        <f t="shared" si="1"/>
-        <v>56</v>
+        <f t="shared" ref="D36:D57" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <v>90</v>
       </c>
       <c r="E36">
-        <v>11680</v>
+        <v>15220</v>
       </c>
       <c r="F36" s="16">
-        <f t="shared" ref="F36:F42" si="3">IF(B36 &gt;  0,E36-B36, 0)</f>
-        <v>28</v>
+        <f t="shared" ref="F36:F47" si="5">IF(B36 &gt;  0,E36-B36, 0)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="16" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B37" s="16">
-        <v>11810</v>
+        <v>16484</v>
       </c>
       <c r="C37" s="16">
-        <v>11870</v>
+        <v>16574</v>
       </c>
       <c r="D37" s="16">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="E37">
-        <v>11839</v>
-      </c>
-      <c r="F37" s="16">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="16">
-        <v>12121</v>
+        <v>17011</v>
       </c>
       <c r="C38" s="16">
-        <v>12181</v>
+        <v>17101</v>
       </c>
       <c r="D38" s="16">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" si="4"/>
+        <v>90</v>
       </c>
       <c r="E38">
-        <v>12150</v>
+        <v>17027</v>
       </c>
       <c r="F38" s="16">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="16" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B39" s="16">
-        <v>12635</v>
+        <v>17525</v>
       </c>
       <c r="C39" s="16">
-        <v>12695</v>
+        <v>17615</v>
       </c>
       <c r="D39" s="16">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" si="4"/>
+        <v>90</v>
       </c>
       <c r="E39">
-        <v>12664</v>
+        <v>17541</v>
       </c>
       <c r="F39" s="16">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="16" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B40" s="16">
-        <v>13099</v>
+        <v>18058</v>
       </c>
       <c r="C40" s="16">
-        <v>13187</v>
+        <v>18298</v>
       </c>
       <c r="D40" s="16">
-        <f t="shared" si="1"/>
-        <v>88</v>
+        <f t="shared" si="4"/>
+        <v>240</v>
       </c>
       <c r="E40">
-        <v>13117</v>
+        <v>18074</v>
       </c>
       <c r="F40" s="16">
-        <f t="shared" si="3"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="16">
-        <v>13343</v>
-      </c>
-      <c r="C41" s="16">
-        <v>13431</v>
-      </c>
-      <c r="D41" s="16">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="E41">
-        <v>13361</v>
-      </c>
-      <c r="F41" s="16">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
+      <c r="A41" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B42" s="16">
-        <v>14307</v>
+        <v>18356</v>
       </c>
       <c r="C42" s="16">
-        <v>14395</v>
+        <v>18596</v>
       </c>
       <c r="D42" s="16">
-        <f t="shared" si="1"/>
-        <v>88</v>
+        <f t="shared" si="4"/>
+        <v>240</v>
       </c>
       <c r="E42">
-        <v>14325</v>
+        <v>18372</v>
       </c>
       <c r="F42" s="16">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18.75">
-      <c r="A43" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="16">
+        <v>18742</v>
+      </c>
+      <c r="C43" s="16">
+        <v>18982</v>
+      </c>
+      <c r="D43" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E43">
+        <v>18758</v>
+      </c>
+      <c r="F43" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="22"/>
+      <c r="A44" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="16">
+        <v>18974</v>
+      </c>
+      <c r="C44" s="16">
+        <v>19214</v>
+      </c>
+      <c r="D44" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E44">
+        <v>18990</v>
+      </c>
+      <c r="F44" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="16" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B45" s="16">
-        <v>15202</v>
+        <v>19152</v>
       </c>
       <c r="C45" s="16">
-        <v>15292</v>
+        <v>19392</v>
       </c>
       <c r="D45" s="16">
-        <f t="shared" ref="D45:D66" si="4">IF(B45 &gt;  0,C45-B45, 0)</f>
-        <v>90</v>
+        <f t="shared" si="4"/>
+        <v>240</v>
       </c>
       <c r="E45">
-        <v>15220</v>
+        <v>19168</v>
       </c>
       <c r="F45" s="16">
-        <f t="shared" ref="F45:F56" si="5">IF(B45 &gt;  0,E45-B45, 0)</f>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="16" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B46" s="16">
-        <v>16484</v>
+        <v>19206</v>
       </c>
       <c r="C46" s="16">
-        <v>16574</v>
+        <v>19447</v>
       </c>
       <c r="D46" s="16">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>241</v>
+      </c>
+      <c r="E46">
+        <v>19223</v>
+      </c>
+      <c r="F46" s="16">
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="16" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B47" s="16">
-        <v>17011</v>
+        <v>19281</v>
       </c>
       <c r="C47" s="16">
-        <v>17101</v>
+        <v>19522</v>
       </c>
       <c r="D47" s="16">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>241</v>
       </c>
       <c r="E47">
-        <v>17027</v>
+        <v>19299</v>
       </c>
       <c r="F47" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B48" s="16">
-        <v>17525</v>
+        <v>19350</v>
       </c>
       <c r="C48" s="16">
-        <v>17615</v>
+        <v>19591</v>
       </c>
       <c r="D48" s="16">
         <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-      <c r="E48">
-        <v>17541</v>
-      </c>
-      <c r="F48" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="16" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B49" s="16">
-        <v>18058</v>
+        <v>19374</v>
       </c>
       <c r="C49" s="16">
-        <v>18298</v>
+        <v>19615</v>
       </c>
       <c r="D49" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
-      </c>
-      <c r="E49">
-        <v>18074</v>
-      </c>
-      <c r="F49" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="22"/>
+      <c r="A50" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="16">
+        <v>19461</v>
+      </c>
+      <c r="C50" s="16">
+        <v>19703</v>
+      </c>
+      <c r="D50" s="16">
+        <f t="shared" si="4"/>
+        <v>242</v>
+      </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="16" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B51" s="16">
-        <v>18356</v>
+        <v>19706</v>
       </c>
       <c r="C51" s="16">
-        <v>18596</v>
+        <v>19949</v>
       </c>
       <c r="D51" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
-      </c>
-      <c r="E51">
-        <v>18372</v>
-      </c>
-      <c r="F51" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="16" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B52" s="16">
-        <v>18742</v>
+        <v>20114</v>
       </c>
       <c r="C52" s="16">
-        <v>18982</v>
+        <v>20359</v>
       </c>
       <c r="D52" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
-      </c>
-      <c r="E52">
-        <v>18758</v>
-      </c>
-      <c r="F52" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="16" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B53" s="16">
-        <v>18974</v>
+        <v>20117</v>
       </c>
       <c r="C53" s="16">
-        <v>19214</v>
+        <v>20363</v>
       </c>
       <c r="D53" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
-      </c>
-      <c r="E53">
-        <v>18990</v>
-      </c>
-      <c r="F53" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="16" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B54" s="16">
-        <v>19152</v>
+        <v>20257</v>
       </c>
       <c r="C54" s="16">
-        <v>19392</v>
+        <v>20512</v>
       </c>
       <c r="D54" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
-      </c>
-      <c r="E54">
-        <v>19168</v>
-      </c>
-      <c r="F54" s="16">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="16" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="B55" s="16">
-        <v>19206</v>
+        <v>20537</v>
       </c>
       <c r="C55" s="16">
-        <v>19447</v>
+        <v>20832</v>
       </c>
       <c r="D55" s="16">
         <f t="shared" si="4"/>
-        <v>241</v>
+        <v>295</v>
       </c>
       <c r="E55">
-        <v>19223</v>
+        <v>20600</v>
       </c>
       <c r="F55" s="16">
-        <f t="shared" si="5"/>
-        <v>17</v>
+        <f t="shared" ref="F55:F57" si="6">IF(B55 &gt;  0,E55-B55, 0)</f>
+        <v>63</v>
+      </c>
+      <c r="G55" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="16" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="B56" s="16">
-        <v>19281</v>
+        <v>21051</v>
       </c>
       <c r="C56" s="16">
-        <v>19522</v>
+        <v>21346</v>
       </c>
       <c r="D56" s="16">
         <f t="shared" si="4"/>
-        <v>241</v>
+        <v>295</v>
       </c>
       <c r="E56">
-        <v>19299</v>
+        <v>21114</v>
       </c>
       <c r="F56" s="16">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>63</v>
+      </c>
+      <c r="G56" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="16" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B57" s="16">
-        <v>19350</v>
+        <v>21617</v>
       </c>
       <c r="C57" s="16">
-        <v>19591</v>
+        <v>22007</v>
       </c>
       <c r="D57" s="16">
         <f t="shared" si="4"/>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" s="16">
-        <v>19374</v>
-      </c>
-      <c r="C58" s="16">
-        <v>19615</v>
-      </c>
-      <c r="D58" s="16">
-        <f t="shared" si="4"/>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="16">
-        <v>19461</v>
-      </c>
-      <c r="C59" s="16">
-        <v>19703</v>
-      </c>
-      <c r="D59" s="16">
-        <f t="shared" si="4"/>
-        <v>242</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="16">
-        <v>19706</v>
-      </c>
-      <c r="C60" s="16">
-        <v>19949</v>
-      </c>
-      <c r="D60" s="16">
-        <f t="shared" si="4"/>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" s="16">
-        <v>20114</v>
-      </c>
-      <c r="C61" s="16">
-        <v>20359</v>
-      </c>
-      <c r="D61" s="16">
-        <f t="shared" si="4"/>
-        <v>245</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B62" s="16">
-        <v>20117</v>
-      </c>
-      <c r="C62" s="16">
-        <v>20363</v>
-      </c>
-      <c r="D62" s="16">
-        <f t="shared" si="4"/>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B63" s="16">
-        <v>20257</v>
-      </c>
-      <c r="C63" s="16">
-        <v>20512</v>
-      </c>
-      <c r="D63" s="16">
-        <f t="shared" si="4"/>
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B64" s="16">
-        <v>20537</v>
-      </c>
-      <c r="C64" s="16">
-        <v>20832</v>
-      </c>
-      <c r="D64" s="16">
-        <f t="shared" si="4"/>
-        <v>295</v>
-      </c>
-      <c r="E64">
-        <v>20600</v>
-      </c>
-      <c r="F64" s="16">
-        <f t="shared" ref="F64:F66" si="6">IF(B64 &gt;  0,E64-B64, 0)</f>
-        <v>63</v>
-      </c>
-      <c r="G64" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B65" s="16">
-        <v>21051</v>
-      </c>
-      <c r="C65" s="16">
-        <v>21346</v>
-      </c>
-      <c r="D65" s="16">
-        <f t="shared" si="4"/>
-        <v>295</v>
-      </c>
-      <c r="E65">
-        <v>21114</v>
-      </c>
-      <c r="F65" s="16">
-        <f t="shared" si="6"/>
-        <v>63</v>
-      </c>
-      <c r="G65" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B66" s="16">
-        <v>21617</v>
-      </c>
-      <c r="C66" s="16">
-        <v>22007</v>
-      </c>
-      <c r="D66" s="16">
-        <f t="shared" si="4"/>
         <v>390</v>
       </c>
-      <c r="E66">
+      <c r="E57">
         <v>21615</v>
       </c>
-      <c r="F66" s="16">
+      <c r="F57" s="16">
         <f t="shared" si="6"/>
         <v>-2</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G57" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2024,7 +1872,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A34:F34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
NSMB - World 5 begin
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>1-1</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>Checkpoint</t>
+  </si>
+  <si>
+    <t>Me</t>
   </si>
 </sst>
 </file>
@@ -798,8 +801,8 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1086,6 +1089,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="20" t="s">
@@ -1097,6 +1101,7 @@
       <c r="E16" s="21"/>
       <c r="F16" s="20"/>
       <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="16" t="s">
@@ -1112,6 +1117,8 @@
         <f t="shared" si="1"/>
         <v>880</v>
       </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="16" t="s">
@@ -1127,6 +1134,8 @@
         <f t="shared" si="1"/>
         <v>903</v>
       </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="16" t="s">
@@ -1142,6 +1151,8 @@
         <f t="shared" si="1"/>
         <v>919</v>
       </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="16" t="s">
@@ -1154,6 +1165,7 @@
         <f t="shared" si="1"/>
         <v>-7351</v>
       </c>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="16" t="s">
@@ -1363,16 +1375,19 @@
       <c r="A30" s="16" t="s">
         <v>73</v>
       </c>
+      <c r="B30" s="16">
+        <v>11140</v>
+      </c>
       <c r="D30" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-11140</v>
       </c>
       <c r="E30">
         <v>12664</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -1395,35 +1410,41 @@
       <c r="A32" s="16" t="s">
         <v>56</v>
       </c>
+      <c r="B32" s="16">
+        <v>11592</v>
+      </c>
       <c r="D32" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-11592</v>
       </c>
       <c r="E32">
         <v>13361</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>76</v>
       </c>
+      <c r="B33" s="16">
+        <v>12540</v>
+      </c>
       <c r="D33" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-12540</v>
       </c>
       <c r="E33">
         <v>14325</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="18.75">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18.75">
       <c r="A34" s="28" t="s">
         <v>77</v>
       </c>
@@ -1433,7 +1454,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:8">
       <c r="A35" s="24" t="s">
         <v>78</v>
       </c>
@@ -1442,111 +1463,123 @@
       <c r="D35" s="22"/>
       <c r="E35" s="23"/>
       <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="16">
-        <v>15202</v>
-      </c>
-      <c r="C36" s="16">
-        <v>15292</v>
+        <v>12987</v>
       </c>
       <c r="D36" s="16">
         <f t="shared" ref="D36:D57" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
-        <v>90</v>
+        <v>-12987</v>
       </c>
       <c r="E36">
         <v>15220</v>
       </c>
       <c r="F36" s="16">
         <f t="shared" ref="F36:F47" si="5">IF(B36 &gt;  0,E36-B36, 0)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>2233</v>
+      </c>
+      <c r="G36" s="16">
+        <v>15202</v>
+      </c>
+      <c r="H36" s="16">
+        <v>15292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B37" s="16">
+        <v>13217</v>
+      </c>
+      <c r="D37" s="16">
+        <f t="shared" si="4"/>
+        <v>-13217</v>
+      </c>
+      <c r="G37" s="16">
         <v>16484</v>
       </c>
-      <c r="C37" s="16">
+      <c r="H37" s="16">
         <v>16574</v>
       </c>
-      <c r="D37" s="16">
-        <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="16">
-        <v>17011</v>
-      </c>
-      <c r="C38" s="16">
-        <v>17101</v>
-      </c>
       <c r="D38" s="16">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>17027</v>
       </c>
       <c r="F38" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G38" s="16">
+        <v>17011</v>
+      </c>
+      <c r="H38" s="16">
+        <v>17101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="16">
-        <v>17525</v>
-      </c>
-      <c r="C39" s="16">
-        <v>17615</v>
-      </c>
       <c r="D39" s="16">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>17541</v>
       </c>
       <c r="F39" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G39" s="16">
+        <v>17525</v>
+      </c>
+      <c r="H39" s="16">
+        <v>17615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="16">
-        <v>18058</v>
-      </c>
-      <c r="C40" s="16">
-        <v>18298</v>
-      </c>
       <c r="D40" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>18074</v>
       </c>
       <c r="F40" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G40" s="16">
+        <v>18058</v>
+      </c>
+      <c r="H40" s="16">
+        <v>18298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="24" t="s">
         <v>94</v>
       </c>
@@ -1555,317 +1588,310 @@
       <c r="D41" s="22"/>
       <c r="E41" s="23"/>
       <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="16">
-        <v>18356</v>
-      </c>
-      <c r="C42" s="16">
-        <v>18596</v>
-      </c>
       <c r="D42" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>18372</v>
       </c>
       <c r="F42" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G42" s="16">
+        <v>18356</v>
+      </c>
+      <c r="H42" s="16">
+        <v>18596</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="16">
-        <v>18742</v>
-      </c>
-      <c r="C43" s="16">
-        <v>18982</v>
-      </c>
       <c r="D43" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>18758</v>
       </c>
       <c r="F43" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16">
+        <v>18742</v>
+      </c>
+      <c r="H43" s="16">
+        <v>18982</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="16">
-        <v>18974</v>
-      </c>
-      <c r="C44" s="16">
-        <v>19214</v>
-      </c>
       <c r="D44" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>18990</v>
       </c>
       <c r="F44" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G44" s="16">
+        <v>18974</v>
+      </c>
+      <c r="H44" s="16">
+        <v>19214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="16">
-        <v>19152</v>
-      </c>
-      <c r="C45" s="16">
-        <v>19392</v>
-      </c>
       <c r="D45" s="16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>19168</v>
       </c>
       <c r="F45" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G45" s="16">
+        <v>19152</v>
+      </c>
+      <c r="H45" s="16">
+        <v>19392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="16">
-        <v>19206</v>
-      </c>
-      <c r="C46" s="16">
-        <v>19447</v>
-      </c>
       <c r="D46" s="16">
         <f t="shared" si="4"/>
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>19223</v>
       </c>
       <c r="F46" s="16">
         <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G46" s="16">
+        <v>19206</v>
+      </c>
+      <c r="H46" s="16">
+        <v>19447</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="16">
-        <v>19281</v>
-      </c>
-      <c r="C47" s="16">
-        <v>19522</v>
-      </c>
       <c r="D47" s="16">
         <f t="shared" si="4"/>
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>19299</v>
       </c>
       <c r="F47" s="16">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <v>19281</v>
+      </c>
+      <c r="H47" s="16">
+        <v>19522</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="16">
+      <c r="D48" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="16">
         <v>19350</v>
       </c>
-      <c r="C48" s="16">
+      <c r="H48" s="16">
         <v>19591</v>
       </c>
-      <c r="D48" s="16">
-        <f t="shared" si="4"/>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="16">
+      <c r="D49" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="16">
         <v>19374</v>
       </c>
-      <c r="C49" s="16">
+      <c r="H49" s="16">
         <v>19615</v>
       </c>
-      <c r="D49" s="16">
-        <f t="shared" si="4"/>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="16">
+      <c r="D50" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="16">
         <v>19461</v>
       </c>
-      <c r="C50" s="16">
+      <c r="H50" s="16">
         <v>19703</v>
       </c>
-      <c r="D50" s="16">
-        <f t="shared" si="4"/>
-        <v>242</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="16">
+      <c r="D51" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="16">
         <v>19706</v>
       </c>
-      <c r="C51" s="16">
+      <c r="H51" s="16">
         <v>19949</v>
       </c>
-      <c r="D51" s="16">
-        <f t="shared" si="4"/>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="16">
+      <c r="D52" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="16">
         <v>20114</v>
       </c>
-      <c r="C52" s="16">
+      <c r="H52" s="16">
         <v>20359</v>
       </c>
-      <c r="D52" s="16">
-        <f t="shared" si="4"/>
-        <v>245</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="16">
+      <c r="D53" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="16">
         <v>20117</v>
       </c>
-      <c r="C53" s="16">
+      <c r="H53" s="16">
         <v>20363</v>
       </c>
-      <c r="D53" s="16">
-        <f t="shared" si="4"/>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="16">
+      <c r="D54" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="16">
         <v>20257</v>
       </c>
-      <c r="C54" s="16">
+      <c r="H54" s="16">
         <v>20512</v>
       </c>
-      <c r="D54" s="16">
-        <f t="shared" si="4"/>
-        <v>255</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="16">
-        <v>20537</v>
-      </c>
-      <c r="C55" s="16">
-        <v>20832</v>
-      </c>
       <c r="D55" s="16">
         <f t="shared" si="4"/>
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="E55">
         <v>20600</v>
       </c>
       <c r="F55" s="16">
         <f t="shared" ref="F55:F57" si="6">IF(B55 &gt;  0,E55-B55, 0)</f>
-        <v>63</v>
-      </c>
-      <c r="G55" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="G55" s="16">
+        <v>20537</v>
+      </c>
+      <c r="H55" s="16">
+        <v>20832</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="16">
-        <v>21051</v>
-      </c>
-      <c r="C56" s="16">
-        <v>21346</v>
-      </c>
       <c r="D56" s="16">
         <f t="shared" si="4"/>
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>21114</v>
       </c>
       <c r="F56" s="16">
         <f t="shared" si="6"/>
-        <v>63</v>
-      </c>
-      <c r="G56" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="G56" s="16">
+        <v>21051</v>
+      </c>
+      <c r="H56" s="16">
+        <v>21346</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="16">
-        <v>21617</v>
-      </c>
-      <c r="C57" s="16">
-        <v>22007</v>
-      </c>
       <c r="D57" s="16">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>21615</v>
       </c>
       <c r="F57" s="16">
         <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="G57" t="s">
-        <v>98</v>
+        <v>0</v>
+      </c>
+      <c r="G57" s="16">
+        <v>21617</v>
+      </c>
+      <c r="H57" s="16">
+        <v>22007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 5-1 Done except for possible map manipulation.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -801,8 +801,8 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1186,14 +1186,14 @@
       <c r="E22" s="21"/>
       <c r="F22" s="20"/>
       <c r="I22" s="13">
-        <v>9852</v>
+        <v>13217</v>
       </c>
       <c r="J22" s="13">
-        <v>11335</v>
+        <v>15452</v>
       </c>
       <c r="K22" s="13">
         <f>J22-I22</f>
-        <v>1483</v>
+        <v>2235</v>
       </c>
       <c r="L22" s="13">
         <v>5057</v>
@@ -1263,11 +1263,11 @@
       </c>
       <c r="I24">
         <f>SUM(I22:I23)</f>
-        <v>9869</v>
+        <v>13234</v>
       </c>
       <c r="J24">
         <f>SUM(J22:J23)</f>
-        <v>11344</v>
+        <v>15461</v>
       </c>
       <c r="L24">
         <f>SUM(L22:L23)</f>
@@ -1502,9 +1502,12 @@
       <c r="B37" s="16">
         <v>13217</v>
       </c>
+      <c r="C37" s="16">
+        <v>15452</v>
+      </c>
       <c r="D37" s="16">
         <f t="shared" si="4"/>
-        <v>-13217</v>
+        <v>2235</v>
       </c>
       <c r="G37" s="16">
         <v>16484</v>

</xml_diff>

<commit_message>
NSMB - a version of 5-2 but it gets 336 on the timer because I sacrificed one trying to get hit the ? block so it wouldn't be on the map anymore.  Time to find a frame somewhere.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="111">
   <si>
     <t>1-1</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>Me</t>
+  </si>
+  <si>
+    <t>Enter 5-2</t>
+  </si>
+  <si>
+    <t>1st move</t>
   </si>
 </sst>
 </file>
@@ -801,8 +807,8 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1186,14 +1192,14 @@
       <c r="E22" s="21"/>
       <c r="F22" s="20"/>
       <c r="I22" s="13">
-        <v>13217</v>
+        <v>16243</v>
       </c>
       <c r="J22" s="13">
-        <v>15452</v>
+        <v>18855</v>
       </c>
       <c r="K22" s="13">
         <f>J22-I22</f>
-        <v>2235</v>
+        <v>2612</v>
       </c>
       <c r="L22" s="13">
         <v>5057</v>
@@ -1263,11 +1269,11 @@
       </c>
       <c r="I24">
         <f>SUM(I22:I23)</f>
-        <v>13234</v>
+        <v>16260</v>
       </c>
       <c r="J24">
         <f>SUM(J22:J23)</f>
-        <v>15461</v>
+        <v>18864</v>
       </c>
       <c r="L24">
         <f>SUM(L22:L23)</f>
@@ -1520,16 +1526,19 @@
       <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="B38" s="16">
+        <v>14776</v>
+      </c>
       <c r="D38" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-14776</v>
       </c>
       <c r="E38">
         <v>17027</v>
       </c>
       <c r="F38" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2251</v>
       </c>
       <c r="G38" s="16">
         <v>17011</v>
@@ -1596,18 +1605,21 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="16" t="s">
-        <v>79</v>
+        <v>109</v>
+      </c>
+      <c r="B42" s="16">
+        <v>15781</v>
       </c>
       <c r="D42" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-15781</v>
       </c>
       <c r="E42">
         <v>18372</v>
       </c>
       <c r="F42" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2591</v>
       </c>
       <c r="G42" s="16">
         <v>18356</v>
@@ -1620,16 +1632,19 @@
       <c r="A43" s="16" t="s">
         <v>20</v>
       </c>
+      <c r="B43" s="16">
+        <v>16148</v>
+      </c>
       <c r="D43" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-16148</v>
       </c>
       <c r="E43">
         <v>18758</v>
       </c>
       <c r="F43" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2610</v>
       </c>
       <c r="G43" s="16">
         <v>18742</v>
@@ -1640,7 +1655,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="16" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D44" s="16">
         <f t="shared" si="4"/>
@@ -1653,12 +1668,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G44" s="16">
-        <v>18974</v>
-      </c>
-      <c r="H44" s="16">
-        <v>19214</v>
-      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="16" t="s">
@@ -1820,9 +1831,12 @@
       <c r="A54" s="16" t="s">
         <v>20</v>
       </c>
+      <c r="B54" s="16">
+        <v>17646</v>
+      </c>
       <c r="D54" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-17646</v>
       </c>
       <c r="G54" s="16">
         <v>20257</v>
@@ -1835,16 +1849,19 @@
       <c r="A55" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="B55" s="16">
+        <v>17913</v>
+      </c>
       <c r="D55" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-17913</v>
       </c>
       <c r="E55">
         <v>20600</v>
       </c>
       <c r="F55" s="16">
         <f t="shared" ref="F55:F57" si="6">IF(B55 &gt;  0,E55-B55, 0)</f>
-        <v>0</v>
+        <v>2687</v>
       </c>
       <c r="G55" s="16">
         <v>20537</v>

</xml_diff>

<commit_message>
NSMB - 5-2 - 6 frames saved in 5-2 thanks to terrotim.  Now comes the fun part, getting that hammer bros at the ghost house after 5-3.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
   <si>
     <t>1-1</t>
   </si>
@@ -349,7 +349,28 @@
     <t>Enter 5-2</t>
   </si>
   <si>
-    <t>1st move</t>
+    <t>Map First move</t>
+  </si>
+  <si>
+    <t>Checkpoint 9</t>
+  </si>
+  <si>
+    <t>Checkpoitn Rail 460xxxxx</t>
+  </si>
+  <si>
+    <t>Checkpoint 995</t>
+  </si>
+  <si>
+    <t>Checkpoint 1500</t>
+  </si>
+  <si>
+    <t>Checkpoint 2107/2106</t>
+  </si>
+  <si>
+    <t>Checkpoint 3094/3093</t>
+  </si>
+  <si>
+    <t>Checkpoint 3442</t>
   </si>
 </sst>
 </file>
@@ -804,11 +825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1483,9 +1504,12 @@
       <c r="B36" s="16">
         <v>12987</v>
       </c>
+      <c r="C36" s="16">
+        <v>15235</v>
+      </c>
       <c r="D36" s="16">
-        <f t="shared" ref="D36:D57" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
-        <v>-12987</v>
+        <f t="shared" ref="D36:D55" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <v>2248</v>
       </c>
       <c r="E36">
         <v>15220</v>
@@ -1509,11 +1533,11 @@
         <v>13217</v>
       </c>
       <c r="C37" s="16">
-        <v>15452</v>
+        <v>15489</v>
       </c>
       <c r="D37" s="16">
         <f t="shared" si="4"/>
-        <v>2235</v>
+        <v>2272</v>
       </c>
       <c r="G37" s="16">
         <v>16484</v>
@@ -1529,9 +1553,12 @@
       <c r="B38" s="16">
         <v>14776</v>
       </c>
+      <c r="C38" s="16">
+        <v>17048</v>
+      </c>
       <c r="D38" s="16">
         <f t="shared" si="4"/>
-        <v>-14776</v>
+        <v>2272</v>
       </c>
       <c r="E38">
         <v>17027</v>
@@ -1551,16 +1578,22 @@
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
+      <c r="B39" s="16">
+        <v>15290</v>
+      </c>
+      <c r="C39" s="16">
+        <v>17562</v>
+      </c>
       <c r="D39" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2272</v>
       </c>
       <c r="E39">
         <v>17541</v>
       </c>
       <c r="F39" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2251</v>
       </c>
       <c r="G39" s="16">
         <v>17525</v>
@@ -1571,18 +1604,24 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="16" t="s">
-        <v>51</v>
+        <v>110</v>
+      </c>
+      <c r="B40" s="16">
+        <v>15631</v>
+      </c>
+      <c r="C40" s="16">
+        <v>18105</v>
       </c>
       <c r="D40" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2474</v>
       </c>
       <c r="E40">
         <v>18074</v>
       </c>
       <c r="F40" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2443</v>
       </c>
       <c r="G40" s="16">
         <v>18058</v>
@@ -1610,9 +1649,12 @@
       <c r="B42" s="16">
         <v>15781</v>
       </c>
+      <c r="C42" s="16">
+        <v>18403</v>
+      </c>
       <c r="D42" s="16">
         <f t="shared" si="4"/>
-        <v>-15781</v>
+        <v>2622</v>
       </c>
       <c r="E42">
         <v>18372</v>
@@ -1621,12 +1663,8 @@
         <f t="shared" si="5"/>
         <v>2591</v>
       </c>
-      <c r="G42" s="16">
-        <v>18356</v>
-      </c>
-      <c r="H42" s="16">
-        <v>18596</v>
-      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="16" t="s">
@@ -1635,9 +1673,12 @@
       <c r="B43" s="16">
         <v>16148</v>
       </c>
+      <c r="C43" s="16">
+        <v>18789</v>
+      </c>
       <c r="D43" s="16">
         <f t="shared" si="4"/>
-        <v>-16148</v>
+        <v>2641</v>
       </c>
       <c r="E43">
         <v>18758</v>
@@ -1646,273 +1687,243 @@
         <f t="shared" si="5"/>
         <v>2610</v>
       </c>
-      <c r="G43" s="16">
-        <v>18742</v>
-      </c>
-      <c r="H43" s="16">
-        <v>18982</v>
-      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="B44" s="16">
+        <v>16363</v>
+      </c>
+      <c r="C44" s="16">
+        <v>19022</v>
       </c>
       <c r="D44" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2659</v>
       </c>
       <c r="E44">
         <v>18990</v>
       </c>
       <c r="F44" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2627</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="16" t="s">
-        <v>85</v>
+        <v>112</v>
+      </c>
+      <c r="B45" s="16">
+        <v>16557</v>
+      </c>
+      <c r="C45" s="16">
+        <v>19216</v>
       </c>
       <c r="D45" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2659</v>
       </c>
       <c r="E45">
         <v>19168</v>
       </c>
       <c r="F45" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="16">
-        <v>19152</v>
-      </c>
-      <c r="H45" s="16">
-        <v>19392</v>
-      </c>
+        <v>2611</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="16" t="s">
-        <v>86</v>
+        <v>113</v>
+      </c>
+      <c r="B46" s="16">
+        <v>16685</v>
+      </c>
+      <c r="C46" s="16">
+        <v>19344</v>
       </c>
       <c r="D46" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2659</v>
       </c>
       <c r="E46">
         <v>19223</v>
       </c>
       <c r="F46" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="16">
-        <v>19206</v>
-      </c>
-      <c r="H46" s="16">
-        <v>19447</v>
-      </c>
+        <v>2538</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="16" t="s">
-        <v>87</v>
+        <v>114</v>
+      </c>
+      <c r="B47" s="16">
+        <v>16859</v>
+      </c>
+      <c r="C47" s="16">
+        <v>19523</v>
       </c>
       <c r="D47" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2664</v>
       </c>
       <c r="E47">
         <v>19299</v>
       </c>
       <c r="F47" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="16">
-        <v>19281</v>
-      </c>
-      <c r="H47" s="16">
-        <v>19522</v>
-      </c>
+        <v>2440</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="16" t="s">
-        <v>88</v>
+        <v>115</v>
+      </c>
+      <c r="B48" s="16">
+        <v>17061</v>
+      </c>
+      <c r="C48" s="16">
+        <v>19725</v>
       </c>
       <c r="D48" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="16">
-        <v>19350</v>
-      </c>
-      <c r="H48" s="16">
-        <v>19591</v>
-      </c>
+        <v>2664</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="16" t="s">
-        <v>89</v>
+        <v>116</v>
+      </c>
+      <c r="B49" s="16">
+        <v>17390</v>
+      </c>
+      <c r="C49" s="16">
+        <v>20054</v>
       </c>
       <c r="D49" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="16">
-        <v>19374</v>
-      </c>
-      <c r="H49" s="16">
-        <v>19615</v>
-      </c>
+        <v>2664</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="16" t="s">
-        <v>90</v>
+        <v>117</v>
+      </c>
+      <c r="B50" s="16">
+        <v>17549</v>
+      </c>
+      <c r="C50" s="16">
+        <v>20197</v>
       </c>
       <c r="D50" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="16">
-        <v>19461</v>
-      </c>
-      <c r="H50" s="16">
-        <v>19703</v>
-      </c>
+        <v>2648</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="16" t="s">
-        <v>91</v>
+        <v>20</v>
+      </c>
+      <c r="B51" s="16">
+        <v>17569</v>
+      </c>
+      <c r="C51" s="16">
+        <v>20233</v>
       </c>
       <c r="D51" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="16">
-        <v>19706</v>
-      </c>
-      <c r="H51" s="16">
-        <v>19949</v>
-      </c>
+        <v>2664</v>
+      </c>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="16" t="s">
-        <v>92</v>
+        <v>46</v>
+      </c>
+      <c r="B52" s="16">
+        <v>17640</v>
+      </c>
+      <c r="C52" s="16">
+        <v>20304</v>
       </c>
       <c r="D52" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G52" s="16">
-        <v>20114</v>
-      </c>
-      <c r="H52" s="16">
-        <v>20359</v>
-      </c>
+        <v>2664</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="16" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="D53" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G53" s="16">
-        <v>20117</v>
-      </c>
-      <c r="H53" s="16">
-        <v>20363</v>
-      </c>
+      <c r="E53">
+        <v>20600</v>
+      </c>
+      <c r="F53" s="16">
+        <f t="shared" ref="F53:F55" si="6">IF(B53 &gt;  0,E53-B53, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" s="16">
-        <v>17646</v>
+        <v>46</v>
       </c>
       <c r="D54" s="16">
         <f t="shared" si="4"/>
-        <v>-17646</v>
-      </c>
-      <c r="G54" s="16">
-        <v>20257</v>
-      </c>
-      <c r="H54" s="16">
-        <v>20512</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>21114</v>
+      </c>
+      <c r="F54" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="16">
-        <v>17913</v>
+        <v>95</v>
       </c>
       <c r="D55" s="16">
         <f t="shared" si="4"/>
-        <v>-17913</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>20600</v>
+        <v>21615</v>
       </c>
       <c r="F55" s="16">
-        <f t="shared" ref="F55:F57" si="6">IF(B55 &gt;  0,E55-B55, 0)</f>
-        <v>2687</v>
-      </c>
-      <c r="G55" s="16">
-        <v>20537</v>
-      </c>
-      <c r="H55" s="16">
-        <v>20832</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D56" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>21114</v>
-      </c>
-      <c r="F56" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G56" s="16">
-        <v>21051</v>
-      </c>
-      <c r="H56" s="16">
-        <v>21346</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>21615</v>
-      </c>
-      <c r="F57" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G57" s="16">
-        <v>21617</v>
-      </c>
-      <c r="H57" s="16">
-        <v>22007</v>
-      </c>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
NSMB - fix map movements after 5-1, lost 17 frames to luck manipluation.  TODO: copy/paste 5-2.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="122">
   <si>
     <t>1-1</t>
   </si>
@@ -371,6 +371,18 @@
   </si>
   <si>
     <t>Checkpoint 3442</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>WIN</t>
+  </si>
+  <si>
+    <t>15290 possible</t>
   </si>
 </sst>
 </file>
@@ -828,8 +840,8 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1452,7 +1464,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:11">
       <c r="A33" s="16" t="s">
         <v>76</v>
       </c>
@@ -1471,7 +1483,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="18.75">
+    <row r="34" spans="1:11" ht="18.75">
       <c r="A34" s="28" t="s">
         <v>77</v>
       </c>
@@ -1481,7 +1493,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:11">
       <c r="A35" s="24" t="s">
         <v>78</v>
       </c>
@@ -1496,8 +1508,14 @@
       <c r="H35" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="J35">
+        <v>76</v>
+      </c>
+      <c r="K35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -1524,8 +1542,14 @@
       <c r="H36" s="16">
         <v>15292</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="J36">
+        <v>77</v>
+      </c>
+      <c r="K36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="16" t="s">
         <v>95</v>
       </c>
@@ -1545,8 +1569,11 @@
       <c r="H37" s="16">
         <v>16574</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="J37">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
@@ -1573,27 +1600,33 @@
       <c r="H38" s="16">
         <v>17101</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="J38">
+        <v>79</v>
+      </c>
+      <c r="K38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="16">
-        <v>15290</v>
+        <v>15307</v>
       </c>
       <c r="C39" s="16">
         <v>17562</v>
       </c>
       <c r="D39" s="16">
         <f t="shared" si="4"/>
-        <v>2272</v>
+        <v>2255</v>
       </c>
       <c r="E39">
         <v>17541</v>
       </c>
       <c r="F39" s="16">
         <f t="shared" si="5"/>
-        <v>2251</v>
+        <v>2234</v>
       </c>
       <c r="G39" s="16">
         <v>17525</v>
@@ -1601,27 +1634,33 @@
       <c r="H39" s="16">
         <v>17615</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="s">
+        <v>121</v>
+      </c>
+      <c r="J39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="16" t="s">
         <v>110</v>
       </c>
       <c r="B40" s="16">
-        <v>15631</v>
+        <v>15573</v>
       </c>
       <c r="C40" s="16">
         <v>18105</v>
       </c>
       <c r="D40" s="16">
         <f t="shared" si="4"/>
-        <v>2474</v>
+        <v>2532</v>
       </c>
       <c r="E40">
         <v>18074</v>
       </c>
       <c r="F40" s="16">
         <f t="shared" si="5"/>
-        <v>2443</v>
+        <v>2501</v>
       </c>
       <c r="G40" s="16">
         <v>18058</v>
@@ -1629,8 +1668,11 @@
       <c r="H40" s="16">
         <v>18298</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="J40">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="24" t="s">
         <v>94</v>
       </c>
@@ -1641,32 +1683,43 @@
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="J41">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="16" t="s">
         <v>109</v>
       </c>
       <c r="B42" s="16">
-        <v>15781</v>
+        <v>15722</v>
       </c>
       <c r="C42" s="16">
         <v>18403</v>
       </c>
       <c r="D42" s="16">
         <f t="shared" si="4"/>
-        <v>2622</v>
+        <v>2681</v>
       </c>
       <c r="E42">
         <v>18372</v>
       </c>
       <c r="F42" s="16">
         <f t="shared" si="5"/>
-        <v>2591</v>
+        <v>2650</v>
       </c>
       <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="H42" s="16">
+        <v>15781</v>
+      </c>
+      <c r="J42">
+        <v>83</v>
+      </c>
+      <c r="K42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="16" t="s">
         <v>20</v>
       </c>
@@ -1689,8 +1742,11 @@
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="J43">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="16" t="s">
         <v>111</v>
       </c>
@@ -1713,8 +1769,14 @@
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="J44">
+        <v>85</v>
+      </c>
+      <c r="K44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="16" t="s">
         <v>112</v>
       </c>
@@ -1737,8 +1799,11 @@
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="J45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="16" t="s">
         <v>113</v>
       </c>
@@ -1761,8 +1826,11 @@
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="J46">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="16" t="s">
         <v>114</v>
       </c>
@@ -1785,8 +1853,11 @@
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="J47">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="16" t="s">
         <v>115</v>
       </c>
@@ -1802,8 +1873,11 @@
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="J48">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="16" t="s">
         <v>116</v>
       </c>
@@ -1819,8 +1893,11 @@
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="J49">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="16" t="s">
         <v>117</v>
       </c>
@@ -1836,8 +1913,11 @@
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="J50">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="16" t="s">
         <v>20</v>
       </c>
@@ -1853,8 +1933,14 @@
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="J51">
+        <v>92</v>
+      </c>
+      <c r="K51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="16" t="s">
         <v>46</v>
       </c>
@@ -1870,8 +1956,20 @@
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52">
+        <v>95090</v>
+      </c>
+      <c r="J52">
+        <v>93</v>
+      </c>
+      <c r="K52" t="s">
+        <v>120</v>
+      </c>
+      <c r="L52">
+        <v>94790</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="16" t="s">
         <v>45</v>
       </c>
@@ -1889,7 +1987,7 @@
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:12">
       <c r="A54" s="16" t="s">
         <v>46</v>
       </c>
@@ -1907,7 +2005,7 @@
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:12">
       <c r="A55" s="16" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
NSMB - 5-3 done, 5-G up to manipulating the mini-mushroom done.  3837 ahead of TRT's movie including all the emulation lag differences.  Without those lag differences, I no longer have any idea how much ahead.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="135">
   <si>
     <t>1-1</t>
   </si>
@@ -383,6 +383,45 @@
   </si>
   <si>
     <t>15290 possible</t>
+  </si>
+  <si>
+    <t>Enter 5-3</t>
+  </si>
+  <si>
+    <t>Checkpoint 2676</t>
+  </si>
+  <si>
+    <t>Checkpoint 2869</t>
+  </si>
+  <si>
+    <t>Checkpoint 3080</t>
+  </si>
+  <si>
+    <t>Checkpoint 3355/3356</t>
+  </si>
+  <si>
+    <t>Checkpoint 3484/3485</t>
+  </si>
+  <si>
+    <t>Checkpoint 3692/3693</t>
+  </si>
+  <si>
+    <t>Level end</t>
+  </si>
+  <si>
+    <t>Enter 5-G</t>
+  </si>
+  <si>
+    <t>1st move</t>
+  </si>
+  <si>
+    <t>Hit block</t>
+  </si>
+  <si>
+    <t>Checkpoint 10400</t>
+  </si>
+  <si>
+    <t>Get mini-mario</t>
   </si>
 </sst>
 </file>
@@ -837,11 +876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1350,6 +1389,12 @@
         <f t="shared" si="1"/>
         <v>-9674</v>
       </c>
+      <c r="I26">
+        <v>16182</v>
+      </c>
+      <c r="J26">
+        <v>16243</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="16" t="s">
@@ -1526,7 +1571,7 @@
         <v>15235</v>
       </c>
       <c r="D36" s="16">
-        <f t="shared" ref="D36:D55" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <f t="shared" ref="D36:D69" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
         <v>2248</v>
       </c>
       <c r="E36">
@@ -2022,6 +2067,224 @@
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="16">
+        <v>18945</v>
+      </c>
+      <c r="C56" s="16">
+        <v>22185</v>
+      </c>
+      <c r="D56" s="16">
+        <f t="shared" si="4"/>
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" s="16">
+        <v>19177</v>
+      </c>
+      <c r="C57" s="16">
+        <v>22443</v>
+      </c>
+      <c r="D57" s="16">
+        <f t="shared" si="4"/>
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="16">
+        <v>20120</v>
+      </c>
+      <c r="C58" s="16">
+        <v>23386</v>
+      </c>
+      <c r="D58" s="16">
+        <f t="shared" si="4"/>
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="16">
+        <v>20187</v>
+      </c>
+      <c r="C59" s="16">
+        <v>23453</v>
+      </c>
+      <c r="D59" s="16">
+        <f t="shared" si="4"/>
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="16">
+        <v>20258</v>
+      </c>
+      <c r="C60" s="16">
+        <v>23524</v>
+      </c>
+      <c r="D60" s="16">
+        <f t="shared" si="4"/>
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="16">
+        <v>20351</v>
+      </c>
+      <c r="C61" s="16">
+        <v>23618</v>
+      </c>
+      <c r="D61" s="16">
+        <f t="shared" si="4"/>
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="16">
+        <v>20394</v>
+      </c>
+      <c r="C62" s="16">
+        <v>23661</v>
+      </c>
+      <c r="D62" s="16">
+        <f t="shared" si="4"/>
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" s="16">
+        <v>20465</v>
+      </c>
+      <c r="C63" s="16">
+        <v>23733</v>
+      </c>
+      <c r="D63" s="16">
+        <f t="shared" si="4"/>
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="16">
+        <v>20658</v>
+      </c>
+      <c r="C64" s="16">
+        <v>23926</v>
+      </c>
+      <c r="D64" s="16">
+        <f t="shared" si="4"/>
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" s="16">
+        <v>21172</v>
+      </c>
+      <c r="C65" s="16">
+        <v>24440</v>
+      </c>
+      <c r="D65" s="16">
+        <f t="shared" si="4"/>
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="16">
+        <v>21661</v>
+      </c>
+      <c r="C66" s="16">
+        <v>25475</v>
+      </c>
+      <c r="D66" s="16">
+        <f t="shared" si="4"/>
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="16">
+        <v>21890</v>
+      </c>
+      <c r="C67" s="16">
+        <v>25726</v>
+      </c>
+      <c r="D67" s="16">
+        <f t="shared" si="4"/>
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="16">
+        <v>21929</v>
+      </c>
+      <c r="C68" s="16">
+        <v>25765</v>
+      </c>
+      <c r="D68" s="16">
+        <f t="shared" si="4"/>
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="16">
+        <v>21995</v>
+      </c>
+      <c r="C69" s="16">
+        <v>25832</v>
+      </c>
+      <c r="D69" s="16">
+        <f t="shared" si="4"/>
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="16">
+        <v>25957</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
NSMB - got a mini-mushroom!
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="136">
   <si>
     <t>1-1</t>
   </si>
@@ -373,15 +373,6 @@
     <t>Checkpoint 3442</t>
   </si>
   <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>WIN</t>
-  </si>
-  <si>
     <t>15290 possible</t>
   </si>
   <si>
@@ -422,13 +413,25 @@
   </si>
   <si>
     <t>Get mini-mario</t>
+  </si>
+  <si>
+    <t>Hit HB</t>
+  </si>
+  <si>
+    <t>Fireflower</t>
+  </si>
+  <si>
+    <t>Score:</t>
+  </si>
+  <si>
+    <t>Bshell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,6 +449,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -537,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -582,6 +593,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,11 +889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1509,7 +1522,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:9">
       <c r="A33" s="16" t="s">
         <v>76</v>
       </c>
@@ -1528,7 +1541,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18.75">
+    <row r="34" spans="1:9" ht="18.75">
       <c r="A34" s="28" t="s">
         <v>77</v>
       </c>
@@ -1538,7 +1551,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:9">
       <c r="A35" s="24" t="s">
         <v>78</v>
       </c>
@@ -1553,14 +1566,8 @@
       <c r="H35" t="s">
         <v>59</v>
       </c>
-      <c r="J35">
-        <v>76</v>
-      </c>
-      <c r="K35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>15235</v>
       </c>
       <c r="D36" s="16">
-        <f t="shared" ref="D36:D69" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <f t="shared" ref="D36:D70" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
         <v>2248</v>
       </c>
       <c r="E36">
@@ -1587,14 +1594,8 @@
       <c r="H36" s="16">
         <v>15292</v>
       </c>
-      <c r="J36">
-        <v>77</v>
-      </c>
-      <c r="K36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="16" t="s">
         <v>95</v>
       </c>
@@ -1614,11 +1615,8 @@
       <c r="H37" s="16">
         <v>16574</v>
       </c>
-      <c r="J37">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
@@ -1645,14 +1643,8 @@
       <c r="H38" s="16">
         <v>17101</v>
       </c>
-      <c r="J38">
-        <v>79</v>
-      </c>
-      <c r="K38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -1680,13 +1672,10 @@
         <v>17615</v>
       </c>
       <c r="I39" t="s">
-        <v>121</v>
-      </c>
-      <c r="J39">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="16" t="s">
         <v>110</v>
       </c>
@@ -1713,11 +1702,8 @@
       <c r="H40" s="16">
         <v>18298</v>
       </c>
-      <c r="J40">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="24" t="s">
         <v>94</v>
       </c>
@@ -1728,11 +1714,8 @@
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-      <c r="J41">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="16" t="s">
         <v>109</v>
       </c>
@@ -1757,14 +1740,8 @@
       <c r="H42" s="16">
         <v>15781</v>
       </c>
-      <c r="J42">
-        <v>83</v>
-      </c>
-      <c r="K42" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="16" t="s">
         <v>20</v>
       </c>
@@ -1787,11 +1764,8 @@
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
-      <c r="J43">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="16" t="s">
         <v>111</v>
       </c>
@@ -1814,14 +1788,8 @@
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
-      <c r="J44">
-        <v>85</v>
-      </c>
-      <c r="K44" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="16" t="s">
         <v>112</v>
       </c>
@@ -1844,11 +1812,8 @@
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
-      <c r="J45">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="16" t="s">
         <v>113</v>
       </c>
@@ -1871,11 +1836,8 @@
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
-      <c r="J46">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="16" t="s">
         <v>114</v>
       </c>
@@ -1898,11 +1860,8 @@
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-      <c r="J47">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="16" t="s">
         <v>115</v>
       </c>
@@ -1918,11 +1877,8 @@
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
-      <c r="J48">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="16" t="s">
         <v>116</v>
       </c>
@@ -1938,11 +1894,8 @@
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="16"/>
-      <c r="J49">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="16" t="s">
         <v>117</v>
       </c>
@@ -1958,11 +1911,8 @@
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
-      <c r="J50">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="16" t="s">
         <v>20</v>
       </c>
@@ -1978,14 +1928,8 @@
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-      <c r="J51">
-        <v>92</v>
-      </c>
-      <c r="K51" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="16" t="s">
         <v>46</v>
       </c>
@@ -2004,17 +1948,8 @@
       <c r="I52">
         <v>95090</v>
       </c>
-      <c r="J52">
-        <v>93</v>
-      </c>
-      <c r="K52" t="s">
-        <v>120</v>
-      </c>
-      <c r="L52">
-        <v>94790</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="16" t="s">
         <v>45</v>
       </c>
@@ -2032,7 +1967,7 @@
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:15">
       <c r="A54" s="16" t="s">
         <v>46</v>
       </c>
@@ -2050,7 +1985,7 @@
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:15">
       <c r="A55" s="16" t="s">
         <v>95</v>
       </c>
@@ -2068,9 +2003,9 @@
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:15">
       <c r="A56" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B56" s="16">
         <v>18945</v>
@@ -2083,7 +2018,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:15">
       <c r="A57" s="16" t="s">
         <v>95</v>
       </c>
@@ -2097,10 +2032,25 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="G57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H57" s="30">
+        <v>139920</v>
+      </c>
+      <c r="J57" s="30">
+        <v>140020</v>
+      </c>
+      <c r="L57" s="30">
+        <v>141120</v>
+      </c>
+      <c r="N57" s="30">
+        <v>141220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B58" s="16">
         <v>20120</v>
@@ -2112,10 +2062,34 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="G58" t="s">
+        <v>134</v>
+      </c>
+      <c r="H58" s="31">
+        <v>22088</v>
+      </c>
+      <c r="I58" t="s">
+        <v>135</v>
+      </c>
+      <c r="J58" s="31">
+        <v>221088</v>
+      </c>
+      <c r="K58" t="s">
+        <v>135</v>
+      </c>
+      <c r="L58" s="31">
+        <v>22088</v>
+      </c>
+      <c r="M58" t="s">
+        <v>135</v>
+      </c>
+      <c r="N58" s="31">
+        <v>22088</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B59" s="16">
         <v>20187</v>
@@ -2127,10 +2101,25 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="H59">
+        <v>22089</v>
+      </c>
+      <c r="I59" t="s">
+        <v>135</v>
+      </c>
+      <c r="J59">
+        <v>22089</v>
+      </c>
+      <c r="L59">
+        <v>22089</v>
+      </c>
+      <c r="N59">
+        <v>22089</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B60" s="16">
         <v>20258</v>
@@ -2142,10 +2131,32 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="H60">
+        <f>H59+1</f>
+        <v>22090</v>
+      </c>
+      <c r="I60" t="s">
+        <v>135</v>
+      </c>
+      <c r="J60">
+        <f>J59+1</f>
+        <v>22090</v>
+      </c>
+      <c r="L60">
+        <f>L59+1</f>
+        <v>22090</v>
+      </c>
+      <c r="N60">
+        <f>N59+1</f>
+        <v>22090</v>
+      </c>
+      <c r="O60" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B61" s="16">
         <v>20351</v>
@@ -2157,10 +2168,26 @@
         <f t="shared" si="4"/>
         <v>3267</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="H61">
+        <f t="shared" ref="H61:H90" si="7">H60+1</f>
+        <v>22091</v>
+      </c>
+      <c r="J61">
+        <f t="shared" ref="J61:J90" si="8">J60+1</f>
+        <v>22091</v>
+      </c>
+      <c r="L61">
+        <f t="shared" ref="L61:L87" si="9">L60+1</f>
+        <v>22091</v>
+      </c>
+      <c r="N61">
+        <f t="shared" ref="N61:N87" si="10">N60+1</f>
+        <v>22091</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B62" s="16">
         <v>20394</v>
@@ -2172,10 +2199,26 @@
         <f t="shared" si="4"/>
         <v>3267</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="H62">
+        <f t="shared" si="7"/>
+        <v>22092</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="8"/>
+        <v>22092</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="9"/>
+        <v>22092</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="10"/>
+        <v>22092</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B63" s="16">
         <v>20465</v>
@@ -2187,8 +2230,30 @@
         <f t="shared" si="4"/>
         <v>3268</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="H63">
+        <f t="shared" si="7"/>
+        <v>22093</v>
+      </c>
+      <c r="I63" t="s">
+        <v>135</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="8"/>
+        <v>22093</v>
+      </c>
+      <c r="K63" t="s">
+        <v>135</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="9"/>
+        <v>22093</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="10"/>
+        <v>22093</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="16" t="s">
         <v>45</v>
       </c>
@@ -2202,10 +2267,32 @@
         <f t="shared" si="4"/>
         <v>3268</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="H64">
+        <f t="shared" si="7"/>
+        <v>22094</v>
+      </c>
+      <c r="I64" t="s">
+        <v>135</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="8"/>
+        <v>22094</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="9"/>
+        <v>22094</v>
+      </c>
+      <c r="M64" t="s">
+        <v>135</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="10"/>
+        <v>22094</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B65" s="16">
         <v>21172</v>
@@ -2217,10 +2304,29 @@
         <f t="shared" si="4"/>
         <v>3268</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="H65">
+        <f t="shared" si="7"/>
+        <v>22095</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="8"/>
+        <v>22095</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="9"/>
+        <v>22095</v>
+      </c>
+      <c r="M65" t="s">
+        <v>135</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="10"/>
+        <v>22095</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B66" s="16">
         <v>21661</v>
@@ -2232,10 +2338,26 @@
         <f t="shared" si="4"/>
         <v>3814</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="H66">
+        <f t="shared" si="7"/>
+        <v>22096</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="8"/>
+        <v>22096</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="9"/>
+        <v>22096</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="10"/>
+        <v>22096</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B67" s="16">
         <v>21890</v>
@@ -2247,10 +2369,29 @@
         <f t="shared" si="4"/>
         <v>3836</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="H67">
+        <f t="shared" si="7"/>
+        <v>22097</v>
+      </c>
+      <c r="I67" t="s">
+        <v>135</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="8"/>
+        <v>22097</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="9"/>
+        <v>22097</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="10"/>
+        <v>22097</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B68" s="16">
         <v>21929</v>
@@ -2262,10 +2403,29 @@
         <f t="shared" si="4"/>
         <v>3836</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="H68">
+        <f t="shared" si="7"/>
+        <v>22098</v>
+      </c>
+      <c r="I68" t="s">
+        <v>133</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="8"/>
+        <v>22098</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="9"/>
+        <v>22098</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="10"/>
+        <v>22098</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B69" s="16">
         <v>21995</v>
@@ -2277,13 +2437,415 @@
         <f t="shared" si="4"/>
         <v>3837</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="H69">
+        <f t="shared" si="7"/>
+        <v>22099</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="8"/>
+        <v>22099</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="9"/>
+        <v>22099</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="10"/>
+        <v>22099</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="B70" s="16">
+        <v>22090</v>
       </c>
       <c r="C70" s="16">
+        <v>25927</v>
+      </c>
+      <c r="D70" s="16">
+        <f t="shared" si="4"/>
+        <v>3837</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="7"/>
+        <v>22100</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="8"/>
+        <v>22100</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="9"/>
+        <v>22100</v>
+      </c>
+      <c r="M70" t="s">
+        <v>135</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="10"/>
+        <v>22100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="A71" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="16">
         <v>25957</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="7"/>
+        <v>22101</v>
+      </c>
+      <c r="I71" t="s">
+        <v>135</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="8"/>
+        <v>22101</v>
+      </c>
+      <c r="K71" t="s">
+        <v>135</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="9"/>
+        <v>22101</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="10"/>
+        <v>22101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
+      <c r="H72">
+        <f t="shared" si="7"/>
+        <v>22102</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="8"/>
+        <v>22102</v>
+      </c>
+      <c r="K72" t="s">
+        <v>135</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="9"/>
+        <v>22102</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="10"/>
+        <v>22102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
+      <c r="H73">
+        <f t="shared" si="7"/>
+        <v>22103</v>
+      </c>
+      <c r="I73" t="s">
+        <v>135</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="8"/>
+        <v>22103</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="9"/>
+        <v>22103</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="10"/>
+        <v>22103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
+      <c r="H74">
+        <f t="shared" si="7"/>
+        <v>22104</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="8"/>
+        <v>22104</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="9"/>
+        <v>22104</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="10"/>
+        <v>22104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="H75">
+        <f t="shared" si="7"/>
+        <v>22105</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="8"/>
+        <v>22105</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="9"/>
+        <v>22105</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="10"/>
+        <v>22105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="H76">
+        <f t="shared" si="7"/>
+        <v>22106</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="8"/>
+        <v>22106</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="9"/>
+        <v>22106</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="10"/>
+        <v>22106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="H77">
+        <f t="shared" si="7"/>
+        <v>22107</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="8"/>
+        <v>22107</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="9"/>
+        <v>22107</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="10"/>
+        <v>22107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="H78">
+        <f t="shared" si="7"/>
+        <v>22108</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="8"/>
+        <v>22108</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="9"/>
+        <v>22108</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="10"/>
+        <v>22108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="H79">
+        <f t="shared" si="7"/>
+        <v>22109</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="8"/>
+        <v>22109</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="9"/>
+        <v>22109</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="10"/>
+        <v>22109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
+      <c r="H80">
+        <f t="shared" si="7"/>
+        <v>22110</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="8"/>
+        <v>22110</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="9"/>
+        <v>22110</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="10"/>
+        <v>22110</v>
+      </c>
+      <c r="O80" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="8:14">
+      <c r="H81">
+        <f t="shared" si="7"/>
+        <v>22111</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="8"/>
+        <v>22111</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="9"/>
+        <v>22111</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="10"/>
+        <v>22111</v>
+      </c>
+    </row>
+    <row r="82" spans="8:14">
+      <c r="H82">
+        <f t="shared" si="7"/>
+        <v>22112</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="8"/>
+        <v>22112</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="9"/>
+        <v>22112</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="10"/>
+        <v>22112</v>
+      </c>
+    </row>
+    <row r="83" spans="8:14">
+      <c r="H83">
+        <f t="shared" si="7"/>
+        <v>22113</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="8"/>
+        <v>22113</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="9"/>
+        <v>22113</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="10"/>
+        <v>22113</v>
+      </c>
+    </row>
+    <row r="84" spans="8:14">
+      <c r="H84">
+        <f t="shared" si="7"/>
+        <v>22114</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="8"/>
+        <v>22114</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="9"/>
+        <v>22114</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="10"/>
+        <v>22114</v>
+      </c>
+    </row>
+    <row r="85" spans="8:14">
+      <c r="H85">
+        <f t="shared" si="7"/>
+        <v>22115</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="8"/>
+        <v>22115</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="9"/>
+        <v>22115</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="10"/>
+        <v>22115</v>
+      </c>
+    </row>
+    <row r="86" spans="8:14">
+      <c r="H86">
+        <f t="shared" si="7"/>
+        <v>22116</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="8"/>
+        <v>22116</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="9"/>
+        <v>22116</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="10"/>
+        <v>22116</v>
+      </c>
+    </row>
+    <row r="87" spans="8:14">
+      <c r="H87">
+        <f t="shared" si="7"/>
+        <v>22117</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="8"/>
+        <v>22117</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="9"/>
+        <v>22117</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="10"/>
+        <v>22117</v>
+      </c>
+    </row>
+    <row r="88" spans="8:14">
+      <c r="H88">
+        <f t="shared" si="7"/>
+        <v>22118</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="8"/>
+        <v>22118</v>
+      </c>
+    </row>
+    <row r="89" spans="8:14">
+      <c r="H89">
+        <f t="shared" si="7"/>
+        <v>22119</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="8"/>
+        <v>22119</v>
+      </c>
+    </row>
+    <row r="90" spans="8:14">
+      <c r="H90">
+        <f t="shared" si="7"/>
+        <v>22120</v>
+      </c>
+      <c r="I90" t="s">
+        <v>135</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="8"/>
+        <v>22120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 5-G up to hitting the vine block, 2 frames ahead from the point of those blocks being bashed to the vine, 4 frames overaul (luck manipulation).  I'm not satisfied with this version, I think I can save more frames.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
   <si>
     <t>1-1</t>
   </si>
@@ -425,13 +425,31 @@
   </si>
   <si>
     <t>Bshell</t>
+  </si>
+  <si>
+    <t>1st bash</t>
+  </si>
+  <si>
+    <t>2nd bash</t>
+  </si>
+  <si>
+    <t>Checkpoint 206</t>
+  </si>
+  <si>
+    <t>Checkpoint 224</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>Hit vine block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +474,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -548,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -588,13 +614,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,8 +919,8 @@
   <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,14 +960,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="I2" s="13">
         <v>9674</v>
       </c>
@@ -1048,14 +1075,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7"/>
       <c r="H7"/>
     </row>
@@ -1542,14 +1569,14 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.75">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="24" t="s">
@@ -1578,7 +1605,7 @@
         <v>15235</v>
       </c>
       <c r="D36" s="16">
-        <f t="shared" ref="D36:D70" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <f t="shared" ref="D36:D77" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
         <v>2248</v>
       </c>
       <c r="E36">
@@ -2035,16 +2062,16 @@
       <c r="G57" t="s">
         <v>134</v>
       </c>
-      <c r="H57" s="30">
+      <c r="H57" s="25">
         <v>139920</v>
       </c>
-      <c r="J57" s="30">
+      <c r="J57" s="25">
         <v>140020</v>
       </c>
-      <c r="L57" s="30">
+      <c r="L57" s="25">
         <v>141120</v>
       </c>
-      <c r="N57" s="30">
+      <c r="N57" s="25">
         <v>141220</v>
       </c>
     </row>
@@ -2065,25 +2092,25 @@
       <c r="G58" t="s">
         <v>134</v>
       </c>
-      <c r="H58" s="31">
+      <c r="H58" s="26">
         <v>22088</v>
       </c>
       <c r="I58" t="s">
         <v>135</v>
       </c>
-      <c r="J58" s="31">
+      <c r="J58" s="26">
         <v>221088</v>
       </c>
       <c r="K58" t="s">
         <v>135</v>
       </c>
-      <c r="L58" s="31">
+      <c r="L58" s="26">
         <v>22088</v>
       </c>
       <c r="M58" t="s">
         <v>135</v>
       </c>
-      <c r="N58" s="31">
+      <c r="N58" s="26">
         <v>22088</v>
       </c>
     </row>
@@ -2492,8 +2519,15 @@
       <c r="A71" s="16" t="s">
         <v>131</v>
       </c>
+      <c r="B71" s="16">
+        <v>22121</v>
+      </c>
       <c r="C71" s="16">
         <v>25957</v>
+      </c>
+      <c r="D71" s="16">
+        <f t="shared" si="4"/>
+        <v>3836</v>
       </c>
       <c r="H71">
         <f t="shared" si="7"/>
@@ -2519,6 +2553,19 @@
       </c>
     </row>
     <row r="72" spans="1:15">
+      <c r="A72" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" s="16">
+        <v>22330</v>
+      </c>
+      <c r="C72" s="16">
+        <v>26163</v>
+      </c>
+      <c r="D72" s="16">
+        <f t="shared" si="4"/>
+        <v>3833</v>
+      </c>
       <c r="H72">
         <f t="shared" si="7"/>
         <v>22102</v>
@@ -2540,6 +2587,19 @@
       </c>
     </row>
     <row r="73" spans="1:15">
+      <c r="A73" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" s="16">
+        <v>22372</v>
+      </c>
+      <c r="C73" s="16">
+        <v>26202</v>
+      </c>
+      <c r="D73" s="16">
+        <f t="shared" si="4"/>
+        <v>3830</v>
+      </c>
       <c r="H73">
         <f t="shared" si="7"/>
         <v>22103</v>
@@ -2561,6 +2621,19 @@
       </c>
     </row>
     <row r="74" spans="1:15">
+      <c r="A74" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" s="16">
+        <v>22388</v>
+      </c>
+      <c r="C74" s="16">
+        <v>26218</v>
+      </c>
+      <c r="D74" s="16">
+        <f t="shared" si="4"/>
+        <v>3830</v>
+      </c>
       <c r="H74">
         <f t="shared" si="7"/>
         <v>22104</v>
@@ -2579,6 +2652,19 @@
       </c>
     </row>
     <row r="75" spans="1:15">
+      <c r="A75" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="16">
+        <v>22421</v>
+      </c>
+      <c r="C75" s="16">
+        <v>26262</v>
+      </c>
+      <c r="D75" s="16">
+        <f t="shared" si="4"/>
+        <v>3841</v>
+      </c>
       <c r="H75">
         <f t="shared" si="7"/>
         <v>22105</v>
@@ -2597,6 +2683,19 @@
       </c>
     </row>
     <row r="76" spans="1:15">
+      <c r="A76" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="16">
+        <v>22454</v>
+      </c>
+      <c r="C76" s="16">
+        <v>26286</v>
+      </c>
+      <c r="D76" s="16">
+        <f t="shared" si="4"/>
+        <v>3832</v>
+      </c>
       <c r="H76">
         <f t="shared" si="7"/>
         <v>22106</v>
@@ -2615,6 +2714,19 @@
       </c>
     </row>
     <row r="77" spans="1:15">
+      <c r="A77" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="16">
+        <v>22739</v>
+      </c>
+      <c r="C77" s="16">
+        <v>26571</v>
+      </c>
+      <c r="D77" s="16">
+        <f t="shared" si="4"/>
+        <v>3832</v>
+      </c>
       <c r="H77">
         <f t="shared" si="7"/>
         <v>22107</v>
@@ -2896,14 +3008,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -2966,14 +3078,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
@@ -3496,14 +3608,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="24" t="s">

</xml_diff>

<commit_message>
NSMB - 5-G done pending confirmation that the left shaft isnt' faster, and possible map manipulation.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="143">
   <si>
     <t>1-1</t>
   </si>
@@ -418,15 +418,6 @@
     <t>Hit HB</t>
   </si>
   <si>
-    <t>Fireflower</t>
-  </si>
-  <si>
-    <t>Score:</t>
-  </si>
-  <si>
-    <t>Bshell</t>
-  </si>
-  <si>
     <t>1st bash</t>
   </si>
   <si>
@@ -443,6 +434,18 @@
   </si>
   <si>
     <t>Hit vine block</t>
+  </si>
+  <si>
+    <t>Grab vine *imprecise compare</t>
+  </si>
+  <si>
+    <t>Checkpoint 1137</t>
+  </si>
+  <si>
+    <t>End level</t>
+  </si>
+  <si>
+    <t>Enter 5-C</t>
   </si>
 </sst>
 </file>
@@ -616,12 +619,12 @@
     <xf numFmtId="16" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,11 +919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O90"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -960,14 +963,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="I2" s="13">
         <v>9674</v>
       </c>
@@ -1075,14 +1078,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7"/>
       <c r="H7"/>
     </row>
@@ -1569,14 +1572,14 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.75">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="24" t="s">
@@ -1605,7 +1608,7 @@
         <v>15235</v>
       </c>
       <c r="D36" s="16">
-        <f t="shared" ref="D36:D77" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <f t="shared" ref="D36:D83" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
         <v>2248</v>
       </c>
       <c r="E36">
@@ -1905,7 +1908,7 @@
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:14">
       <c r="A49" s="16" t="s">
         <v>116</v>
       </c>
@@ -1922,7 +1925,7 @@
       <c r="G49" s="16"/>
       <c r="H49" s="16"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:14">
       <c r="A50" s="16" t="s">
         <v>117</v>
       </c>
@@ -1939,7 +1942,7 @@
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:14">
       <c r="A51" s="16" t="s">
         <v>20</v>
       </c>
@@ -1956,7 +1959,7 @@
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:14">
       <c r="A52" s="16" t="s">
         <v>46</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>95090</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:14">
       <c r="A53" s="16" t="s">
         <v>45</v>
       </c>
@@ -1994,7 +1997,7 @@
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:14">
       <c r="A54" s="16" t="s">
         <v>46</v>
       </c>
@@ -2012,7 +2015,7 @@
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:14">
       <c r="A55" s="16" t="s">
         <v>95</v>
       </c>
@@ -2030,7 +2033,7 @@
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:14">
       <c r="A56" s="16" t="s">
         <v>119</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:14">
       <c r="A57" s="16" t="s">
         <v>95</v>
       </c>
@@ -2059,23 +2062,12 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-      <c r="G57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H57" s="25">
-        <v>139920</v>
-      </c>
-      <c r="J57" s="25">
-        <v>140020</v>
-      </c>
-      <c r="L57" s="25">
-        <v>141120</v>
-      </c>
-      <c r="N57" s="25">
-        <v>141220</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="H57" s="25"/>
+      <c r="J57" s="25"/>
+      <c r="L57" s="25"/>
+      <c r="N57" s="25"/>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="16" t="s">
         <v>120</v>
       </c>
@@ -2089,32 +2081,12 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-      <c r="G58" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="26">
-        <v>22088</v>
-      </c>
-      <c r="I58" t="s">
-        <v>135</v>
-      </c>
-      <c r="J58" s="26">
-        <v>221088</v>
-      </c>
-      <c r="K58" t="s">
-        <v>135</v>
-      </c>
-      <c r="L58" s="26">
-        <v>22088</v>
-      </c>
-      <c r="M58" t="s">
-        <v>135</v>
-      </c>
-      <c r="N58" s="26">
-        <v>22088</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="H58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="N58" s="26"/>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="16" t="s">
         <v>121</v>
       </c>
@@ -2128,23 +2100,8 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-      <c r="H59">
-        <v>22089</v>
-      </c>
-      <c r="I59" t="s">
-        <v>135</v>
-      </c>
-      <c r="J59">
-        <v>22089</v>
-      </c>
-      <c r="L59">
-        <v>22089</v>
-      </c>
-      <c r="N59">
-        <v>22089</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15">
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="16" t="s">
         <v>122</v>
       </c>
@@ -2158,30 +2115,8 @@
         <f t="shared" si="4"/>
         <v>3266</v>
       </c>
-      <c r="H60">
-        <f>H59+1</f>
-        <v>22090</v>
-      </c>
-      <c r="I60" t="s">
-        <v>135</v>
-      </c>
-      <c r="J60">
-        <f>J59+1</f>
-        <v>22090</v>
-      </c>
-      <c r="L60">
-        <f>L59+1</f>
-        <v>22090</v>
-      </c>
-      <c r="N60">
-        <f>N59+1</f>
-        <v>22090</v>
-      </c>
-      <c r="O60" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15">
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" s="16" t="s">
         <v>123</v>
       </c>
@@ -2195,24 +2130,8 @@
         <f t="shared" si="4"/>
         <v>3267</v>
       </c>
-      <c r="H61">
-        <f t="shared" ref="H61:H90" si="7">H60+1</f>
-        <v>22091</v>
-      </c>
-      <c r="J61">
-        <f t="shared" ref="J61:J90" si="8">J60+1</f>
-        <v>22091</v>
-      </c>
-      <c r="L61">
-        <f t="shared" ref="L61:L87" si="9">L60+1</f>
-        <v>22091</v>
-      </c>
-      <c r="N61">
-        <f t="shared" ref="N61:N87" si="10">N60+1</f>
-        <v>22091</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15">
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" s="16" t="s">
         <v>124</v>
       </c>
@@ -2226,24 +2145,8 @@
         <f t="shared" si="4"/>
         <v>3267</v>
       </c>
-      <c r="H62">
-        <f t="shared" si="7"/>
-        <v>22092</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="8"/>
-        <v>22092</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="9"/>
-        <v>22092</v>
-      </c>
-      <c r="N62">
-        <f t="shared" si="10"/>
-        <v>22092</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15">
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="16" t="s">
         <v>125</v>
       </c>
@@ -2257,30 +2160,8 @@
         <f t="shared" si="4"/>
         <v>3268</v>
       </c>
-      <c r="H63">
-        <f t="shared" si="7"/>
-        <v>22093</v>
-      </c>
-      <c r="I63" t="s">
-        <v>135</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="8"/>
-        <v>22093</v>
-      </c>
-      <c r="K63" t="s">
-        <v>135</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="9"/>
-        <v>22093</v>
-      </c>
-      <c r="N63">
-        <f t="shared" si="10"/>
-        <v>22093</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" s="16" t="s">
         <v>45</v>
       </c>
@@ -2294,30 +2175,8 @@
         <f t="shared" si="4"/>
         <v>3268</v>
       </c>
-      <c r="H64">
-        <f t="shared" si="7"/>
-        <v>22094</v>
-      </c>
-      <c r="I64" t="s">
-        <v>135</v>
-      </c>
-      <c r="J64">
-        <f t="shared" si="8"/>
-        <v>22094</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="9"/>
-        <v>22094</v>
-      </c>
-      <c r="M64" t="s">
-        <v>135</v>
-      </c>
-      <c r="N64">
-        <f t="shared" si="10"/>
-        <v>22094</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15">
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="16" t="s">
         <v>126</v>
       </c>
@@ -2331,27 +2190,8 @@
         <f t="shared" si="4"/>
         <v>3268</v>
       </c>
-      <c r="H65">
-        <f t="shared" si="7"/>
-        <v>22095</v>
-      </c>
-      <c r="J65">
-        <f t="shared" si="8"/>
-        <v>22095</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="9"/>
-        <v>22095</v>
-      </c>
-      <c r="M65" t="s">
-        <v>135</v>
-      </c>
-      <c r="N65">
-        <f t="shared" si="10"/>
-        <v>22095</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15">
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="16" t="s">
         <v>127</v>
       </c>
@@ -2365,24 +2205,8 @@
         <f t="shared" si="4"/>
         <v>3814</v>
       </c>
-      <c r="H66">
-        <f t="shared" si="7"/>
-        <v>22096</v>
-      </c>
-      <c r="J66">
-        <f t="shared" si="8"/>
-        <v>22096</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="9"/>
-        <v>22096</v>
-      </c>
-      <c r="N66">
-        <f t="shared" si="10"/>
-        <v>22096</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15">
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="16" t="s">
         <v>128</v>
       </c>
@@ -2396,27 +2220,8 @@
         <f t="shared" si="4"/>
         <v>3836</v>
       </c>
-      <c r="H67">
-        <f t="shared" si="7"/>
-        <v>22097</v>
-      </c>
-      <c r="I67" t="s">
-        <v>135</v>
-      </c>
-      <c r="J67">
-        <f t="shared" si="8"/>
-        <v>22097</v>
-      </c>
-      <c r="L67">
-        <f t="shared" si="9"/>
-        <v>22097</v>
-      </c>
-      <c r="N67">
-        <f t="shared" si="10"/>
-        <v>22097</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15">
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="16" t="s">
         <v>129</v>
       </c>
@@ -2430,27 +2235,8 @@
         <f t="shared" si="4"/>
         <v>3836</v>
       </c>
-      <c r="H68">
-        <f t="shared" si="7"/>
-        <v>22098</v>
-      </c>
-      <c r="I68" t="s">
-        <v>133</v>
-      </c>
-      <c r="J68">
-        <f t="shared" si="8"/>
-        <v>22098</v>
-      </c>
-      <c r="L68">
-        <f t="shared" si="9"/>
-        <v>22098</v>
-      </c>
-      <c r="N68">
-        <f t="shared" si="10"/>
-        <v>22098</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15">
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="16" t="s">
         <v>130</v>
       </c>
@@ -2464,24 +2250,8 @@
         <f t="shared" si="4"/>
         <v>3837</v>
       </c>
-      <c r="H69">
-        <f t="shared" si="7"/>
-        <v>22099</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="8"/>
-        <v>22099</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="9"/>
-        <v>22099</v>
-      </c>
-      <c r="N69">
-        <f t="shared" si="10"/>
-        <v>22099</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15">
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="16" t="s">
         <v>132</v>
       </c>
@@ -2495,27 +2265,8 @@
         <f t="shared" si="4"/>
         <v>3837</v>
       </c>
-      <c r="H70">
-        <f t="shared" si="7"/>
-        <v>22100</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="8"/>
-        <v>22100</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="9"/>
-        <v>22100</v>
-      </c>
-      <c r="M70" t="s">
-        <v>135</v>
-      </c>
-      <c r="N70">
-        <f t="shared" si="10"/>
-        <v>22100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15">
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="16" t="s">
         <v>131</v>
       </c>
@@ -2529,32 +2280,10 @@
         <f t="shared" si="4"/>
         <v>3836</v>
       </c>
-      <c r="H71">
-        <f t="shared" si="7"/>
-        <v>22101</v>
-      </c>
-      <c r="I71" t="s">
-        <v>135</v>
-      </c>
-      <c r="J71">
-        <f t="shared" si="8"/>
-        <v>22101</v>
-      </c>
-      <c r="K71" t="s">
-        <v>135</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="9"/>
-        <v>22101</v>
-      </c>
-      <c r="N71">
-        <f t="shared" si="10"/>
-        <v>22101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15">
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B72" s="16">
         <v>22330</v>
@@ -2566,29 +2295,10 @@
         <f t="shared" si="4"/>
         <v>3833</v>
       </c>
-      <c r="H72">
-        <f t="shared" si="7"/>
-        <v>22102</v>
-      </c>
-      <c r="J72">
-        <f t="shared" si="8"/>
-        <v>22102</v>
-      </c>
-      <c r="K72" t="s">
-        <v>135</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="9"/>
-        <v>22102</v>
-      </c>
-      <c r="N72">
-        <f t="shared" si="10"/>
-        <v>22102</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15">
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B73" s="16">
         <v>22372</v>
@@ -2600,29 +2310,10 @@
         <f t="shared" si="4"/>
         <v>3830</v>
       </c>
-      <c r="H73">
-        <f t="shared" si="7"/>
-        <v>22103</v>
-      </c>
-      <c r="I73" t="s">
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="J73">
-        <f t="shared" si="8"/>
-        <v>22103</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="9"/>
-        <v>22103</v>
-      </c>
-      <c r="N73">
-        <f t="shared" si="10"/>
-        <v>22103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15">
-      <c r="A74" s="16" t="s">
-        <v>138</v>
       </c>
       <c r="B74" s="16">
         <v>22388</v>
@@ -2634,26 +2325,10 @@
         <f t="shared" si="4"/>
         <v>3830</v>
       </c>
-      <c r="H74">
-        <f t="shared" si="7"/>
-        <v>22104</v>
-      </c>
-      <c r="J74">
-        <f t="shared" si="8"/>
-        <v>22104</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="9"/>
-        <v>22104</v>
-      </c>
-      <c r="N74">
-        <f t="shared" si="10"/>
-        <v>22104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15">
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B75" s="16">
         <v>22421</v>
@@ -2665,26 +2340,10 @@
         <f t="shared" si="4"/>
         <v>3841</v>
       </c>
-      <c r="H75">
-        <f t="shared" si="7"/>
-        <v>22105</v>
-      </c>
-      <c r="J75">
-        <f t="shared" si="8"/>
-        <v>22105</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="9"/>
-        <v>22105</v>
-      </c>
-      <c r="N75">
-        <f t="shared" si="10"/>
-        <v>22105</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15">
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B76" s="16">
         <v>22454</v>
@@ -2696,268 +2355,118 @@
         <f t="shared" si="4"/>
         <v>3832</v>
       </c>
-      <c r="H76">
-        <f t="shared" si="7"/>
-        <v>22106</v>
-      </c>
-      <c r="J76">
-        <f t="shared" si="8"/>
-        <v>22106</v>
-      </c>
-      <c r="L76">
-        <f t="shared" si="9"/>
-        <v>22106</v>
-      </c>
-      <c r="N76">
-        <f t="shared" si="10"/>
-        <v>22106</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15">
-      <c r="A77" s="32" t="s">
-        <v>141</v>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="27" t="s">
+        <v>138</v>
       </c>
       <c r="B77" s="16">
-        <v>22739</v>
+        <v>22708</v>
       </c>
       <c r="C77" s="16">
         <v>26571</v>
       </c>
       <c r="D77" s="16">
         <f t="shared" si="4"/>
-        <v>3832</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="7"/>
-        <v>22107</v>
-      </c>
-      <c r="J77">
-        <f t="shared" si="8"/>
-        <v>22107</v>
-      </c>
-      <c r="L77">
-        <f t="shared" si="9"/>
-        <v>22107</v>
-      </c>
-      <c r="N77">
-        <f t="shared" si="10"/>
-        <v>22107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15">
-      <c r="H78">
-        <f t="shared" si="7"/>
-        <v>22108</v>
-      </c>
-      <c r="J78">
-        <f t="shared" si="8"/>
-        <v>22108</v>
-      </c>
-      <c r="L78">
-        <f t="shared" si="9"/>
-        <v>22108</v>
-      </c>
-      <c r="N78">
-        <f t="shared" si="10"/>
-        <v>22108</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15">
-      <c r="H79">
-        <f t="shared" si="7"/>
-        <v>22109</v>
-      </c>
-      <c r="J79">
-        <f t="shared" si="8"/>
-        <v>22109</v>
-      </c>
-      <c r="L79">
-        <f t="shared" si="9"/>
-        <v>22109</v>
-      </c>
-      <c r="N79">
-        <f t="shared" si="10"/>
-        <v>22109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15">
-      <c r="H80">
-        <f t="shared" si="7"/>
-        <v>22110</v>
-      </c>
-      <c r="J80">
-        <f t="shared" si="8"/>
-        <v>22110</v>
-      </c>
-      <c r="L80">
-        <f t="shared" si="9"/>
-        <v>22110</v>
-      </c>
-      <c r="N80">
-        <f t="shared" si="10"/>
-        <v>22110</v>
-      </c>
-      <c r="O80" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="81" spans="8:14">
-      <c r="H81">
-        <f t="shared" si="7"/>
-        <v>22111</v>
-      </c>
-      <c r="J81">
-        <f t="shared" si="8"/>
-        <v>22111</v>
-      </c>
-      <c r="L81">
-        <f t="shared" si="9"/>
-        <v>22111</v>
-      </c>
-      <c r="N81">
-        <f t="shared" si="10"/>
-        <v>22111</v>
-      </c>
-    </row>
-    <row r="82" spans="8:14">
-      <c r="H82">
-        <f t="shared" si="7"/>
-        <v>22112</v>
-      </c>
-      <c r="J82">
-        <f t="shared" si="8"/>
-        <v>22112</v>
-      </c>
-      <c r="L82">
-        <f t="shared" si="9"/>
-        <v>22112</v>
-      </c>
-      <c r="N82">
-        <f t="shared" si="10"/>
-        <v>22112</v>
-      </c>
-    </row>
-    <row r="83" spans="8:14">
-      <c r="H83">
-        <f t="shared" si="7"/>
-        <v>22113</v>
-      </c>
-      <c r="J83">
-        <f t="shared" si="8"/>
-        <v>22113</v>
-      </c>
-      <c r="L83">
-        <f t="shared" si="9"/>
-        <v>22113</v>
-      </c>
-      <c r="N83">
-        <f t="shared" si="10"/>
-        <v>22113</v>
-      </c>
-    </row>
-    <row r="84" spans="8:14">
-      <c r="H84">
-        <f t="shared" si="7"/>
-        <v>22114</v>
-      </c>
-      <c r="J84">
-        <f t="shared" si="8"/>
-        <v>22114</v>
-      </c>
-      <c r="L84">
-        <f t="shared" si="9"/>
-        <v>22114</v>
-      </c>
-      <c r="N84">
-        <f t="shared" si="10"/>
-        <v>22114</v>
-      </c>
-    </row>
-    <row r="85" spans="8:14">
-      <c r="H85">
-        <f t="shared" si="7"/>
-        <v>22115</v>
-      </c>
-      <c r="J85">
-        <f t="shared" si="8"/>
-        <v>22115</v>
-      </c>
-      <c r="L85">
-        <f t="shared" si="9"/>
-        <v>22115</v>
-      </c>
-      <c r="N85">
-        <f t="shared" si="10"/>
-        <v>22115</v>
-      </c>
-    </row>
-    <row r="86" spans="8:14">
-      <c r="H86">
-        <f t="shared" si="7"/>
-        <v>22116</v>
-      </c>
-      <c r="J86">
-        <f t="shared" si="8"/>
-        <v>22116</v>
-      </c>
-      <c r="L86">
-        <f t="shared" si="9"/>
-        <v>22116</v>
-      </c>
-      <c r="N86">
-        <f t="shared" si="10"/>
-        <v>22116</v>
-      </c>
-    </row>
-    <row r="87" spans="8:14">
-      <c r="H87">
-        <f t="shared" si="7"/>
-        <v>22117</v>
-      </c>
-      <c r="J87">
-        <f t="shared" si="8"/>
-        <v>22117</v>
-      </c>
-      <c r="L87">
-        <f t="shared" si="9"/>
-        <v>22117</v>
-      </c>
-      <c r="N87">
-        <f t="shared" si="10"/>
-        <v>22117</v>
-      </c>
-    </row>
-    <row r="88" spans="8:14">
-      <c r="H88">
-        <f t="shared" si="7"/>
-        <v>22118</v>
-      </c>
-      <c r="J88">
-        <f t="shared" si="8"/>
-        <v>22118</v>
-      </c>
-    </row>
-    <row r="89" spans="8:14">
-      <c r="H89">
-        <f t="shared" si="7"/>
-        <v>22119</v>
-      </c>
-      <c r="J89">
-        <f t="shared" si="8"/>
-        <v>22119</v>
-      </c>
-    </row>
-    <row r="90" spans="8:14">
-      <c r="H90">
-        <f t="shared" si="7"/>
-        <v>22120</v>
-      </c>
-      <c r="I90" t="s">
-        <v>135</v>
-      </c>
-      <c r="J90">
-        <f t="shared" si="8"/>
-        <v>22120</v>
+        <v>3863</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78" s="16">
+        <v>22829</v>
+      </c>
+      <c r="C78" s="16">
+        <v>26694</v>
+      </c>
+      <c r="D78" s="16">
+        <f t="shared" si="4"/>
+        <v>3865</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="16">
+        <v>23205</v>
+      </c>
+      <c r="C79" s="16">
+        <v>27067</v>
+      </c>
+      <c r="D79" s="16">
+        <f t="shared" si="4"/>
+        <v>3862</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80" s="16">
+        <v>23849</v>
+      </c>
+      <c r="C80" s="16">
+        <v>27731</v>
+      </c>
+      <c r="D80" s="16">
+        <f t="shared" si="4"/>
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" s="16">
+        <v>24266</v>
+      </c>
+      <c r="C81" s="16">
+        <v>28148</v>
+      </c>
+      <c r="D81" s="16">
+        <f t="shared" si="4"/>
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" s="16">
+        <v>24570</v>
+      </c>
+      <c r="C82" s="16">
+        <v>28462</v>
+      </c>
+      <c r="D82" s="16">
+        <f t="shared" si="4"/>
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="16">
+        <v>25088</v>
+      </c>
+      <c r="C83" s="16">
+        <v>28980</v>
+      </c>
+      <c r="D83" s="16">
+        <f t="shared" si="4"/>
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" s="16">
+        <v>29893</v>
       </c>
     </row>
   </sheetData>
@@ -3008,14 +2517,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -3078,14 +2587,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
@@ -3608,14 +3117,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="24" t="s">

</xml_diff>

<commit_message>
NSMB - up to world 8 !
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="146">
   <si>
     <t>1-1</t>
   </si>
@@ -446,6 +446,15 @@
   </si>
   <si>
     <t>Enter 5-C</t>
+  </si>
+  <si>
+    <t>Descend into cannon</t>
+  </si>
+  <si>
+    <t>World 8</t>
+  </si>
+  <si>
+    <t>Enter 8-1</t>
   </si>
 </sst>
 </file>
@@ -492,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +541,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -625,6 +640,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,11 +939,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N84"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1608,7 +1628,7 @@
         <v>15235</v>
       </c>
       <c r="D36" s="16">
-        <f t="shared" ref="D36:D83" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
+        <f t="shared" ref="D36:D87" si="4">IF(B36 &gt;  0,C36-B36, 0)</f>
         <v>2248</v>
       </c>
       <c r="E36">
@@ -2416,7 +2436,7 @@
         <v>3882</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:6">
       <c r="A81" s="16" t="s">
         <v>37</v>
       </c>
@@ -2431,7 +2451,7 @@
         <v>3882</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:6">
       <c r="A82" s="16" t="s">
         <v>45</v>
       </c>
@@ -2446,7 +2466,7 @@
         <v>3892</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:6">
       <c r="A83" s="16" t="s">
         <v>141</v>
       </c>
@@ -2461,19 +2481,122 @@
         <v>3892</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:6">
       <c r="A84" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="B84" s="16">
+        <v>25472</v>
+      </c>
       <c r="C84" s="16">
         <v>29893</v>
       </c>
+      <c r="D84" s="16">
+        <f t="shared" si="4"/>
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85" s="16">
+        <v>25697</v>
+      </c>
+      <c r="C85" s="16">
+        <v>30136</v>
+      </c>
+      <c r="D85" s="16">
+        <f t="shared" si="4"/>
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B86" s="16">
+        <v>25830</v>
+      </c>
+      <c r="C86" s="16">
+        <v>30269</v>
+      </c>
+      <c r="D86" s="16">
+        <f t="shared" si="4"/>
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B87" s="16">
+        <v>26420</v>
+      </c>
+      <c r="C87" s="16">
+        <v>30859</v>
+      </c>
+      <c r="D87" s="16">
+        <f t="shared" si="4"/>
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="18.75">
+      <c r="A88" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="34"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="B89" s="36"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="36"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B90" s="16">
+        <v>26790</v>
+      </c>
+      <c r="C90" s="16">
+        <v>31594</v>
+      </c>
+      <c r="D90" s="16">
+        <f t="shared" ref="D90:D91" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="16">
+        <v>27017</v>
+      </c>
+      <c r="C91" s="16">
+        <v>31842</v>
+      </c>
+      <c r="D91" s="16">
+        <f t="shared" si="7"/>
+        <v>4825</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A88:F88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
NSMB - Starting 8-2
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="149">
   <si>
     <t>1-1</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>Enter 8-1</t>
+  </si>
+  <si>
+    <t>Enter 8-2</t>
+  </si>
+  <si>
+    <t>Checkpoint 2005</t>
+  </si>
+  <si>
+    <t>Mario touch ground</t>
   </si>
 </sst>
 </file>
@@ -635,6 +644,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -642,9 +654,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,11 +948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -983,14 +992,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="I2" s="13">
         <v>9674</v>
       </c>
@@ -1098,14 +1107,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
       <c r="G7"/>
       <c r="H7"/>
     </row>
@@ -1592,14 +1601,14 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.75">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="24" t="s">
@@ -2542,24 +2551,24 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="18.75">
-      <c r="A88" s="33" t="s">
+      <c r="A88" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="B88" s="33"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="34"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="35" t="s">
+      <c r="A89" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="B89" s="36"/>
-      <c r="C89" s="36"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="36"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="29"/>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="16" t="s">
@@ -2572,7 +2581,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D91" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D98" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2589,6 +2598,111 @@
       <c r="D91" s="16">
         <f t="shared" si="7"/>
         <v>4825</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B92" s="16">
+        <v>27730</v>
+      </c>
+      <c r="C92" s="16">
+        <v>32556</v>
+      </c>
+      <c r="D92" s="16">
+        <f t="shared" si="7"/>
+        <v>4826</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93" s="16">
+        <v>28335</v>
+      </c>
+      <c r="C93" s="16">
+        <v>33163</v>
+      </c>
+      <c r="D93" s="16">
+        <f t="shared" si="7"/>
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="16">
+        <v>28853</v>
+      </c>
+      <c r="C94" s="16">
+        <v>33681</v>
+      </c>
+      <c r="D94" s="16">
+        <f t="shared" si="7"/>
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B95" s="16">
+        <v>29213</v>
+      </c>
+      <c r="C95" s="16">
+        <v>34468</v>
+      </c>
+      <c r="D95" s="16">
+        <f t="shared" si="7"/>
+        <v>5255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" s="16">
+        <v>29438</v>
+      </c>
+      <c r="C96" s="16">
+        <v>34713</v>
+      </c>
+      <c r="D96" s="16">
+        <f t="shared" si="7"/>
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" s="16">
+        <v>29585</v>
+      </c>
+      <c r="C97" s="16">
+        <v>34860</v>
+      </c>
+      <c r="D97" s="16">
+        <f t="shared" si="7"/>
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B98" s="16">
+        <v>29708</v>
+      </c>
+      <c r="C98" s="16">
+        <v>34998</v>
+      </c>
+      <c r="D98" s="16">
+        <f t="shared" si="7"/>
+        <v>5290</v>
       </c>
     </row>
   </sheetData>
@@ -2640,14 +2754,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -2710,14 +2824,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
@@ -3240,14 +3354,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="24" t="s">

</xml_diff>

<commit_message>
NSMB - first segmet of 8-2 done.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="151">
   <si>
     <t>1-1</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>Mario touch ground</t>
+  </si>
+  <si>
+    <t>1st up after button</t>
+  </si>
+  <si>
+    <t>Speed = -1</t>
   </si>
 </sst>
 </file>
@@ -948,11 +954,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N98"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J88" sqref="J88:L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2581,7 +2587,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D98" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D101" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2701,6 +2707,51 @@
         <v>34998</v>
       </c>
       <c r="D98" s="16">
+        <f t="shared" si="7"/>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B99" s="16">
+        <v>29848</v>
+      </c>
+      <c r="C99" s="16">
+        <v>35137</v>
+      </c>
+      <c r="D99" s="16">
+        <f t="shared" si="7"/>
+        <v>5289</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B100" s="16">
+        <v>29894</v>
+      </c>
+      <c r="C100" s="16">
+        <v>35181</v>
+      </c>
+      <c r="D100" s="16">
+        <f t="shared" si="7"/>
+        <v>5287</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" s="16">
+        <v>30331</v>
+      </c>
+      <c r="C101" s="16">
+        <v>35621</v>
+      </c>
+      <c r="D101" s="16">
         <f t="shared" si="7"/>
         <v>5290</v>
       </c>

</xml_diff>

<commit_message>
NSMB - Several more rooms of 8-2 done
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="154">
   <si>
     <t>1-1</t>
   </si>
@@ -470,6 +470,15 @@
   </si>
   <si>
     <t>Speed = -1</t>
+  </si>
+  <si>
+    <t>Rail 93650944 (after turn)</t>
+  </si>
+  <si>
+    <t>Black screens</t>
+  </si>
+  <si>
+    <t>Black screen (water scene)</t>
   </si>
 </sst>
 </file>
@@ -954,11 +963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J88" sqref="J88:L91"/>
+      <selection pane="bottomLeft" activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2451,7 +2460,7 @@
         <v>3882</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:10">
       <c r="A81" s="16" t="s">
         <v>37</v>
       </c>
@@ -2466,7 +2475,7 @@
         <v>3882</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:10">
       <c r="A82" s="16" t="s">
         <v>45</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>3892</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:10">
       <c r="A83" s="16" t="s">
         <v>141</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>3892</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:10">
       <c r="A84" s="16" t="s">
         <v>142</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>4421</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:10">
       <c r="A85" s="16" t="s">
         <v>95</v>
       </c>
@@ -2526,7 +2535,7 @@
         <v>4439</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:10">
       <c r="A86" s="16" t="s">
         <v>143</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>4439</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:10">
       <c r="A87" s="16" t="s">
         <v>141</v>
       </c>
@@ -2556,7 +2565,7 @@
         <v>4439</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="18.75">
+    <row r="88" spans="1:10" ht="18.75">
       <c r="A88" s="36" t="s">
         <v>144</v>
       </c>
@@ -2566,7 +2575,7 @@
       <c r="E88" s="37"/>
       <c r="F88" s="37"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:10">
       <c r="A89" s="28" t="s">
         <v>145</v>
       </c>
@@ -2576,7 +2585,7 @@
       <c r="E89" s="30"/>
       <c r="F89" s="29"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:10">
       <c r="A90" s="16" t="s">
         <v>145</v>
       </c>
@@ -2587,11 +2596,11 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D101" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D106" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:10">
       <c r="A91" s="16" t="s">
         <v>95</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>4825</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:10">
       <c r="A92" s="16" t="s">
         <v>147</v>
       </c>
@@ -2621,7 +2630,7 @@
         <v>4826</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:10">
       <c r="A93" s="16" t="s">
         <v>45</v>
       </c>
@@ -2635,8 +2644,14 @@
         <f t="shared" si="7"/>
         <v>4828</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="I93">
+        <v>31543</v>
+      </c>
+      <c r="J93">
+        <v>36872</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="16" t="s">
         <v>141</v>
       </c>
@@ -2651,7 +2666,7 @@
         <v>4828</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:10">
       <c r="A95" s="16" t="s">
         <v>146</v>
       </c>
@@ -2666,7 +2681,7 @@
         <v>5255</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:10">
       <c r="A96" s="16" t="s">
         <v>95</v>
       </c>
@@ -2754,6 +2769,81 @@
       <c r="D101" s="16">
         <f t="shared" si="7"/>
         <v>5290</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B102" s="16">
+        <v>30698</v>
+      </c>
+      <c r="C102" s="16">
+        <v>35992</v>
+      </c>
+      <c r="D102" s="16">
+        <f t="shared" si="7"/>
+        <v>5294</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B103" s="16">
+        <v>30992</v>
+      </c>
+      <c r="C103" s="16">
+        <v>36290</v>
+      </c>
+      <c r="D103" s="16">
+        <f t="shared" si="7"/>
+        <v>5298</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B104" s="16">
+        <v>31261</v>
+      </c>
+      <c r="C104" s="16">
+        <v>36576</v>
+      </c>
+      <c r="D104" s="16">
+        <f t="shared" si="7"/>
+        <v>5315</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" s="16">
+        <v>31543</v>
+      </c>
+      <c r="C105" s="16">
+        <v>36872</v>
+      </c>
+      <c r="D105" s="16">
+        <f t="shared" si="7"/>
+        <v>5329</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106" s="16">
+        <v>31909</v>
+      </c>
+      <c r="C106" s="16">
+        <v>37235</v>
+      </c>
+      <c r="D106" s="16">
+        <f t="shared" si="7"/>
+        <v>5326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-2 done
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
   <si>
     <t>1-1</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t>Black screen (water scene)</t>
+  </si>
+  <si>
+    <t>Black screen (water)</t>
+  </si>
+  <si>
+    <t>Enter 8-F1</t>
   </si>
 </sst>
 </file>
@@ -963,11 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N106"/>
+  <dimension ref="A1:N111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J94" sqref="J94"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2596,7 +2602,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D106" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D111" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2665,6 +2671,12 @@
         <f t="shared" si="7"/>
         <v>4828</v>
       </c>
+      <c r="I94">
+        <v>17</v>
+      </c>
+      <c r="J94">
+        <v>8</v>
+      </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="16" t="s">
@@ -2680,6 +2692,14 @@
         <f t="shared" si="7"/>
         <v>5255</v>
       </c>
+      <c r="I95">
+        <f>SUM(I93:I94)</f>
+        <v>31560</v>
+      </c>
+      <c r="J95">
+        <f>SUM(J93:J94)</f>
+        <v>36880</v>
+      </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="16" t="s">
@@ -2836,14 +2856,89 @@
         <v>153</v>
       </c>
       <c r="B106" s="16">
-        <v>31909</v>
+        <v>31906</v>
       </c>
       <c r="C106" s="16">
         <v>37235</v>
       </c>
       <c r="D106" s="16">
         <f t="shared" si="7"/>
-        <v>5326</v>
+        <v>5329</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107" s="16">
+        <v>32382</v>
+      </c>
+      <c r="C107" s="16">
+        <v>37736</v>
+      </c>
+      <c r="D107" s="16">
+        <f t="shared" si="7"/>
+        <v>5354</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B108" s="16">
+        <v>32646</v>
+      </c>
+      <c r="C108" s="16">
+        <v>38007</v>
+      </c>
+      <c r="D108" s="16">
+        <f t="shared" si="7"/>
+        <v>5361</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B109" s="16">
+        <v>33164</v>
+      </c>
+      <c r="C109" s="16">
+        <v>38525</v>
+      </c>
+      <c r="D109" s="16">
+        <f t="shared" si="7"/>
+        <v>5361</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B110" s="16">
+        <v>33599</v>
+      </c>
+      <c r="C110" s="16">
+        <v>39462</v>
+      </c>
+      <c r="D110" s="16">
+        <f t="shared" si="7"/>
+        <v>5863</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B111" s="16">
+        <v>33826</v>
+      </c>
+      <c r="C111" s="16">
+        <v>39712</v>
+      </c>
+      <c r="D111" s="16">
+        <f t="shared" si="7"/>
+        <v>5886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - some of 8-F1 done.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
   <si>
     <t>1-1</t>
   </si>
@@ -485,6 +485,21 @@
   </si>
   <si>
     <t>Enter 8-F1</t>
+  </si>
+  <si>
+    <t>Checkpoint 580</t>
+  </si>
+  <si>
+    <t>Checkpoint 618</t>
+  </si>
+  <si>
+    <t>Frame ruled out due to moving logs</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2 coins remaining</t>
   </si>
 </sst>
 </file>
@@ -969,11 +984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N111"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B112" sqref="B112"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2602,7 +2617,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D111" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D116" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2716,7 +2731,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:7">
       <c r="A97" s="16" t="s">
         <v>20</v>
       </c>
@@ -2731,7 +2746,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:7">
       <c r="A98" s="16" t="s">
         <v>148</v>
       </c>
@@ -2746,7 +2761,7 @@
         <v>5290</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:7">
       <c r="A99" s="16" t="s">
         <v>150</v>
       </c>
@@ -2761,7 +2776,7 @@
         <v>5289</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:7">
       <c r="A100" s="16" t="s">
         <v>149</v>
       </c>
@@ -2776,7 +2791,7 @@
         <v>5287</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:7">
       <c r="A101" s="16" t="s">
         <v>20</v>
       </c>
@@ -2791,7 +2806,7 @@
         <v>5290</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:7">
       <c r="A102" s="16" t="s">
         <v>151</v>
       </c>
@@ -2806,7 +2821,7 @@
         <v>5294</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:7">
       <c r="A103" s="16" t="s">
         <v>152</v>
       </c>
@@ -2821,7 +2836,7 @@
         <v>5298</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:7">
       <c r="A104" s="16" t="s">
         <v>152</v>
       </c>
@@ -2836,7 +2851,7 @@
         <v>5315</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:7">
       <c r="A105" s="16" t="s">
         <v>46</v>
       </c>
@@ -2851,7 +2866,7 @@
         <v>5329</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:7">
       <c r="A106" s="16" t="s">
         <v>153</v>
       </c>
@@ -2866,7 +2881,7 @@
         <v>5329</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:7">
       <c r="A107" s="16" t="s">
         <v>154</v>
       </c>
@@ -2881,7 +2896,7 @@
         <v>5354</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:7">
       <c r="A108" s="16" t="s">
         <v>45</v>
       </c>
@@ -2896,7 +2911,7 @@
         <v>5361</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:7">
       <c r="A109" s="16" t="s">
         <v>141</v>
       </c>
@@ -2911,7 +2926,7 @@
         <v>5361</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:7">
       <c r="A110" s="16" t="s">
         <v>155</v>
       </c>
@@ -2926,7 +2941,7 @@
         <v>5863</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:7">
       <c r="A111" s="16" t="s">
         <v>95</v>
       </c>
@@ -2939,6 +2954,75 @@
       <c r="D111" s="16">
         <f t="shared" si="7"/>
         <v>5886</v>
+      </c>
+      <c r="G111" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B112" s="16">
+        <v>34022</v>
+      </c>
+      <c r="C112" s="16">
+        <v>39911</v>
+      </c>
+      <c r="D112" s="16">
+        <f t="shared" si="7"/>
+        <v>5889</v>
+      </c>
+      <c r="G112" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B113" s="16">
+        <v>34385</v>
+      </c>
+      <c r="C113" s="16">
+        <v>40279</v>
+      </c>
+      <c r="D113" s="16">
+        <f t="shared" si="7"/>
+        <v>5894</v>
+      </c>
+      <c r="G113" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B114" s="16">
+        <v>34776</v>
+      </c>
+      <c r="C114" s="16">
+        <v>40661</v>
+      </c>
+      <c r="D114" s="16">
+        <f t="shared" ref="D114" si="8">IF(B114 &gt;  0,C114-B114, 0)</f>
+        <v>5885</v>
+      </c>
+      <c r="G114">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" s="16">
+        <v>41485</v>
+      </c>
+      <c r="D115" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-F1 up to boss fight.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="163">
   <si>
     <t>1-1</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>2 coins remaining</t>
+  </si>
+  <si>
+    <t>Wall bounce dust</t>
+  </si>
+  <si>
+    <t>Checkpoint 626</t>
   </si>
 </sst>
 </file>
@@ -984,11 +990,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N115"/>
+  <dimension ref="A1:N119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2617,7 +2623,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D116" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D119" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2955,9 +2961,6 @@
         <f t="shared" si="7"/>
         <v>5886</v>
       </c>
-      <c r="G111" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="16" t="s">
@@ -2974,10 +2977,10 @@
         <v>5889</v>
       </c>
       <c r="G112" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="16" t="s">
         <v>157</v>
       </c>
@@ -2995,34 +2998,108 @@
         <v>159</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:10">
       <c r="A114" s="16" t="s">
         <v>160</v>
       </c>
       <c r="B114" s="16">
-        <v>34776</v>
+        <v>34767</v>
       </c>
       <c r="C114" s="16">
         <v>40661</v>
       </c>
       <c r="D114" s="16">
-        <f t="shared" ref="D114" si="8">IF(B114 &gt;  0,C114-B114, 0)</f>
-        <v>5885</v>
-      </c>
-      <c r="G114">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
+        <f t="shared" ref="D114:D118" si="8">IF(B114 &gt;  0,C114-B114, 0)</f>
+        <v>5894</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B115" s="16">
+        <v>34904</v>
+      </c>
+      <c r="C115" s="16">
+        <v>40799</v>
+      </c>
+      <c r="D115" s="16">
+        <f t="shared" si="8"/>
+        <v>5895</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B116" s="16">
+        <v>34950</v>
+      </c>
+      <c r="C116" s="16">
+        <v>40846</v>
+      </c>
+      <c r="D116" s="16">
+        <f t="shared" si="8"/>
+        <v>5896</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B117" s="16">
+        <v>35025</v>
+      </c>
+      <c r="C117" s="16">
+        <v>40921</v>
+      </c>
+      <c r="D117" s="16">
+        <f t="shared" si="8"/>
+        <v>5896</v>
+      </c>
+      <c r="H117">
+        <v>41175</v>
+      </c>
+      <c r="J117">
+        <f>35282-74</f>
+        <v>35208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B118" s="16">
+        <v>35282</v>
+      </c>
+      <c r="C118" s="16">
+        <v>41175</v>
+      </c>
+      <c r="D118" s="16">
+        <f t="shared" si="8"/>
+        <v>5893</v>
+      </c>
+      <c r="H118">
+        <v>41101</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C115" s="16">
+      <c r="B119" s="16">
+        <v>35587</v>
+      </c>
+      <c r="C119" s="16">
         <v>41485</v>
       </c>
-      <c r="D115" s="16">
+      <c r="D119" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5898</v>
+      </c>
+      <c r="H119">
+        <f>H117-H118</f>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-F1 done but with bad HB manipulation
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="164">
   <si>
     <t>1-1</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>Checkpoint 626</t>
+  </si>
+  <si>
+    <t>Boss - 4000 appears</t>
   </si>
 </sst>
 </file>
@@ -990,11 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2623,7 +2626,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D119" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D121" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2980,7 +2983,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:7">
       <c r="A113" s="16" t="s">
         <v>157</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:7">
       <c r="A114" s="16" t="s">
         <v>160</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>5894</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:7">
       <c r="A115" s="16" t="s">
         <v>161</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>5895</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:7">
       <c r="A116" s="16" t="s">
         <v>161</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>5896</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:7">
       <c r="A117" s="16" t="s">
         <v>161</v>
       </c>
@@ -3057,15 +3060,8 @@
         <f t="shared" si="8"/>
         <v>5896</v>
       </c>
-      <c r="H117">
-        <v>41175</v>
-      </c>
-      <c r="J117">
-        <f>35282-74</f>
-        <v>35208</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" s="16" t="s">
         <v>162</v>
       </c>
@@ -3079,11 +3075,8 @@
         <f t="shared" si="8"/>
         <v>5893</v>
       </c>
-      <c r="H118">
-        <v>41101</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="16" t="s">
         <v>37</v>
       </c>
@@ -3097,9 +3090,35 @@
         <f t="shared" si="7"/>
         <v>5898</v>
       </c>
-      <c r="H119">
-        <f>H117-H118</f>
-        <v>74</v>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B120" s="16">
+        <v>35856</v>
+      </c>
+      <c r="C120" s="16">
+        <v>41774</v>
+      </c>
+      <c r="D120" s="16">
+        <f t="shared" si="7"/>
+        <v>5918</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B121" s="16">
+        <v>36493</v>
+      </c>
+      <c r="C121" s="16">
+        <v>42408</v>
+      </c>
+      <c r="D121" s="16">
+        <f t="shared" si="7"/>
+        <v>5915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - got the right hammer bros manipulation but it only wants to give a mini-mushroom /o\
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="165">
   <si>
     <t>1-1</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>Boss - 4000 appears</t>
+  </si>
+  <si>
+    <t>Enter 8-3</t>
   </si>
 </sst>
 </file>
@@ -993,11 +996,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:N124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2626,7 +2629,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D121" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D123" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -3111,14 +3114,49 @@
         <v>126</v>
       </c>
       <c r="B121" s="16">
-        <v>36493</v>
+        <v>36497</v>
       </c>
       <c r="C121" s="16">
         <v>42408</v>
       </c>
       <c r="D121" s="16">
         <f t="shared" si="7"/>
-        <v>5915</v>
+        <v>5911</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B122" s="16">
+        <v>37189</v>
+      </c>
+      <c r="C122" s="16">
+        <v>43787</v>
+      </c>
+      <c r="D122" s="16">
+        <f t="shared" si="7"/>
+        <v>6598</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B123" s="16">
+        <v>37416</v>
+      </c>
+      <c r="C123" s="16">
+        <v>44032</v>
+      </c>
+      <c r="D123" s="16">
+        <f t="shared" si="7"/>
+        <v>6616</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="C124" s="16">
+        <v>44249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 9 frames faster upon entering 8-3.  Still can't avoid the mini-mushroom though.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -3144,14 +3144,14 @@
         <v>128</v>
       </c>
       <c r="B123" s="16">
-        <v>37416</v>
+        <v>37409</v>
       </c>
       <c r="C123" s="16">
         <v>44032</v>
       </c>
       <c r="D123" s="16">
         <f t="shared" si="7"/>
-        <v>6616</v>
+        <v>6623</v>
       </c>
     </row>
     <row r="124" spans="1:7">

</xml_diff>

<commit_message>
NSMB - 8-3 Done & some of 8-4
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="169">
   <si>
     <t>1-1</t>
   </si>
@@ -512,6 +512,18 @@
   </si>
   <si>
     <t>Enter 8-3</t>
+  </si>
+  <si>
+    <t>Checkpoint Rail 12582912</t>
+  </si>
+  <si>
+    <t>Checkpoint 460</t>
+  </si>
+  <si>
+    <t>Cehckpiont 1449</t>
+  </si>
+  <si>
+    <t>Enter 8-4</t>
   </si>
 </sst>
 </file>
@@ -996,11 +1008,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N124"/>
+  <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2629,7 +2641,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D123" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D132" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -2986,7 +2998,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:11">
       <c r="A113" s="16" t="s">
         <v>157</v>
       </c>
@@ -3004,7 +3016,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:11">
       <c r="A114" s="16" t="s">
         <v>160</v>
       </c>
@@ -3019,7 +3031,7 @@
         <v>5894</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:11">
       <c r="A115" s="16" t="s">
         <v>161</v>
       </c>
@@ -3034,7 +3046,7 @@
         <v>5895</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:11">
       <c r="A116" s="16" t="s">
         <v>161</v>
       </c>
@@ -3048,8 +3060,14 @@
         <f t="shared" si="8"/>
         <v>5896</v>
       </c>
-    </row>
-    <row r="117" spans="1:7">
+      <c r="J116">
+        <v>35610</v>
+      </c>
+      <c r="K116">
+        <v>35604</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="16" t="s">
         <v>161</v>
       </c>
@@ -3064,7 +3082,7 @@
         <v>5896</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:11">
       <c r="A118" s="16" t="s">
         <v>162</v>
       </c>
@@ -3079,7 +3097,7 @@
         <v>5893</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:11">
       <c r="A119" s="16" t="s">
         <v>37</v>
       </c>
@@ -3094,7 +3112,7 @@
         <v>5898</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:11">
       <c r="A120" s="16" t="s">
         <v>163</v>
       </c>
@@ -3109,7 +3127,7 @@
         <v>5918</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:11">
       <c r="A121" s="16" t="s">
         <v>126</v>
       </c>
@@ -3124,39 +3142,169 @@
         <v>5911</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:11">
       <c r="A122" s="16" t="s">
         <v>164</v>
       </c>
       <c r="B122" s="16">
-        <v>37189</v>
+        <v>37222</v>
       </c>
       <c r="C122" s="16">
         <v>43787</v>
       </c>
       <c r="D122" s="16">
         <f t="shared" si="7"/>
-        <v>6598</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
+        <v>6565</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="16" t="s">
         <v>128</v>
       </c>
       <c r="B123" s="16">
-        <v>37409</v>
+        <v>37448</v>
       </c>
       <c r="C123" s="16">
         <v>44032</v>
       </c>
       <c r="D123" s="16">
         <f t="shared" si="7"/>
-        <v>6623</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
+        <v>6584</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="16">
+        <v>37664</v>
+      </c>
       <c r="C124" s="16">
         <v>44249</v>
+      </c>
+      <c r="D124" s="16">
+        <f t="shared" si="7"/>
+        <v>6585</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B125" s="16">
+        <v>37919</v>
+      </c>
+      <c r="C125" s="16">
+        <v>44527</v>
+      </c>
+      <c r="D125" s="16">
+        <f t="shared" si="7"/>
+        <v>6608</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B126" s="16">
+        <v>39165</v>
+      </c>
+      <c r="C126" s="16">
+        <v>45775</v>
+      </c>
+      <c r="D126" s="16">
+        <f t="shared" si="7"/>
+        <v>6610</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B127" s="16">
+        <v>39722</v>
+      </c>
+      <c r="C127" s="16">
+        <v>46333</v>
+      </c>
+      <c r="D127" s="16">
+        <f t="shared" si="7"/>
+        <v>6611</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128" s="16">
+        <v>41771</v>
+      </c>
+      <c r="C128" s="16">
+        <v>48401</v>
+      </c>
+      <c r="D128" s="16">
+        <f t="shared" si="7"/>
+        <v>6630</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B129" s="16">
+        <v>42012</v>
+      </c>
+      <c r="C129" s="16">
+        <v>48651</v>
+      </c>
+      <c r="D129" s="16">
+        <f t="shared" si="7"/>
+        <v>6639</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130" s="16">
+        <v>42526</v>
+      </c>
+      <c r="C130" s="16">
+        <v>49165</v>
+      </c>
+      <c r="D130" s="16">
+        <f t="shared" si="7"/>
+        <v>6639</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="16">
+        <v>42919</v>
+      </c>
+      <c r="C131" s="16">
+        <v>49956</v>
+      </c>
+      <c r="D131" s="16">
+        <f t="shared" si="7"/>
+        <v>7037</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B132" s="16">
+        <v>43147</v>
+      </c>
+      <c r="C132" s="16">
+        <v>50203</v>
+      </c>
+      <c r="D132" s="16">
+        <f t="shared" si="7"/>
+        <v>7056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - Fix desync in 8-3 but of course bad map movement.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -1012,7 +1012,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B133" sqref="B133"/>
+      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3252,14 +3252,14 @@
         <v>45</v>
       </c>
       <c r="B129" s="16">
-        <v>42012</v>
+        <v>42009</v>
       </c>
       <c r="C129" s="16">
         <v>48651</v>
       </c>
       <c r="D129" s="16">
         <f t="shared" si="7"/>
-        <v>6639</v>
+        <v>6642</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3267,14 +3267,14 @@
         <v>141</v>
       </c>
       <c r="B130" s="16">
-        <v>42526</v>
+        <v>42523</v>
       </c>
       <c r="C130" s="16">
         <v>49165</v>
       </c>
       <c r="D130" s="16">
         <f t="shared" si="7"/>
-        <v>6639</v>
+        <v>6642</v>
       </c>
     </row>
     <row r="131" spans="1:4">

</xml_diff>

<commit_message>
NSMB - 8-4 done.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="170">
   <si>
     <t>1-1</t>
   </si>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>Cehckpiont 1449</t>
+  </si>
+  <si>
+    <t>Enter 8-C</t>
   </si>
   <si>
     <t>Enter 8-4</t>
@@ -1008,11 +1011,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N132"/>
+  <dimension ref="A1:N135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2641,7 +2644,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D132" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D135" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -3279,17 +3282,17 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B131" s="16">
-        <v>42919</v>
+        <v>42949</v>
       </c>
       <c r="C131" s="16">
         <v>49956</v>
       </c>
       <c r="D131" s="16">
         <f t="shared" si="7"/>
-        <v>7037</v>
+        <v>7007</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3297,14 +3300,59 @@
         <v>95</v>
       </c>
       <c r="B132" s="16">
-        <v>43147</v>
+        <v>43175</v>
       </c>
       <c r="C132" s="16">
         <v>50203</v>
       </c>
       <c r="D132" s="16">
         <f t="shared" si="7"/>
-        <v>7056</v>
+        <v>7028</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B133" s="16">
+        <v>44628</v>
+      </c>
+      <c r="C133" s="16">
+        <v>51659</v>
+      </c>
+      <c r="D133" s="16">
+        <f t="shared" si="7"/>
+        <v>7031</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B134" s="16">
+        <v>45146</v>
+      </c>
+      <c r="C134" s="16">
+        <v>52177</v>
+      </c>
+      <c r="D134" s="16">
+        <f t="shared" si="7"/>
+        <v>7031</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B135" s="16">
+        <v>45524</v>
+      </c>
+      <c r="C135" s="16">
+        <v>52978</v>
+      </c>
+      <c r="D135" s="16">
+        <f t="shared" si="7"/>
+        <v>7454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8-C done.  9163 frames ahead upon entering 8-5
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="179">
   <si>
     <t>1-1</t>
   </si>
@@ -527,6 +527,33 @@
   </si>
   <si>
     <t>Enter 8-4</t>
+  </si>
+  <si>
+    <t>Checkpoint 89</t>
+  </si>
+  <si>
+    <t>Checkpoint 404</t>
+  </si>
+  <si>
+    <t>Checkpoint 1037</t>
+  </si>
+  <si>
+    <t>Checkpoint 1534</t>
+  </si>
+  <si>
+    <t>Checkpoint 1836</t>
+  </si>
+  <si>
+    <t>Checkpoitn 2224</t>
+  </si>
+  <si>
+    <t>Checkpoint 2586</t>
+  </si>
+  <si>
+    <t>Touch button</t>
+  </si>
+  <si>
+    <t>Enter 8-5</t>
   </si>
 </sst>
 </file>
@@ -1011,11 +1038,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N135"/>
+  <dimension ref="A1:N148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2644,7 +2671,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D135" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D148" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -3353,6 +3380,201 @@
       <c r="D135" s="16">
         <f t="shared" si="7"/>
         <v>7454</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B136" s="16">
+        <v>45752</v>
+      </c>
+      <c r="C136" s="16">
+        <v>53228</v>
+      </c>
+      <c r="D136" s="16">
+        <f t="shared" si="7"/>
+        <v>7476</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B137" s="16">
+        <v>45830</v>
+      </c>
+      <c r="C137" s="16">
+        <v>53306</v>
+      </c>
+      <c r="D137" s="16">
+        <f t="shared" si="7"/>
+        <v>7476</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B138" s="16">
+        <v>45929</v>
+      </c>
+      <c r="C138" s="16">
+        <v>53405</v>
+      </c>
+      <c r="D138" s="16">
+        <f t="shared" si="7"/>
+        <v>7476</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B139" s="16">
+        <v>46124</v>
+      </c>
+      <c r="C139" s="16">
+        <v>53602</v>
+      </c>
+      <c r="D139" s="16">
+        <f t="shared" si="7"/>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B140" s="16">
+        <v>46279</v>
+      </c>
+      <c r="C140" s="16">
+        <v>53758</v>
+      </c>
+      <c r="D140" s="16">
+        <f t="shared" si="7"/>
+        <v>7479</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B141" s="16">
+        <v>46376</v>
+      </c>
+      <c r="C141" s="16">
+        <v>53854</v>
+      </c>
+      <c r="D141" s="16">
+        <f t="shared" si="7"/>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B142" s="16">
+        <v>46504</v>
+      </c>
+      <c r="C142" s="16">
+        <v>53982</v>
+      </c>
+      <c r="D142" s="16">
+        <f t="shared" si="7"/>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B143" s="16">
+        <v>46624</v>
+      </c>
+      <c r="C143" s="16">
+        <v>54102</v>
+      </c>
+      <c r="D143" s="16">
+        <f t="shared" si="7"/>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B144" s="16">
+        <v>46876</v>
+      </c>
+      <c r="C144" s="16">
+        <v>54354</v>
+      </c>
+      <c r="D144" s="16">
+        <f t="shared" si="7"/>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B145" s="16">
+        <v>47892</v>
+      </c>
+      <c r="C145" s="16">
+        <v>55387</v>
+      </c>
+      <c r="D145" s="16">
+        <f t="shared" si="7"/>
+        <v>7495</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B146" s="16">
+        <v>48805</v>
+      </c>
+      <c r="C146" s="16">
+        <v>56300</v>
+      </c>
+      <c r="D146" s="16">
+        <f t="shared" si="7"/>
+        <v>7495</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B147" s="16">
+        <v>50431</v>
+      </c>
+      <c r="C147" s="16">
+        <v>59573</v>
+      </c>
+      <c r="D147" s="16">
+        <f t="shared" si="7"/>
+        <v>9142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B148" s="16">
+        <v>50658</v>
+      </c>
+      <c r="C148" s="16">
+        <v>59821</v>
+      </c>
+      <c r="D148" s="16">
+        <f t="shared" si="7"/>
+        <v>9163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - up through half of 8-6
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="193">
   <si>
     <t>1-1</t>
   </si>
@@ -544,9 +544,6 @@
     <t>Checkpoint 1836</t>
   </si>
   <si>
-    <t>Checkpoitn 2224</t>
-  </si>
-  <si>
     <t>Checkpoint 2586</t>
   </si>
   <si>
@@ -554,6 +551,51 @@
   </si>
   <si>
     <t>Enter 8-5</t>
+  </si>
+  <si>
+    <t>Checkpoint 2224</t>
+  </si>
+  <si>
+    <t>Checkpoint 271</t>
+  </si>
+  <si>
+    <t>Checkpoint 596/595</t>
+  </si>
+  <si>
+    <t>Checkoint 872/870</t>
+  </si>
+  <si>
+    <t>Checkpoint 1293/1291</t>
+  </si>
+  <si>
+    <t>Checkpoint 1945</t>
+  </si>
+  <si>
+    <t>Checkpoint 2354</t>
+  </si>
+  <si>
+    <t>Checkpoitn 2941</t>
+  </si>
+  <si>
+    <t>Get Flag</t>
+  </si>
+  <si>
+    <t>Enter 8-6</t>
+  </si>
+  <si>
+    <t>Land 1st Orange plat</t>
+  </si>
+  <si>
+    <t>Jump block</t>
+  </si>
+  <si>
+    <t>Jump Pipe</t>
+  </si>
+  <si>
+    <t>Push on spring</t>
+  </si>
+  <si>
+    <t>Spring off 2nd spring (sparks)</t>
   </si>
 </sst>
 </file>
@@ -1038,11 +1080,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N148"/>
+  <dimension ref="A1:N167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2671,7 +2713,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D148" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D167" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -3474,7 +3516,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="16" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B142" s="16">
         <v>46504</v>
@@ -3489,7 +3531,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B143" s="16">
         <v>46624</v>
@@ -3519,7 +3561,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B145" s="16">
         <v>47892</v>
@@ -3549,7 +3591,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B147" s="16">
         <v>50431</v>
@@ -3575,6 +3617,288 @@
       <c r="D148" s="16">
         <f t="shared" si="7"/>
         <v>9163</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B149" s="16">
+        <v>50797</v>
+      </c>
+      <c r="C149" s="16">
+        <v>59960</v>
+      </c>
+      <c r="D149" s="16">
+        <f t="shared" si="7"/>
+        <v>9163</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B150" s="16">
+        <v>50904</v>
+      </c>
+      <c r="C150" s="16">
+        <v>60068</v>
+      </c>
+      <c r="D150" s="16">
+        <f t="shared" si="7"/>
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B151" s="16">
+        <v>50995</v>
+      </c>
+      <c r="C151" s="16">
+        <v>60159</v>
+      </c>
+      <c r="D151" s="16">
+        <f t="shared" si="7"/>
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B152" s="16">
+        <v>51135</v>
+      </c>
+      <c r="C152" s="16">
+        <v>60299</v>
+      </c>
+      <c r="D152" s="16">
+        <f t="shared" si="7"/>
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B153" s="16">
+        <v>51352</v>
+      </c>
+      <c r="C153" s="16">
+        <v>60517</v>
+      </c>
+      <c r="D153" s="16">
+        <f t="shared" si="7"/>
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B154" s="16">
+        <v>51487</v>
+      </c>
+      <c r="C154" s="16">
+        <v>60652</v>
+      </c>
+      <c r="D154" s="16">
+        <f t="shared" si="7"/>
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B155" s="16">
+        <v>51681</v>
+      </c>
+      <c r="C155" s="16">
+        <v>60846</v>
+      </c>
+      <c r="D155" s="16">
+        <f t="shared" si="7"/>
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B156" s="16">
+        <v>52080</v>
+      </c>
+      <c r="C156" s="16">
+        <v>61248</v>
+      </c>
+      <c r="D156" s="16">
+        <f t="shared" si="7"/>
+        <v>9168</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B157" s="16">
+        <v>52250</v>
+      </c>
+      <c r="C157" s="16">
+        <v>61427</v>
+      </c>
+      <c r="D157" s="16">
+        <f t="shared" si="7"/>
+        <v>9177</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B158" s="16">
+        <v>52768</v>
+      </c>
+      <c r="C158" s="16">
+        <v>61945</v>
+      </c>
+      <c r="D158" s="16">
+        <f t="shared" si="7"/>
+        <v>9177</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B159" s="16">
+        <v>53104</v>
+      </c>
+      <c r="C159" s="16">
+        <v>62610</v>
+      </c>
+      <c r="D159" s="16">
+        <f t="shared" si="7"/>
+        <v>9506</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B160" s="16">
+        <v>53332</v>
+      </c>
+      <c r="C160" s="16">
+        <v>62861</v>
+      </c>
+      <c r="D160" s="16">
+        <f t="shared" si="7"/>
+        <v>9529</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B161" s="16">
+        <v>53477</v>
+      </c>
+      <c r="C161" s="16">
+        <v>63021</v>
+      </c>
+      <c r="D161" s="16">
+        <f t="shared" si="7"/>
+        <v>9544</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B162" s="16">
+        <v>53562</v>
+      </c>
+      <c r="C162" s="16">
+        <v>63110</v>
+      </c>
+      <c r="D162" s="16">
+        <f t="shared" si="7"/>
+        <v>9548</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="B163" s="16">
+        <v>53643</v>
+      </c>
+      <c r="C163" s="16">
+        <v>63206</v>
+      </c>
+      <c r="D163" s="16">
+        <f t="shared" si="7"/>
+        <v>9563</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B164" s="16">
+        <v>53813</v>
+      </c>
+      <c r="C164" s="16">
+        <v>63376</v>
+      </c>
+      <c r="D164" s="16">
+        <f t="shared" si="7"/>
+        <v>9563</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B165" s="16">
+        <v>53851</v>
+      </c>
+      <c r="C165" s="16">
+        <v>63425</v>
+      </c>
+      <c r="D165" s="16">
+        <f t="shared" si="7"/>
+        <v>9574</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B166" s="16">
+        <v>53952</v>
+      </c>
+      <c r="C166" s="16">
+        <v>63540</v>
+      </c>
+      <c r="D166" s="16">
+        <f t="shared" si="7"/>
+        <v>9588</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B167" s="16">
+        <v>54007</v>
+      </c>
+      <c r="C167" s="16">
+        <v>63597</v>
+      </c>
+      <c r="D167" s="16">
+        <f t="shared" si="7"/>
+        <v>9590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-7 Begin
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="195">
   <si>
     <t>1-1</t>
   </si>
@@ -596,6 +596,12 @@
   </si>
   <si>
     <t>Spring off 2nd spring (sparks)</t>
+  </si>
+  <si>
+    <t>Begin Pipe Enter</t>
+  </si>
+  <si>
+    <t>Enter 8-7</t>
   </si>
 </sst>
 </file>
@@ -1080,11 +1086,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N167"/>
+  <dimension ref="A1:N174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B168" sqref="B168"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2713,7 +2719,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D167" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D174" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -3899,6 +3905,111 @@
       <c r="D167" s="16">
         <f t="shared" si="7"/>
         <v>9590</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B168" s="16">
+        <v>54209</v>
+      </c>
+      <c r="C168" s="16">
+        <v>63819</v>
+      </c>
+      <c r="D168" s="16">
+        <f t="shared" si="7"/>
+        <v>9610</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B169" s="16">
+        <v>54368</v>
+      </c>
+      <c r="C169" s="16">
+        <v>64047</v>
+      </c>
+      <c r="D169" s="16">
+        <f t="shared" si="7"/>
+        <v>9679</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B170" s="16">
+        <v>54651</v>
+      </c>
+      <c r="C170" s="16">
+        <v>64335</v>
+      </c>
+      <c r="D170" s="16">
+        <f t="shared" si="7"/>
+        <v>9684</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B171" s="16">
+        <v>54872</v>
+      </c>
+      <c r="C171" s="16">
+        <v>64568</v>
+      </c>
+      <c r="D171" s="16">
+        <f t="shared" si="7"/>
+        <v>9696</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B172" s="16">
+        <v>55390</v>
+      </c>
+      <c r="C172" s="16">
+        <v>65086</v>
+      </c>
+      <c r="D172" s="16">
+        <f t="shared" si="7"/>
+        <v>9696</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B173" s="16">
+        <v>55725</v>
+      </c>
+      <c r="C173" s="16">
+        <v>65479</v>
+      </c>
+      <c r="D173" s="16">
+        <f t="shared" si="7"/>
+        <v>9754</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B174" s="16">
+        <v>55958</v>
+      </c>
+      <c r="C174" s="16">
+        <v>66009</v>
+      </c>
+      <c r="D174" s="16">
+        <f t="shared" si="7"/>
+        <v>10051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - Begin 8-8
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="209">
   <si>
     <t>1-1</t>
   </si>
@@ -602,6 +602,48 @@
   </si>
   <si>
     <t>Enter 8-7</t>
+  </si>
+  <si>
+    <t>Checkpoint 791</t>
+  </si>
+  <si>
+    <t>Land on Koopa</t>
+  </si>
+  <si>
+    <t>Checkpoint 1702</t>
+  </si>
+  <si>
+    <t>Checkpoint 1927</t>
+  </si>
+  <si>
+    <t>Checkpoint 2230</t>
+  </si>
+  <si>
+    <t>Checkpoint 2421</t>
+  </si>
+  <si>
+    <t>Checkpoint 2550</t>
+  </si>
+  <si>
+    <t>Checkpoint 2927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkpoint </t>
+  </si>
+  <si>
+    <t>Checkpoint 3271</t>
+  </si>
+  <si>
+    <t>Checkpoint 3576</t>
+  </si>
+  <si>
+    <t>Enter 8-8</t>
+  </si>
+  <si>
+    <t>Blast out of pipe</t>
+  </si>
+  <si>
+    <t>End lLevel</t>
   </si>
 </sst>
 </file>
@@ -1086,11 +1128,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N174"/>
+  <dimension ref="A1:N191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2719,7 +2761,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D174" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D191" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -4010,6 +4052,261 @@
       <c r="D174" s="16">
         <f t="shared" si="7"/>
         <v>10051</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B175" s="16">
+        <v>56265</v>
+      </c>
+      <c r="C175" s="16">
+        <v>66317</v>
+      </c>
+      <c r="D175" s="16">
+        <f t="shared" si="7"/>
+        <v>10052</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B176" s="16">
+        <v>56378</v>
+      </c>
+      <c r="C176" s="16">
+        <v>66431</v>
+      </c>
+      <c r="D176" s="16">
+        <f t="shared" si="7"/>
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B177" s="16">
+        <v>56428</v>
+      </c>
+      <c r="C177" s="16">
+        <v>66483</v>
+      </c>
+      <c r="D177" s="16">
+        <f t="shared" si="7"/>
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B178" s="16">
+        <v>56640</v>
+      </c>
+      <c r="C178" s="16">
+        <v>66695</v>
+      </c>
+      <c r="D178" s="16">
+        <f t="shared" si="7"/>
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B179" s="16">
+        <v>56715</v>
+      </c>
+      <c r="C179" s="16">
+        <v>66770</v>
+      </c>
+      <c r="D179" s="16">
+        <f t="shared" si="7"/>
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B180" s="16">
+        <v>56898</v>
+      </c>
+      <c r="C180" s="16">
+        <v>66954</v>
+      </c>
+      <c r="D180" s="16">
+        <f t="shared" si="7"/>
+        <v>10056</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B181" s="16">
+        <v>56982</v>
+      </c>
+      <c r="C181" s="16">
+        <v>67039</v>
+      </c>
+      <c r="D181" s="16">
+        <f t="shared" si="7"/>
+        <v>10057</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B182" s="16">
+        <v>57020</v>
+      </c>
+      <c r="C182" s="16">
+        <v>67079</v>
+      </c>
+      <c r="D182" s="16">
+        <f t="shared" si="7"/>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B183" s="16">
+        <v>57085</v>
+      </c>
+      <c r="C183" s="16">
+        <v>67144</v>
+      </c>
+      <c r="D183" s="16">
+        <f t="shared" si="7"/>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B184" s="16">
+        <v>57134</v>
+      </c>
+      <c r="C184" s="16">
+        <v>67193</v>
+      </c>
+      <c r="D184" s="16">
+        <f t="shared" si="7"/>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B185" s="16">
+        <v>57234</v>
+      </c>
+      <c r="C185" s="16">
+        <v>67293</v>
+      </c>
+      <c r="D185" s="16">
+        <f t="shared" si="7"/>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B186" s="16">
+        <v>57309</v>
+      </c>
+      <c r="C186" s="16">
+        <v>67368</v>
+      </c>
+      <c r="D186" s="16">
+        <f t="shared" si="7"/>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B187" s="16">
+        <v>57531</v>
+      </c>
+      <c r="C187" s="16">
+        <v>67591</v>
+      </c>
+      <c r="D187" s="16">
+        <f t="shared" si="7"/>
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B188" s="16">
+        <v>57771</v>
+      </c>
+      <c r="C188" s="16">
+        <v>67831</v>
+      </c>
+      <c r="D188" s="16">
+        <f t="shared" si="7"/>
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B189" s="16">
+        <v>58289</v>
+      </c>
+      <c r="C189" s="16">
+        <v>68349</v>
+      </c>
+      <c r="D189" s="16">
+        <f t="shared" si="7"/>
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B190" s="16">
+        <v>58622</v>
+      </c>
+      <c r="C190" s="16">
+        <v>69018</v>
+      </c>
+      <c r="D190" s="16">
+        <f t="shared" si="7"/>
+        <v>10396</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B191" s="16">
+        <v>58848</v>
+      </c>
+      <c r="C191" s="16">
+        <v>69265</v>
+      </c>
+      <c r="D191" s="16">
+        <f t="shared" si="7"/>
+        <v>10417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-8 & some of 8-F2 done.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="215">
   <si>
     <t>1-1</t>
   </si>
@@ -644,6 +644,24 @@
   </si>
   <si>
     <t>End lLevel</t>
+  </si>
+  <si>
+    <t>Checkpoint 1633</t>
+  </si>
+  <si>
+    <t>Checkpoint 1946/1944</t>
+  </si>
+  <si>
+    <t>Checkpoint 2388/2385</t>
+  </si>
+  <si>
+    <t>Checkpoint 2896/2895</t>
+  </si>
+  <si>
+    <t>Enter 8-F2</t>
+  </si>
+  <si>
+    <t>Platform 1st Move</t>
   </si>
 </sst>
 </file>
@@ -1128,11 +1146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N191"/>
+  <dimension ref="A1:N200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B192" sqref="B192"/>
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2761,7 +2779,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D191" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D200" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -4307,6 +4325,141 @@
       <c r="D191" s="16">
         <f t="shared" si="7"/>
         <v>10417</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B192" s="16">
+        <v>59432</v>
+      </c>
+      <c r="C192" s="16">
+        <v>69850</v>
+      </c>
+      <c r="D192" s="16">
+        <f t="shared" si="7"/>
+        <v>10418</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B193" s="16">
+        <v>59610</v>
+      </c>
+      <c r="C193" s="16">
+        <v>70031</v>
+      </c>
+      <c r="D193" s="16">
+        <f t="shared" si="7"/>
+        <v>10421</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B194" s="16">
+        <v>59716</v>
+      </c>
+      <c r="C194" s="16">
+        <v>70137</v>
+      </c>
+      <c r="D194" s="16">
+        <f t="shared" si="7"/>
+        <v>10421</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B195" s="16">
+        <v>59863</v>
+      </c>
+      <c r="C195" s="16">
+        <v>70285</v>
+      </c>
+      <c r="D195" s="16">
+        <f t="shared" si="7"/>
+        <v>10422</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B196" s="16">
+        <v>60022</v>
+      </c>
+      <c r="C196" s="16">
+        <v>70444</v>
+      </c>
+      <c r="D196" s="16">
+        <f t="shared" si="7"/>
+        <v>10422</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B197" s="16">
+        <v>60540</v>
+      </c>
+      <c r="C197" s="16">
+        <v>70962</v>
+      </c>
+      <c r="D197" s="16">
+        <f t="shared" si="7"/>
+        <v>10422</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B198" s="16">
+        <v>60909</v>
+      </c>
+      <c r="C198" s="16">
+        <v>71707</v>
+      </c>
+      <c r="D198" s="16">
+        <f t="shared" si="7"/>
+        <v>10798</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B199" s="16">
+        <v>61137</v>
+      </c>
+      <c r="C199" s="16">
+        <v>71957</v>
+      </c>
+      <c r="D199" s="16">
+        <f t="shared" si="7"/>
+        <v>10820</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B200" s="16">
+        <v>61238</v>
+      </c>
+      <c r="C200" s="16">
+        <v>72069</v>
+      </c>
+      <c r="D200" s="16">
+        <f t="shared" si="7"/>
+        <v>10831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-F2 - Up to boss fight.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="217">
   <si>
     <t>1-1</t>
   </si>
@@ -662,6 +662,12 @@
   </si>
   <si>
     <t>Platform 1st Move</t>
+  </si>
+  <si>
+    <t>Get 4000 on boss</t>
+  </si>
+  <si>
+    <t>Enter 8-Final</t>
   </si>
 </sst>
 </file>
@@ -1146,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N200"/>
+  <dimension ref="A1:N207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B201" sqref="B201"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2779,7 +2785,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D200" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D201" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -4460,6 +4466,69 @@
       <c r="D200" s="16">
         <f t="shared" si="7"/>
         <v>10831</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B201" s="16">
+        <v>69043</v>
+      </c>
+      <c r="C201" s="16">
+        <v>79905</v>
+      </c>
+      <c r="D201" s="16">
+        <f t="shared" si="7"/>
+        <v>10862</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C202" s="16">
+        <v>80190</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C203" s="16">
+        <v>80786</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C204" s="16">
+        <v>82543</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C205" s="16">
+        <v>82799</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C206" s="16">
+        <v>83249</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C207" s="16">
+        <v>83800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - Boss done
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -1156,7 +1156,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
+      <selection pane="bottomLeft" activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2785,7 +2785,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D201" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D202" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -4487,8 +4487,15 @@
       <c r="A202" s="16" t="s">
         <v>215</v>
       </c>
+      <c r="B202" s="16">
+        <v>69309</v>
+      </c>
       <c r="C202" s="16">
         <v>80190</v>
+      </c>
+      <c r="D202" s="16">
+        <f t="shared" si="7"/>
+        <v>10881</v>
       </c>
     </row>
     <row r="203" spans="1:4">

</xml_diff>

<commit_message>
NSMB - Most of last stage done!
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="220">
   <si>
     <t>1-1</t>
   </si>
@@ -668,6 +668,15 @@
   </si>
   <si>
     <t>Enter 8-Final</t>
+  </si>
+  <si>
+    <t>Note: not an absolute measure point</t>
+  </si>
+  <si>
+    <t>Checkpoint 1657</t>
+  </si>
+  <si>
+    <t>Approx (camera angle diffs)</t>
   </si>
 </sst>
 </file>
@@ -1152,11 +1161,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N207"/>
+  <dimension ref="A1:N216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B203" sqref="B203"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2785,7 +2794,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D202" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D216" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -4348,7 +4357,7 @@
         <v>10418</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:7">
       <c r="A193" s="16" t="s">
         <v>210</v>
       </c>
@@ -4363,7 +4372,7 @@
         <v>10421</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:7">
       <c r="A194" s="16" t="s">
         <v>211</v>
       </c>
@@ -4378,7 +4387,7 @@
         <v>10421</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:7">
       <c r="A195" s="16" t="s">
         <v>212</v>
       </c>
@@ -4393,7 +4402,7 @@
         <v>10422</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:7">
       <c r="A196" s="16" t="s">
         <v>45</v>
       </c>
@@ -4408,7 +4417,7 @@
         <v>10422</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:7">
       <c r="A197" s="16" t="s">
         <v>83</v>
       </c>
@@ -4423,7 +4432,7 @@
         <v>10422</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:7">
       <c r="A198" s="16" t="s">
         <v>213</v>
       </c>
@@ -4438,7 +4447,7 @@
         <v>10798</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:7">
       <c r="A199" s="16" t="s">
         <v>95</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>10820</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:7">
       <c r="A200" s="16" t="s">
         <v>214</v>
       </c>
@@ -4468,7 +4477,7 @@
         <v>10831</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:7">
       <c r="A201" s="16" t="s">
         <v>37</v>
       </c>
@@ -4483,7 +4492,7 @@
         <v>10862</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:7">
       <c r="A202" s="16" t="s">
         <v>215</v>
       </c>
@@ -4498,44 +4507,208 @@
         <v>10881</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:7">
       <c r="A203" s="16" t="s">
         <v>83</v>
       </c>
+      <c r="B203" s="16">
+        <v>69906</v>
+      </c>
       <c r="C203" s="16">
         <v>80786</v>
       </c>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="D203" s="16">
+        <f t="shared" si="7"/>
+        <v>10880</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7">
       <c r="A204" s="16" t="s">
         <v>216</v>
       </c>
+      <c r="B204" s="16">
+        <v>70786</v>
+      </c>
       <c r="C204" s="16">
         <v>82543</v>
       </c>
-    </row>
-    <row r="205" spans="1:4">
+      <c r="D204" s="16">
+        <f t="shared" si="7"/>
+        <v>11757</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7">
       <c r="A205" s="16" t="s">
         <v>95</v>
       </c>
+      <c r="B205" s="16">
+        <v>71017</v>
+      </c>
       <c r="C205" s="16">
         <v>82799</v>
       </c>
-    </row>
-    <row r="206" spans="1:4">
+      <c r="D205" s="16">
+        <f t="shared" si="7"/>
+        <v>11782</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7">
       <c r="A206" s="16" t="s">
         <v>37</v>
       </c>
+      <c r="B206" s="16">
+        <v>71467</v>
+      </c>
       <c r="C206" s="16">
         <v>83249</v>
       </c>
-    </row>
-    <row r="207" spans="1:4">
+      <c r="D206" s="16">
+        <f t="shared" si="7"/>
+        <v>11782</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
       <c r="A207" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B207" s="16">
+        <v>71725</v>
+      </c>
+      <c r="C207" s="16">
+        <v>83509</v>
+      </c>
+      <c r="D207" s="16">
+        <f t="shared" si="7"/>
+        <v>11784</v>
+      </c>
+      <c r="G207" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7">
+      <c r="A208" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C207" s="16">
+      <c r="B208" s="16">
+        <v>72016</v>
+      </c>
+      <c r="C208" s="16">
         <v>83800</v>
+      </c>
+      <c r="D208" s="16">
+        <f t="shared" si="7"/>
+        <v>11784</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7">
+      <c r="A209" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B209" s="16">
+        <v>72323</v>
+      </c>
+      <c r="C209" s="16">
+        <v>84128</v>
+      </c>
+      <c r="D209" s="16">
+        <f t="shared" si="7"/>
+        <v>11805</v>
+      </c>
+      <c r="G209" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
+      <c r="A210" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B210" s="16">
+        <v>72665</v>
+      </c>
+      <c r="C210" s="16">
+        <v>84487</v>
+      </c>
+      <c r="D210" s="16">
+        <f t="shared" si="7"/>
+        <v>11822</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
+      <c r="A211" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B211" s="16">
+        <v>73412</v>
+      </c>
+      <c r="C211" s="16">
+        <v>85239</v>
+      </c>
+      <c r="D211" s="16">
+        <f t="shared" si="7"/>
+        <v>11827</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7">
+      <c r="A212" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B212" s="16">
+        <v>73958</v>
+      </c>
+      <c r="C212" s="16">
+        <v>85786</v>
+      </c>
+      <c r="D212" s="16">
+        <f t="shared" si="7"/>
+        <v>11828</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="B213" s="16">
+        <v>74154</v>
+      </c>
+      <c r="C213" s="16">
+        <v>85983</v>
+      </c>
+      <c r="D213" s="16">
+        <f t="shared" si="7"/>
+        <v>11829</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
+      <c r="B214" s="16">
+        <v>74292</v>
+      </c>
+      <c r="C214" s="16">
+        <v>86121</v>
+      </c>
+      <c r="D214" s="16">
+        <f t="shared" si="7"/>
+        <v>11829</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
+      <c r="B215" s="16">
+        <v>74361</v>
+      </c>
+      <c r="C215" s="16">
+        <v>86190</v>
+      </c>
+      <c r="D215" s="16">
+        <f t="shared" si="7"/>
+        <v>11829</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7">
+      <c r="B216" s="16">
+        <v>74597</v>
+      </c>
+      <c r="C216" s="16">
+        <v>86424</v>
+      </c>
+      <c r="D216" s="16">
+        <f t="shared" si="7"/>
+        <v>11827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - movie done!!
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="231">
   <si>
     <t>1-1</t>
   </si>
@@ -677,6 +677,39 @@
   </si>
   <si>
     <t>Approx (camera angle diffs)</t>
+  </si>
+  <si>
+    <t>Speed = 2</t>
+  </si>
+  <si>
+    <t>Checkpoint 7/4</t>
+  </si>
+  <si>
+    <t>Checkpoint 305/304</t>
+  </si>
+  <si>
+    <t>Checkpoint 738/736</t>
+  </si>
+  <si>
+    <t>Checkpoint 1505/1503</t>
+  </si>
+  <si>
+    <t>Checkpoint 1742/1740</t>
+  </si>
+  <si>
+    <t>Checkpoint 2158</t>
+  </si>
+  <si>
+    <t>Enter Final Door</t>
+  </si>
+  <si>
+    <t>Speed = 0</t>
+  </si>
+  <si>
+    <t>End Input</t>
+  </si>
+  <si>
+    <t>Touch Button</t>
   </si>
 </sst>
 </file>
@@ -1161,11 +1194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N216"/>
+  <dimension ref="A1:N227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B217" sqref="B217"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B228" sqref="B228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2794,7 +2827,7 @@
         <v>31594</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" ref="D90:D216" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
+        <f t="shared" ref="D90:D227" si="7">IF(B90 &gt;  0,C90-B90, 0)</f>
         <v>4804</v>
       </c>
     </row>
@@ -4664,51 +4697,228 @@
       </c>
     </row>
     <row r="213" spans="1:7">
+      <c r="A213" s="16" t="s">
+        <v>107</v>
+      </c>
       <c r="B213" s="16">
-        <v>74154</v>
+        <v>74749</v>
       </c>
       <c r="C213" s="16">
-        <v>85983</v>
+        <v>86590</v>
       </c>
       <c r="D213" s="16">
         <f t="shared" si="7"/>
-        <v>11829</v>
+        <v>11841</v>
       </c>
     </row>
     <row r="214" spans="1:7">
+      <c r="A214" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="B214" s="16">
-        <v>74292</v>
+        <v>74982</v>
       </c>
       <c r="C214" s="16">
-        <v>86121</v>
+        <v>86830</v>
       </c>
       <c r="D214" s="16">
         <f t="shared" si="7"/>
-        <v>11829</v>
+        <v>11848</v>
       </c>
     </row>
     <row r="215" spans="1:7">
+      <c r="A215" s="16" t="s">
+        <v>220</v>
+      </c>
       <c r="B215" s="16">
-        <v>74361</v>
+        <v>75107</v>
       </c>
       <c r="C215" s="16">
-        <v>86190</v>
+        <v>86956</v>
       </c>
       <c r="D215" s="16">
-        <f t="shared" si="7"/>
-        <v>11829</v>
+        <f t="shared" ref="D215" si="9">IF(B215 &gt;  0,C215-B215, 0)</f>
+        <v>11849</v>
       </c>
     </row>
     <row r="216" spans="1:7">
+      <c r="A216" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="B216" s="16">
-        <v>74597</v>
+        <v>75280</v>
       </c>
       <c r="C216" s="16">
-        <v>86424</v>
+        <v>87129</v>
       </c>
       <c r="D216" s="16">
         <f t="shared" si="7"/>
-        <v>11827</v>
+        <v>11849</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
+      <c r="A217" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B217" s="16">
+        <v>75591</v>
+      </c>
+      <c r="C217" s="16">
+        <v>87443</v>
+      </c>
+      <c r="D217" s="16">
+        <f t="shared" si="7"/>
+        <v>11852</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B218" s="16">
+        <v>75741</v>
+      </c>
+      <c r="C218" s="16">
+        <v>87604</v>
+      </c>
+      <c r="D218" s="16">
+        <f t="shared" si="7"/>
+        <v>11863</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B219" s="16">
+        <v>75828</v>
+      </c>
+      <c r="C219" s="16">
+        <v>87692</v>
+      </c>
+      <c r="D219" s="16">
+        <f t="shared" si="7"/>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B220" s="16">
+        <v>75972</v>
+      </c>
+      <c r="C220" s="16">
+        <v>87836</v>
+      </c>
+      <c r="D220" s="16">
+        <f t="shared" si="7"/>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B221" s="16">
+        <v>76227</v>
+      </c>
+      <c r="C221" s="16">
+        <v>88091</v>
+      </c>
+      <c r="D221" s="16">
+        <f t="shared" si="7"/>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B222" s="16">
+        <v>76306</v>
+      </c>
+      <c r="C222" s="16">
+        <v>88170</v>
+      </c>
+      <c r="D222" s="16">
+        <f t="shared" si="7"/>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B223" s="16">
+        <v>76444</v>
+      </c>
+      <c r="C223" s="16">
+        <v>88308</v>
+      </c>
+      <c r="D223" s="16">
+        <f t="shared" si="7"/>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7">
+      <c r="A224" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B224" s="16">
+        <v>76741</v>
+      </c>
+      <c r="C224" s="16">
+        <v>88605</v>
+      </c>
+      <c r="D224" s="16">
+        <f t="shared" si="7"/>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B225" s="16">
+        <v>77063</v>
+      </c>
+      <c r="C225" s="16">
+        <v>88946</v>
+      </c>
+      <c r="D225" s="16">
+        <f t="shared" si="7"/>
+        <v>11883</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B226" s="16">
+        <v>77862</v>
+      </c>
+      <c r="C226" s="16">
+        <v>89784</v>
+      </c>
+      <c r="D226" s="16">
+        <f t="shared" si="7"/>
+        <v>11922</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="B227" s="16">
+        <v>77899</v>
+      </c>
+      <c r="C227" s="16">
+        <v>89784</v>
+      </c>
+      <c r="D227" s="16">
+        <f t="shared" si="7"/>
+        <v>11885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - Fix desync and begin preparing release folder.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -1198,7 +1198,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B228" sqref="B228"/>
+      <selection pane="bottomLeft" activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4896,14 +4896,14 @@
         <v>229</v>
       </c>
       <c r="B226" s="16">
-        <v>77862</v>
+        <v>77866</v>
       </c>
       <c r="C226" s="16">
         <v>89784</v>
       </c>
       <c r="D226" s="16">
         <f t="shared" si="7"/>
-        <v>11922</v>
+        <v>11918</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -4911,14 +4911,14 @@
         <v>230</v>
       </c>
       <c r="B227" s="16">
-        <v>77899</v>
+        <v>77902</v>
       </c>
       <c r="C227" s="16">
         <v>89784</v>
       </c>
       <c r="D227" s="16">
         <f t="shared" si="7"/>
-        <v>11885</v>
+        <v>11882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - Up to end of 1-2, 1-1 improved by 2 frames, 1-2 pasted from previous WIP
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="235">
   <si>
     <t>1-1</t>
   </si>
@@ -719,6 +719,9 @@
   </si>
   <si>
     <t>V5</t>
+  </si>
+  <si>
+    <t>"+2 to last time"</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1256,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1282,7 +1285,7 @@
       <c r="F1" s="38"/>
       <c r="G1">
         <f>E237</f>
-        <v>20</v>
+        <v>-52</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="19.5" thickTop="1">
@@ -1420,14 +1423,17 @@
         <v>45</v>
       </c>
       <c r="B13" s="16">
-        <v>4096</v>
+        <v>4094</v>
       </c>
       <c r="C13" s="16">
         <v>4146</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" ref="D13:D35" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>234</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1445,10 +1451,6 @@
       <c r="D14" s="16">
         <f t="shared" si="1"/>
         <v>50</v>
-      </c>
-      <c r="E14">
-        <f>D14-D9</f>
-        <v>20</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -1480,12 +1482,15 @@
       <c r="A17" s="16" t="s">
         <v>53</v>
       </c>
+      <c r="B17" s="16">
+        <v>5005</v>
+      </c>
       <c r="C17" s="16">
         <v>5057</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -1548,7 +1553,7 @@
       </c>
       <c r="E21">
         <f>D21-D17</f>
-        <v>0</v>
+        <v>-52</v>
       </c>
       <c r="G21" s="13"/>
     </row>
@@ -4129,7 +4134,7 @@
       <c r="D237" s="31"/>
       <c r="E237" s="32">
         <f>SUM(E1:E236)</f>
-        <v>20</v>
+        <v>-52</v>
       </c>
       <c r="F237" s="32" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
NSMB - 1-2 & 1-F of TRT copy/pasted into main wip, but bad luck after 1-F, needs to be manipulated.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -1255,8 +1255,8 @@
   <dimension ref="A1:I237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1285,7 +1285,7 @@
       <c r="F1" s="38"/>
       <c r="G1">
         <f>E237</f>
-        <v>-52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="19.5" thickTop="1">
@@ -1528,14 +1528,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="16">
-        <v>6864</v>
+        <v>6946</v>
       </c>
       <c r="C20" s="16">
         <v>6951</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1561,9 +1561,12 @@
       <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
+      <c r="B22" s="16">
+        <v>7769</v>
+      </c>
       <c r="D22" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7769</v>
       </c>
     </row>
     <row r="23" spans="1:9" outlineLevel="1">
@@ -1584,14 +1587,14 @@
         <v>75</v>
       </c>
       <c r="B24" s="16">
-        <v>8308</v>
+        <v>8176</v>
       </c>
       <c r="C24" s="16">
         <v>8406</v>
       </c>
       <c r="D24" s="16">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:9" outlineLevel="1">
@@ -1658,28 +1661,34 @@
       <c r="A30" s="18" t="s">
         <v>45</v>
       </c>
+      <c r="B30" s="16">
+        <v>10525</v>
+      </c>
       <c r="C30" s="16">
         <v>10626</v>
       </c>
       <c r="D30" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:9" outlineLevel="1">
       <c r="A31" s="16" t="s">
         <v>73</v>
       </c>
+      <c r="B31" s="16">
+        <v>11039</v>
+      </c>
       <c r="C31" s="16">
         <v>11140</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="E31">
         <f>D31-D25</f>
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1">
@@ -1694,12 +1703,15 @@
       <c r="A33" s="16" t="s">
         <v>212</v>
       </c>
+      <c r="B33" s="16">
+        <v>11512</v>
+      </c>
       <c r="C33" s="16">
         <v>11592</v>
       </c>
       <c r="D33" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:5" outlineLevel="1">
@@ -4134,7 +4146,7 @@
       <c r="D237" s="31"/>
       <c r="E237" s="32">
         <f>SUM(E1:E236)</f>
-        <v>-52</v>
+        <v>49</v>
       </c>
       <c r="F237" s="32" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
NSMB - Up to World 5 recorded, I haven't compared frame counts to Yoshi's WIP yet
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="135" windowWidth="16080" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="V4" sheetId="4" r:id="rId1"/>
+    <sheet name="V5" sheetId="4" r:id="rId1"/>
     <sheet name="V3" sheetId="2" r:id="rId2"/>
     <sheet name="V1" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="235">
   <si>
     <t>1-1</t>
   </si>
@@ -818,7 +818,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -895,11 +895,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -955,6 +964,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1252,11 +1262,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I237"/>
+  <dimension ref="A1:I236"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1264,6 +1274,7 @@
     <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="16"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1">
@@ -1284,7 +1295,7 @@
       </c>
       <c r="F1" s="38"/>
       <c r="G1">
-        <f>E237</f>
+        <f>E236</f>
         <v>49</v>
       </c>
     </row>
@@ -1429,7 +1440,7 @@
         <v>4146</v>
       </c>
       <c r="D13" s="16">
-        <f t="shared" ref="D13:D35" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
+        <f t="shared" ref="D13:D34" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
         <v>52</v>
       </c>
       <c r="E13" t="s">
@@ -1656,8 +1667,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" outlineLevel="1">
+      <c r="H29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29">
+        <v>11039</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A30" s="18" t="s">
         <v>45</v>
       </c>
@@ -1671,8 +1688,14 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" outlineLevel="1">
+      <c r="H30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="41">
+        <v>11390</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A31" s="16" t="s">
         <v>73</v>
       </c>
@@ -1690,6 +1713,10 @@
         <f>D31-D25</f>
         <v>101</v>
       </c>
+      <c r="I31">
+        <f>I30-I29</f>
+        <v>351</v>
+      </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1">
       <c r="A32" s="20" t="s">
@@ -1716,655 +1743,664 @@
     </row>
     <row r="34" spans="1:5" outlineLevel="1">
       <c r="A34" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="B34" s="16">
+        <v>12463</v>
+      </c>
+      <c r="C34" s="16">
+        <v>12540</v>
       </c>
       <c r="D34" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" outlineLevel="1">
-      <c r="A35" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18.75">
+      <c r="A35" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+    </row>
+    <row r="36" spans="1:5" outlineLevel="1">
+      <c r="A36" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="1:5" outlineLevel="1">
+      <c r="A37" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="16">
+        <v>12911</v>
+      </c>
+      <c r="C37" s="16">
+        <v>12987</v>
+      </c>
+      <c r="D37" s="16">
+        <f t="shared" ref="D37:D84" si="2">IF(B37 &gt;  0,C37-B37, 0)</f>
         <v>76</v>
       </c>
-      <c r="C35" s="16">
-        <v>12540</v>
-      </c>
-      <c r="D35" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="18.75" collapsed="1">
-      <c r="A36" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-    </row>
-    <row r="37" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A37" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-    </row>
-    <row r="38" spans="1:5" hidden="1" outlineLevel="1">
+    </row>
+    <row r="38" spans="1:5" outlineLevel="1">
       <c r="A38" s="16" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C38" s="16">
-        <v>12987</v>
+        <v>13217</v>
       </c>
       <c r="D38" s="16">
-        <f t="shared" ref="D38:D85" si="2">IF(B38 &gt;  0,C38-B38, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" outlineLevel="1">
       <c r="A39" s="16" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="C39" s="16">
-        <v>13217</v>
+        <v>14776</v>
       </c>
       <c r="D39" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="40" spans="1:5" outlineLevel="1">
       <c r="A40" s="16" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C40" s="16">
-        <v>14776</v>
+        <v>15307</v>
       </c>
       <c r="D40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="41" spans="1:5" outlineLevel="1">
       <c r="A41" s="16" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="C41" s="16">
-        <v>15307</v>
+        <v>15573</v>
       </c>
       <c r="D41" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A42" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="16">
-        <v>15573</v>
-      </c>
-      <c r="D42" s="16">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" outlineLevel="1">
+      <c r="A42" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" outlineLevel="1">
+      <c r="A43" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="16">
+        <v>15722</v>
+      </c>
+      <c r="D43" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A43" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-    </row>
-    <row r="44" spans="1:5" hidden="1" outlineLevel="1">
+    </row>
+    <row r="44" spans="1:5" outlineLevel="1">
       <c r="A44" s="16" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C44" s="16">
-        <v>15722</v>
+        <v>15947</v>
       </c>
       <c r="D44" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="45" spans="1:5" outlineLevel="1">
       <c r="A45" s="16" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="C45" s="16">
-        <v>15947</v>
+        <v>16087</v>
       </c>
       <c r="D45" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:5" outlineLevel="1">
       <c r="A46" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="16">
-        <v>16087</v>
+        <v>17508</v>
       </c>
       <c r="D46" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="47" spans="1:5" outlineLevel="1">
       <c r="A47" s="16" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C47" s="16">
-        <v>17508</v>
+        <v>17579</v>
       </c>
       <c r="D47" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="48" spans="1:5" outlineLevel="1">
       <c r="A48" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" s="16">
-        <v>17579</v>
+        <v>17846</v>
       </c>
       <c r="D48" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="49" spans="1:9" outlineLevel="1">
       <c r="A49" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C49" s="16">
-        <v>17846</v>
+        <v>18368</v>
       </c>
       <c r="D49" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1" outlineLevel="1">
-      <c r="A50" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="16">
-        <v>18368</v>
-      </c>
-      <c r="D50" s="16">
+      <c r="E49">
+        <f>D49-D44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" outlineLevel="1">
+      <c r="A50" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+    </row>
+    <row r="51" spans="1:9" outlineLevel="1">
+      <c r="A51" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="16">
+        <v>18945</v>
+      </c>
+      <c r="D51" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E50">
-        <f>D50-D45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" hidden="1" outlineLevel="1">
-      <c r="A51" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-    </row>
-    <row r="52" spans="1:9" hidden="1" outlineLevel="1">
+    </row>
+    <row r="52" spans="1:9" outlineLevel="1">
       <c r="A52" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C52" s="16">
-        <v>18945</v>
+        <v>19177</v>
       </c>
       <c r="D52" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="E52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="I52" s="25"/>
+    </row>
+    <row r="53" spans="1:9" outlineLevel="1">
       <c r="A53" s="16" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C53" s="16">
-        <v>19177</v>
+        <v>20120</v>
       </c>
       <c r="D53" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="I53" s="25"/>
-    </row>
-    <row r="54" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="E53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" outlineLevel="1">
       <c r="A54" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C54" s="16">
-        <v>20120</v>
+        <v>20187</v>
       </c>
       <c r="D54" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="I54" s="26"/>
-    </row>
-    <row r="55" spans="1:9" hidden="1" outlineLevel="1">
+    </row>
+    <row r="55" spans="1:9" outlineLevel="1">
       <c r="A55" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C55" s="16">
-        <v>20187</v>
+        <v>20258</v>
       </c>
       <c r="D55" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="56" spans="1:9" outlineLevel="1">
       <c r="A56" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C56" s="16">
-        <v>20258</v>
+        <v>20351</v>
       </c>
       <c r="D56" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="57" spans="1:9" outlineLevel="1">
       <c r="A57" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C57" s="16">
-        <v>20351</v>
+        <v>20394</v>
       </c>
       <c r="D57" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="58" spans="1:9" outlineLevel="1">
       <c r="A58" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C58" s="16">
-        <v>20394</v>
+        <v>20465</v>
       </c>
       <c r="D58" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="59" spans="1:9" outlineLevel="1">
       <c r="A59" s="16" t="s">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="C59" s="16">
-        <v>20465</v>
+        <v>20658</v>
       </c>
       <c r="D59" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="60" spans="1:9" outlineLevel="1">
       <c r="A60" s="16" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="C60" s="16">
-        <v>20658</v>
+        <v>21172</v>
       </c>
       <c r="D60" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" outlineLevel="1">
-      <c r="A61" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61" s="16">
-        <v>21172</v>
-      </c>
-      <c r="D61" s="16">
+    <row r="61" spans="1:9" outlineLevel="1">
+      <c r="A61" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+    </row>
+    <row r="62" spans="1:9" outlineLevel="1">
+      <c r="A62" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" s="16">
+        <v>21661</v>
+      </c>
+      <c r="D62" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" outlineLevel="1">
-      <c r="A62" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-    </row>
-    <row r="63" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="63" spans="1:9" outlineLevel="1">
       <c r="A63" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C63" s="16">
-        <v>21661</v>
+        <v>21890</v>
       </c>
       <c r="D63" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" outlineLevel="1">
+    <row r="64" spans="1:9" outlineLevel="1">
       <c r="A64" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C64" s="16">
-        <v>21890</v>
+        <v>21929</v>
       </c>
       <c r="D64" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="65" spans="1:5" outlineLevel="1">
       <c r="A65" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C65" s="16">
-        <v>21929</v>
+        <v>21995</v>
       </c>
       <c r="D65" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="66" spans="1:5" outlineLevel="1">
       <c r="A66" s="16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C66" s="16">
-        <v>21995</v>
+        <v>22090</v>
       </c>
       <c r="D66" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="67" spans="1:5" outlineLevel="1">
       <c r="A67" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C67" s="16">
-        <v>22090</v>
+        <v>22121</v>
       </c>
       <c r="D67" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="68" spans="1:5" outlineLevel="1">
       <c r="A68" s="16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C68" s="16">
-        <v>22121</v>
+        <v>22330</v>
       </c>
       <c r="D68" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="69" spans="1:5" outlineLevel="1">
       <c r="A69" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C69" s="16">
-        <v>22330</v>
+        <v>22372</v>
       </c>
       <c r="D69" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="70" spans="1:5" outlineLevel="1">
       <c r="A70" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C70" s="16">
-        <v>22372</v>
+        <v>22388</v>
       </c>
       <c r="D70" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="71" spans="1:5" outlineLevel="1">
       <c r="A71" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C71" s="16">
-        <v>22388</v>
+        <v>22421</v>
       </c>
       <c r="D71" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="72" spans="1:5" outlineLevel="1">
       <c r="A72" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C72" s="16">
-        <v>22421</v>
+        <v>22454</v>
       </c>
       <c r="D72" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A73" s="16" t="s">
-        <v>125</v>
+    <row r="73" spans="1:5" outlineLevel="1">
+      <c r="A73" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="C73" s="16">
-        <v>22454</v>
+        <v>22708</v>
       </c>
       <c r="D73" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A74" s="27" t="s">
-        <v>126</v>
+    <row r="74" spans="1:5" outlineLevel="1">
+      <c r="A74" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="C74" s="16">
-        <v>22708</v>
+        <v>22829</v>
       </c>
       <c r="D74" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="75" spans="1:5" outlineLevel="1">
       <c r="A75" s="16" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C75" s="16">
-        <v>22829</v>
+        <v>23205</v>
       </c>
       <c r="D75" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="76" spans="1:5" outlineLevel="1">
       <c r="A76" s="16" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="C76" s="16">
-        <v>23205</v>
+        <v>23849</v>
       </c>
       <c r="D76" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="77" spans="1:5" outlineLevel="1">
       <c r="A77" s="16" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="C77" s="16">
-        <v>23849</v>
+        <v>24266</v>
       </c>
       <c r="D77" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="78" spans="1:5" outlineLevel="1">
       <c r="A78" s="16" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C78" s="16">
-        <v>24266</v>
+        <v>24570</v>
       </c>
       <c r="D78" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="79" spans="1:5" outlineLevel="1">
       <c r="A79" s="16" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C79" s="16">
-        <v>24570</v>
+        <v>25088</v>
       </c>
       <c r="D79" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A80" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C80" s="16">
-        <v>25088</v>
-      </c>
-      <c r="D80" s="16">
+      <c r="E79">
+        <f>D79-D63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" outlineLevel="1">
+      <c r="A80" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+    </row>
+    <row r="81" spans="1:5" outlineLevel="1">
+      <c r="A81" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C81" s="16">
+        <v>25472</v>
+      </c>
+      <c r="D81" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E80">
-        <f>D80-D64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A81" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-    </row>
-    <row r="82" spans="1:5" hidden="1" outlineLevel="1">
+    </row>
+    <row r="82" spans="1:5" outlineLevel="1">
       <c r="A82" s="16" t="s">
-        <v>216</v>
+        <v>95</v>
       </c>
       <c r="C82" s="16">
-        <v>25472</v>
+        <v>25697</v>
       </c>
       <c r="D82" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="83" spans="1:5" outlineLevel="1">
       <c r="A83" s="16" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="C83" s="16">
-        <v>25697</v>
+        <v>25830</v>
       </c>
       <c r="D83" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="84" spans="1:5" outlineLevel="1">
       <c r="A84" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C84" s="16">
-        <v>25830</v>
+        <v>26420</v>
       </c>
       <c r="D84" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A85" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C85" s="16">
-        <v>26420</v>
-      </c>
-      <c r="D85" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="18.75" collapsed="1">
-      <c r="A86" s="36" t="s">
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="18.75" collapsed="1">
+      <c r="A85" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="36"/>
+    </row>
+    <row r="86" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A86" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
     </row>
     <row r="87" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A87" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
+      <c r="A87" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" s="16">
+        <v>26790</v>
+      </c>
+      <c r="D87" s="16">
+        <f t="shared" ref="D87:D235" si="3">IF(B87 &gt;  0,C87-B87, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A88" s="16" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="C88" s="16">
-        <v>26790</v>
+        <v>27017</v>
       </c>
       <c r="D88" s="16">
-        <f t="shared" ref="D88:D236" si="3">IF(B88 &gt;  0,C88-B88, 0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A89" s="16" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="C89" s="16">
-        <v>27017</v>
+        <v>27730</v>
       </c>
       <c r="D89" s="16">
         <f t="shared" si="3"/>
@@ -2373,10 +2409,10 @@
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A90" s="16" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="C90" s="16">
-        <v>27730</v>
+        <v>28335</v>
       </c>
       <c r="D90" s="16">
         <f t="shared" si="3"/>
@@ -2385,46 +2421,46 @@
     </row>
     <row r="91" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A91" s="16" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C91" s="16">
-        <v>28335</v>
+        <v>28853</v>
       </c>
       <c r="D91" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E91">
+        <f>D91-D88</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A92" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C92" s="16">
-        <v>28853</v>
-      </c>
-      <c r="D92" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E92">
-        <f>D92-D89</f>
-        <v>0</v>
-      </c>
+      <c r="A92" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
     </row>
     <row r="93" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A93" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B93" s="29"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="29"/>
+      <c r="A93" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C93" s="16">
+        <v>29213</v>
+      </c>
+      <c r="D93" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A94" s="16" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C94" s="16">
-        <v>29213</v>
+        <v>29438</v>
       </c>
       <c r="D94" s="16">
         <f t="shared" si="3"/>
@@ -2433,10 +2469,10 @@
     </row>
     <row r="95" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A95" s="16" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="C95" s="16">
-        <v>29438</v>
+        <v>29585</v>
       </c>
       <c r="D95" s="16">
         <f t="shared" si="3"/>
@@ -2445,10 +2481,10 @@
     </row>
     <row r="96" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A96" s="16" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="C96" s="16">
-        <v>29585</v>
+        <v>29708</v>
       </c>
       <c r="D96" s="16">
         <f t="shared" si="3"/>
@@ -2457,10 +2493,10 @@
     </row>
     <row r="97" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A97" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C97" s="16">
-        <v>29708</v>
+        <v>29848</v>
       </c>
       <c r="D97" s="16">
         <f t="shared" si="3"/>
@@ -2469,10 +2505,10 @@
     </row>
     <row r="98" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A98" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C98" s="16">
-        <v>29848</v>
+        <v>29894</v>
       </c>
       <c r="D98" s="16">
         <f t="shared" si="3"/>
@@ -2481,10 +2517,10 @@
     </row>
     <row r="99" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A99" s="16" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="C99" s="16">
-        <v>29894</v>
+        <v>30331</v>
       </c>
       <c r="D99" s="16">
         <f t="shared" si="3"/>
@@ -2493,10 +2529,10 @@
     </row>
     <row r="100" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A100" s="16" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="C100" s="16">
-        <v>30331</v>
+        <v>30698</v>
       </c>
       <c r="D100" s="16">
         <f t="shared" si="3"/>
@@ -2505,10 +2541,10 @@
     </row>
     <row r="101" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A101" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C101" s="16">
-        <v>30698</v>
+        <v>30992</v>
       </c>
       <c r="D101" s="16">
         <f t="shared" si="3"/>
@@ -2520,7 +2556,7 @@
         <v>139</v>
       </c>
       <c r="C102" s="16">
-        <v>30992</v>
+        <v>31261</v>
       </c>
       <c r="D102" s="16">
         <f t="shared" si="3"/>
@@ -2529,10 +2565,10 @@
     </row>
     <row r="103" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A103" s="16" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="C103" s="16">
-        <v>31261</v>
+        <v>31543</v>
       </c>
       <c r="D103" s="16">
         <f t="shared" si="3"/>
@@ -2541,10 +2577,10 @@
     </row>
     <row r="104" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A104" s="16" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="C104" s="16">
-        <v>31543</v>
+        <v>31906</v>
       </c>
       <c r="D104" s="16">
         <f t="shared" si="3"/>
@@ -2553,10 +2589,10 @@
     </row>
     <row r="105" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A105" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C105" s="16">
-        <v>31906</v>
+        <v>32382</v>
       </c>
       <c r="D105" s="16">
         <f t="shared" si="3"/>
@@ -2565,10 +2601,10 @@
     </row>
     <row r="106" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A106" s="16" t="s">
-        <v>141</v>
+        <v>45</v>
       </c>
       <c r="C106" s="16">
-        <v>32382</v>
+        <v>32646</v>
       </c>
       <c r="D106" s="16">
         <f t="shared" si="3"/>
@@ -2577,46 +2613,46 @@
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A107" s="16" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C107" s="16">
-        <v>32646</v>
+        <v>33164</v>
       </c>
       <c r="D107" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E107">
+        <f>D107-D94</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A108" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C108" s="16">
-        <v>33164</v>
-      </c>
-      <c r="D108" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E108">
-        <f>D108-D95</f>
-        <v>0</v>
-      </c>
+      <c r="A108" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="29"/>
     </row>
     <row r="109" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A109" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B109" s="29"/>
-      <c r="C109" s="29"/>
-      <c r="D109" s="29"/>
+      <c r="A109" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C109" s="16">
+        <v>33599</v>
+      </c>
+      <c r="D109" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A110" s="16" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="C110" s="16">
-        <v>33599</v>
+        <v>33826</v>
       </c>
       <c r="D110" s="16">
         <f t="shared" si="3"/>
@@ -2625,10 +2661,10 @@
     </row>
     <row r="111" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A111" s="16" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C111" s="16">
-        <v>33826</v>
+        <v>34022</v>
       </c>
       <c r="D111" s="16">
         <f t="shared" si="3"/>
@@ -2637,10 +2673,10 @@
     </row>
     <row r="112" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A112" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C112" s="16">
-        <v>34022</v>
+        <v>34385</v>
       </c>
       <c r="D112" s="16">
         <f t="shared" si="3"/>
@@ -2649,25 +2685,25 @@
     </row>
     <row r="113" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A113" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C113" s="16">
-        <v>34385</v>
+        <v>34767</v>
       </c>
       <c r="D113" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D113:D117" si="4">IF(B113 &gt;  0,C113-B113, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A114" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C114" s="16">
-        <v>34767</v>
+        <v>34904</v>
       </c>
       <c r="D114" s="16">
-        <f t="shared" ref="D114:D118" si="4">IF(B114 &gt;  0,C114-B114, 0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2676,7 +2712,7 @@
         <v>146</v>
       </c>
       <c r="C115" s="16">
-        <v>34904</v>
+        <v>34950</v>
       </c>
       <c r="D115" s="16">
         <f t="shared" si="4"/>
@@ -2688,7 +2724,7 @@
         <v>146</v>
       </c>
       <c r="C116" s="16">
-        <v>34950</v>
+        <v>35025</v>
       </c>
       <c r="D116" s="16">
         <f t="shared" si="4"/>
@@ -2697,10 +2733,10 @@
     </row>
     <row r="117" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A117" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C117" s="16">
-        <v>35025</v>
+        <v>35282</v>
       </c>
       <c r="D117" s="16">
         <f t="shared" si="4"/>
@@ -2709,22 +2745,22 @@
     </row>
     <row r="118" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A118" s="16" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="C118" s="16">
-        <v>35282</v>
+        <v>35587</v>
       </c>
       <c r="D118" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A119" s="16" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="C119" s="16">
-        <v>35587</v>
+        <v>35856</v>
       </c>
       <c r="D119" s="16">
         <f t="shared" si="3"/>
@@ -2733,46 +2769,46 @@
     </row>
     <row r="120" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A120" s="16" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="C120" s="16">
-        <v>35856</v>
+        <v>36497</v>
       </c>
       <c r="D120" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E120">
+        <f>D120-D110</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A121" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C121" s="16">
-        <v>36497</v>
-      </c>
-      <c r="D121" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E121">
-        <f>D121-D111</f>
-        <v>0</v>
-      </c>
+      <c r="A121" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B121" s="29"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="29"/>
     </row>
     <row r="122" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A122" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="B122" s="29"/>
-      <c r="C122" s="29"/>
-      <c r="D122" s="29"/>
+      <c r="A122" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C122" s="16">
+        <v>37222</v>
+      </c>
+      <c r="D122" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A123" s="16" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="C123" s="16">
-        <v>37222</v>
+        <v>37448</v>
       </c>
       <c r="D123" s="16">
         <f t="shared" si="3"/>
@@ -2781,10 +2817,10 @@
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A124" s="16" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="C124" s="16">
-        <v>37448</v>
+        <v>37664</v>
       </c>
       <c r="D124" s="16">
         <f t="shared" si="3"/>
@@ -2793,10 +2829,10 @@
     </row>
     <row r="125" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A125" s="16" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="C125" s="16">
-        <v>37664</v>
+        <v>37919</v>
       </c>
       <c r="D125" s="16">
         <f t="shared" si="3"/>
@@ -2805,10 +2841,10 @@
     </row>
     <row r="126" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A126" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C126" s="16">
-        <v>37919</v>
+        <v>39165</v>
       </c>
       <c r="D126" s="16">
         <f t="shared" si="3"/>
@@ -2817,10 +2853,10 @@
     </row>
     <row r="127" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A127" s="16" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="C127" s="16">
-        <v>39165</v>
+        <v>39722</v>
       </c>
       <c r="D127" s="16">
         <f t="shared" si="3"/>
@@ -2829,10 +2865,10 @@
     </row>
     <row r="128" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A128" s="16" t="s">
-        <v>217</v>
+        <v>72</v>
       </c>
       <c r="C128" s="16">
-        <v>39722</v>
+        <v>41771</v>
       </c>
       <c r="D128" s="16">
         <f t="shared" si="3"/>
@@ -2841,10 +2877,10 @@
     </row>
     <row r="129" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A129" s="16" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C129" s="16">
-        <v>41771</v>
+        <v>42009</v>
       </c>
       <c r="D129" s="16">
         <f t="shared" si="3"/>
@@ -2853,46 +2889,46 @@
     </row>
     <row r="130" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A130" s="16" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C130" s="16">
-        <v>42009</v>
+        <v>42523</v>
       </c>
       <c r="D130" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E130">
+        <f>D130-D123</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A131" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C131" s="16">
-        <v>42523</v>
-      </c>
-      <c r="D131" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E131">
-        <f>D131-D124</f>
-        <v>0</v>
-      </c>
+      <c r="A131" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B131" s="29"/>
+      <c r="C131" s="29"/>
+      <c r="D131" s="29"/>
     </row>
     <row r="132" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A132" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="B132" s="29"/>
-      <c r="C132" s="29"/>
-      <c r="D132" s="29"/>
+      <c r="A132" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C132" s="16">
+        <v>42949</v>
+      </c>
+      <c r="D132" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A133" s="16" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
       <c r="C133" s="16">
-        <v>42949</v>
+        <v>43175</v>
       </c>
       <c r="D133" s="16">
         <f t="shared" si="3"/>
@@ -2901,10 +2937,10 @@
     </row>
     <row r="134" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A134" s="16" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="C134" s="16">
-        <v>43175</v>
+        <v>44628</v>
       </c>
       <c r="D134" s="16">
         <f t="shared" si="3"/>
@@ -2913,46 +2949,46 @@
     </row>
     <row r="135" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A135" s="16" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C135" s="16">
-        <v>44628</v>
+        <v>45146</v>
       </c>
       <c r="D135" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E135">
+        <f>D135-D133</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A136" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C136" s="16">
-        <v>45146</v>
-      </c>
-      <c r="D136" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E136">
-        <f>D136-D134</f>
-        <v>0</v>
-      </c>
+      <c r="A136" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="29"/>
     </row>
     <row r="137" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A137" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="B137" s="29"/>
-      <c r="C137" s="29"/>
-      <c r="D137" s="29"/>
+      <c r="A137" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C137" s="16">
+        <v>45524</v>
+      </c>
+      <c r="D137" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A138" s="16" t="s">
-        <v>225</v>
+        <v>95</v>
       </c>
       <c r="C138" s="16">
-        <v>45524</v>
+        <v>45752</v>
       </c>
       <c r="D138" s="16">
         <f t="shared" si="3"/>
@@ -2961,10 +2997,10 @@
     </row>
     <row r="139" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A139" s="16" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="C139" s="16">
-        <v>45752</v>
+        <v>45830</v>
       </c>
       <c r="D139" s="16">
         <f t="shared" si="3"/>
@@ -2973,10 +3009,10 @@
     </row>
     <row r="140" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A140" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140" s="16">
-        <v>45830</v>
+        <v>45929</v>
       </c>
       <c r="D140" s="16">
         <f t="shared" si="3"/>
@@ -2985,10 +3021,10 @@
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A141" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C141" s="16">
-        <v>45929</v>
+        <v>46124</v>
       </c>
       <c r="D141" s="16">
         <f t="shared" si="3"/>
@@ -2997,10 +3033,10 @@
     </row>
     <row r="142" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A142" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C142" s="16">
-        <v>46124</v>
+        <v>46279</v>
       </c>
       <c r="D142" s="16">
         <f t="shared" si="3"/>
@@ -3009,10 +3045,10 @@
     </row>
     <row r="143" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A143" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C143" s="16">
-        <v>46279</v>
+        <v>46376</v>
       </c>
       <c r="D143" s="16">
         <f t="shared" si="3"/>
@@ -3021,10 +3057,10 @@
     </row>
     <row r="144" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A144" s="16" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C144" s="16">
-        <v>46376</v>
+        <v>46504</v>
       </c>
       <c r="D144" s="16">
         <f t="shared" si="3"/>
@@ -3033,10 +3069,10 @@
     </row>
     <row r="145" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A145" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C145" s="16">
-        <v>46504</v>
+        <v>46624</v>
       </c>
       <c r="D145" s="16">
         <f t="shared" si="3"/>
@@ -3045,10 +3081,10 @@
     </row>
     <row r="146" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A146" s="16" t="s">
-        <v>158</v>
+        <v>37</v>
       </c>
       <c r="C146" s="16">
-        <v>46624</v>
+        <v>46876</v>
       </c>
       <c r="D146" s="16">
         <f t="shared" si="3"/>
@@ -3057,10 +3093,10 @@
     </row>
     <row r="147" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A147" s="16" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="C147" s="16">
-        <v>46876</v>
+        <v>47892</v>
       </c>
       <c r="D147" s="16">
         <f t="shared" si="3"/>
@@ -3069,46 +3105,46 @@
     </row>
     <row r="148" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A148" s="16" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="C148" s="16">
-        <v>47892</v>
+        <v>48805</v>
       </c>
       <c r="D148" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E148">
+        <f>D148-D138</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="149" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A149" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C149" s="16">
-        <v>48805</v>
-      </c>
-      <c r="D149" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E149">
-        <f>D149-D139</f>
-        <v>0</v>
-      </c>
+      <c r="A149" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B149" s="29"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="29"/>
     </row>
     <row r="150" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A150" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="B150" s="29"/>
-      <c r="C150" s="29"/>
-      <c r="D150" s="29"/>
+      <c r="A150" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C150" s="16">
+        <v>50431</v>
+      </c>
+      <c r="D150" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="151" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A151" s="16" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="C151" s="16">
-        <v>50431</v>
+        <v>50658</v>
       </c>
       <c r="D151" s="16">
         <f t="shared" si="3"/>
@@ -3117,10 +3153,10 @@
     </row>
     <row r="152" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A152" s="16" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="C152" s="16">
-        <v>50658</v>
+        <v>50797</v>
       </c>
       <c r="D152" s="16">
         <f t="shared" si="3"/>
@@ -3129,10 +3165,10 @@
     </row>
     <row r="153" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A153" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C153" s="16">
-        <v>50797</v>
+        <v>50904</v>
       </c>
       <c r="D153" s="16">
         <f t="shared" si="3"/>
@@ -3141,10 +3177,10 @@
     </row>
     <row r="154" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A154" s="16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C154" s="16">
-        <v>50904</v>
+        <v>50995</v>
       </c>
       <c r="D154" s="16">
         <f t="shared" si="3"/>
@@ -3153,10 +3189,10 @@
     </row>
     <row r="155" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A155" s="16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C155" s="16">
-        <v>50995</v>
+        <v>51135</v>
       </c>
       <c r="D155" s="16">
         <f t="shared" si="3"/>
@@ -3165,10 +3201,10 @@
     </row>
     <row r="156" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A156" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C156" s="16">
-        <v>51135</v>
+        <v>51352</v>
       </c>
       <c r="D156" s="16">
         <f t="shared" si="3"/>
@@ -3177,10 +3213,10 @@
     </row>
     <row r="157" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A157" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C157" s="16">
-        <v>51352</v>
+        <v>51487</v>
       </c>
       <c r="D157" s="16">
         <f t="shared" si="3"/>
@@ -3189,10 +3225,10 @@
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A158" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C158" s="16">
-        <v>51487</v>
+        <v>51681</v>
       </c>
       <c r="D158" s="16">
         <f t="shared" si="3"/>
@@ -3201,10 +3237,10 @@
     </row>
     <row r="159" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A159" s="16" t="s">
-        <v>168</v>
+        <v>72</v>
       </c>
       <c r="C159" s="16">
-        <v>51681</v>
+        <v>52080</v>
       </c>
       <c r="D159" s="16">
         <f t="shared" si="3"/>
@@ -3213,10 +3249,10 @@
     </row>
     <row r="160" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A160" s="16" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="C160" s="16">
-        <v>52080</v>
+        <v>52250</v>
       </c>
       <c r="D160" s="16">
         <f t="shared" si="3"/>
@@ -3225,46 +3261,46 @@
     </row>
     <row r="161" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A161" s="16" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="C161" s="16">
-        <v>52250</v>
+        <v>52768</v>
       </c>
       <c r="D161" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E161">
+        <f>D161-D151</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="162" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A162" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C162" s="16">
-        <v>52768</v>
-      </c>
-      <c r="D162" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E162">
-        <f>D162-D152</f>
-        <v>0</v>
-      </c>
+      <c r="A162" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B162" s="29"/>
+      <c r="C162" s="29"/>
+      <c r="D162" s="29"/>
     </row>
     <row r="163" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A163" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="B163" s="29"/>
-      <c r="C163" s="29"/>
-      <c r="D163" s="29"/>
+      <c r="A163" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C163" s="16">
+        <v>53104</v>
+      </c>
+      <c r="D163" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="164" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A164" s="16" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="C164" s="16">
-        <v>53104</v>
+        <v>53332</v>
       </c>
       <c r="D164" s="16">
         <f t="shared" si="3"/>
@@ -3273,10 +3309,10 @@
     </row>
     <row r="165" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A165" s="16" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
       <c r="C165" s="16">
-        <v>53332</v>
+        <v>53477</v>
       </c>
       <c r="D165" s="16">
         <f t="shared" si="3"/>
@@ -3285,10 +3321,10 @@
     </row>
     <row r="166" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A166" s="16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C166" s="16">
-        <v>53477</v>
+        <v>53562</v>
       </c>
       <c r="D166" s="16">
         <f t="shared" si="3"/>
@@ -3297,10 +3333,10 @@
     </row>
     <row r="167" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A167" s="16" t="s">
-        <v>173</v>
+        <v>104</v>
       </c>
       <c r="C167" s="16">
-        <v>53562</v>
+        <v>53643</v>
       </c>
       <c r="D167" s="16">
         <f t="shared" si="3"/>
@@ -3312,7 +3348,7 @@
         <v>104</v>
       </c>
       <c r="C168" s="16">
-        <v>53643</v>
+        <v>53813</v>
       </c>
       <c r="D168" s="16">
         <f t="shared" si="3"/>
@@ -3321,10 +3357,10 @@
     </row>
     <row r="169" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A169" s="16" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="C169" s="16">
-        <v>53813</v>
+        <v>53851</v>
       </c>
       <c r="D169" s="16">
         <f t="shared" si="3"/>
@@ -3333,10 +3369,10 @@
     </row>
     <row r="170" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A170" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C170" s="16">
-        <v>53851</v>
+        <v>53952</v>
       </c>
       <c r="D170" s="16">
         <f t="shared" si="3"/>
@@ -3345,10 +3381,10 @@
     </row>
     <row r="171" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A171" s="16" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C171" s="16">
-        <v>53952</v>
+        <v>54007</v>
       </c>
       <c r="D171" s="16">
         <f t="shared" si="3"/>
@@ -3357,10 +3393,10 @@
     </row>
     <row r="172" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A172" s="16" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="C172" s="16">
-        <v>54007</v>
+        <v>54209</v>
       </c>
       <c r="D172" s="16">
         <f t="shared" si="3"/>
@@ -3369,10 +3405,10 @@
     </row>
     <row r="173" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A173" s="16" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="C173" s="16">
-        <v>54209</v>
+        <v>54368</v>
       </c>
       <c r="D173" s="16">
         <f t="shared" si="3"/>
@@ -3381,10 +3417,10 @@
     </row>
     <row r="174" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A174" s="16" t="s">
-        <v>176</v>
+        <v>46</v>
       </c>
       <c r="C174" s="16">
-        <v>54368</v>
+        <v>54651</v>
       </c>
       <c r="D174" s="16">
         <f t="shared" si="3"/>
@@ -3393,10 +3429,10 @@
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A175" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C175" s="16">
-        <v>54651</v>
+        <v>54872</v>
       </c>
       <c r="D175" s="16">
         <f t="shared" si="3"/>
@@ -3405,202 +3441,202 @@
     </row>
     <row r="176" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A176" s="16" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C176" s="16">
-        <v>54872</v>
+        <v>55390</v>
       </c>
       <c r="D176" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A177" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C177" s="16">
-        <v>55390</v>
-      </c>
-      <c r="D177" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E177">
-        <f>D177-D165</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A178" s="28" t="s">
+      <c r="E176">
+        <f>D176-D164</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A177" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="B178" s="29"/>
-      <c r="C178" s="29"/>
-      <c r="D178" s="29"/>
-    </row>
-    <row r="179" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="B177" s="29"/>
+      <c r="C177" s="29"/>
+      <c r="D177" s="29"/>
+    </row>
+    <row r="178" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A178" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C178" s="16">
+        <v>55725</v>
+      </c>
+      <c r="D178" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A179" s="16" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="C179" s="16">
-        <v>55725</v>
+        <v>55958</v>
       </c>
       <c r="D179" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="180" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A180" s="16" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="C180" s="16">
-        <v>55958</v>
+        <v>56265</v>
       </c>
       <c r="D180" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="181" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A181" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C181" s="16">
-        <v>56265</v>
+        <v>56378</v>
       </c>
       <c r="D181" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="182" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A182" s="16" t="s">
-        <v>179</v>
+        <v>88</v>
       </c>
       <c r="C182" s="16">
-        <v>56378</v>
+        <v>56428</v>
       </c>
       <c r="D182" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="183" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A183" s="16" t="s">
-        <v>88</v>
+        <v>180</v>
       </c>
       <c r="C183" s="16">
-        <v>56428</v>
+        <v>56640</v>
       </c>
       <c r="D183" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="184" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A184" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C184" s="16">
-        <v>56640</v>
+        <v>56715</v>
       </c>
       <c r="D184" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="185" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A185" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C185" s="16">
-        <v>56715</v>
+        <v>56898</v>
       </c>
       <c r="D185" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="186" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A186" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C186" s="16">
-        <v>56898</v>
+        <v>56982</v>
       </c>
       <c r="D186" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="187" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A187" s="16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C187" s="16">
-        <v>56982</v>
+        <v>57020</v>
       </c>
       <c r="D187" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="188" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A188" s="16" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C188" s="16">
-        <v>57020</v>
+        <v>57085</v>
       </c>
       <c r="D188" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="189" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A189" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C189" s="16">
-        <v>57085</v>
+        <v>57134</v>
       </c>
       <c r="D189" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="190" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A190" s="16" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C190" s="16">
-        <v>57134</v>
+        <v>57234</v>
       </c>
       <c r="D190" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="191" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A191" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C191" s="16">
-        <v>57234</v>
+        <v>57309</v>
       </c>
       <c r="D191" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="192" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A192" s="16" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C192" s="16">
-        <v>57309</v>
+        <v>57531</v>
       </c>
       <c r="D192" s="16">
         <f t="shared" si="3"/>
@@ -3609,10 +3645,10 @@
     </row>
     <row r="193" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A193" s="16" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C193" s="16">
-        <v>57531</v>
+        <v>57771</v>
       </c>
       <c r="D193" s="16">
         <f t="shared" si="3"/>
@@ -3621,46 +3657,46 @@
     </row>
     <row r="194" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A194" s="16" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="C194" s="16">
-        <v>57771</v>
+        <v>58289</v>
       </c>
       <c r="D194" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E194">
+        <f>D194-D179</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="195" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A195" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C195" s="16">
-        <v>58289</v>
-      </c>
-      <c r="D195" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E195">
-        <f>D195-D180</f>
-        <v>0</v>
-      </c>
+      <c r="A195" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="B195" s="29"/>
+      <c r="C195" s="29"/>
+      <c r="D195" s="29"/>
     </row>
     <row r="196" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A196" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="B196" s="29"/>
-      <c r="C196" s="29"/>
-      <c r="D196" s="29"/>
+      <c r="A196" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C196" s="16">
+        <v>58622</v>
+      </c>
+      <c r="D196" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="197" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A197" s="16" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="C197" s="16">
-        <v>58622</v>
+        <v>58848</v>
       </c>
       <c r="D197" s="16">
         <f t="shared" si="3"/>
@@ -3669,10 +3705,10 @@
     </row>
     <row r="198" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A198" s="16" t="s">
-        <v>95</v>
+        <v>191</v>
       </c>
       <c r="C198" s="16">
-        <v>58848</v>
+        <v>59432</v>
       </c>
       <c r="D198" s="16">
         <f t="shared" si="3"/>
@@ -3681,10 +3717,10 @@
     </row>
     <row r="199" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A199" s="16" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C199" s="16">
-        <v>59432</v>
+        <v>59610</v>
       </c>
       <c r="D199" s="16">
         <f t="shared" si="3"/>
@@ -3693,10 +3729,10 @@
     </row>
     <row r="200" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A200" s="16" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C200" s="16">
-        <v>59610</v>
+        <v>59716</v>
       </c>
       <c r="D200" s="16">
         <f t="shared" si="3"/>
@@ -3705,10 +3741,10 @@
     </row>
     <row r="201" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A201" s="16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C201" s="16">
-        <v>59716</v>
+        <v>59863</v>
       </c>
       <c r="D201" s="16">
         <f t="shared" si="3"/>
@@ -3717,10 +3753,10 @@
     </row>
     <row r="202" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A202" s="16" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="C202" s="16">
-        <v>59863</v>
+        <v>60022</v>
       </c>
       <c r="D202" s="16">
         <f t="shared" si="3"/>
@@ -3729,46 +3765,46 @@
     </row>
     <row r="203" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A203" s="16" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C203" s="16">
-        <v>60022</v>
+        <v>60540</v>
       </c>
       <c r="D203" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E203">
+        <f>D203-D197</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="204" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A204" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C204" s="16">
-        <v>60540</v>
-      </c>
-      <c r="D204" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E204">
-        <f>D204-D198</f>
-        <v>0</v>
-      </c>
+      <c r="A204" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="B204" s="29"/>
+      <c r="C204" s="29"/>
+      <c r="D204" s="29"/>
     </row>
     <row r="205" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A205" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="B205" s="29"/>
-      <c r="C205" s="29"/>
-      <c r="D205" s="29"/>
+      <c r="A205" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C205" s="16">
+        <v>60909</v>
+      </c>
+      <c r="D205" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="206" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A206" s="16" t="s">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="C206" s="16">
-        <v>60909</v>
+        <v>61137</v>
       </c>
       <c r="D206" s="16">
         <f t="shared" si="3"/>
@@ -3777,10 +3813,10 @@
     </row>
     <row r="207" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A207" s="16" t="s">
-        <v>95</v>
+        <v>196</v>
       </c>
       <c r="C207" s="16">
-        <v>61137</v>
+        <v>61238</v>
       </c>
       <c r="D207" s="16">
         <f t="shared" si="3"/>
@@ -3789,10 +3825,10 @@
     </row>
     <row r="208" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A208" s="16" t="s">
-        <v>196</v>
+        <v>37</v>
       </c>
       <c r="C208" s="16">
-        <v>61238</v>
+        <v>69043</v>
       </c>
       <c r="D208" s="16">
         <f t="shared" si="3"/>
@@ -3801,10 +3837,10 @@
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A209" s="16" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="C209" s="16">
-        <v>69043</v>
+        <v>69309</v>
       </c>
       <c r="D209" s="16">
         <f t="shared" si="3"/>
@@ -3813,46 +3849,46 @@
     </row>
     <row r="210" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A210" s="16" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
       <c r="C210" s="16">
-        <v>69309</v>
+        <v>69906</v>
       </c>
       <c r="D210" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E210">
+        <f>D210-D206</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="211" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A211" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C211" s="16">
-        <v>69906</v>
-      </c>
-      <c r="D211" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E211">
-        <f>D211-D207</f>
-        <v>0</v>
-      </c>
+      <c r="A211" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B211" s="29"/>
+      <c r="C211" s="29"/>
+      <c r="D211" s="29"/>
     </row>
     <row r="212" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A212" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="B212" s="29"/>
-      <c r="C212" s="29"/>
-      <c r="D212" s="29"/>
+      <c r="A212" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C212" s="16">
+        <v>70786</v>
+      </c>
+      <c r="D212" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="213" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A213" s="16" t="s">
-        <v>198</v>
+        <v>95</v>
       </c>
       <c r="C213" s="16">
-        <v>70786</v>
+        <v>71017</v>
       </c>
       <c r="D213" s="16">
         <f t="shared" si="3"/>
@@ -3861,10 +3897,10 @@
     </row>
     <row r="214" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A214" s="16" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C214" s="16">
-        <v>71017</v>
+        <v>71467</v>
       </c>
       <c r="D214" s="16">
         <f t="shared" si="3"/>
@@ -3873,10 +3909,10 @@
     </row>
     <row r="215" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A215" s="16" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="C215" s="16">
-        <v>71467</v>
+        <v>71725</v>
       </c>
       <c r="D215" s="16">
         <f t="shared" si="3"/>
@@ -3885,10 +3921,10 @@
     </row>
     <row r="216" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A216" s="16" t="s">
-        <v>159</v>
+        <v>37</v>
       </c>
       <c r="C216" s="16">
-        <v>71725</v>
+        <v>72016</v>
       </c>
       <c r="D216" s="16">
         <f t="shared" si="3"/>
@@ -3897,10 +3933,10 @@
     </row>
     <row r="217" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A217" s="16" t="s">
-        <v>37</v>
+        <v>199</v>
       </c>
       <c r="C217" s="16">
-        <v>72016</v>
+        <v>72323</v>
       </c>
       <c r="D217" s="16">
         <f t="shared" si="3"/>
@@ -3909,10 +3945,10 @@
     </row>
     <row r="218" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A218" s="16" t="s">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="C218" s="16">
-        <v>72323</v>
+        <v>72665</v>
       </c>
       <c r="D218" s="16">
         <f t="shared" si="3"/>
@@ -3924,7 +3960,7 @@
         <v>37</v>
       </c>
       <c r="C219" s="16">
-        <v>72665</v>
+        <v>73412</v>
       </c>
       <c r="D219" s="16">
         <f t="shared" si="3"/>
@@ -3936,7 +3972,7 @@
         <v>37</v>
       </c>
       <c r="C220" s="16">
-        <v>73412</v>
+        <v>73958</v>
       </c>
       <c r="D220" s="16">
         <f t="shared" si="3"/>
@@ -3945,10 +3981,10 @@
     </row>
     <row r="221" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A221" s="16" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="C221" s="16">
-        <v>73958</v>
+        <v>74749</v>
       </c>
       <c r="D221" s="16">
         <f t="shared" si="3"/>
@@ -3957,10 +3993,10 @@
     </row>
     <row r="222" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A222" s="16" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="C222" s="16">
-        <v>74749</v>
+        <v>74982</v>
       </c>
       <c r="D222" s="16">
         <f t="shared" si="3"/>
@@ -3969,25 +4005,25 @@
     </row>
     <row r="223" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A223" s="16" t="s">
-        <v>37</v>
+        <v>200</v>
       </c>
       <c r="C223" s="16">
-        <v>74982</v>
+        <v>75107</v>
       </c>
       <c r="D223" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D223" si="5">IF(B223 &gt;  0,C223-B223, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A224" s="16" t="s">
-        <v>200</v>
+        <v>37</v>
       </c>
       <c r="C224" s="16">
-        <v>75107</v>
+        <v>75280</v>
       </c>
       <c r="D224" s="16">
-        <f t="shared" ref="D224" si="5">IF(B224 &gt;  0,C224-B224, 0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3996,7 +4032,7 @@
         <v>37</v>
       </c>
       <c r="C225" s="16">
-        <v>75280</v>
+        <v>75591</v>
       </c>
       <c r="D225" s="16">
         <f t="shared" si="3"/>
@@ -4005,10 +4041,10 @@
     </row>
     <row r="226" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A226" s="16" t="s">
-        <v>37</v>
+        <v>201</v>
       </c>
       <c r="C226" s="16">
-        <v>75591</v>
+        <v>75741</v>
       </c>
       <c r="D226" s="16">
         <f t="shared" si="3"/>
@@ -4017,10 +4053,10 @@
     </row>
     <row r="227" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A227" s="16" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C227" s="16">
-        <v>75741</v>
+        <v>75828</v>
       </c>
       <c r="D227" s="16">
         <f t="shared" si="3"/>
@@ -4029,10 +4065,10 @@
     </row>
     <row r="228" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A228" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C228" s="16">
-        <v>75828</v>
+        <v>75972</v>
       </c>
       <c r="D228" s="16">
         <f t="shared" si="3"/>
@@ -4041,10 +4077,10 @@
     </row>
     <row r="229" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A229" s="16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C229" s="16">
-        <v>75972</v>
+        <v>76227</v>
       </c>
       <c r="D229" s="16">
         <f t="shared" si="3"/>
@@ -4053,10 +4089,10 @@
     </row>
     <row r="230" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A230" s="16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C230" s="16">
-        <v>76227</v>
+        <v>76306</v>
       </c>
       <c r="D230" s="16">
         <f t="shared" si="3"/>
@@ -4065,10 +4101,10 @@
     </row>
     <row r="231" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A231" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C231" s="16">
-        <v>76306</v>
+        <v>76444</v>
       </c>
       <c r="D231" s="16">
         <f t="shared" si="3"/>
@@ -4077,10 +4113,10 @@
     </row>
     <row r="232" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A232" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C232" s="16">
-        <v>76444</v>
+        <v>76741</v>
       </c>
       <c r="D232" s="16">
         <f t="shared" si="3"/>
@@ -4089,10 +4125,10 @@
     </row>
     <row r="233" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A233" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C233" s="16">
-        <v>76741</v>
+        <v>77063</v>
       </c>
       <c r="D233" s="16">
         <f t="shared" si="3"/>
@@ -4101,54 +4137,42 @@
     </row>
     <row r="234" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A234" s="16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C234" s="16">
-        <v>77063</v>
+        <v>77866</v>
       </c>
       <c r="D234" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" outlineLevel="1">
+    <row r="235" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A235" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C235" s="16">
-        <v>77866</v>
+        <v>77902</v>
       </c>
       <c r="D235" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A236" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C236" s="16">
-        <v>77902</v>
-      </c>
-      <c r="D236" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E236" s="30">
-        <f>D236-D214</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" s="32" customFormat="1" ht="16.5" hidden="1" outlineLevel="1" thickTop="1" thickBot="1">
-      <c r="A237" s="31"/>
-      <c r="B237" s="31"/>
-      <c r="C237" s="31"/>
-      <c r="D237" s="31"/>
-      <c r="E237" s="32">
-        <f>SUM(E1:E236)</f>
+      <c r="E235" s="30">
+        <f>D235-D213</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" s="32" customFormat="1" ht="16.5" hidden="1" outlineLevel="1" thickTop="1" thickBot="1">
+      <c r="A236" s="31"/>
+      <c r="B236" s="31"/>
+      <c r="C236" s="31"/>
+      <c r="D236" s="31"/>
+      <c r="E236" s="32">
+        <f>SUM(E1:E235)</f>
         <v>49</v>
       </c>
-      <c r="F237" s="32" t="s">
+      <c r="F236" s="32" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4156,8 +4180,8 @@
   <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A85:D85"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4170,8 +4194,8 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
NSMB - updated spreadsheet for framecounts for V4, V5, and Yoshi's WIP up to world 5, and added a few more WIPs
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="232">
   <si>
     <t>1-1</t>
   </si>
@@ -319,18 +319,6 @@
     <t>V4</t>
   </si>
   <si>
-    <t>Checkpoint 759</t>
-  </si>
-  <si>
-    <t>Checkpoint 936</t>
-  </si>
-  <si>
-    <t>Checkpoint 2626</t>
-  </si>
-  <si>
-    <t>Mario appears</t>
-  </si>
-  <si>
     <t>Checkpoint</t>
   </si>
   <si>
@@ -715,13 +703,16 @@
     <t>Total in game</t>
   </si>
   <si>
-    <t>In Level Improvements:</t>
-  </si>
-  <si>
     <t>V5</t>
   </si>
   <si>
-    <t>"+2 to last time"</t>
+    <t>Yoshi</t>
+  </si>
+  <si>
+    <t>Checkpoint 937</t>
+  </si>
+  <si>
+    <t>Note: 10154 is possible, but doesn't matter due to waiting for 465 on the timer</t>
   </si>
 </sst>
 </file>
@@ -818,7 +809,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -856,17 +847,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -890,14 +870,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="double">
         <color indexed="64"/>
@@ -953,18 +928,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,27 +1237,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I236"/>
+  <dimension ref="A1:H228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="16"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="16"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>99</v>
@@ -1290,1204 +1266,1334 @@
       <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="F1" s="38"/>
-      <c r="G1">
-        <f>E236</f>
+      <c r="E1" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="A2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+    </row>
+    <row r="3" spans="1:6" outlineLevel="1">
+      <c r="A3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="16">
+        <v>460</v>
+      </c>
+      <c r="C3" s="16">
+        <v>477</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D5" si="0">IF(B3 &gt;  0,C3-B3, 0)</f>
+        <v>17</v>
+      </c>
+      <c r="E3" s="16">
+        <v>460</v>
+      </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F5" si="1">IF(B3 &gt;  0,E3-B3, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" outlineLevel="1">
+      <c r="A4" s="16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="1:7" outlineLevel="1">
-      <c r="A3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="16">
-        <f>IF(B3 &gt;  0,C3-B3, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" outlineLevel="1">
-      <c r="A4" s="16" t="s">
-        <v>48</v>
+      <c r="B4" s="16">
+        <v>2451</v>
       </c>
       <c r="C4" s="16">
-        <v>476</v>
+        <v>2481</v>
       </c>
       <c r="D4" s="16">
-        <f t="shared" ref="D4:D6" si="0">IF(B4 &gt;  0,C4-B4, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" outlineLevel="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E4" s="16">
+        <v>2451</v>
+      </c>
+      <c r="F4" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" outlineLevel="1">
       <c r="A5" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2547</v>
       </c>
       <c r="C5" s="16">
-        <v>2937</v>
+        <v>2579</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" outlineLevel="1">
-      <c r="A6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="16">
-        <v>2549</v>
-      </c>
-      <c r="C6" s="16">
-        <v>2579</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2547</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="13" customFormat="1" ht="18.75">
+      <c r="A6" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+    </row>
+    <row r="7" spans="1:6" outlineLevel="1">
+      <c r="A7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" outlineLevel="1">
+      <c r="A8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2776</v>
+      </c>
+      <c r="C8" s="16">
+        <v>2806</v>
+      </c>
+      <c r="D8" s="16">
+        <f>IF(B8 &gt;  0,C8-B8, 0)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" outlineLevel="1">
-      <c r="A8" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" outlineLevel="1">
+      <c r="E8" s="16">
+        <v>2776</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" ref="F8:F26" si="2">IF(B8 &gt;  0,E8-B8, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" outlineLevel="1">
       <c r="A9" s="16" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
       <c r="B9" s="16">
-        <v>2776</v>
+        <v>3120</v>
       </c>
       <c r="C9" s="16">
-        <v>2806</v>
+        <v>3151</v>
       </c>
       <c r="D9" s="16">
         <f>IF(B9 &gt;  0,C9-B9, 0)</f>
-        <v>30</v>
-      </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" outlineLevel="1">
+        <v>31</v>
+      </c>
+      <c r="E9" s="16">
+        <v>3120</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" outlineLevel="1">
       <c r="A10" s="16" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="B10" s="16">
-        <v>3062</v>
+        <v>4094</v>
       </c>
       <c r="C10" s="16">
-        <v>3093</v>
+        <v>4146</v>
       </c>
       <c r="D10" s="16">
-        <f>IF(B10 &gt;  0,C10-B10, 0)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" outlineLevel="1">
+        <f t="shared" ref="D10:D26" si="3">IF(B10 &gt;  0,C10-B10, 0)</f>
+        <v>52</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4096</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" outlineLevel="1">
       <c r="A11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="16">
+        <v>4612</v>
+      </c>
+      <c r="C11" s="16">
+        <v>4664</v>
+      </c>
+      <c r="D11" s="16">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="E11" s="16">
+        <v>4614</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" outlineLevel="1">
+      <c r="A12" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" outlineLevel="1">
+      <c r="A13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="16">
+        <v>5005</v>
+      </c>
+      <c r="C13" s="16">
+        <v>5057</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="E13" s="16">
+        <v>5007</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" outlineLevel="1">
+      <c r="A14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="16">
+        <v>6946</v>
+      </c>
+      <c r="C14" s="16">
+        <v>7029</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="E14" s="16">
+        <v>6951</v>
+      </c>
+      <c r="F14" s="16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" outlineLevel="1">
+      <c r="A15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="16">
+        <v>7255</v>
+      </c>
+      <c r="C15" s="16">
+        <v>7351</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="E15" s="16">
+        <v>7260</v>
+      </c>
+      <c r="F15" s="16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" outlineLevel="1">
+      <c r="A16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="16">
+        <v>7769</v>
+      </c>
+      <c r="C16" s="16">
+        <v>7865</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="E16" s="16">
+        <v>7774</v>
+      </c>
+      <c r="F16" s="16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" outlineLevel="1">
+      <c r="A17" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8" outlineLevel="1">
+      <c r="A18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="16">
+        <v>8317</v>
+      </c>
+      <c r="C18" s="16">
+        <v>8406</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="E18" s="16">
+        <v>8308</v>
+      </c>
+      <c r="F18" s="16">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" outlineLevel="1">
+      <c r="A19" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="16">
+        <v>8545</v>
+      </c>
+      <c r="C19" s="16">
+        <v>8632</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="E19" s="16">
+        <v>8536</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" outlineLevel="1">
+      <c r="A20" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="16">
+        <v>9532</v>
+      </c>
+      <c r="C20" s="16">
+        <v>9637</v>
+      </c>
+      <c r="D20" s="16">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="E20" s="16">
+        <v>9523</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" outlineLevel="1">
+      <c r="A21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16">
+        <v>10158</v>
+      </c>
+      <c r="C21" s="16">
+        <v>10327</v>
+      </c>
+      <c r="D21" s="16">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="E21" s="16">
+        <v>10219</v>
+      </c>
+      <c r="F21" s="16">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" outlineLevel="1">
+      <c r="A22" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="16">
+        <v>10525</v>
+      </c>
+      <c r="C22" s="16">
+        <v>10626</v>
+      </c>
+      <c r="D22" s="16">
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
-      <c r="C11" s="16">
-        <v>3151</v>
-      </c>
-      <c r="D11" s="16">
-        <f>IF(B11 &gt;  0,C11-B11, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" outlineLevel="1">
-      <c r="A12" s="16" t="s">
+      <c r="E22" s="16">
+        <v>10518</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="H22" s="38"/>
+    </row>
+    <row r="23" spans="1:8" outlineLevel="1">
+      <c r="A23" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="16">
+        <v>11039</v>
+      </c>
+      <c r="C23" s="16">
+        <v>11140</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
+      <c r="E23" s="16">
+        <v>11032</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" outlineLevel="1">
+      <c r="A24" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" outlineLevel="1">
+      <c r="A25" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="16">
+        <v>11512</v>
+      </c>
+      <c r="C25" s="16">
+        <v>11592</v>
+      </c>
+      <c r="D25" s="16">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="E25" s="16">
+        <v>11479</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" si="2"/>
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" outlineLevel="1">
+      <c r="A26" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="16">
+        <v>12463</v>
+      </c>
+      <c r="C26" s="16">
+        <v>12540</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="E26" s="16">
+        <v>12425</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" si="2"/>
+        <v>-38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18.75">
+      <c r="A27" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+    </row>
+    <row r="28" spans="1:8" outlineLevel="1">
+      <c r="A28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+    </row>
+    <row r="29" spans="1:8" outlineLevel="1">
+      <c r="A29" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="16">
+        <v>12911</v>
+      </c>
+      <c r="C29" s="16">
+        <v>12987</v>
+      </c>
+      <c r="D29" s="16">
+        <f t="shared" ref="D29:D76" si="4">IF(B29 &gt;  0,C29-B29, 0)</f>
+        <v>76</v>
+      </c>
+      <c r="E29" s="16">
+        <v>12873</v>
+      </c>
+      <c r="F29" s="16">
+        <f t="shared" ref="F29" si="5">IF(B29 &gt;  0,E29-B29, 0)</f>
+        <v>-38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" outlineLevel="1">
+      <c r="A30" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="16">
+        <v>13217</v>
+      </c>
+      <c r="D30" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" outlineLevel="1">
+      <c r="A31" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="16">
+        <v>14776</v>
+      </c>
+      <c r="D31" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" outlineLevel="1">
+      <c r="A32" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="16">
+        <v>15307</v>
+      </c>
+      <c r="D32" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" outlineLevel="1">
+      <c r="A33" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="16">
-        <v>3712</v>
-      </c>
-      <c r="D12" s="16">
-        <f>IF(B12 &gt;  0,C12-B12, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" outlineLevel="1">
-      <c r="A13" s="16" t="s">
+      <c r="C33" s="16">
+        <v>15573</v>
+      </c>
+      <c r="D33" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" outlineLevel="1">
+      <c r="A34" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" outlineLevel="1">
+      <c r="A35" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="16">
+        <v>15722</v>
+      </c>
+      <c r="D35" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" outlineLevel="1">
+      <c r="A36" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="16">
+        <v>15947</v>
+      </c>
+      <c r="D36" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" outlineLevel="1">
+      <c r="A37" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="16">
+        <v>16087</v>
+      </c>
+      <c r="D37" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" outlineLevel="1">
+      <c r="A38" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="16">
+        <v>17508</v>
+      </c>
+      <c r="D38" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" outlineLevel="1">
+      <c r="A39" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="16">
+        <v>17579</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" outlineLevel="1">
+      <c r="A40" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="16">
-        <v>4094</v>
-      </c>
-      <c r="C13" s="16">
-        <v>4146</v>
-      </c>
-      <c r="D13" s="16">
-        <f t="shared" ref="D13:D34" si="1">IF(B13 &gt;  0,C13-B13, 0)</f>
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>234</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" outlineLevel="1">
-      <c r="A14" s="16" t="s">
+      <c r="C40" s="16">
+        <v>17846</v>
+      </c>
+      <c r="D40" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" outlineLevel="1">
+      <c r="A41" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="16">
-        <v>4614</v>
-      </c>
-      <c r="C14" s="16">
-        <v>4664</v>
-      </c>
-      <c r="D14" s="16">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" outlineLevel="1">
-      <c r="A15" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" outlineLevel="1">
-      <c r="A16" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:9" outlineLevel="1">
-      <c r="A17" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="16">
-        <v>5005</v>
-      </c>
-      <c r="C17" s="16">
-        <v>5057</v>
-      </c>
-      <c r="D17" s="16">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:9" outlineLevel="1">
-      <c r="A18" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="16">
-        <v>5296</v>
-      </c>
-      <c r="D18" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" outlineLevel="1">
-      <c r="A19" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="16">
-        <v>6823</v>
-      </c>
-      <c r="D19" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" outlineLevel="1">
-      <c r="A20" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="16">
-        <v>6946</v>
-      </c>
-      <c r="C20" s="16">
-        <v>6951</v>
-      </c>
-      <c r="D20" s="16">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:9" outlineLevel="1">
-      <c r="A21" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="16">
-        <v>7351</v>
-      </c>
-      <c r="D21" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f>D21-D17</f>
-        <v>-52</v>
-      </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" outlineLevel="1">
-      <c r="A22" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="16">
-        <v>7769</v>
-      </c>
-      <c r="D22" s="16">
-        <f t="shared" si="1"/>
-        <v>-7769</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" outlineLevel="1">
-      <c r="A23" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" outlineLevel="1">
-      <c r="A24" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="16">
-        <v>8176</v>
-      </c>
-      <c r="C24" s="16">
-        <v>8406</v>
-      </c>
-      <c r="D24" s="16">
-        <f t="shared" si="1"/>
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" outlineLevel="1">
-      <c r="A25" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="16">
-        <v>8632</v>
-      </c>
-      <c r="D25" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" outlineLevel="1">
-      <c r="A26" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="16">
-        <v>9637</v>
-      </c>
-      <c r="D26" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" outlineLevel="1">
-      <c r="A27" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="16">
-        <v>9674</v>
-      </c>
-      <c r="D27" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" outlineLevel="1">
-      <c r="A28" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="16">
-        <v>9816</v>
-      </c>
-      <c r="D28" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" outlineLevel="1">
-      <c r="A29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="16">
-        <v>10327</v>
-      </c>
-      <c r="D29" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
-        <v>114</v>
-      </c>
-      <c r="I29">
-        <v>11039</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A30" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="16">
-        <v>10525</v>
-      </c>
-      <c r="C30" s="16">
-        <v>10626</v>
-      </c>
-      <c r="D30" s="16">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="H30" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="41">
-        <v>11390</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A31" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="16">
-        <v>11039</v>
-      </c>
-      <c r="C31" s="16">
-        <v>11140</v>
-      </c>
-      <c r="D31" s="16">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="E31">
-        <f>D31-D25</f>
-        <v>101</v>
-      </c>
-      <c r="I31">
-        <f>I30-I29</f>
-        <v>351</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" outlineLevel="1">
-      <c r="A32" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="33" spans="1:5" outlineLevel="1">
-      <c r="A33" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B33" s="16">
-        <v>11512</v>
-      </c>
-      <c r="C33" s="16">
-        <v>11592</v>
-      </c>
-      <c r="D33" s="16">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" outlineLevel="1">
-      <c r="A34" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="16">
-        <v>12463</v>
-      </c>
-      <c r="C34" s="16">
-        <v>12540</v>
-      </c>
-      <c r="D34" s="16">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="18.75">
-      <c r="A35" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-    </row>
-    <row r="36" spans="1:5" outlineLevel="1">
-      <c r="A36" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-    </row>
-    <row r="37" spans="1:5" outlineLevel="1">
-      <c r="A37" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="16">
-        <v>12911</v>
-      </c>
-      <c r="C37" s="16">
-        <v>12987</v>
-      </c>
-      <c r="D37" s="16">
-        <f t="shared" ref="D37:D84" si="2">IF(B37 &gt;  0,C37-B37, 0)</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" outlineLevel="1">
-      <c r="A38" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="16">
-        <v>13217</v>
-      </c>
-      <c r="D38" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" outlineLevel="1">
-      <c r="A39" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="16">
-        <v>14776</v>
-      </c>
-      <c r="D39" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" outlineLevel="1">
-      <c r="A40" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="16">
-        <v>15307</v>
-      </c>
-      <c r="D40" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" outlineLevel="1">
-      <c r="A41" s="16" t="s">
-        <v>106</v>
-      </c>
       <c r="C41" s="16">
-        <v>15573</v>
+        <v>18368</v>
       </c>
       <c r="D41" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="16">
+        <f>D41-D36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" outlineLevel="1">
       <c r="A42" s="24" t="s">
-        <v>94</v>
+        <v>209</v>
       </c>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
     </row>
-    <row r="43" spans="1:5" outlineLevel="1">
+    <row r="43" spans="1:8" outlineLevel="1">
       <c r="A43" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" s="16">
-        <v>15722</v>
+        <v>18945</v>
       </c>
       <c r="D43" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" outlineLevel="1">
       <c r="A44" s="16" t="s">
         <v>95</v>
       </c>
       <c r="C44" s="16">
-        <v>15947</v>
+        <v>19177</v>
       </c>
       <c r="D44" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="39"/>
+      <c r="H44" s="25"/>
+    </row>
+    <row r="45" spans="1:8" outlineLevel="1">
       <c r="A45" s="16" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="C45" s="16">
-        <v>16087</v>
+        <v>20120</v>
       </c>
       <c r="D45" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="40"/>
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="1:8" outlineLevel="1">
       <c r="A46" s="16" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="C46" s="16">
-        <v>17508</v>
+        <v>20187</v>
       </c>
       <c r="D46" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" outlineLevel="1">
       <c r="A47" s="16" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C47" s="16">
-        <v>17579</v>
+        <v>20258</v>
       </c>
       <c r="D47" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" outlineLevel="1">
       <c r="A48" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="16">
+        <v>20351</v>
+      </c>
+      <c r="D48" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" outlineLevel="1">
+      <c r="A49" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="16">
+        <v>20394</v>
+      </c>
+      <c r="D49" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" outlineLevel="1">
+      <c r="A50" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="16">
+        <v>20465</v>
+      </c>
+      <c r="D50" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" outlineLevel="1">
+      <c r="A51" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="16">
-        <v>17846</v>
-      </c>
-      <c r="D48" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" outlineLevel="1">
-      <c r="A49" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="16">
-        <v>18368</v>
-      </c>
-      <c r="D49" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <f>D49-D44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" outlineLevel="1">
-      <c r="A50" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-    </row>
-    <row r="51" spans="1:9" outlineLevel="1">
-      <c r="A51" s="16" t="s">
-        <v>107</v>
-      </c>
       <c r="C51" s="16">
-        <v>18945</v>
+        <v>20658</v>
       </c>
       <c r="D51" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" outlineLevel="1">
       <c r="A52" s="16" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C52" s="16">
-        <v>19177</v>
+        <v>21172</v>
       </c>
       <c r="D52" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="I52" s="25"/>
-    </row>
-    <row r="53" spans="1:9" outlineLevel="1">
-      <c r="A53" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="16">
-        <v>20120</v>
-      </c>
-      <c r="D53" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="I53" s="26"/>
-    </row>
-    <row r="54" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" outlineLevel="1">
+      <c r="A53" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+    </row>
+    <row r="54" spans="1:4" outlineLevel="1">
       <c r="A54" s="16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C54" s="16">
-        <v>20187</v>
+        <v>21661</v>
       </c>
       <c r="D54" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" outlineLevel="1">
       <c r="A55" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C55" s="16">
-        <v>20258</v>
+        <v>21890</v>
       </c>
       <c r="D55" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" outlineLevel="1">
       <c r="A56" s="16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C56" s="16">
-        <v>20351</v>
+        <v>21929</v>
       </c>
       <c r="D56" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" outlineLevel="1">
       <c r="A57" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C57" s="16">
-        <v>20394</v>
+        <v>21995</v>
       </c>
       <c r="D57" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" outlineLevel="1">
       <c r="A58" s="16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C58" s="16">
-        <v>20465</v>
+        <v>22090</v>
       </c>
       <c r="D58" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" outlineLevel="1">
       <c r="A59" s="16" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="C59" s="16">
-        <v>20658</v>
+        <v>22121</v>
       </c>
       <c r="D59" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" outlineLevel="1">
       <c r="A60" s="16" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C60" s="16">
-        <v>21172</v>
+        <v>22330</v>
       </c>
       <c r="D60" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" outlineLevel="1">
-      <c r="A61" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-    </row>
-    <row r="62" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" outlineLevel="1">
+      <c r="A61" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="16">
+        <v>22372</v>
+      </c>
+      <c r="D61" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" outlineLevel="1">
       <c r="A62" s="16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C62" s="16">
-        <v>21661</v>
+        <v>22388</v>
       </c>
       <c r="D62" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" outlineLevel="1">
       <c r="A63" s="16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C63" s="16">
-        <v>21890</v>
+        <v>22421</v>
       </c>
       <c r="D63" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" outlineLevel="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" outlineLevel="1">
       <c r="A64" s="16" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C64" s="16">
-        <v>21929</v>
+        <v>22454</v>
       </c>
       <c r="D64" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" outlineLevel="1">
-      <c r="A65" s="16" t="s">
-        <v>118</v>
+      <c r="A65" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="C65" s="16">
-        <v>21995</v>
+        <v>22708</v>
       </c>
       <c r="D65" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" outlineLevel="1">
       <c r="A66" s="16" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C66" s="16">
-        <v>22090</v>
+        <v>22829</v>
       </c>
       <c r="D66" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" outlineLevel="1">
       <c r="A67" s="16" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="C67" s="16">
-        <v>22121</v>
+        <v>23205</v>
       </c>
       <c r="D67" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" outlineLevel="1">
       <c r="A68" s="16" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C68" s="16">
-        <v>22330</v>
+        <v>23849</v>
       </c>
       <c r="D68" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:5" outlineLevel="1">
       <c r="A69" s="16" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="C69" s="16">
-        <v>22372</v>
+        <v>24266</v>
       </c>
       <c r="D69" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" outlineLevel="1">
       <c r="A70" s="16" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="C70" s="16">
-        <v>22388</v>
+        <v>24570</v>
       </c>
       <c r="D70" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5" outlineLevel="1">
       <c r="A71" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C71" s="16">
-        <v>22421</v>
+        <v>25088</v>
       </c>
       <c r="D71" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E71" s="16">
+        <f>D71-D55</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5" outlineLevel="1">
-      <c r="A72" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C72" s="16">
-        <v>22454</v>
-      </c>
-      <c r="D72" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="A72" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
     </row>
     <row r="73" spans="1:5" outlineLevel="1">
-      <c r="A73" s="27" t="s">
-        <v>126</v>
+      <c r="A73" s="16" t="s">
+        <v>212</v>
       </c>
       <c r="C73" s="16">
-        <v>22708</v>
+        <v>25472</v>
       </c>
       <c r="D73" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5" outlineLevel="1">
       <c r="A74" s="16" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C74" s="16">
-        <v>22829</v>
+        <v>25697</v>
       </c>
       <c r="D74" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" outlineLevel="1">
       <c r="A75" s="16" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="C75" s="16">
-        <v>23205</v>
+        <v>25830</v>
       </c>
       <c r="D75" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" outlineLevel="1">
       <c r="A76" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C76" s="16">
+        <v>26420</v>
+      </c>
+      <c r="D76" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="18.75" collapsed="1">
+      <c r="A77" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A78" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+    </row>
+    <row r="79" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A79" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C76" s="16">
-        <v>23849</v>
-      </c>
-      <c r="D76" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" outlineLevel="1">
-      <c r="A77" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C77" s="16">
-        <v>24266</v>
-      </c>
-      <c r="D77" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" outlineLevel="1">
-      <c r="A78" s="16" t="s">
+      <c r="C79" s="16">
+        <v>26790</v>
+      </c>
+      <c r="D79" s="16">
+        <f t="shared" ref="D79:D227" si="6">IF(B79 &gt;  0,C79-B79, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A80" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C80" s="16">
+        <v>27017</v>
+      </c>
+      <c r="D80" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A81" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="16">
+        <v>27730</v>
+      </c>
+      <c r="D81" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A82" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C78" s="16">
-        <v>24570</v>
-      </c>
-      <c r="D78" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" outlineLevel="1">
-      <c r="A79" s="16" t="s">
+      <c r="C82" s="16">
+        <v>28335</v>
+      </c>
+      <c r="D82" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A83" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" s="16">
+        <v>28853</v>
+      </c>
+      <c r="D83" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="16">
+        <f>D83-D80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A84" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+    </row>
+    <row r="85" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A85" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C79" s="16">
-        <v>25088</v>
-      </c>
-      <c r="D79" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <f>D79-D63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" outlineLevel="1">
-      <c r="A80" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-    </row>
-    <row r="81" spans="1:5" outlineLevel="1">
-      <c r="A81" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="C81" s="16">
-        <v>25472</v>
-      </c>
-      <c r="D81" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" outlineLevel="1">
-      <c r="A82" s="16" t="s">
+      <c r="C85" s="16">
+        <v>29213</v>
+      </c>
+      <c r="D85" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A86" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="16">
-        <v>25697</v>
-      </c>
-      <c r="D82" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" outlineLevel="1">
-      <c r="A83" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C83" s="16">
-        <v>25830</v>
-      </c>
-      <c r="D83" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" outlineLevel="1">
-      <c r="A84" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C84" s="16">
-        <v>26420</v>
-      </c>
-      <c r="D84" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="18.75" collapsed="1">
-      <c r="A85" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-    </row>
-    <row r="86" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A86" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
+      <c r="C86" s="16">
+        <v>29438</v>
+      </c>
+      <c r="D86" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A87" s="16" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="C87" s="16">
-        <v>26790</v>
+        <v>29585</v>
       </c>
       <c r="D87" s="16">
-        <f t="shared" ref="D87:D235" si="3">IF(B87 &gt;  0,C87-B87, 0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A88" s="16" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="C88" s="16">
-        <v>27017</v>
+        <v>29708</v>
       </c>
       <c r="D88" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A89" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C89" s="16">
-        <v>27730</v>
+        <v>29848</v>
       </c>
       <c r="D89" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A90" s="16" t="s">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="C90" s="16">
-        <v>28335</v>
+        <v>29894</v>
       </c>
       <c r="D90" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A91" s="16" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="C91" s="16">
-        <v>28853</v>
+        <v>30331</v>
       </c>
       <c r="D91" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E91">
-        <f>D91-D88</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A92" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B92" s="29"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="29"/>
+      <c r="A92" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C92" s="16">
+        <v>30698</v>
+      </c>
+      <c r="D92" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A93" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C93" s="16">
-        <v>29213</v>
+        <v>30992</v>
       </c>
       <c r="D93" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A94" s="16" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="C94" s="16">
-        <v>29438</v>
+        <v>31261</v>
       </c>
       <c r="D94" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A95" s="16" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C95" s="16">
-        <v>29585</v>
+        <v>31543</v>
       </c>
       <c r="D95" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A96" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C96" s="16">
-        <v>29708</v>
+        <v>31906</v>
       </c>
       <c r="D96" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2496,82 +2602,82 @@
         <v>137</v>
       </c>
       <c r="C97" s="16">
-        <v>29848</v>
+        <v>32382</v>
       </c>
       <c r="D97" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A98" s="16" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C98" s="16">
-        <v>29894</v>
+        <v>32646</v>
       </c>
       <c r="D98" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A99" s="16" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="C99" s="16">
-        <v>30331</v>
+        <v>33164</v>
       </c>
       <c r="D99" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E99" s="16">
+        <f>D99-D86</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A100" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C100" s="16">
-        <v>30698</v>
-      </c>
-      <c r="D100" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A100" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
     </row>
     <row r="101" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A101" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C101" s="16">
-        <v>30992</v>
+        <v>33599</v>
       </c>
       <c r="D101" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A102" s="16" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="C102" s="16">
-        <v>31261</v>
+        <v>33826</v>
       </c>
       <c r="D102" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A103" s="16" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="C103" s="16">
-        <v>31543</v>
+        <v>34022</v>
       </c>
       <c r="D103" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2580,10 +2686,10 @@
         <v>140</v>
       </c>
       <c r="C104" s="16">
-        <v>31906</v>
+        <v>34385</v>
       </c>
       <c r="D104" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2592,622 +2698,622 @@
         <v>141</v>
       </c>
       <c r="C105" s="16">
-        <v>32382</v>
+        <v>34767</v>
       </c>
       <c r="D105" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D105:D109" si="7">IF(B105 &gt;  0,C105-B105, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A106" s="16" t="s">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="C106" s="16">
-        <v>32646</v>
+        <v>34904</v>
       </c>
       <c r="D106" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A107" s="16" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C107" s="16">
-        <v>33164</v>
+        <v>34950</v>
       </c>
       <c r="D107" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E107">
-        <f>D107-D94</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A108" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B108" s="29"/>
-      <c r="C108" s="29"/>
-      <c r="D108" s="29"/>
+      <c r="A108" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C108" s="16">
+        <v>35025</v>
+      </c>
+      <c r="D108" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A109" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C109" s="16">
-        <v>33599</v>
+        <v>35282</v>
       </c>
       <c r="D109" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A110" s="16" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C110" s="16">
-        <v>33826</v>
+        <v>35587</v>
       </c>
       <c r="D110" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A111" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C111" s="16">
-        <v>34022</v>
+        <v>35856</v>
       </c>
       <c r="D111" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A112" s="16" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="C112" s="16">
-        <v>34385</v>
+        <v>36497</v>
       </c>
       <c r="D112" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E112" s="16">
+        <f>D112-D102</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A113" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C113" s="16">
-        <v>34767</v>
-      </c>
-      <c r="D113" s="16">
-        <f t="shared" ref="D113:D117" si="4">IF(B113 &gt;  0,C113-B113, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="A113" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
     </row>
     <row r="114" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A114" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C114" s="16">
-        <v>34904</v>
+        <v>37222</v>
       </c>
       <c r="D114" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A115" s="16" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="C115" s="16">
-        <v>34950</v>
+        <v>37448</v>
       </c>
       <c r="D115" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A116" s="16" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="C116" s="16">
-        <v>35025</v>
+        <v>37664</v>
       </c>
       <c r="D116" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A117" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C117" s="16">
-        <v>35282</v>
+        <v>37919</v>
       </c>
       <c r="D117" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A118" s="16" t="s">
-        <v>37</v>
+        <v>147</v>
       </c>
       <c r="C118" s="16">
-        <v>35587</v>
+        <v>39165</v>
       </c>
       <c r="D118" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A119" s="16" t="s">
-        <v>148</v>
+        <v>213</v>
       </c>
       <c r="C119" s="16">
-        <v>35856</v>
+        <v>39722</v>
       </c>
       <c r="D119" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A120" s="16" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="C120" s="16">
-        <v>36497</v>
+        <v>41771</v>
       </c>
       <c r="D120" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E120">
-        <f>D120-D110</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A121" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="B121" s="29"/>
-      <c r="C121" s="29"/>
-      <c r="D121" s="29"/>
+      <c r="A121" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C121" s="16">
+        <v>42009</v>
+      </c>
+      <c r="D121" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A122" s="16" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="C122" s="16">
-        <v>37222</v>
+        <v>42523</v>
       </c>
       <c r="D122" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E122" s="16">
+        <f>D122-D115</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A123" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C123" s="16">
-        <v>37448</v>
-      </c>
-      <c r="D123" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A123" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="29"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A124" s="16" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="C124" s="16">
-        <v>37664</v>
+        <v>42949</v>
       </c>
       <c r="D124" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A125" s="16" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="C125" s="16">
-        <v>37919</v>
+        <v>43175</v>
       </c>
       <c r="D125" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A126" s="16" t="s">
-        <v>151</v>
+        <v>45</v>
       </c>
       <c r="C126" s="16">
-        <v>39165</v>
+        <v>44628</v>
       </c>
       <c r="D126" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A127" s="16" t="s">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="C127" s="16">
-        <v>39722</v>
+        <v>45146</v>
       </c>
       <c r="D127" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E127" s="16">
+        <f>D127-D125</f>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A128" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C128" s="16">
-        <v>41771</v>
-      </c>
-      <c r="D128" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A128" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B128" s="29"/>
+      <c r="C128" s="29"/>
+      <c r="D128" s="29"/>
     </row>
     <row r="129" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A129" s="16" t="s">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="C129" s="16">
-        <v>42009</v>
+        <v>45524</v>
       </c>
       <c r="D129" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A130" s="16" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="C130" s="16">
-        <v>42523</v>
+        <v>45752</v>
       </c>
       <c r="D130" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E130">
-        <f>D130-D123</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A131" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="B131" s="29"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="29"/>
+      <c r="A131" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C131" s="16">
+        <v>45830</v>
+      </c>
+      <c r="D131" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="132" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A132" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C132" s="16">
-        <v>42949</v>
+        <v>45929</v>
       </c>
       <c r="D132" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A133" s="16" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="C133" s="16">
-        <v>43175</v>
+        <v>46124</v>
       </c>
       <c r="D133" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A134" s="16" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="C134" s="16">
-        <v>44628</v>
+        <v>46279</v>
       </c>
       <c r="D134" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A135" s="16" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="C135" s="16">
-        <v>45146</v>
+        <v>46376</v>
       </c>
       <c r="D135" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E135">
-        <f>D135-D133</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A136" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="B136" s="29"/>
-      <c r="C136" s="29"/>
-      <c r="D136" s="29"/>
+      <c r="A136" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C136" s="16">
+        <v>46504</v>
+      </c>
+      <c r="D136" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A137" s="16" t="s">
-        <v>225</v>
+        <v>154</v>
       </c>
       <c r="C137" s="16">
-        <v>45524</v>
+        <v>46624</v>
       </c>
       <c r="D137" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A138" s="16" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C138" s="16">
-        <v>45752</v>
+        <v>46876</v>
       </c>
       <c r="D138" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A139" s="16" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C139" s="16">
-        <v>45830</v>
+        <v>47892</v>
       </c>
       <c r="D139" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A140" s="16" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="C140" s="16">
-        <v>45929</v>
+        <v>48805</v>
       </c>
       <c r="D140" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E140" s="16">
+        <f>D140-D130</f>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A141" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C141" s="16">
-        <v>46124</v>
-      </c>
-      <c r="D141" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A141" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B141" s="29"/>
+      <c r="C141" s="29"/>
+      <c r="D141" s="29"/>
     </row>
     <row r="142" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A142" s="16" t="s">
         <v>156</v>
       </c>
       <c r="C142" s="16">
-        <v>46279</v>
+        <v>50431</v>
       </c>
       <c r="D142" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A143" s="16" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="C143" s="16">
-        <v>46376</v>
+        <v>50658</v>
       </c>
       <c r="D143" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A144" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C144" s="16">
-        <v>46504</v>
+        <v>50797</v>
       </c>
       <c r="D144" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A145" s="16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C145" s="16">
-        <v>46624</v>
+        <v>50904</v>
       </c>
       <c r="D145" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A146" s="16" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="C146" s="16">
-        <v>46876</v>
+        <v>50995</v>
       </c>
       <c r="D146" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A147" s="16" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C147" s="16">
-        <v>47892</v>
+        <v>51135</v>
       </c>
       <c r="D147" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A148" s="16" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="C148" s="16">
-        <v>48805</v>
+        <v>51352</v>
       </c>
       <c r="D148" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E148">
-        <f>D148-D138</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A149" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="B149" s="29"/>
-      <c r="C149" s="29"/>
-      <c r="D149" s="29"/>
+      <c r="A149" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C149" s="16">
+        <v>51487</v>
+      </c>
+      <c r="D149" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A150" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C150" s="16">
-        <v>50431</v>
+        <v>51681</v>
       </c>
       <c r="D150" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A151" s="16" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C151" s="16">
-        <v>50658</v>
+        <v>52080</v>
       </c>
       <c r="D151" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A152" s="16" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C152" s="16">
-        <v>50797</v>
+        <v>52250</v>
       </c>
       <c r="D152" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A153" s="16" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="C153" s="16">
-        <v>50904</v>
+        <v>52768</v>
       </c>
       <c r="D153" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E153" s="16">
+        <f>D153-D143</f>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A154" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="C154" s="16">
-        <v>50995</v>
-      </c>
-      <c r="D154" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A154" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B154" s="29"/>
+      <c r="C154" s="29"/>
+      <c r="D154" s="29"/>
     </row>
     <row r="155" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A155" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C155" s="16">
-        <v>51135</v>
+        <v>53104</v>
       </c>
       <c r="D155" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A156" s="16" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="C156" s="16">
-        <v>51352</v>
+        <v>53332</v>
       </c>
       <c r="D156" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3216,502 +3322,502 @@
         <v>167</v>
       </c>
       <c r="C157" s="16">
-        <v>51487</v>
+        <v>53477</v>
       </c>
       <c r="D157" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A158" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C158" s="16">
-        <v>51681</v>
+        <v>53562</v>
       </c>
       <c r="D158" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A159" s="16" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C159" s="16">
-        <v>52080</v>
+        <v>53643</v>
       </c>
       <c r="D159" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A160" s="16" t="s">
-        <v>169</v>
+        <v>100</v>
       </c>
       <c r="C160" s="16">
-        <v>52250</v>
+        <v>53813</v>
       </c>
       <c r="D160" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A161" s="16" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="C161" s="16">
-        <v>52768</v>
+        <v>53851</v>
       </c>
       <c r="D161" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E161">
-        <f>D161-D151</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A162" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="B162" s="29"/>
-      <c r="C162" s="29"/>
-      <c r="D162" s="29"/>
+      <c r="A162" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C162" s="16">
+        <v>53952</v>
+      </c>
+      <c r="D162" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="163" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A163" s="16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C163" s="16">
-        <v>53104</v>
+        <v>54007</v>
       </c>
       <c r="D163" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A164" s="16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C164" s="16">
-        <v>53332</v>
+        <v>54209</v>
       </c>
       <c r="D164" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A165" s="16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C165" s="16">
-        <v>53477</v>
+        <v>54368</v>
       </c>
       <c r="D165" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A166" s="16" t="s">
-        <v>173</v>
+        <v>46</v>
       </c>
       <c r="C166" s="16">
-        <v>53562</v>
+        <v>54651</v>
       </c>
       <c r="D166" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A167" s="16" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="C167" s="16">
-        <v>53643</v>
+        <v>54872</v>
       </c>
       <c r="D167" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A168" s="16" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C168" s="16">
-        <v>53813</v>
+        <v>55390</v>
       </c>
       <c r="D168" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E168" s="16">
+        <f>D168-D156</f>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A169" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="C169" s="16">
-        <v>53851</v>
-      </c>
-      <c r="D169" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A169" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B169" s="29"/>
+      <c r="C169" s="29"/>
+      <c r="D169" s="29"/>
     </row>
     <row r="170" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A170" s="16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C170" s="16">
-        <v>53952</v>
+        <v>55725</v>
       </c>
       <c r="D170" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A171" s="16" t="s">
-        <v>175</v>
+        <v>95</v>
       </c>
       <c r="C171" s="16">
-        <v>54007</v>
+        <v>55958</v>
       </c>
       <c r="D171" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A172" s="16" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="C172" s="16">
-        <v>54209</v>
+        <v>56265</v>
       </c>
       <c r="D172" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A173" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C173" s="16">
-        <v>54368</v>
+        <v>56378</v>
       </c>
       <c r="D173" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A174" s="16" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C174" s="16">
-        <v>54651</v>
+        <v>56428</v>
       </c>
       <c r="D174" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A175" s="16" t="s">
-        <v>45</v>
+        <v>176</v>
       </c>
       <c r="C175" s="16">
-        <v>54872</v>
+        <v>56640</v>
       </c>
       <c r="D175" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A176" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C176" s="16">
+        <v>56715</v>
+      </c>
+      <c r="D176" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A177" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C177" s="16">
+        <v>56898</v>
+      </c>
+      <c r="D177" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A178" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C178" s="16">
+        <v>56982</v>
+      </c>
+      <c r="D178" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A179" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C179" s="16">
+        <v>57020</v>
+      </c>
+      <c r="D179" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A180" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C180" s="16">
+        <v>57085</v>
+      </c>
+      <c r="D180" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A181" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C181" s="16">
+        <v>57134</v>
+      </c>
+      <c r="D181" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A182" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C182" s="16">
+        <v>57234</v>
+      </c>
+      <c r="D182" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A183" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C183" s="16">
+        <v>57309</v>
+      </c>
+      <c r="D183" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A184" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C184" s="16">
+        <v>57531</v>
+      </c>
+      <c r="D184" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A185" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C185" s="16">
+        <v>57771</v>
+      </c>
+      <c r="D185" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A186" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C176" s="16">
-        <v>55390</v>
-      </c>
-      <c r="D176" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E176">
-        <f>D176-D164</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A177" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="B177" s="29"/>
-      <c r="C177" s="29"/>
-      <c r="D177" s="29"/>
-    </row>
-    <row r="178" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A178" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="C178" s="16">
-        <v>55725</v>
-      </c>
-      <c r="D178" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A179" s="16" t="s">
+      <c r="C186" s="16">
+        <v>58289</v>
+      </c>
+      <c r="D186" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E186" s="16">
+        <f>D186-D171</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A187" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B187" s="29"/>
+      <c r="C187" s="29"/>
+      <c r="D187" s="29"/>
+    </row>
+    <row r="188" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A188" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C188" s="16">
+        <v>58622</v>
+      </c>
+      <c r="D188" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A189" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C179" s="16">
-        <v>55958</v>
-      </c>
-      <c r="D179" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A180" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="C180" s="16">
-        <v>56265</v>
-      </c>
-      <c r="D180" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A181" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="C181" s="16">
-        <v>56378</v>
-      </c>
-      <c r="D181" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A182" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C182" s="16">
-        <v>56428</v>
-      </c>
-      <c r="D182" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A183" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C183" s="16">
-        <v>56640</v>
-      </c>
-      <c r="D183" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A184" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C184" s="16">
-        <v>56715</v>
-      </c>
-      <c r="D184" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A185" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="C185" s="16">
-        <v>56898</v>
-      </c>
-      <c r="D185" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A186" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="C186" s="16">
-        <v>56982</v>
-      </c>
-      <c r="D186" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A187" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="C187" s="16">
-        <v>57020</v>
-      </c>
-      <c r="D187" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A188" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C188" s="16">
-        <v>57085</v>
-      </c>
-      <c r="D188" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" hidden="1" outlineLevel="1">
-      <c r="A189" s="16" t="s">
-        <v>185</v>
-      </c>
       <c r="C189" s="16">
-        <v>57134</v>
+        <v>58848</v>
       </c>
       <c r="D189" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A190" s="16" t="s">
         <v>187</v>
       </c>
       <c r="C190" s="16">
-        <v>57234</v>
+        <v>59432</v>
       </c>
       <c r="D190" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A191" s="16" t="s">
         <v>188</v>
       </c>
       <c r="C191" s="16">
-        <v>57309</v>
+        <v>59610</v>
       </c>
       <c r="D191" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A192" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C192" s="16">
-        <v>57531</v>
+        <v>59716</v>
       </c>
       <c r="D192" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A193" s="16" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="C193" s="16">
-        <v>57771</v>
+        <v>59863</v>
       </c>
       <c r="D193" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A194" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C194" s="16">
+        <v>60022</v>
+      </c>
+      <c r="D194" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A195" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C194" s="16">
-        <v>58289</v>
-      </c>
-      <c r="D194" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E194">
-        <f>D194-D179</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A195" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="B195" s="29"/>
-      <c r="C195" s="29"/>
-      <c r="D195" s="29"/>
+      <c r="C195" s="16">
+        <v>60540</v>
+      </c>
+      <c r="D195" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E195" s="16">
+        <f>D195-D189</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="196" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A196" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C196" s="16">
-        <v>58622</v>
-      </c>
-      <c r="D196" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="A196" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B196" s="29"/>
+      <c r="C196" s="29"/>
+      <c r="D196" s="29"/>
     </row>
     <row r="197" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A197" s="16" t="s">
-        <v>95</v>
+        <v>191</v>
       </c>
       <c r="C197" s="16">
-        <v>58848</v>
+        <v>60909</v>
       </c>
       <c r="D197" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A198" s="16" t="s">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="C198" s="16">
-        <v>59432</v>
+        <v>61137</v>
       </c>
       <c r="D198" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3720,106 +3826,106 @@
         <v>192</v>
       </c>
       <c r="C199" s="16">
-        <v>59610</v>
+        <v>61238</v>
       </c>
       <c r="D199" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A200" s="16" t="s">
-        <v>193</v>
+        <v>37</v>
       </c>
       <c r="C200" s="16">
-        <v>59716</v>
+        <v>69043</v>
       </c>
       <c r="D200" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A201" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C201" s="16">
-        <v>59863</v>
+        <v>69309</v>
       </c>
       <c r="D201" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A202" s="16" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C202" s="16">
-        <v>60022</v>
+        <v>69906</v>
       </c>
       <c r="D202" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E202" s="16">
+        <f>D202-D198</f>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A203" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C203" s="16">
-        <v>60540</v>
-      </c>
-      <c r="D203" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E203">
-        <f>D203-D197</f>
-        <v>0</v>
-      </c>
+      <c r="A203" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B203" s="29"/>
+      <c r="C203" s="29"/>
+      <c r="D203" s="29"/>
     </row>
     <row r="204" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A204" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="B204" s="29"/>
-      <c r="C204" s="29"/>
-      <c r="D204" s="29"/>
+      <c r="A204" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C204" s="16">
+        <v>70786</v>
+      </c>
+      <c r="D204" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="205" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A205" s="16" t="s">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="C205" s="16">
-        <v>60909</v>
+        <v>71017</v>
       </c>
       <c r="D205" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A206" s="16" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C206" s="16">
-        <v>61137</v>
+        <v>71467</v>
       </c>
       <c r="D206" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A207" s="16" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="C207" s="16">
-        <v>61238</v>
+        <v>71725</v>
       </c>
       <c r="D207" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3828,361 +3934,267 @@
         <v>37</v>
       </c>
       <c r="C208" s="16">
-        <v>69043</v>
+        <v>72016</v>
       </c>
       <c r="D208" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A209" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C209" s="16">
-        <v>69309</v>
+        <v>72323</v>
       </c>
       <c r="D209" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A210" s="16" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="C210" s="16">
-        <v>69906</v>
+        <v>72665</v>
       </c>
       <c r="D210" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E210">
-        <f>D210-D206</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A211" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="B211" s="29"/>
-      <c r="C211" s="29"/>
-      <c r="D211" s="29"/>
-    </row>
-    <row r="212" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A211" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C211" s="16">
+        <v>73412</v>
+      </c>
+      <c r="D211" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A212" s="16" t="s">
-        <v>198</v>
+        <v>37</v>
       </c>
       <c r="C212" s="16">
-        <v>70786</v>
+        <v>73958</v>
       </c>
       <c r="D212" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A213" s="16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C213" s="16">
-        <v>71017</v>
+        <v>74749</v>
       </c>
       <c r="D213" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A214" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C214" s="16">
-        <v>71467</v>
+        <v>74982</v>
       </c>
       <c r="D214" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A215" s="16" t="s">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="C215" s="16">
-        <v>71725</v>
+        <v>75107</v>
       </c>
       <c r="D215" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" ref="D215" si="8">IF(B215 &gt;  0,C215-B215, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A216" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C216" s="16">
-        <v>72016</v>
+        <v>75280</v>
       </c>
       <c r="D216" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A217" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C217" s="16">
+        <v>75591</v>
+      </c>
+      <c r="D217" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A218" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C218" s="16">
+        <v>75741</v>
+      </c>
+      <c r="D218" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A219" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C219" s="16">
+        <v>75828</v>
+      </c>
+      <c r="D219" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A220" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="C217" s="16">
-        <v>72323</v>
-      </c>
-      <c r="D217" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A218" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C218" s="16">
-        <v>72665</v>
-      </c>
-      <c r="D218" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A219" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C219" s="16">
-        <v>73412</v>
-      </c>
-      <c r="D219" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A220" s="16" t="s">
-        <v>37</v>
-      </c>
       <c r="C220" s="16">
-        <v>73958</v>
+        <v>75972</v>
       </c>
       <c r="D220" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A221" s="16" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="C221" s="16">
-        <v>74749</v>
+        <v>76227</v>
       </c>
       <c r="D221" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A222" s="16" t="s">
-        <v>37</v>
+        <v>201</v>
       </c>
       <c r="C222" s="16">
-        <v>74982</v>
+        <v>76306</v>
       </c>
       <c r="D222" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A223" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C223" s="16">
-        <v>75107</v>
+        <v>76444</v>
       </c>
       <c r="D223" s="16">
-        <f t="shared" ref="D223" si="5">IF(B223 &gt;  0,C223-B223, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A224" s="16" t="s">
-        <v>37</v>
+        <v>203</v>
       </c>
       <c r="C224" s="16">
-        <v>75280</v>
+        <v>76741</v>
       </c>
       <c r="D224" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A225" s="16" t="s">
-        <v>37</v>
+        <v>204</v>
       </c>
       <c r="C225" s="16">
-        <v>75591</v>
+        <v>77063</v>
       </c>
       <c r="D225" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A226" s="16" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C226" s="16">
-        <v>75741</v>
+        <v>77866</v>
       </c>
       <c r="D226" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" hidden="1" outlineLevel="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A227" s="16" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C227" s="16">
-        <v>75828</v>
+        <v>77902</v>
       </c>
       <c r="D227" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A228" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="C228" s="16">
-        <v>75972</v>
-      </c>
-      <c r="D228" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A229" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="C229" s="16">
-        <v>76227</v>
-      </c>
-      <c r="D229" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A230" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="C230" s="16">
-        <v>76306</v>
-      </c>
-      <c r="D230" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A231" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="C231" s="16">
-        <v>76444</v>
-      </c>
-      <c r="D231" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A232" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C232" s="16">
-        <v>76741</v>
-      </c>
-      <c r="D232" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A233" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C233" s="16">
-        <v>77063</v>
-      </c>
-      <c r="D233" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" hidden="1" outlineLevel="1">
-      <c r="A234" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="C234" s="16">
-        <v>77866</v>
-      </c>
-      <c r="D234" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A235" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C235" s="16">
-        <v>77902</v>
-      </c>
-      <c r="D235" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E235" s="30">
-        <f>D235-D213</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" s="32" customFormat="1" ht="16.5" hidden="1" outlineLevel="1" thickTop="1" thickBot="1">
-      <c r="A236" s="31"/>
-      <c r="B236" s="31"/>
-      <c r="C236" s="31"/>
-      <c r="D236" s="31"/>
-      <c r="E236" s="32">
-        <f>SUM(E1:E235)</f>
-        <v>49</v>
-      </c>
-      <c r="F236" s="32" t="s">
-        <v>231</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E227" s="41">
+        <f>D227-D205</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" s="31" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+      <c r="A228" s="30"/>
+      <c r="B228" s="30"/>
+      <c r="C228" s="30"/>
+      <c r="D228" s="30"/>
+      <c r="E228" s="30">
+        <f>SUM(E1:E227)</f>
+        <v>141969</v>
+      </c>
+      <c r="F228" s="30" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A77:D77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4226,14 +4238,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -4296,14 +4308,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
@@ -4826,14 +4838,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="24" t="s">

</xml_diff>

<commit_message>
NSMB - cleanup - Move Yoshi's world 5 savestate to the LevelSavestates/World 5 savestate.  Merge spreadsheets.  Remove unneeded movie file, move another into a Misc folder.  The purpose of that folder is for alternate versions of levels (that are equally fast) or for interesting but slower tricks discovered.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="4" r:id="rId1"/>
-    <sheet name="V3" sheetId="2" r:id="rId2"/>
-    <sheet name="V1" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="V4" sheetId="5" r:id="rId2"/>
+    <sheet name="V3" sheetId="2" r:id="rId3"/>
+    <sheet name="V1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="239">
   <si>
     <t>1-1</t>
   </si>
@@ -716,6 +717,24 @@
   </si>
   <si>
     <t>Note: 10154 is possible, but doesn't matter due to waiting for 465 on the timer.</t>
+  </si>
+  <si>
+    <t>Mario appears</t>
+  </si>
+  <si>
+    <t>Checkpoint 2626</t>
+  </si>
+  <si>
+    <t>Checkpoint 936</t>
+  </si>
+  <si>
+    <t>Checkpoint 759</t>
+  </si>
+  <si>
+    <t>In Level Improvements:</t>
+  </si>
+  <si>
+    <t>terrot</t>
   </si>
 </sst>
 </file>
@@ -812,7 +831,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -882,11 +901,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -943,6 +982,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,7 +1286,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4209,10 +4251,3502 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:I236"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="16"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="43"/>
+      <c r="G1">
+        <f>E236</f>
+        <v>723</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" ht="19.5" collapsed="1" thickTop="1">
+      <c r="A2" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+    </row>
+    <row r="3" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="16">
+        <v>355</v>
+      </c>
+      <c r="D3" s="16">
+        <f>IF(B3 &gt;  0,C3-B3, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="16">
+        <v>476</v>
+      </c>
+      <c r="C4" s="16">
+        <v>517</v>
+      </c>
+      <c r="D4" s="16">
+        <f>IF(B4 &gt;  0,C4-B4, 0)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2937</v>
+      </c>
+      <c r="C5" s="16">
+        <v>2937</v>
+      </c>
+      <c r="D5" s="16">
+        <f>IF(B5 &gt;  0,C5-B5, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="16">
+        <v>2579</v>
+      </c>
+      <c r="C6" s="16">
+        <v>3038</v>
+      </c>
+      <c r="D6" s="16">
+        <f>IF(B6 &gt;  0,C6-B6, 0)</f>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="18.75" collapsed="1">
+      <c r="A7" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+    </row>
+    <row r="8" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A8" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="16">
+        <v>2806</v>
+      </c>
+      <c r="C9" s="16">
+        <v>3285</v>
+      </c>
+      <c r="D9" s="16">
+        <f>IF(B9 &gt;  0,C9-B9, 0)</f>
+        <v>479</v>
+      </c>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A10" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="16">
+        <v>3093</v>
+      </c>
+      <c r="C10" s="16">
+        <v>3571</v>
+      </c>
+      <c r="D10" s="16">
+        <f>IF(B10 &gt;  0,C10-B10, 0)</f>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A11" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" s="16">
+        <v>3151</v>
+      </c>
+      <c r="C11" s="16">
+        <v>3630</v>
+      </c>
+      <c r="D11" s="16">
+        <f>IF(B11 &gt;  0,C11-B11, 0)</f>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A12" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" s="16">
+        <v>3712</v>
+      </c>
+      <c r="C12" s="16">
+        <v>4192</v>
+      </c>
+      <c r="D12" s="16">
+        <f>IF(B12 &gt;  0,C12-B12, 0)</f>
+        <v>480</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="16">
+        <v>4146</v>
+      </c>
+      <c r="C13" s="16">
+        <v>4627</v>
+      </c>
+      <c r="D13" s="16">
+        <f>IF(B13 &gt;  0,C13-B13, 0)</f>
+        <v>481</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="16">
+        <v>4664</v>
+      </c>
+      <c r="C14" s="16">
+        <v>5145</v>
+      </c>
+      <c r="D14" s="16">
+        <f>IF(B14 &gt;  0,C14-B14, 0)</f>
+        <v>481</v>
+      </c>
+      <c r="E14">
+        <f>D14-D9</f>
+        <v>2</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17">
+        <v>5738</v>
+      </c>
+      <c r="D15" s="16">
+        <f>IF(B15 &gt;  0,C15-B15, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" hidden="1" outlineLevel="1">
+      <c r="A16" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="16">
+        <v>5057</v>
+      </c>
+      <c r="C17" s="16">
+        <v>5937</v>
+      </c>
+      <c r="D17" s="16">
+        <f>IF(B17 &gt;  0,C17-B17, 0)</f>
+        <v>880</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A18" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="16">
+        <v>5296</v>
+      </c>
+      <c r="C18" s="16">
+        <v>6199</v>
+      </c>
+      <c r="D18" s="16">
+        <f>IF(B18 &gt;  0,C18-B18, 0)</f>
+        <v>903</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A19" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="16">
+        <v>6823</v>
+      </c>
+      <c r="C19" s="16">
+        <v>7742</v>
+      </c>
+      <c r="D19" s="16">
+        <f>IF(B19 &gt;  0,C19-B19, 0)</f>
+        <v>919</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="16">
+        <v>7351</v>
+      </c>
+      <c r="C20" s="16">
+        <v>8272</v>
+      </c>
+      <c r="D20" s="16">
+        <f>IF(B20 &gt;  0,C20-B20, 0)</f>
+        <v>921</v>
+      </c>
+      <c r="E20">
+        <f>D20-D17</f>
+        <v>41</v>
+      </c>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="16">
+        <v>8786</v>
+      </c>
+      <c r="D21" s="16">
+        <f>IF(B21 &gt;  0,C21-B21, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A22" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="16">
+        <v>8406</v>
+      </c>
+      <c r="C23" s="16">
+        <v>9830</v>
+      </c>
+      <c r="D23" s="16">
+        <f>IF(B23 &gt;  0,C23-B23, 0)</f>
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A24" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="16">
+        <v>8632</v>
+      </c>
+      <c r="C24" s="16">
+        <v>10077</v>
+      </c>
+      <c r="D24" s="16">
+        <f>IF(B24 &gt;  0,C24-B24, 0)</f>
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A25" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="16">
+        <v>9637</v>
+      </c>
+      <c r="C25" s="16">
+        <v>11112</v>
+      </c>
+      <c r="D25" s="16">
+        <f>IF(B25 &gt;  0,C25-B25, 0)</f>
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A26" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="16">
+        <v>9674</v>
+      </c>
+      <c r="D26" s="16">
+        <f>IF(B26 &gt;  0,C26-B26, 0)</f>
+        <v>-9674</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A27" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="16">
+        <v>9816</v>
+      </c>
+      <c r="C27" s="16">
+        <v>11292</v>
+      </c>
+      <c r="D27" s="16">
+        <f>IF(B27 &gt;  0,C27-B27, 0)</f>
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="16">
+        <v>10327</v>
+      </c>
+      <c r="C28" s="16">
+        <v>11807</v>
+      </c>
+      <c r="D28" s="16">
+        <f>IF(B28 &gt;  0,C28-B28, 0)</f>
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="16">
+        <v>10626</v>
+      </c>
+      <c r="C29" s="16">
+        <v>12118</v>
+      </c>
+      <c r="D29" s="16">
+        <f>IF(B29 &gt;  0,C29-B29, 0)</f>
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A30" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="16">
+        <v>11140</v>
+      </c>
+      <c r="C30" s="16">
+        <v>12632</v>
+      </c>
+      <c r="D30" s="16">
+        <f>IF(B30 &gt;  0,C30-B30, 0)</f>
+        <v>1492</v>
+      </c>
+      <c r="E30">
+        <f>D30-D24</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A31" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+    </row>
+    <row r="32" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A32" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B32" s="16">
+        <v>11592</v>
+      </c>
+      <c r="C32" s="16">
+        <v>13368</v>
+      </c>
+      <c r="D32" s="16">
+        <f>IF(B32 &gt;  0,C32-B32, 0)</f>
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A33" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="16">
+        <v>13611</v>
+      </c>
+      <c r="D33" s="16">
+        <f>IF(B33 &gt;  0,C33-B33, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A34" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="16">
+        <v>12540</v>
+      </c>
+      <c r="C34" s="16">
+        <v>14342</v>
+      </c>
+      <c r="D34" s="16">
+        <f>IF(B34 &gt;  0,C34-B34, 0)</f>
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18.75" collapsed="1">
+      <c r="A35" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+    </row>
+    <row r="36" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A36" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A37" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="16">
+        <v>12987</v>
+      </c>
+      <c r="C37" s="16">
+        <v>15235</v>
+      </c>
+      <c r="D37" s="16">
+        <f>IF(B37 &gt;  0,C37-B37, 0)</f>
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A38" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="16">
+        <v>13217</v>
+      </c>
+      <c r="C38" s="16">
+        <v>15489</v>
+      </c>
+      <c r="D38" s="16">
+        <f>IF(B38 &gt;  0,C38-B38, 0)</f>
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A39" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="16">
+        <v>14776</v>
+      </c>
+      <c r="C39" s="16">
+        <v>17048</v>
+      </c>
+      <c r="D39" s="16">
+        <f>IF(B39 &gt;  0,C39-B39, 0)</f>
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A40" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="16">
+        <v>15307</v>
+      </c>
+      <c r="C40" s="16">
+        <v>17562</v>
+      </c>
+      <c r="D40" s="16">
+        <f>IF(B40 &gt;  0,C40-B40, 0)</f>
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A41" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="16">
+        <v>15573</v>
+      </c>
+      <c r="C41" s="16">
+        <v>18105</v>
+      </c>
+      <c r="D41" s="16">
+        <f>IF(B41 &gt;  0,C41-B41, 0)</f>
+        <v>2532</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A42" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A43" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="16">
+        <v>15722</v>
+      </c>
+      <c r="C43" s="16">
+        <v>18403</v>
+      </c>
+      <c r="D43" s="16">
+        <f>IF(B43 &gt;  0,C43-B43, 0)</f>
+        <v>2681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A44" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="16">
+        <v>15947</v>
+      </c>
+      <c r="C44" s="16">
+        <v>18649</v>
+      </c>
+      <c r="D44" s="16">
+        <f>IF(B44 &gt;  0,C44-B44, 0)</f>
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A45" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="16">
+        <v>16087</v>
+      </c>
+      <c r="C45" s="16">
+        <v>18789</v>
+      </c>
+      <c r="D45" s="16">
+        <f>IF(B45 &gt;  0,C45-B45, 0)</f>
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A46" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="16">
+        <v>17508</v>
+      </c>
+      <c r="C46" s="16">
+        <v>20233</v>
+      </c>
+      <c r="D46" s="16">
+        <f>IF(B46 &gt;  0,C46-B46, 0)</f>
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A47" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16">
+        <v>17579</v>
+      </c>
+      <c r="C47" s="16">
+        <v>20304</v>
+      </c>
+      <c r="D47" s="16">
+        <f>IF(B47 &gt;  0,C47-B47, 0)</f>
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A48" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="16">
+        <v>17846</v>
+      </c>
+      <c r="C48" s="16">
+        <v>20584</v>
+      </c>
+      <c r="D48" s="16">
+        <f>IF(B48 &gt;  0,C48-B48, 0)</f>
+        <v>2738</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A49" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="16">
+        <v>18368</v>
+      </c>
+      <c r="C49" s="16">
+        <v>21098</v>
+      </c>
+      <c r="D49" s="16">
+        <f>IF(B49 &gt;  0,C49-B49, 0)</f>
+        <v>2730</v>
+      </c>
+      <c r="E49">
+        <f>D49-D44</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A50" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+    </row>
+    <row r="51" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A51" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="16">
+        <v>18945</v>
+      </c>
+      <c r="C51" s="16">
+        <v>22185</v>
+      </c>
+      <c r="D51" s="16">
+        <f>IF(B51 &gt;  0,C51-B51, 0)</f>
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A52" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="16">
+        <v>19177</v>
+      </c>
+      <c r="C52" s="16">
+        <v>22443</v>
+      </c>
+      <c r="D52" s="16">
+        <f>IF(B52 &gt;  0,C52-B52, 0)</f>
+        <v>3266</v>
+      </c>
+      <c r="E52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="I52" s="25"/>
+    </row>
+    <row r="53" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A53" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="16">
+        <v>20120</v>
+      </c>
+      <c r="C53" s="16">
+        <v>23386</v>
+      </c>
+      <c r="D53" s="16">
+        <f>IF(B53 &gt;  0,C53-B53, 0)</f>
+        <v>3266</v>
+      </c>
+      <c r="E53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A54" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="16">
+        <v>20187</v>
+      </c>
+      <c r="C54" s="16">
+        <v>23453</v>
+      </c>
+      <c r="D54" s="16">
+        <f>IF(B54 &gt;  0,C54-B54, 0)</f>
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A55" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="16">
+        <v>20258</v>
+      </c>
+      <c r="C55" s="16">
+        <v>23524</v>
+      </c>
+      <c r="D55" s="16">
+        <f>IF(B55 &gt;  0,C55-B55, 0)</f>
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A56" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="16">
+        <v>20351</v>
+      </c>
+      <c r="C56" s="16">
+        <v>23618</v>
+      </c>
+      <c r="D56" s="16">
+        <f>IF(B56 &gt;  0,C56-B56, 0)</f>
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A57" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="16">
+        <v>20394</v>
+      </c>
+      <c r="C57" s="16">
+        <v>23661</v>
+      </c>
+      <c r="D57" s="16">
+        <f>IF(B57 &gt;  0,C57-B57, 0)</f>
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A58" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="16">
+        <v>20465</v>
+      </c>
+      <c r="C58" s="16">
+        <v>23733</v>
+      </c>
+      <c r="D58" s="16">
+        <f>IF(B58 &gt;  0,C58-B58, 0)</f>
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A59" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="16">
+        <v>20658</v>
+      </c>
+      <c r="C59" s="16">
+        <v>23926</v>
+      </c>
+      <c r="D59" s="16">
+        <f>IF(B59 &gt;  0,C59-B59, 0)</f>
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A60" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="16">
+        <v>21172</v>
+      </c>
+      <c r="C60" s="16">
+        <v>24440</v>
+      </c>
+      <c r="D60" s="16">
+        <f>IF(B60 &gt;  0,C60-B60, 0)</f>
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A61" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+    </row>
+    <row r="62" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A62" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="16">
+        <v>21661</v>
+      </c>
+      <c r="C62" s="16">
+        <v>25475</v>
+      </c>
+      <c r="D62" s="16">
+        <f>IF(B62 &gt;  0,C62-B62, 0)</f>
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A63" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="16">
+        <v>21890</v>
+      </c>
+      <c r="C63" s="16">
+        <v>25726</v>
+      </c>
+      <c r="D63" s="16">
+        <f>IF(B63 &gt;  0,C63-B63, 0)</f>
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" hidden="1" outlineLevel="1">
+      <c r="A64" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="16">
+        <v>21929</v>
+      </c>
+      <c r="C64" s="16">
+        <v>25765</v>
+      </c>
+      <c r="D64" s="16">
+        <f>IF(B64 &gt;  0,C64-B64, 0)</f>
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A65" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="16">
+        <v>21995</v>
+      </c>
+      <c r="C65" s="16">
+        <v>25832</v>
+      </c>
+      <c r="D65" s="16">
+        <f>IF(B65 &gt;  0,C65-B65, 0)</f>
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A66" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B66" s="16">
+        <v>22090</v>
+      </c>
+      <c r="C66" s="16">
+        <v>25927</v>
+      </c>
+      <c r="D66" s="16">
+        <f>IF(B66 &gt;  0,C66-B66, 0)</f>
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A67" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="16">
+        <v>22121</v>
+      </c>
+      <c r="C67" s="16">
+        <v>25957</v>
+      </c>
+      <c r="D67" s="16">
+        <f>IF(B67 &gt;  0,C67-B67, 0)</f>
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A68" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="16">
+        <v>22330</v>
+      </c>
+      <c r="C68" s="16">
+        <v>26163</v>
+      </c>
+      <c r="D68" s="16">
+        <f>IF(B68 &gt;  0,C68-B68, 0)</f>
+        <v>3833</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A69" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="16">
+        <v>22372</v>
+      </c>
+      <c r="C69" s="16">
+        <v>26202</v>
+      </c>
+      <c r="D69" s="16">
+        <f>IF(B69 &gt;  0,C69-B69, 0)</f>
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A70" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="16">
+        <v>22388</v>
+      </c>
+      <c r="C70" s="16">
+        <v>26218</v>
+      </c>
+      <c r="D70" s="16">
+        <f>IF(B70 &gt;  0,C70-B70, 0)</f>
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A71" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="16">
+        <v>22421</v>
+      </c>
+      <c r="C71" s="16">
+        <v>26262</v>
+      </c>
+      <c r="D71" s="16">
+        <f>IF(B71 &gt;  0,C71-B71, 0)</f>
+        <v>3841</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A72" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B72" s="16">
+        <v>22454</v>
+      </c>
+      <c r="C72" s="16">
+        <v>26286</v>
+      </c>
+      <c r="D72" s="16">
+        <f>IF(B72 &gt;  0,C72-B72, 0)</f>
+        <v>3832</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A73" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B73" s="16">
+        <v>22708</v>
+      </c>
+      <c r="C73" s="16">
+        <v>26571</v>
+      </c>
+      <c r="D73" s="16">
+        <f>IF(B73 &gt;  0,C73-B73, 0)</f>
+        <v>3863</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A74" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" s="16">
+        <v>22829</v>
+      </c>
+      <c r="C74" s="16">
+        <v>26694</v>
+      </c>
+      <c r="D74" s="16">
+        <f>IF(B74 &gt;  0,C74-B74, 0)</f>
+        <v>3865</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A75" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" s="16">
+        <v>23205</v>
+      </c>
+      <c r="C75" s="16">
+        <v>27067</v>
+      </c>
+      <c r="D75" s="16">
+        <f>IF(B75 &gt;  0,C75-B75, 0)</f>
+        <v>3862</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A76" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" s="16">
+        <v>23849</v>
+      </c>
+      <c r="C76" s="16">
+        <v>27731</v>
+      </c>
+      <c r="D76" s="16">
+        <f>IF(B76 &gt;  0,C76-B76, 0)</f>
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A77" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B77" s="16">
+        <v>24266</v>
+      </c>
+      <c r="C77" s="16">
+        <v>28148</v>
+      </c>
+      <c r="D77" s="16">
+        <f>IF(B77 &gt;  0,C77-B77, 0)</f>
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A78" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B78" s="16">
+        <v>24570</v>
+      </c>
+      <c r="C78" s="16">
+        <v>28462</v>
+      </c>
+      <c r="D78" s="16">
+        <f>IF(B78 &gt;  0,C78-B78, 0)</f>
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A79" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="16">
+        <v>25088</v>
+      </c>
+      <c r="C79" s="16">
+        <v>28980</v>
+      </c>
+      <c r="D79" s="16">
+        <f>IF(B79 &gt;  0,C79-B79, 0)</f>
+        <v>3892</v>
+      </c>
+      <c r="E79">
+        <f>D79-D63</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A80" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+    </row>
+    <row r="81" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A81" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81" s="16">
+        <v>25472</v>
+      </c>
+      <c r="C81" s="16">
+        <v>29893</v>
+      </c>
+      <c r="D81" s="16">
+        <f>IF(B81 &gt;  0,C81-B81, 0)</f>
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A82" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B82" s="16">
+        <v>25697</v>
+      </c>
+      <c r="C82" s="16">
+        <v>30136</v>
+      </c>
+      <c r="D82" s="16">
+        <f>IF(B82 &gt;  0,C82-B82, 0)</f>
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A83" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" s="16">
+        <v>25830</v>
+      </c>
+      <c r="C83" s="16">
+        <v>30269</v>
+      </c>
+      <c r="D83" s="16">
+        <f>IF(B83 &gt;  0,C83-B83, 0)</f>
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="A84" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B84" s="16">
+        <v>26420</v>
+      </c>
+      <c r="C84" s="16">
+        <v>30859</v>
+      </c>
+      <c r="D84" s="16">
+        <f>IF(B84 &gt;  0,C84-B84, 0)</f>
+        <v>4439</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="18.75">
+      <c r="A85" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B85" s="36"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="36"/>
+    </row>
+    <row r="86" spans="1:5" outlineLevel="1">
+      <c r="A86" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+    </row>
+    <row r="87" spans="1:5" outlineLevel="1">
+      <c r="A87" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="16">
+        <v>26790</v>
+      </c>
+      <c r="C87" s="16">
+        <v>31594</v>
+      </c>
+      <c r="D87" s="16">
+        <f>IF(B87 &gt;  0,C87-B87, 0)</f>
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" outlineLevel="1">
+      <c r="A88" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" s="16">
+        <v>27017</v>
+      </c>
+      <c r="C88" s="16">
+        <v>31842</v>
+      </c>
+      <c r="D88" s="16">
+        <f>IF(B88 &gt;  0,C88-B88, 0)</f>
+        <v>4825</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" outlineLevel="1">
+      <c r="A89" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B89" s="16">
+        <v>27730</v>
+      </c>
+      <c r="C89" s="16">
+        <v>32556</v>
+      </c>
+      <c r="D89" s="16">
+        <f>IF(B89 &gt;  0,C89-B89, 0)</f>
+        <v>4826</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" outlineLevel="1">
+      <c r="A90" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90" s="16">
+        <v>28335</v>
+      </c>
+      <c r="C90" s="16">
+        <v>33163</v>
+      </c>
+      <c r="D90" s="16">
+        <f>IF(B90 &gt;  0,C90-B90, 0)</f>
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" outlineLevel="1">
+      <c r="A91" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B91" s="16">
+        <v>28853</v>
+      </c>
+      <c r="C91" s="16">
+        <v>33681</v>
+      </c>
+      <c r="D91" s="16">
+        <f>IF(B91 &gt;  0,C91-B91, 0)</f>
+        <v>4828</v>
+      </c>
+      <c r="E91">
+        <f>D91-D88</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" outlineLevel="1">
+      <c r="A92" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+    </row>
+    <row r="93" spans="1:5" outlineLevel="1">
+      <c r="A93" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B93" s="16">
+        <v>29213</v>
+      </c>
+      <c r="C93" s="16">
+        <v>34468</v>
+      </c>
+      <c r="D93" s="16">
+        <f>IF(B93 &gt;  0,C93-B93, 0)</f>
+        <v>5255</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" outlineLevel="1">
+      <c r="A94" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="16">
+        <v>29438</v>
+      </c>
+      <c r="C94" s="16">
+        <v>34713</v>
+      </c>
+      <c r="D94" s="16">
+        <f>IF(B94 &gt;  0,C94-B94, 0)</f>
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" outlineLevel="1">
+      <c r="A95" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" s="16">
+        <v>29585</v>
+      </c>
+      <c r="C95" s="16">
+        <v>34860</v>
+      </c>
+      <c r="D95" s="16">
+        <f>IF(B95 &gt;  0,C95-B95, 0)</f>
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" outlineLevel="1">
+      <c r="A96" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B96" s="16">
+        <v>29708</v>
+      </c>
+      <c r="C96" s="16">
+        <v>34998</v>
+      </c>
+      <c r="D96" s="16">
+        <f>IF(B96 &gt;  0,C96-B96, 0)</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" outlineLevel="1">
+      <c r="A97" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B97" s="16">
+        <v>29848</v>
+      </c>
+      <c r="C97" s="16">
+        <v>35137</v>
+      </c>
+      <c r="D97" s="16">
+        <f>IF(B97 &gt;  0,C97-B97, 0)</f>
+        <v>5289</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" outlineLevel="1">
+      <c r="A98" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B98" s="16">
+        <v>29894</v>
+      </c>
+      <c r="C98" s="16">
+        <v>35181</v>
+      </c>
+      <c r="D98" s="16">
+        <f>IF(B98 &gt;  0,C98-B98, 0)</f>
+        <v>5287</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" outlineLevel="1">
+      <c r="A99" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" s="16">
+        <v>30331</v>
+      </c>
+      <c r="C99" s="16">
+        <v>35621</v>
+      </c>
+      <c r="D99" s="16">
+        <f>IF(B99 &gt;  0,C99-B99, 0)</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" outlineLevel="1">
+      <c r="A100" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B100" s="16">
+        <v>30698</v>
+      </c>
+      <c r="C100" s="16">
+        <v>35992</v>
+      </c>
+      <c r="D100" s="16">
+        <f>IF(B100 &gt;  0,C100-B100, 0)</f>
+        <v>5294</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" outlineLevel="1">
+      <c r="A101" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B101" s="16">
+        <v>30992</v>
+      </c>
+      <c r="C101" s="16">
+        <v>36290</v>
+      </c>
+      <c r="D101" s="16">
+        <f>IF(B101 &gt;  0,C101-B101, 0)</f>
+        <v>5298</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" outlineLevel="1">
+      <c r="A102" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B102" s="16">
+        <v>31261</v>
+      </c>
+      <c r="C102" s="16">
+        <v>36576</v>
+      </c>
+      <c r="D102" s="16">
+        <f>IF(B102 &gt;  0,C102-B102, 0)</f>
+        <v>5315</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" outlineLevel="1">
+      <c r="A103" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" s="16">
+        <v>31543</v>
+      </c>
+      <c r="C103" s="16">
+        <v>36872</v>
+      </c>
+      <c r="D103" s="16">
+        <f>IF(B103 &gt;  0,C103-B103, 0)</f>
+        <v>5329</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" outlineLevel="1">
+      <c r="A104" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B104" s="16">
+        <v>31906</v>
+      </c>
+      <c r="C104" s="16">
+        <v>37235</v>
+      </c>
+      <c r="D104" s="16">
+        <f>IF(B104 &gt;  0,C104-B104, 0)</f>
+        <v>5329</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" outlineLevel="1">
+      <c r="A105" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B105" s="16">
+        <v>32382</v>
+      </c>
+      <c r="C105" s="16">
+        <v>37736</v>
+      </c>
+      <c r="D105" s="16">
+        <f>IF(B105 &gt;  0,C105-B105, 0)</f>
+        <v>5354</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" outlineLevel="1">
+      <c r="A106" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B106" s="16">
+        <v>32646</v>
+      </c>
+      <c r="C106" s="16">
+        <v>38007</v>
+      </c>
+      <c r="D106" s="16">
+        <f>IF(B106 &gt;  0,C106-B106, 0)</f>
+        <v>5361</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" outlineLevel="1">
+      <c r="A107" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B107" s="16">
+        <v>33164</v>
+      </c>
+      <c r="C107" s="16">
+        <v>38525</v>
+      </c>
+      <c r="D107" s="16">
+        <f>IF(B107 &gt;  0,C107-B107, 0)</f>
+        <v>5361</v>
+      </c>
+      <c r="E107">
+        <f>D107-D94</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" outlineLevel="1">
+      <c r="A108" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="29"/>
+    </row>
+    <row r="109" spans="1:5" outlineLevel="1">
+      <c r="A109" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B109" s="16">
+        <v>33599</v>
+      </c>
+      <c r="C109" s="16">
+        <v>39462</v>
+      </c>
+      <c r="D109" s="16">
+        <f>IF(B109 &gt;  0,C109-B109, 0)</f>
+        <v>5863</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" outlineLevel="1">
+      <c r="A110" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B110" s="16">
+        <v>33826</v>
+      </c>
+      <c r="C110" s="16">
+        <v>39712</v>
+      </c>
+      <c r="D110" s="16">
+        <f>IF(B110 &gt;  0,C110-B110, 0)</f>
+        <v>5886</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" outlineLevel="1">
+      <c r="A111" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B111" s="16">
+        <v>34022</v>
+      </c>
+      <c r="C111" s="16">
+        <v>39911</v>
+      </c>
+      <c r="D111" s="16">
+        <f>IF(B111 &gt;  0,C111-B111, 0)</f>
+        <v>5889</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" outlineLevel="1">
+      <c r="A112" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B112" s="16">
+        <v>34385</v>
+      </c>
+      <c r="C112" s="16">
+        <v>40279</v>
+      </c>
+      <c r="D112" s="16">
+        <f>IF(B112 &gt;  0,C112-B112, 0)</f>
+        <v>5894</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" outlineLevel="1">
+      <c r="A113" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="16">
+        <v>34767</v>
+      </c>
+      <c r="C113" s="16">
+        <v>40661</v>
+      </c>
+      <c r="D113" s="16">
+        <f>IF(B113 &gt;  0,C113-B113, 0)</f>
+        <v>5894</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" outlineLevel="1">
+      <c r="A114" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B114" s="16">
+        <v>34904</v>
+      </c>
+      <c r="C114" s="16">
+        <v>40799</v>
+      </c>
+      <c r="D114" s="16">
+        <f>IF(B114 &gt;  0,C114-B114, 0)</f>
+        <v>5895</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" outlineLevel="1">
+      <c r="A115" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B115" s="16">
+        <v>34950</v>
+      </c>
+      <c r="C115" s="16">
+        <v>40846</v>
+      </c>
+      <c r="D115" s="16">
+        <f>IF(B115 &gt;  0,C115-B115, 0)</f>
+        <v>5896</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" outlineLevel="1">
+      <c r="A116" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B116" s="16">
+        <v>35025</v>
+      </c>
+      <c r="C116" s="16">
+        <v>40921</v>
+      </c>
+      <c r="D116" s="16">
+        <f>IF(B116 &gt;  0,C116-B116, 0)</f>
+        <v>5896</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" outlineLevel="1">
+      <c r="A117" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B117" s="16">
+        <v>35282</v>
+      </c>
+      <c r="C117" s="16">
+        <v>41175</v>
+      </c>
+      <c r="D117" s="16">
+        <f>IF(B117 &gt;  0,C117-B117, 0)</f>
+        <v>5893</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" outlineLevel="1">
+      <c r="A118" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B118" s="16">
+        <v>35587</v>
+      </c>
+      <c r="C118" s="16">
+        <v>41485</v>
+      </c>
+      <c r="D118" s="16">
+        <f>IF(B118 &gt;  0,C118-B118, 0)</f>
+        <v>5898</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" outlineLevel="1">
+      <c r="A119" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B119" s="16">
+        <v>35856</v>
+      </c>
+      <c r="C119" s="16">
+        <v>41774</v>
+      </c>
+      <c r="D119" s="16">
+        <f>IF(B119 &gt;  0,C119-B119, 0)</f>
+        <v>5918</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" outlineLevel="1">
+      <c r="A120" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B120" s="16">
+        <v>36497</v>
+      </c>
+      <c r="C120" s="16">
+        <v>42408</v>
+      </c>
+      <c r="D120" s="16">
+        <f>IF(B120 &gt;  0,C120-B120, 0)</f>
+        <v>5911</v>
+      </c>
+      <c r="E120">
+        <f>D120-D110</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" outlineLevel="1">
+      <c r="A121" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B121" s="29"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="29"/>
+    </row>
+    <row r="122" spans="1:5" outlineLevel="1">
+      <c r="A122" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B122" s="16">
+        <v>37222</v>
+      </c>
+      <c r="C122" s="16">
+        <v>43787</v>
+      </c>
+      <c r="D122" s="16">
+        <f>IF(B122 &gt;  0,C122-B122, 0)</f>
+        <v>6565</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" outlineLevel="1">
+      <c r="A123" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B123" s="16">
+        <v>37448</v>
+      </c>
+      <c r="C123" s="16">
+        <v>44032</v>
+      </c>
+      <c r="D123" s="16">
+        <f>IF(B123 &gt;  0,C123-B123, 0)</f>
+        <v>6584</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" outlineLevel="1">
+      <c r="A124" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="16">
+        <v>37664</v>
+      </c>
+      <c r="C124" s="16">
+        <v>44249</v>
+      </c>
+      <c r="D124" s="16">
+        <f>IF(B124 &gt;  0,C124-B124, 0)</f>
+        <v>6585</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" outlineLevel="1">
+      <c r="A125" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B125" s="16">
+        <v>37919</v>
+      </c>
+      <c r="C125" s="16">
+        <v>44527</v>
+      </c>
+      <c r="D125" s="16">
+        <f>IF(B125 &gt;  0,C125-B125, 0)</f>
+        <v>6608</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" outlineLevel="1">
+      <c r="A126" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B126" s="16">
+        <v>39165</v>
+      </c>
+      <c r="C126" s="16">
+        <v>45775</v>
+      </c>
+      <c r="D126" s="16">
+        <f>IF(B126 &gt;  0,C126-B126, 0)</f>
+        <v>6610</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" outlineLevel="1">
+      <c r="A127" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B127" s="16">
+        <v>39722</v>
+      </c>
+      <c r="C127" s="16">
+        <v>46333</v>
+      </c>
+      <c r="D127" s="16">
+        <f>IF(B127 &gt;  0,C127-B127, 0)</f>
+        <v>6611</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" outlineLevel="1">
+      <c r="A128" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128" s="16">
+        <v>41771</v>
+      </c>
+      <c r="C128" s="16">
+        <v>48401</v>
+      </c>
+      <c r="D128" s="16">
+        <f>IF(B128 &gt;  0,C128-B128, 0)</f>
+        <v>6630</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" outlineLevel="1">
+      <c r="A129" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B129" s="16">
+        <v>42009</v>
+      </c>
+      <c r="C129" s="16">
+        <v>48651</v>
+      </c>
+      <c r="D129" s="16">
+        <f>IF(B129 &gt;  0,C129-B129, 0)</f>
+        <v>6642</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" outlineLevel="1">
+      <c r="A130" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B130" s="16">
+        <v>42523</v>
+      </c>
+      <c r="C130" s="16">
+        <v>49165</v>
+      </c>
+      <c r="D130" s="16">
+        <f>IF(B130 &gt;  0,C130-B130, 0)</f>
+        <v>6642</v>
+      </c>
+      <c r="E130">
+        <f>D130-D123</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" outlineLevel="1">
+      <c r="A131" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B131" s="29"/>
+      <c r="C131" s="29"/>
+      <c r="D131" s="29"/>
+    </row>
+    <row r="132" spans="1:5" outlineLevel="1">
+      <c r="A132" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B132" s="16">
+        <v>42949</v>
+      </c>
+      <c r="C132" s="16">
+        <v>49956</v>
+      </c>
+      <c r="D132" s="16">
+        <f>IF(B132 &gt;  0,C132-B132, 0)</f>
+        <v>7007</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" outlineLevel="1">
+      <c r="A133" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B133" s="16">
+        <v>43175</v>
+      </c>
+      <c r="C133" s="16">
+        <v>50203</v>
+      </c>
+      <c r="D133" s="16">
+        <f>IF(B133 &gt;  0,C133-B133, 0)</f>
+        <v>7028</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" outlineLevel="1">
+      <c r="A134" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B134" s="16">
+        <v>44628</v>
+      </c>
+      <c r="C134" s="16">
+        <v>51659</v>
+      </c>
+      <c r="D134" s="16">
+        <f>IF(B134 &gt;  0,C134-B134, 0)</f>
+        <v>7031</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" outlineLevel="1">
+      <c r="A135" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B135" s="16">
+        <v>45146</v>
+      </c>
+      <c r="C135" s="16">
+        <v>52177</v>
+      </c>
+      <c r="D135" s="16">
+        <f>IF(B135 &gt;  0,C135-B135, 0)</f>
+        <v>7031</v>
+      </c>
+      <c r="E135">
+        <f>D135-D133</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" outlineLevel="1">
+      <c r="A136" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="29"/>
+    </row>
+    <row r="137" spans="1:5" outlineLevel="1">
+      <c r="A137" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B137" s="16">
+        <v>45524</v>
+      </c>
+      <c r="C137" s="16">
+        <v>52978</v>
+      </c>
+      <c r="D137" s="16">
+        <f>IF(B137 &gt;  0,C137-B137, 0)</f>
+        <v>7454</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" outlineLevel="1">
+      <c r="A138" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B138" s="16">
+        <v>45752</v>
+      </c>
+      <c r="C138" s="16">
+        <v>53228</v>
+      </c>
+      <c r="D138" s="16">
+        <f>IF(B138 &gt;  0,C138-B138, 0)</f>
+        <v>7476</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" outlineLevel="1">
+      <c r="A139" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B139" s="16">
+        <v>45830</v>
+      </c>
+      <c r="C139" s="16">
+        <v>53306</v>
+      </c>
+      <c r="D139" s="16">
+        <f>IF(B139 &gt;  0,C139-B139, 0)</f>
+        <v>7476</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" outlineLevel="1">
+      <c r="A140" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B140" s="16">
+        <v>45929</v>
+      </c>
+      <c r="C140" s="16">
+        <v>53405</v>
+      </c>
+      <c r="D140" s="16">
+        <f>IF(B140 &gt;  0,C140-B140, 0)</f>
+        <v>7476</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" outlineLevel="1">
+      <c r="A141" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B141" s="16">
+        <v>46124</v>
+      </c>
+      <c r="C141" s="16">
+        <v>53602</v>
+      </c>
+      <c r="D141" s="16">
+        <f>IF(B141 &gt;  0,C141-B141, 0)</f>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" outlineLevel="1">
+      <c r="A142" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B142" s="16">
+        <v>46279</v>
+      </c>
+      <c r="C142" s="16">
+        <v>53758</v>
+      </c>
+      <c r="D142" s="16">
+        <f>IF(B142 &gt;  0,C142-B142, 0)</f>
+        <v>7479</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" outlineLevel="1">
+      <c r="A143" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B143" s="16">
+        <v>46376</v>
+      </c>
+      <c r="C143" s="16">
+        <v>53854</v>
+      </c>
+      <c r="D143" s="16">
+        <f>IF(B143 &gt;  0,C143-B143, 0)</f>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" outlineLevel="1">
+      <c r="A144" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B144" s="16">
+        <v>46504</v>
+      </c>
+      <c r="C144" s="16">
+        <v>53982</v>
+      </c>
+      <c r="D144" s="16">
+        <f>IF(B144 &gt;  0,C144-B144, 0)</f>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" outlineLevel="1">
+      <c r="A145" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B145" s="16">
+        <v>46624</v>
+      </c>
+      <c r="C145" s="16">
+        <v>54102</v>
+      </c>
+      <c r="D145" s="16">
+        <f>IF(B145 &gt;  0,C145-B145, 0)</f>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" outlineLevel="1">
+      <c r="A146" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B146" s="16">
+        <v>46876</v>
+      </c>
+      <c r="C146" s="16">
+        <v>54354</v>
+      </c>
+      <c r="D146" s="16">
+        <f>IF(B146 &gt;  0,C146-B146, 0)</f>
+        <v>7478</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" outlineLevel="1">
+      <c r="A147" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B147" s="16">
+        <v>47892</v>
+      </c>
+      <c r="C147" s="16">
+        <v>55387</v>
+      </c>
+      <c r="D147" s="16">
+        <f>IF(B147 &gt;  0,C147-B147, 0)</f>
+        <v>7495</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" outlineLevel="1">
+      <c r="A148" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B148" s="16">
+        <v>48805</v>
+      </c>
+      <c r="C148" s="16">
+        <v>56300</v>
+      </c>
+      <c r="D148" s="16">
+        <f>IF(B148 &gt;  0,C148-B148, 0)</f>
+        <v>7495</v>
+      </c>
+      <c r="E148">
+        <f>D148-D138</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" outlineLevel="1">
+      <c r="A149" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B149" s="29"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="29"/>
+    </row>
+    <row r="150" spans="1:5" outlineLevel="1">
+      <c r="A150" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B150" s="16">
+        <v>50431</v>
+      </c>
+      <c r="C150" s="16">
+        <v>59573</v>
+      </c>
+      <c r="D150" s="16">
+        <f>IF(B150 &gt;  0,C150-B150, 0)</f>
+        <v>9142</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" outlineLevel="1">
+      <c r="A151" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B151" s="16">
+        <v>50658</v>
+      </c>
+      <c r="C151" s="16">
+        <v>59821</v>
+      </c>
+      <c r="D151" s="16">
+        <f>IF(B151 &gt;  0,C151-B151, 0)</f>
+        <v>9163</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" outlineLevel="1">
+      <c r="A152" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B152" s="16">
+        <v>50797</v>
+      </c>
+      <c r="C152" s="16">
+        <v>59960</v>
+      </c>
+      <c r="D152" s="16">
+        <f>IF(B152 &gt;  0,C152-B152, 0)</f>
+        <v>9163</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" outlineLevel="1">
+      <c r="A153" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B153" s="16">
+        <v>50904</v>
+      </c>
+      <c r="C153" s="16">
+        <v>60068</v>
+      </c>
+      <c r="D153" s="16">
+        <f>IF(B153 &gt;  0,C153-B153, 0)</f>
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" outlineLevel="1">
+      <c r="A154" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B154" s="16">
+        <v>50995</v>
+      </c>
+      <c r="C154" s="16">
+        <v>60159</v>
+      </c>
+      <c r="D154" s="16">
+        <f>IF(B154 &gt;  0,C154-B154, 0)</f>
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" outlineLevel="1">
+      <c r="A155" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B155" s="16">
+        <v>51135</v>
+      </c>
+      <c r="C155" s="16">
+        <v>60299</v>
+      </c>
+      <c r="D155" s="16">
+        <f>IF(B155 &gt;  0,C155-B155, 0)</f>
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" outlineLevel="1">
+      <c r="A156" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B156" s="16">
+        <v>51352</v>
+      </c>
+      <c r="C156" s="16">
+        <v>60517</v>
+      </c>
+      <c r="D156" s="16">
+        <f>IF(B156 &gt;  0,C156-B156, 0)</f>
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" outlineLevel="1">
+      <c r="A157" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B157" s="16">
+        <v>51487</v>
+      </c>
+      <c r="C157" s="16">
+        <v>60652</v>
+      </c>
+      <c r="D157" s="16">
+        <f>IF(B157 &gt;  0,C157-B157, 0)</f>
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" outlineLevel="1">
+      <c r="A158" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B158" s="16">
+        <v>51681</v>
+      </c>
+      <c r="C158" s="16">
+        <v>60846</v>
+      </c>
+      <c r="D158" s="16">
+        <f>IF(B158 &gt;  0,C158-B158, 0)</f>
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" outlineLevel="1">
+      <c r="A159" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B159" s="16">
+        <v>52080</v>
+      </c>
+      <c r="C159" s="16">
+        <v>61248</v>
+      </c>
+      <c r="D159" s="16">
+        <f>IF(B159 &gt;  0,C159-B159, 0)</f>
+        <v>9168</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" outlineLevel="1">
+      <c r="A160" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B160" s="16">
+        <v>52250</v>
+      </c>
+      <c r="C160" s="16">
+        <v>61427</v>
+      </c>
+      <c r="D160" s="16">
+        <f>IF(B160 &gt;  0,C160-B160, 0)</f>
+        <v>9177</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" outlineLevel="1">
+      <c r="A161" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B161" s="16">
+        <v>52768</v>
+      </c>
+      <c r="C161" s="16">
+        <v>61945</v>
+      </c>
+      <c r="D161" s="16">
+        <f>IF(B161 &gt;  0,C161-B161, 0)</f>
+        <v>9177</v>
+      </c>
+      <c r="E161">
+        <f>D161-D151</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" outlineLevel="1">
+      <c r="A162" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B162" s="29"/>
+      <c r="C162" s="29"/>
+      <c r="D162" s="29"/>
+    </row>
+    <row r="163" spans="1:5" outlineLevel="1">
+      <c r="A163" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B163" s="16">
+        <v>53104</v>
+      </c>
+      <c r="C163" s="16">
+        <v>62610</v>
+      </c>
+      <c r="D163" s="16">
+        <f>IF(B163 &gt;  0,C163-B163, 0)</f>
+        <v>9506</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" outlineLevel="1">
+      <c r="A164" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B164" s="16">
+        <v>53332</v>
+      </c>
+      <c r="C164" s="16">
+        <v>62861</v>
+      </c>
+      <c r="D164" s="16">
+        <f>IF(B164 &gt;  0,C164-B164, 0)</f>
+        <v>9529</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" outlineLevel="1">
+      <c r="A165" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B165" s="16">
+        <v>53477</v>
+      </c>
+      <c r="C165" s="16">
+        <v>63021</v>
+      </c>
+      <c r="D165" s="16">
+        <f>IF(B165 &gt;  0,C165-B165, 0)</f>
+        <v>9544</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" outlineLevel="1">
+      <c r="A166" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B166" s="16">
+        <v>53562</v>
+      </c>
+      <c r="C166" s="16">
+        <v>63110</v>
+      </c>
+      <c r="D166" s="16">
+        <f>IF(B166 &gt;  0,C166-B166, 0)</f>
+        <v>9548</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" outlineLevel="1">
+      <c r="A167" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B167" s="16">
+        <v>53643</v>
+      </c>
+      <c r="C167" s="16">
+        <v>63206</v>
+      </c>
+      <c r="D167" s="16">
+        <f>IF(B167 &gt;  0,C167-B167, 0)</f>
+        <v>9563</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" outlineLevel="1">
+      <c r="A168" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B168" s="16">
+        <v>53813</v>
+      </c>
+      <c r="C168" s="16">
+        <v>63376</v>
+      </c>
+      <c r="D168" s="16">
+        <f>IF(B168 &gt;  0,C168-B168, 0)</f>
+        <v>9563</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" outlineLevel="1">
+      <c r="A169" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B169" s="16">
+        <v>53851</v>
+      </c>
+      <c r="C169" s="16">
+        <v>63425</v>
+      </c>
+      <c r="D169" s="16">
+        <f>IF(B169 &gt;  0,C169-B169, 0)</f>
+        <v>9574</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" outlineLevel="1">
+      <c r="A170" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B170" s="16">
+        <v>53952</v>
+      </c>
+      <c r="C170" s="16">
+        <v>63540</v>
+      </c>
+      <c r="D170" s="16">
+        <f>IF(B170 &gt;  0,C170-B170, 0)</f>
+        <v>9588</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" outlineLevel="1">
+      <c r="A171" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171" s="16">
+        <v>54007</v>
+      </c>
+      <c r="C171" s="16">
+        <v>63597</v>
+      </c>
+      <c r="D171" s="16">
+        <f>IF(B171 &gt;  0,C171-B171, 0)</f>
+        <v>9590</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" outlineLevel="1">
+      <c r="A172" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B172" s="16">
+        <v>54209</v>
+      </c>
+      <c r="C172" s="16">
+        <v>63819</v>
+      </c>
+      <c r="D172" s="16">
+        <f>IF(B172 &gt;  0,C172-B172, 0)</f>
+        <v>9610</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" outlineLevel="1">
+      <c r="A173" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B173" s="16">
+        <v>54368</v>
+      </c>
+      <c r="C173" s="16">
+        <v>64047</v>
+      </c>
+      <c r="D173" s="16">
+        <f>IF(B173 &gt;  0,C173-B173, 0)</f>
+        <v>9679</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" outlineLevel="1">
+      <c r="A174" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B174" s="16">
+        <v>54651</v>
+      </c>
+      <c r="C174" s="16">
+        <v>64335</v>
+      </c>
+      <c r="D174" s="16">
+        <f>IF(B174 &gt;  0,C174-B174, 0)</f>
+        <v>9684</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" outlineLevel="1">
+      <c r="A175" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B175" s="16">
+        <v>54872</v>
+      </c>
+      <c r="C175" s="16">
+        <v>64568</v>
+      </c>
+      <c r="D175" s="16">
+        <f>IF(B175 &gt;  0,C175-B175, 0)</f>
+        <v>9696</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" outlineLevel="1">
+      <c r="A176" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B176" s="16">
+        <v>55390</v>
+      </c>
+      <c r="C176" s="16">
+        <v>65086</v>
+      </c>
+      <c r="D176" s="16">
+        <f>IF(B176 &gt;  0,C176-B176, 0)</f>
+        <v>9696</v>
+      </c>
+      <c r="E176">
+        <f>D176-D164</f>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" outlineLevel="1">
+      <c r="A177" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B177" s="29"/>
+      <c r="C177" s="29"/>
+      <c r="D177" s="29"/>
+    </row>
+    <row r="178" spans="1:4" outlineLevel="1">
+      <c r="A178" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B178" s="16">
+        <v>55725</v>
+      </c>
+      <c r="C178" s="16">
+        <v>65479</v>
+      </c>
+      <c r="D178" s="16">
+        <f>IF(B178 &gt;  0,C178-B178, 0)</f>
+        <v>9754</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" outlineLevel="1">
+      <c r="A179" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B179" s="16">
+        <v>55958</v>
+      </c>
+      <c r="C179" s="16">
+        <v>66009</v>
+      </c>
+      <c r="D179" s="16">
+        <f>IF(B179 &gt;  0,C179-B179, 0)</f>
+        <v>10051</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" outlineLevel="1">
+      <c r="A180" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B180" s="16">
+        <v>56265</v>
+      </c>
+      <c r="C180" s="16">
+        <v>66317</v>
+      </c>
+      <c r="D180" s="16">
+        <f>IF(B180 &gt;  0,C180-B180, 0)</f>
+        <v>10052</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" outlineLevel="1">
+      <c r="A181" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B181" s="16">
+        <v>56378</v>
+      </c>
+      <c r="C181" s="16">
+        <v>66431</v>
+      </c>
+      <c r="D181" s="16">
+        <f>IF(B181 &gt;  0,C181-B181, 0)</f>
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" outlineLevel="1">
+      <c r="A182" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B182" s="16">
+        <v>56428</v>
+      </c>
+      <c r="C182" s="16">
+        <v>66483</v>
+      </c>
+      <c r="D182" s="16">
+        <f>IF(B182 &gt;  0,C182-B182, 0)</f>
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" outlineLevel="1">
+      <c r="A183" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B183" s="16">
+        <v>56640</v>
+      </c>
+      <c r="C183" s="16">
+        <v>66695</v>
+      </c>
+      <c r="D183" s="16">
+        <f>IF(B183 &gt;  0,C183-B183, 0)</f>
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" outlineLevel="1">
+      <c r="A184" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B184" s="16">
+        <v>56715</v>
+      </c>
+      <c r="C184" s="16">
+        <v>66770</v>
+      </c>
+      <c r="D184" s="16">
+        <f>IF(B184 &gt;  0,C184-B184, 0)</f>
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" outlineLevel="1">
+      <c r="A185" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B185" s="16">
+        <v>56898</v>
+      </c>
+      <c r="C185" s="16">
+        <v>66954</v>
+      </c>
+      <c r="D185" s="16">
+        <f>IF(B185 &gt;  0,C185-B185, 0)</f>
+        <v>10056</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" outlineLevel="1">
+      <c r="A186" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B186" s="16">
+        <v>56982</v>
+      </c>
+      <c r="C186" s="16">
+        <v>67039</v>
+      </c>
+      <c r="D186" s="16">
+        <f>IF(B186 &gt;  0,C186-B186, 0)</f>
+        <v>10057</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" outlineLevel="1">
+      <c r="A187" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B187" s="16">
+        <v>57020</v>
+      </c>
+      <c r="C187" s="16">
+        <v>67079</v>
+      </c>
+      <c r="D187" s="16">
+        <f>IF(B187 &gt;  0,C187-B187, 0)</f>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" outlineLevel="1">
+      <c r="A188" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B188" s="16">
+        <v>57085</v>
+      </c>
+      <c r="C188" s="16">
+        <v>67144</v>
+      </c>
+      <c r="D188" s="16">
+        <f>IF(B188 &gt;  0,C188-B188, 0)</f>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" outlineLevel="1">
+      <c r="A189" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B189" s="16">
+        <v>57134</v>
+      </c>
+      <c r="C189" s="16">
+        <v>67193</v>
+      </c>
+      <c r="D189" s="16">
+        <f>IF(B189 &gt;  0,C189-B189, 0)</f>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" outlineLevel="1">
+      <c r="A190" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B190" s="16">
+        <v>57234</v>
+      </c>
+      <c r="C190" s="16">
+        <v>67293</v>
+      </c>
+      <c r="D190" s="16">
+        <f>IF(B190 &gt;  0,C190-B190, 0)</f>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" outlineLevel="1">
+      <c r="A191" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B191" s="16">
+        <v>57309</v>
+      </c>
+      <c r="C191" s="16">
+        <v>67368</v>
+      </c>
+      <c r="D191" s="16">
+        <f>IF(B191 &gt;  0,C191-B191, 0)</f>
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" outlineLevel="1">
+      <c r="A192" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B192" s="16">
+        <v>57531</v>
+      </c>
+      <c r="C192" s="16">
+        <v>67591</v>
+      </c>
+      <c r="D192" s="16">
+        <f>IF(B192 &gt;  0,C192-B192, 0)</f>
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" outlineLevel="1">
+      <c r="A193" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B193" s="16">
+        <v>57771</v>
+      </c>
+      <c r="C193" s="16">
+        <v>67831</v>
+      </c>
+      <c r="D193" s="16">
+        <f>IF(B193 &gt;  0,C193-B193, 0)</f>
+        <v>10060</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" outlineLevel="1">
+      <c r="A194" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B194" s="16">
+        <v>58289</v>
+      </c>
+      <c r="C194" s="16">
+        <v>68349</v>
+      </c>
+      <c r="D194" s="16">
+        <f>IF(B194 &gt;  0,C194-B194, 0)</f>
+        <v>10060</v>
+      </c>
+      <c r="E194">
+        <f>D194-D179</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" outlineLevel="1">
+      <c r="A195" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B195" s="29"/>
+      <c r="C195" s="29"/>
+      <c r="D195" s="29"/>
+    </row>
+    <row r="196" spans="1:5" outlineLevel="1">
+      <c r="A196" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B196" s="16">
+        <v>58622</v>
+      </c>
+      <c r="C196" s="16">
+        <v>69018</v>
+      </c>
+      <c r="D196" s="16">
+        <f>IF(B196 &gt;  0,C196-B196, 0)</f>
+        <v>10396</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" outlineLevel="1">
+      <c r="A197" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B197" s="16">
+        <v>58848</v>
+      </c>
+      <c r="C197" s="16">
+        <v>69265</v>
+      </c>
+      <c r="D197" s="16">
+        <f>IF(B197 &gt;  0,C197-B197, 0)</f>
+        <v>10417</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" outlineLevel="1">
+      <c r="A198" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B198" s="16">
+        <v>59432</v>
+      </c>
+      <c r="C198" s="16">
+        <v>69850</v>
+      </c>
+      <c r="D198" s="16">
+        <f>IF(B198 &gt;  0,C198-B198, 0)</f>
+        <v>10418</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" outlineLevel="1">
+      <c r="A199" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B199" s="16">
+        <v>59610</v>
+      </c>
+      <c r="C199" s="16">
+        <v>70031</v>
+      </c>
+      <c r="D199" s="16">
+        <f>IF(B199 &gt;  0,C199-B199, 0)</f>
+        <v>10421</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" outlineLevel="1">
+      <c r="A200" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B200" s="16">
+        <v>59716</v>
+      </c>
+      <c r="C200" s="16">
+        <v>70137</v>
+      </c>
+      <c r="D200" s="16">
+        <f>IF(B200 &gt;  0,C200-B200, 0)</f>
+        <v>10421</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" outlineLevel="1">
+      <c r="A201" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B201" s="16">
+        <v>59863</v>
+      </c>
+      <c r="C201" s="16">
+        <v>70285</v>
+      </c>
+      <c r="D201" s="16">
+        <f>IF(B201 &gt;  0,C201-B201, 0)</f>
+        <v>10422</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" outlineLevel="1">
+      <c r="A202" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B202" s="16">
+        <v>60022</v>
+      </c>
+      <c r="C202" s="16">
+        <v>70444</v>
+      </c>
+      <c r="D202" s="16">
+        <f>IF(B202 &gt;  0,C202-B202, 0)</f>
+        <v>10422</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" outlineLevel="1">
+      <c r="A203" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B203" s="16">
+        <v>60540</v>
+      </c>
+      <c r="C203" s="16">
+        <v>70962</v>
+      </c>
+      <c r="D203" s="16">
+        <f>IF(B203 &gt;  0,C203-B203, 0)</f>
+        <v>10422</v>
+      </c>
+      <c r="E203">
+        <f>D203-D197</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" outlineLevel="1">
+      <c r="A204" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B204" s="29"/>
+      <c r="C204" s="29"/>
+      <c r="D204" s="29"/>
+    </row>
+    <row r="205" spans="1:5" outlineLevel="1">
+      <c r="A205" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B205" s="16">
+        <v>60909</v>
+      </c>
+      <c r="C205" s="16">
+        <v>71707</v>
+      </c>
+      <c r="D205" s="16">
+        <f>IF(B205 &gt;  0,C205-B205, 0)</f>
+        <v>10798</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" outlineLevel="1">
+      <c r="A206" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B206" s="16">
+        <v>61137</v>
+      </c>
+      <c r="C206" s="16">
+        <v>71957</v>
+      </c>
+      <c r="D206" s="16">
+        <f>IF(B206 &gt;  0,C206-B206, 0)</f>
+        <v>10820</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" outlineLevel="1">
+      <c r="A207" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B207" s="16">
+        <v>61238</v>
+      </c>
+      <c r="C207" s="16">
+        <v>72069</v>
+      </c>
+      <c r="D207" s="16">
+        <f>IF(B207 &gt;  0,C207-B207, 0)</f>
+        <v>10831</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" outlineLevel="1">
+      <c r="A208" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B208" s="16">
+        <v>69043</v>
+      </c>
+      <c r="C208" s="16">
+        <v>79905</v>
+      </c>
+      <c r="D208" s="16">
+        <f>IF(B208 &gt;  0,C208-B208, 0)</f>
+        <v>10862</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" outlineLevel="1">
+      <c r="A209" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B209" s="16">
+        <v>69309</v>
+      </c>
+      <c r="C209" s="16">
+        <v>80190</v>
+      </c>
+      <c r="D209" s="16">
+        <f>IF(B209 &gt;  0,C209-B209, 0)</f>
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" outlineLevel="1">
+      <c r="A210" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B210" s="16">
+        <v>69906</v>
+      </c>
+      <c r="C210" s="16">
+        <v>80786</v>
+      </c>
+      <c r="D210" s="16">
+        <f>IF(B210 &gt;  0,C210-B210, 0)</f>
+        <v>10880</v>
+      </c>
+      <c r="E210">
+        <f>D210-D206</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" outlineLevel="1">
+      <c r="A211" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B211" s="29"/>
+      <c r="C211" s="29"/>
+      <c r="D211" s="29"/>
+    </row>
+    <row r="212" spans="1:5" outlineLevel="1">
+      <c r="A212" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B212" s="16">
+        <v>70786</v>
+      </c>
+      <c r="C212" s="16">
+        <v>82543</v>
+      </c>
+      <c r="D212" s="16">
+        <f>IF(B212 &gt;  0,C212-B212, 0)</f>
+        <v>11757</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" outlineLevel="1">
+      <c r="A213" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B213" s="16">
+        <v>71017</v>
+      </c>
+      <c r="C213" s="16">
+        <v>82799</v>
+      </c>
+      <c r="D213" s="16">
+        <f>IF(B213 &gt;  0,C213-B213, 0)</f>
+        <v>11782</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" outlineLevel="1">
+      <c r="A214" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B214" s="16">
+        <v>71467</v>
+      </c>
+      <c r="C214" s="16">
+        <v>83249</v>
+      </c>
+      <c r="D214" s="16">
+        <f>IF(B214 &gt;  0,C214-B214, 0)</f>
+        <v>11782</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" outlineLevel="1">
+      <c r="A215" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B215" s="16">
+        <v>71725</v>
+      </c>
+      <c r="C215" s="16">
+        <v>83509</v>
+      </c>
+      <c r="D215" s="16">
+        <f>IF(B215 &gt;  0,C215-B215, 0)</f>
+        <v>11784</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" outlineLevel="1">
+      <c r="A216" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B216" s="16">
+        <v>72016</v>
+      </c>
+      <c r="C216" s="16">
+        <v>83800</v>
+      </c>
+      <c r="D216" s="16">
+        <f>IF(B216 &gt;  0,C216-B216, 0)</f>
+        <v>11784</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" outlineLevel="1">
+      <c r="A217" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B217" s="16">
+        <v>72323</v>
+      </c>
+      <c r="C217" s="16">
+        <v>84128</v>
+      </c>
+      <c r="D217" s="16">
+        <f>IF(B217 &gt;  0,C217-B217, 0)</f>
+        <v>11805</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" outlineLevel="1">
+      <c r="A218" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B218" s="16">
+        <v>72665</v>
+      </c>
+      <c r="C218" s="16">
+        <v>84487</v>
+      </c>
+      <c r="D218" s="16">
+        <f>IF(B218 &gt;  0,C218-B218, 0)</f>
+        <v>11822</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" outlineLevel="1">
+      <c r="A219" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B219" s="16">
+        <v>73412</v>
+      </c>
+      <c r="C219" s="16">
+        <v>85239</v>
+      </c>
+      <c r="D219" s="16">
+        <f>IF(B219 &gt;  0,C219-B219, 0)</f>
+        <v>11827</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" outlineLevel="1">
+      <c r="A220" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B220" s="16">
+        <v>73958</v>
+      </c>
+      <c r="C220" s="16">
+        <v>85786</v>
+      </c>
+      <c r="D220" s="16">
+        <f>IF(B220 &gt;  0,C220-B220, 0)</f>
+        <v>11828</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" outlineLevel="1">
+      <c r="A221" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B221" s="16">
+        <v>74749</v>
+      </c>
+      <c r="C221" s="16">
+        <v>86590</v>
+      </c>
+      <c r="D221" s="16">
+        <f>IF(B221 &gt;  0,C221-B221, 0)</f>
+        <v>11841</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" outlineLevel="1">
+      <c r="A222" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B222" s="16">
+        <v>74982</v>
+      </c>
+      <c r="C222" s="16">
+        <v>86830</v>
+      </c>
+      <c r="D222" s="16">
+        <f>IF(B222 &gt;  0,C222-B222, 0)</f>
+        <v>11848</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" outlineLevel="1">
+      <c r="A223" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B223" s="16">
+        <v>75107</v>
+      </c>
+      <c r="C223" s="16">
+        <v>86956</v>
+      </c>
+      <c r="D223" s="16">
+        <f>IF(B223 &gt;  0,C223-B223, 0)</f>
+        <v>11849</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" outlineLevel="1">
+      <c r="A224" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B224" s="16">
+        <v>75280</v>
+      </c>
+      <c r="C224" s="16">
+        <v>87129</v>
+      </c>
+      <c r="D224" s="16">
+        <f>IF(B224 &gt;  0,C224-B224, 0)</f>
+        <v>11849</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" outlineLevel="1">
+      <c r="A225" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B225" s="16">
+        <v>75591</v>
+      </c>
+      <c r="C225" s="16">
+        <v>87443</v>
+      </c>
+      <c r="D225" s="16">
+        <f>IF(B225 &gt;  0,C225-B225, 0)</f>
+        <v>11852</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" outlineLevel="1">
+      <c r="A226" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B226" s="16">
+        <v>75741</v>
+      </c>
+      <c r="C226" s="16">
+        <v>87604</v>
+      </c>
+      <c r="D226" s="16">
+        <f>IF(B226 &gt;  0,C226-B226, 0)</f>
+        <v>11863</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" outlineLevel="1">
+      <c r="A227" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B227" s="16">
+        <v>75828</v>
+      </c>
+      <c r="C227" s="16">
+        <v>87692</v>
+      </c>
+      <c r="D227" s="16">
+        <f>IF(B227 &gt;  0,C227-B227, 0)</f>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" outlineLevel="1">
+      <c r="A228" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B228" s="16">
+        <v>75972</v>
+      </c>
+      <c r="C228" s="16">
+        <v>87836</v>
+      </c>
+      <c r="D228" s="16">
+        <f>IF(B228 &gt;  0,C228-B228, 0)</f>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" outlineLevel="1">
+      <c r="A229" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B229" s="16">
+        <v>76227</v>
+      </c>
+      <c r="C229" s="16">
+        <v>88091</v>
+      </c>
+      <c r="D229" s="16">
+        <f>IF(B229 &gt;  0,C229-B229, 0)</f>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" outlineLevel="1">
+      <c r="A230" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B230" s="16">
+        <v>76306</v>
+      </c>
+      <c r="C230" s="16">
+        <v>88170</v>
+      </c>
+      <c r="D230" s="16">
+        <f>IF(B230 &gt;  0,C230-B230, 0)</f>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" outlineLevel="1">
+      <c r="A231" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B231" s="16">
+        <v>76444</v>
+      </c>
+      <c r="C231" s="16">
+        <v>88308</v>
+      </c>
+      <c r="D231" s="16">
+        <f>IF(B231 &gt;  0,C231-B231, 0)</f>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" outlineLevel="1">
+      <c r="A232" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B232" s="16">
+        <v>76741</v>
+      </c>
+      <c r="C232" s="16">
+        <v>88605</v>
+      </c>
+      <c r="D232" s="16">
+        <f>IF(B232 &gt;  0,C232-B232, 0)</f>
+        <v>11864</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" outlineLevel="1">
+      <c r="A233" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B233" s="16">
+        <v>77063</v>
+      </c>
+      <c r="C233" s="16">
+        <v>88946</v>
+      </c>
+      <c r="D233" s="16">
+        <f>IF(B233 &gt;  0,C233-B233, 0)</f>
+        <v>11883</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" outlineLevel="1">
+      <c r="A234" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B234" s="16">
+        <v>77866</v>
+      </c>
+      <c r="C234" s="16">
+        <v>89784</v>
+      </c>
+      <c r="D234" s="16">
+        <f>IF(B234 &gt;  0,C234-B234, 0)</f>
+        <v>11918</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A235" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B235" s="16">
+        <v>77902</v>
+      </c>
+      <c r="C235" s="16">
+        <v>89784</v>
+      </c>
+      <c r="D235" s="16">
+        <f>IF(B235 &gt;  0,C235-B235, 0)</f>
+        <v>11882</v>
+      </c>
+      <c r="E235" s="42">
+        <f>D235-D213</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" s="31" customFormat="1" ht="16.5" outlineLevel="1" thickTop="1" thickBot="1">
+      <c r="A236" s="30"/>
+      <c r="B236" s="30"/>
+      <c r="C236" s="30"/>
+      <c r="D236" s="30"/>
+      <c r="E236" s="31">
+        <f>SUM(E1:E235)</f>
+        <v>723</v>
+      </c>
+      <c r="F236" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -5299,7 +8833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C45"/>
   <sheetViews>
@@ -5805,7 +9339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding an awesome lua script by nitsuja for Sonic Rush that also works for NSMB.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="242">
   <si>
     <t>1-1</t>
   </si>
@@ -735,6 +735,15 @@
   </si>
   <si>
     <t>terrot</t>
+  </si>
+  <si>
+    <t>Enter small pipe</t>
+  </si>
+  <si>
+    <t>Enter pipe (wall jump)</t>
+  </si>
+  <si>
+    <t>Hit P block</t>
   </si>
 </sst>
 </file>
@@ -976,15 +985,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,11 +1291,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I228"/>
+  <dimension ref="A1:I239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1319,14 +1328,14 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:9" outlineLevel="1">
       <c r="A3" s="16" t="s">
@@ -1395,14 +1404,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="13" customFormat="1" ht="18.75">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="I6" s="13" t="s">
         <v>231</v>
       </c>
@@ -1806,14 +1815,14 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
     </row>
     <row r="28" spans="1:8" outlineLevel="1">
       <c r="A28" s="24" t="s">
@@ -2414,12 +2423,12 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" collapsed="1">
-      <c r="A77" s="36" t="s">
+      <c r="A77" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
     </row>
     <row r="78" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A78" s="28" t="s">
@@ -4232,6 +4241,171 @@
       </c>
       <c r="F228" s="30" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B230" s="16">
+        <v>28733</v>
+      </c>
+      <c r="C230" s="16">
+        <v>29213</v>
+      </c>
+      <c r="D230" s="16">
+        <f t="shared" ref="D230:D239" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B231" s="16">
+        <v>29105</v>
+      </c>
+      <c r="C231" s="16">
+        <v>29585</v>
+      </c>
+      <c r="D231" s="16">
+        <f t="shared" si="9"/>
+        <v>480</v>
+      </c>
+      <c r="E231" s="16">
+        <v>29585</v>
+      </c>
+      <c r="F231" s="16">
+        <f t="shared" ref="F231:F235" si="10">IF(B231 &gt;  0,E231-B231, 0)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B232" s="16">
+        <v>29353</v>
+      </c>
+      <c r="C232" s="16">
+        <v>29834</v>
+      </c>
+      <c r="D232" s="16">
+        <f t="shared" si="9"/>
+        <v>481</v>
+      </c>
+      <c r="E232" s="16">
+        <v>29834</v>
+      </c>
+      <c r="F232" s="16">
+        <f t="shared" si="10"/>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="B233" s="16">
+        <v>29360</v>
+      </c>
+      <c r="E233" s="16">
+        <v>29839</v>
+      </c>
+      <c r="F233" s="16">
+        <f t="shared" si="10"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="B234" s="16">
+        <v>29407</v>
+      </c>
+      <c r="E234" s="16">
+        <v>29886</v>
+      </c>
+      <c r="F234" s="16">
+        <f t="shared" si="10"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B235" s="16">
+        <v>29838</v>
+      </c>
+      <c r="C235" s="16">
+        <v>30332</v>
+      </c>
+      <c r="D235" s="16">
+        <f t="shared" si="9"/>
+        <v>494</v>
+      </c>
+      <c r="E235" s="16">
+        <v>30318</v>
+      </c>
+      <c r="F235" s="16">
+        <f t="shared" si="10"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B236" s="16">
+        <v>30494</v>
+      </c>
+      <c r="C236" s="16">
+        <v>30988</v>
+      </c>
+      <c r="D236" s="16">
+        <f t="shared" si="9"/>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B237" s="16">
+        <v>30766</v>
+      </c>
+      <c r="C237" s="16">
+        <v>31261</v>
+      </c>
+      <c r="D237" s="16">
+        <f t="shared" si="9"/>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B238" s="16">
+        <v>31043</v>
+      </c>
+      <c r="C238" s="16">
+        <v>31543</v>
+      </c>
+      <c r="D238" s="16">
+        <f t="shared" si="9"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B239" s="16">
+        <v>31403</v>
+      </c>
+      <c r="C239" s="16">
+        <v>31906</v>
+      </c>
+      <c r="D239" s="16">
+        <f t="shared" si="9"/>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -4281,22 +4455,22 @@
       <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="43"/>
+      <c r="F1" s="42"/>
       <c r="G1">
         <f>E236</f>
         <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" ht="19.5" collapsed="1" thickTop="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A3" s="15" t="s">
@@ -4356,12 +4530,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="18.75" collapsed="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
     </row>
     <row r="8" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A8" s="20" t="s">
@@ -4383,7 +4557,7 @@
         <v>3285</v>
       </c>
       <c r="D9" s="16">
-        <f>IF(B9 &gt;  0,C9-B9, 0)</f>
+        <f t="shared" ref="D9:D15" si="0">IF(B9 &gt;  0,C9-B9, 0)</f>
         <v>479</v>
       </c>
       <c r="F9" s="13"/>
@@ -4399,7 +4573,7 @@
         <v>3571</v>
       </c>
       <c r="D10" s="16">
-        <f>IF(B10 &gt;  0,C10-B10, 0)</f>
+        <f t="shared" si="0"/>
         <v>478</v>
       </c>
     </row>
@@ -4414,7 +4588,7 @@
         <v>3630</v>
       </c>
       <c r="D11" s="16">
-        <f>IF(B11 &gt;  0,C11-B11, 0)</f>
+        <f t="shared" si="0"/>
         <v>479</v>
       </c>
     </row>
@@ -4429,7 +4603,7 @@
         <v>4192</v>
       </c>
       <c r="D12" s="16">
-        <f>IF(B12 &gt;  0,C12-B12, 0)</f>
+        <f t="shared" si="0"/>
         <v>480</v>
       </c>
       <c r="F12" s="13"/>
@@ -4446,7 +4620,7 @@
         <v>4627</v>
       </c>
       <c r="D13" s="16">
-        <f>IF(B13 &gt;  0,C13-B13, 0)</f>
+        <f t="shared" si="0"/>
         <v>481</v>
       </c>
       <c r="F13" s="13"/>
@@ -4463,7 +4637,7 @@
         <v>5145</v>
       </c>
       <c r="D14" s="16">
-        <f>IF(B14 &gt;  0,C14-B14, 0)</f>
+        <f t="shared" si="0"/>
         <v>481</v>
       </c>
       <c r="E14">
@@ -4482,7 +4656,7 @@
         <v>5738</v>
       </c>
       <c r="D15" s="16">
-        <f>IF(B15 &gt;  0,C15-B15, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" s="13"/>
@@ -4605,7 +4779,7 @@
         <v>9830</v>
       </c>
       <c r="D23" s="16">
-        <f>IF(B23 &gt;  0,C23-B23, 0)</f>
+        <f t="shared" ref="D23:D30" si="1">IF(B23 &gt;  0,C23-B23, 0)</f>
         <v>1424</v>
       </c>
     </row>
@@ -4620,7 +4794,7 @@
         <v>10077</v>
       </c>
       <c r="D24" s="16">
-        <f>IF(B24 &gt;  0,C24-B24, 0)</f>
+        <f t="shared" si="1"/>
         <v>1445</v>
       </c>
     </row>
@@ -4635,7 +4809,7 @@
         <v>11112</v>
       </c>
       <c r="D25" s="16">
-        <f>IF(B25 &gt;  0,C25-B25, 0)</f>
+        <f t="shared" si="1"/>
         <v>1475</v>
       </c>
     </row>
@@ -4647,7 +4821,7 @@
         <v>9674</v>
       </c>
       <c r="D26" s="16">
-        <f>IF(B26 &gt;  0,C26-B26, 0)</f>
+        <f t="shared" si="1"/>
         <v>-9674</v>
       </c>
     </row>
@@ -4662,7 +4836,7 @@
         <v>11292</v>
       </c>
       <c r="D27" s="16">
-        <f>IF(B27 &gt;  0,C27-B27, 0)</f>
+        <f t="shared" si="1"/>
         <v>1476</v>
       </c>
     </row>
@@ -4677,7 +4851,7 @@
         <v>11807</v>
       </c>
       <c r="D28" s="16">
-        <f>IF(B28 &gt;  0,C28-B28, 0)</f>
+        <f t="shared" si="1"/>
         <v>1480</v>
       </c>
     </row>
@@ -4692,7 +4866,7 @@
         <v>12118</v>
       </c>
       <c r="D29" s="16">
-        <f>IF(B29 &gt;  0,C29-B29, 0)</f>
+        <f t="shared" si="1"/>
         <v>1492</v>
       </c>
     </row>
@@ -4707,7 +4881,7 @@
         <v>12632</v>
       </c>
       <c r="D30" s="16">
-        <f>IF(B30 &gt;  0,C30-B30, 0)</f>
+        <f t="shared" si="1"/>
         <v>1492</v>
       </c>
       <c r="E30">
@@ -4766,12 +4940,12 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" collapsed="1">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:5" hidden="1" outlineLevel="1">
       <c r="A36" s="24" t="s">
@@ -4878,7 +5052,7 @@
         <v>18403</v>
       </c>
       <c r="D43" s="16">
-        <f>IF(B43 &gt;  0,C43-B43, 0)</f>
+        <f t="shared" ref="D43:D49" si="2">IF(B43 &gt;  0,C43-B43, 0)</f>
         <v>2681</v>
       </c>
     </row>
@@ -4893,7 +5067,7 @@
         <v>18649</v>
       </c>
       <c r="D44" s="16">
-        <f>IF(B44 &gt;  0,C44-B44, 0)</f>
+        <f t="shared" si="2"/>
         <v>2702</v>
       </c>
     </row>
@@ -4908,7 +5082,7 @@
         <v>18789</v>
       </c>
       <c r="D45" s="16">
-        <f>IF(B45 &gt;  0,C45-B45, 0)</f>
+        <f t="shared" si="2"/>
         <v>2702</v>
       </c>
     </row>
@@ -4923,7 +5097,7 @@
         <v>20233</v>
       </c>
       <c r="D46" s="16">
-        <f>IF(B46 &gt;  0,C46-B46, 0)</f>
+        <f t="shared" si="2"/>
         <v>2725</v>
       </c>
     </row>
@@ -4938,7 +5112,7 @@
         <v>20304</v>
       </c>
       <c r="D47" s="16">
-        <f>IF(B47 &gt;  0,C47-B47, 0)</f>
+        <f t="shared" si="2"/>
         <v>2725</v>
       </c>
     </row>
@@ -4953,7 +5127,7 @@
         <v>20584</v>
       </c>
       <c r="D48" s="16">
-        <f>IF(B48 &gt;  0,C48-B48, 0)</f>
+        <f t="shared" si="2"/>
         <v>2738</v>
       </c>
     </row>
@@ -4968,7 +5142,7 @@
         <v>21098</v>
       </c>
       <c r="D49" s="16">
-        <f>IF(B49 &gt;  0,C49-B49, 0)</f>
+        <f t="shared" si="2"/>
         <v>2730</v>
       </c>
       <c r="E49">
@@ -4995,7 +5169,7 @@
         <v>22185</v>
       </c>
       <c r="D51" s="16">
-        <f>IF(B51 &gt;  0,C51-B51, 0)</f>
+        <f t="shared" ref="D51:D60" si="3">IF(B51 &gt;  0,C51-B51, 0)</f>
         <v>3240</v>
       </c>
     </row>
@@ -5010,7 +5184,7 @@
         <v>22443</v>
       </c>
       <c r="D52" s="16">
-        <f>IF(B52 &gt;  0,C52-B52, 0)</f>
+        <f t="shared" si="3"/>
         <v>3266</v>
       </c>
       <c r="E52" s="25"/>
@@ -5028,7 +5202,7 @@
         <v>23386</v>
       </c>
       <c r="D53" s="16">
-        <f>IF(B53 &gt;  0,C53-B53, 0)</f>
+        <f t="shared" si="3"/>
         <v>3266</v>
       </c>
       <c r="E53" s="26"/>
@@ -5046,7 +5220,7 @@
         <v>23453</v>
       </c>
       <c r="D54" s="16">
-        <f>IF(B54 &gt;  0,C54-B54, 0)</f>
+        <f t="shared" si="3"/>
         <v>3266</v>
       </c>
     </row>
@@ -5061,7 +5235,7 @@
         <v>23524</v>
       </c>
       <c r="D55" s="16">
-        <f>IF(B55 &gt;  0,C55-B55, 0)</f>
+        <f t="shared" si="3"/>
         <v>3266</v>
       </c>
     </row>
@@ -5076,7 +5250,7 @@
         <v>23618</v>
       </c>
       <c r="D56" s="16">
-        <f>IF(B56 &gt;  0,C56-B56, 0)</f>
+        <f t="shared" si="3"/>
         <v>3267</v>
       </c>
     </row>
@@ -5091,7 +5265,7 @@
         <v>23661</v>
       </c>
       <c r="D57" s="16">
-        <f>IF(B57 &gt;  0,C57-B57, 0)</f>
+        <f t="shared" si="3"/>
         <v>3267</v>
       </c>
     </row>
@@ -5106,7 +5280,7 @@
         <v>23733</v>
       </c>
       <c r="D58" s="16">
-        <f>IF(B58 &gt;  0,C58-B58, 0)</f>
+        <f t="shared" si="3"/>
         <v>3268</v>
       </c>
     </row>
@@ -5121,7 +5295,7 @@
         <v>23926</v>
       </c>
       <c r="D59" s="16">
-        <f>IF(B59 &gt;  0,C59-B59, 0)</f>
+        <f t="shared" si="3"/>
         <v>3268</v>
       </c>
     </row>
@@ -5136,7 +5310,7 @@
         <v>24440</v>
       </c>
       <c r="D60" s="16">
-        <f>IF(B60 &gt;  0,C60-B60, 0)</f>
+        <f t="shared" si="3"/>
         <v>3268</v>
       </c>
     </row>
@@ -5159,7 +5333,7 @@
         <v>25475</v>
       </c>
       <c r="D62" s="16">
-        <f>IF(B62 &gt;  0,C62-B62, 0)</f>
+        <f t="shared" ref="D62:D79" si="4">IF(B62 &gt;  0,C62-B62, 0)</f>
         <v>3814</v>
       </c>
     </row>
@@ -5174,7 +5348,7 @@
         <v>25726</v>
       </c>
       <c r="D63" s="16">
-        <f>IF(B63 &gt;  0,C63-B63, 0)</f>
+        <f t="shared" si="4"/>
         <v>3836</v>
       </c>
     </row>
@@ -5189,7 +5363,7 @@
         <v>25765</v>
       </c>
       <c r="D64" s="16">
-        <f>IF(B64 &gt;  0,C64-B64, 0)</f>
+        <f t="shared" si="4"/>
         <v>3836</v>
       </c>
     </row>
@@ -5204,7 +5378,7 @@
         <v>25832</v>
       </c>
       <c r="D65" s="16">
-        <f>IF(B65 &gt;  0,C65-B65, 0)</f>
+        <f t="shared" si="4"/>
         <v>3837</v>
       </c>
     </row>
@@ -5219,7 +5393,7 @@
         <v>25927</v>
       </c>
       <c r="D66" s="16">
-        <f>IF(B66 &gt;  0,C66-B66, 0)</f>
+        <f t="shared" si="4"/>
         <v>3837</v>
       </c>
     </row>
@@ -5234,7 +5408,7 @@
         <v>25957</v>
       </c>
       <c r="D67" s="16">
-        <f>IF(B67 &gt;  0,C67-B67, 0)</f>
+        <f t="shared" si="4"/>
         <v>3836</v>
       </c>
     </row>
@@ -5249,7 +5423,7 @@
         <v>26163</v>
       </c>
       <c r="D68" s="16">
-        <f>IF(B68 &gt;  0,C68-B68, 0)</f>
+        <f t="shared" si="4"/>
         <v>3833</v>
       </c>
     </row>
@@ -5264,7 +5438,7 @@
         <v>26202</v>
       </c>
       <c r="D69" s="16">
-        <f>IF(B69 &gt;  0,C69-B69, 0)</f>
+        <f t="shared" si="4"/>
         <v>3830</v>
       </c>
     </row>
@@ -5279,7 +5453,7 @@
         <v>26218</v>
       </c>
       <c r="D70" s="16">
-        <f>IF(B70 &gt;  0,C70-B70, 0)</f>
+        <f t="shared" si="4"/>
         <v>3830</v>
       </c>
     </row>
@@ -5294,7 +5468,7 @@
         <v>26262</v>
       </c>
       <c r="D71" s="16">
-        <f>IF(B71 &gt;  0,C71-B71, 0)</f>
+        <f t="shared" si="4"/>
         <v>3841</v>
       </c>
     </row>
@@ -5309,7 +5483,7 @@
         <v>26286</v>
       </c>
       <c r="D72" s="16">
-        <f>IF(B72 &gt;  0,C72-B72, 0)</f>
+        <f t="shared" si="4"/>
         <v>3832</v>
       </c>
     </row>
@@ -5324,7 +5498,7 @@
         <v>26571</v>
       </c>
       <c r="D73" s="16">
-        <f>IF(B73 &gt;  0,C73-B73, 0)</f>
+        <f t="shared" si="4"/>
         <v>3863</v>
       </c>
     </row>
@@ -5339,7 +5513,7 @@
         <v>26694</v>
       </c>
       <c r="D74" s="16">
-        <f>IF(B74 &gt;  0,C74-B74, 0)</f>
+        <f t="shared" si="4"/>
         <v>3865</v>
       </c>
     </row>
@@ -5354,7 +5528,7 @@
         <v>27067</v>
       </c>
       <c r="D75" s="16">
-        <f>IF(B75 &gt;  0,C75-B75, 0)</f>
+        <f t="shared" si="4"/>
         <v>3862</v>
       </c>
     </row>
@@ -5369,7 +5543,7 @@
         <v>27731</v>
       </c>
       <c r="D76" s="16">
-        <f>IF(B76 &gt;  0,C76-B76, 0)</f>
+        <f t="shared" si="4"/>
         <v>3882</v>
       </c>
     </row>
@@ -5384,7 +5558,7 @@
         <v>28148</v>
       </c>
       <c r="D77" s="16">
-        <f>IF(B77 &gt;  0,C77-B77, 0)</f>
+        <f t="shared" si="4"/>
         <v>3882</v>
       </c>
     </row>
@@ -5399,7 +5573,7 @@
         <v>28462</v>
       </c>
       <c r="D78" s="16">
-        <f>IF(B78 &gt;  0,C78-B78, 0)</f>
+        <f t="shared" si="4"/>
         <v>3892</v>
       </c>
     </row>
@@ -5414,7 +5588,7 @@
         <v>28980</v>
       </c>
       <c r="D79" s="16">
-        <f>IF(B79 &gt;  0,C79-B79, 0)</f>
+        <f t="shared" si="4"/>
         <v>3892</v>
       </c>
       <c r="E79">
@@ -5494,12 +5668,12 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75">
-      <c r="A85" s="36" t="s">
+      <c r="A85" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
     </row>
     <row r="86" spans="1:5" outlineLevel="1">
       <c r="A86" s="28" t="s">
@@ -5607,7 +5781,7 @@
         <v>34468</v>
       </c>
       <c r="D93" s="16">
-        <f>IF(B93 &gt;  0,C93-B93, 0)</f>
+        <f t="shared" ref="D93:D107" si="5">IF(B93 &gt;  0,C93-B93, 0)</f>
         <v>5255</v>
       </c>
     </row>
@@ -5622,7 +5796,7 @@
         <v>34713</v>
       </c>
       <c r="D94" s="16">
-        <f>IF(B94 &gt;  0,C94-B94, 0)</f>
+        <f t="shared" si="5"/>
         <v>5275</v>
       </c>
     </row>
@@ -5637,7 +5811,7 @@
         <v>34860</v>
       </c>
       <c r="D95" s="16">
-        <f>IF(B95 &gt;  0,C95-B95, 0)</f>
+        <f t="shared" si="5"/>
         <v>5275</v>
       </c>
     </row>
@@ -5652,7 +5826,7 @@
         <v>34998</v>
       </c>
       <c r="D96" s="16">
-        <f>IF(B96 &gt;  0,C96-B96, 0)</f>
+        <f t="shared" si="5"/>
         <v>5290</v>
       </c>
     </row>
@@ -5667,7 +5841,7 @@
         <v>35137</v>
       </c>
       <c r="D97" s="16">
-        <f>IF(B97 &gt;  0,C97-B97, 0)</f>
+        <f t="shared" si="5"/>
         <v>5289</v>
       </c>
     </row>
@@ -5682,7 +5856,7 @@
         <v>35181</v>
       </c>
       <c r="D98" s="16">
-        <f>IF(B98 &gt;  0,C98-B98, 0)</f>
+        <f t="shared" si="5"/>
         <v>5287</v>
       </c>
     </row>
@@ -5697,7 +5871,7 @@
         <v>35621</v>
       </c>
       <c r="D99" s="16">
-        <f>IF(B99 &gt;  0,C99-B99, 0)</f>
+        <f t="shared" si="5"/>
         <v>5290</v>
       </c>
     </row>
@@ -5712,7 +5886,7 @@
         <v>35992</v>
       </c>
       <c r="D100" s="16">
-        <f>IF(B100 &gt;  0,C100-B100, 0)</f>
+        <f t="shared" si="5"/>
         <v>5294</v>
       </c>
     </row>
@@ -5727,7 +5901,7 @@
         <v>36290</v>
       </c>
       <c r="D101" s="16">
-        <f>IF(B101 &gt;  0,C101-B101, 0)</f>
+        <f t="shared" si="5"/>
         <v>5298</v>
       </c>
     </row>
@@ -5742,7 +5916,7 @@
         <v>36576</v>
       </c>
       <c r="D102" s="16">
-        <f>IF(B102 &gt;  0,C102-B102, 0)</f>
+        <f t="shared" si="5"/>
         <v>5315</v>
       </c>
     </row>
@@ -5757,7 +5931,7 @@
         <v>36872</v>
       </c>
       <c r="D103" s="16">
-        <f>IF(B103 &gt;  0,C103-B103, 0)</f>
+        <f t="shared" si="5"/>
         <v>5329</v>
       </c>
     </row>
@@ -5772,7 +5946,7 @@
         <v>37235</v>
       </c>
       <c r="D104" s="16">
-        <f>IF(B104 &gt;  0,C104-B104, 0)</f>
+        <f t="shared" si="5"/>
         <v>5329</v>
       </c>
     </row>
@@ -5787,7 +5961,7 @@
         <v>37736</v>
       </c>
       <c r="D105" s="16">
-        <f>IF(B105 &gt;  0,C105-B105, 0)</f>
+        <f t="shared" si="5"/>
         <v>5354</v>
       </c>
     </row>
@@ -5802,7 +5976,7 @@
         <v>38007</v>
       </c>
       <c r="D106" s="16">
-        <f>IF(B106 &gt;  0,C106-B106, 0)</f>
+        <f t="shared" si="5"/>
         <v>5361</v>
       </c>
     </row>
@@ -5817,7 +5991,7 @@
         <v>38525</v>
       </c>
       <c r="D107" s="16">
-        <f>IF(B107 &gt;  0,C107-B107, 0)</f>
+        <f t="shared" si="5"/>
         <v>5361</v>
       </c>
       <c r="E107">
@@ -5844,7 +6018,7 @@
         <v>39462</v>
       </c>
       <c r="D109" s="16">
-        <f>IF(B109 &gt;  0,C109-B109, 0)</f>
+        <f t="shared" ref="D109:D120" si="6">IF(B109 &gt;  0,C109-B109, 0)</f>
         <v>5863</v>
       </c>
     </row>
@@ -5859,7 +6033,7 @@
         <v>39712</v>
       </c>
       <c r="D110" s="16">
-        <f>IF(B110 &gt;  0,C110-B110, 0)</f>
+        <f t="shared" si="6"/>
         <v>5886</v>
       </c>
     </row>
@@ -5874,7 +6048,7 @@
         <v>39911</v>
       </c>
       <c r="D111" s="16">
-        <f>IF(B111 &gt;  0,C111-B111, 0)</f>
+        <f t="shared" si="6"/>
         <v>5889</v>
       </c>
     </row>
@@ -5889,7 +6063,7 @@
         <v>40279</v>
       </c>
       <c r="D112" s="16">
-        <f>IF(B112 &gt;  0,C112-B112, 0)</f>
+        <f t="shared" si="6"/>
         <v>5894</v>
       </c>
     </row>
@@ -5904,7 +6078,7 @@
         <v>40661</v>
       </c>
       <c r="D113" s="16">
-        <f>IF(B113 &gt;  0,C113-B113, 0)</f>
+        <f t="shared" si="6"/>
         <v>5894</v>
       </c>
     </row>
@@ -5919,7 +6093,7 @@
         <v>40799</v>
       </c>
       <c r="D114" s="16">
-        <f>IF(B114 &gt;  0,C114-B114, 0)</f>
+        <f t="shared" si="6"/>
         <v>5895</v>
       </c>
     </row>
@@ -5934,7 +6108,7 @@
         <v>40846</v>
       </c>
       <c r="D115" s="16">
-        <f>IF(B115 &gt;  0,C115-B115, 0)</f>
+        <f t="shared" si="6"/>
         <v>5896</v>
       </c>
     </row>
@@ -5949,7 +6123,7 @@
         <v>40921</v>
       </c>
       <c r="D116" s="16">
-        <f>IF(B116 &gt;  0,C116-B116, 0)</f>
+        <f t="shared" si="6"/>
         <v>5896</v>
       </c>
     </row>
@@ -5964,7 +6138,7 @@
         <v>41175</v>
       </c>
       <c r="D117" s="16">
-        <f>IF(B117 &gt;  0,C117-B117, 0)</f>
+        <f t="shared" si="6"/>
         <v>5893</v>
       </c>
     </row>
@@ -5979,7 +6153,7 @@
         <v>41485</v>
       </c>
       <c r="D118" s="16">
-        <f>IF(B118 &gt;  0,C118-B118, 0)</f>
+        <f t="shared" si="6"/>
         <v>5898</v>
       </c>
     </row>
@@ -5994,7 +6168,7 @@
         <v>41774</v>
       </c>
       <c r="D119" s="16">
-        <f>IF(B119 &gt;  0,C119-B119, 0)</f>
+        <f t="shared" si="6"/>
         <v>5918</v>
       </c>
     </row>
@@ -6009,7 +6183,7 @@
         <v>42408</v>
       </c>
       <c r="D120" s="16">
-        <f>IF(B120 &gt;  0,C120-B120, 0)</f>
+        <f t="shared" si="6"/>
         <v>5911</v>
       </c>
       <c r="E120">
@@ -6036,7 +6210,7 @@
         <v>43787</v>
       </c>
       <c r="D122" s="16">
-        <f>IF(B122 &gt;  0,C122-B122, 0)</f>
+        <f t="shared" ref="D122:D130" si="7">IF(B122 &gt;  0,C122-B122, 0)</f>
         <v>6565</v>
       </c>
     </row>
@@ -6051,7 +6225,7 @@
         <v>44032</v>
       </c>
       <c r="D123" s="16">
-        <f>IF(B123 &gt;  0,C123-B123, 0)</f>
+        <f t="shared" si="7"/>
         <v>6584</v>
       </c>
     </row>
@@ -6066,7 +6240,7 @@
         <v>44249</v>
       </c>
       <c r="D124" s="16">
-        <f>IF(B124 &gt;  0,C124-B124, 0)</f>
+        <f t="shared" si="7"/>
         <v>6585</v>
       </c>
     </row>
@@ -6081,7 +6255,7 @@
         <v>44527</v>
       </c>
       <c r="D125" s="16">
-        <f>IF(B125 &gt;  0,C125-B125, 0)</f>
+        <f t="shared" si="7"/>
         <v>6608</v>
       </c>
     </row>
@@ -6096,7 +6270,7 @@
         <v>45775</v>
       </c>
       <c r="D126" s="16">
-        <f>IF(B126 &gt;  0,C126-B126, 0)</f>
+        <f t="shared" si="7"/>
         <v>6610</v>
       </c>
     </row>
@@ -6111,7 +6285,7 @@
         <v>46333</v>
       </c>
       <c r="D127" s="16">
-        <f>IF(B127 &gt;  0,C127-B127, 0)</f>
+        <f t="shared" si="7"/>
         <v>6611</v>
       </c>
     </row>
@@ -6126,7 +6300,7 @@
         <v>48401</v>
       </c>
       <c r="D128" s="16">
-        <f>IF(B128 &gt;  0,C128-B128, 0)</f>
+        <f t="shared" si="7"/>
         <v>6630</v>
       </c>
     </row>
@@ -6141,7 +6315,7 @@
         <v>48651</v>
       </c>
       <c r="D129" s="16">
-        <f>IF(B129 &gt;  0,C129-B129, 0)</f>
+        <f t="shared" si="7"/>
         <v>6642</v>
       </c>
     </row>
@@ -6156,7 +6330,7 @@
         <v>49165</v>
       </c>
       <c r="D130" s="16">
-        <f>IF(B130 &gt;  0,C130-B130, 0)</f>
+        <f t="shared" si="7"/>
         <v>6642</v>
       </c>
       <c r="E130">
@@ -6255,7 +6429,7 @@
         <v>52978</v>
       </c>
       <c r="D137" s="16">
-        <f>IF(B137 &gt;  0,C137-B137, 0)</f>
+        <f t="shared" ref="D137:D148" si="8">IF(B137 &gt;  0,C137-B137, 0)</f>
         <v>7454</v>
       </c>
     </row>
@@ -6270,7 +6444,7 @@
         <v>53228</v>
       </c>
       <c r="D138" s="16">
-        <f>IF(B138 &gt;  0,C138-B138, 0)</f>
+        <f t="shared" si="8"/>
         <v>7476</v>
       </c>
     </row>
@@ -6285,7 +6459,7 @@
         <v>53306</v>
       </c>
       <c r="D139" s="16">
-        <f>IF(B139 &gt;  0,C139-B139, 0)</f>
+        <f t="shared" si="8"/>
         <v>7476</v>
       </c>
     </row>
@@ -6300,7 +6474,7 @@
         <v>53405</v>
       </c>
       <c r="D140" s="16">
-        <f>IF(B140 &gt;  0,C140-B140, 0)</f>
+        <f t="shared" si="8"/>
         <v>7476</v>
       </c>
     </row>
@@ -6315,7 +6489,7 @@
         <v>53602</v>
       </c>
       <c r="D141" s="16">
-        <f>IF(B141 &gt;  0,C141-B141, 0)</f>
+        <f t="shared" si="8"/>
         <v>7478</v>
       </c>
     </row>
@@ -6330,7 +6504,7 @@
         <v>53758</v>
       </c>
       <c r="D142" s="16">
-        <f>IF(B142 &gt;  0,C142-B142, 0)</f>
+        <f t="shared" si="8"/>
         <v>7479</v>
       </c>
     </row>
@@ -6345,7 +6519,7 @@
         <v>53854</v>
       </c>
       <c r="D143" s="16">
-        <f>IF(B143 &gt;  0,C143-B143, 0)</f>
+        <f t="shared" si="8"/>
         <v>7478</v>
       </c>
     </row>
@@ -6360,7 +6534,7 @@
         <v>53982</v>
       </c>
       <c r="D144" s="16">
-        <f>IF(B144 &gt;  0,C144-B144, 0)</f>
+        <f t="shared" si="8"/>
         <v>7478</v>
       </c>
     </row>
@@ -6375,7 +6549,7 @@
         <v>54102</v>
       </c>
       <c r="D145" s="16">
-        <f>IF(B145 &gt;  0,C145-B145, 0)</f>
+        <f t="shared" si="8"/>
         <v>7478</v>
       </c>
     </row>
@@ -6390,7 +6564,7 @@
         <v>54354</v>
       </c>
       <c r="D146" s="16">
-        <f>IF(B146 &gt;  0,C146-B146, 0)</f>
+        <f t="shared" si="8"/>
         <v>7478</v>
       </c>
     </row>
@@ -6405,7 +6579,7 @@
         <v>55387</v>
       </c>
       <c r="D147" s="16">
-        <f>IF(B147 &gt;  0,C147-B147, 0)</f>
+        <f t="shared" si="8"/>
         <v>7495</v>
       </c>
     </row>
@@ -6420,7 +6594,7 @@
         <v>56300</v>
       </c>
       <c r="D148" s="16">
-        <f>IF(B148 &gt;  0,C148-B148, 0)</f>
+        <f t="shared" si="8"/>
         <v>7495</v>
       </c>
       <c r="E148">
@@ -6447,7 +6621,7 @@
         <v>59573</v>
       </c>
       <c r="D150" s="16">
-        <f>IF(B150 &gt;  0,C150-B150, 0)</f>
+        <f t="shared" ref="D150:D161" si="9">IF(B150 &gt;  0,C150-B150, 0)</f>
         <v>9142</v>
       </c>
     </row>
@@ -6462,7 +6636,7 @@
         <v>59821</v>
       </c>
       <c r="D151" s="16">
-        <f>IF(B151 &gt;  0,C151-B151, 0)</f>
+        <f t="shared" si="9"/>
         <v>9163</v>
       </c>
     </row>
@@ -6477,7 +6651,7 @@
         <v>59960</v>
       </c>
       <c r="D152" s="16">
-        <f>IF(B152 &gt;  0,C152-B152, 0)</f>
+        <f t="shared" si="9"/>
         <v>9163</v>
       </c>
     </row>
@@ -6492,7 +6666,7 @@
         <v>60068</v>
       </c>
       <c r="D153" s="16">
-        <f>IF(B153 &gt;  0,C153-B153, 0)</f>
+        <f t="shared" si="9"/>
         <v>9164</v>
       </c>
     </row>
@@ -6507,7 +6681,7 @@
         <v>60159</v>
       </c>
       <c r="D154" s="16">
-        <f>IF(B154 &gt;  0,C154-B154, 0)</f>
+        <f t="shared" si="9"/>
         <v>9164</v>
       </c>
     </row>
@@ -6522,7 +6696,7 @@
         <v>60299</v>
       </c>
       <c r="D155" s="16">
-        <f>IF(B155 &gt;  0,C155-B155, 0)</f>
+        <f t="shared" si="9"/>
         <v>9164</v>
       </c>
     </row>
@@ -6537,7 +6711,7 @@
         <v>60517</v>
       </c>
       <c r="D156" s="16">
-        <f>IF(B156 &gt;  0,C156-B156, 0)</f>
+        <f t="shared" si="9"/>
         <v>9165</v>
       </c>
     </row>
@@ -6552,7 +6726,7 @@
         <v>60652</v>
       </c>
       <c r="D157" s="16">
-        <f>IF(B157 &gt;  0,C157-B157, 0)</f>
+        <f t="shared" si="9"/>
         <v>9165</v>
       </c>
     </row>
@@ -6567,7 +6741,7 @@
         <v>60846</v>
       </c>
       <c r="D158" s="16">
-        <f>IF(B158 &gt;  0,C158-B158, 0)</f>
+        <f t="shared" si="9"/>
         <v>9165</v>
       </c>
     </row>
@@ -6582,7 +6756,7 @@
         <v>61248</v>
       </c>
       <c r="D159" s="16">
-        <f>IF(B159 &gt;  0,C159-B159, 0)</f>
+        <f t="shared" si="9"/>
         <v>9168</v>
       </c>
     </row>
@@ -6597,7 +6771,7 @@
         <v>61427</v>
       </c>
       <c r="D160" s="16">
-        <f>IF(B160 &gt;  0,C160-B160, 0)</f>
+        <f t="shared" si="9"/>
         <v>9177</v>
       </c>
     </row>
@@ -6612,7 +6786,7 @@
         <v>61945</v>
       </c>
       <c r="D161" s="16">
-        <f>IF(B161 &gt;  0,C161-B161, 0)</f>
+        <f t="shared" si="9"/>
         <v>9177</v>
       </c>
       <c r="E161">
@@ -6639,7 +6813,7 @@
         <v>62610</v>
       </c>
       <c r="D163" s="16">
-        <f>IF(B163 &gt;  0,C163-B163, 0)</f>
+        <f t="shared" ref="D163:D176" si="10">IF(B163 &gt;  0,C163-B163, 0)</f>
         <v>9506</v>
       </c>
     </row>
@@ -6654,7 +6828,7 @@
         <v>62861</v>
       </c>
       <c r="D164" s="16">
-        <f>IF(B164 &gt;  0,C164-B164, 0)</f>
+        <f t="shared" si="10"/>
         <v>9529</v>
       </c>
     </row>
@@ -6669,7 +6843,7 @@
         <v>63021</v>
       </c>
       <c r="D165" s="16">
-        <f>IF(B165 &gt;  0,C165-B165, 0)</f>
+        <f t="shared" si="10"/>
         <v>9544</v>
       </c>
     </row>
@@ -6684,7 +6858,7 @@
         <v>63110</v>
       </c>
       <c r="D166" s="16">
-        <f>IF(B166 &gt;  0,C166-B166, 0)</f>
+        <f t="shared" si="10"/>
         <v>9548</v>
       </c>
     </row>
@@ -6699,7 +6873,7 @@
         <v>63206</v>
       </c>
       <c r="D167" s="16">
-        <f>IF(B167 &gt;  0,C167-B167, 0)</f>
+        <f t="shared" si="10"/>
         <v>9563</v>
       </c>
     </row>
@@ -6714,7 +6888,7 @@
         <v>63376</v>
       </c>
       <c r="D168" s="16">
-        <f>IF(B168 &gt;  0,C168-B168, 0)</f>
+        <f t="shared" si="10"/>
         <v>9563</v>
       </c>
     </row>
@@ -6729,7 +6903,7 @@
         <v>63425</v>
       </c>
       <c r="D169" s="16">
-        <f>IF(B169 &gt;  0,C169-B169, 0)</f>
+        <f t="shared" si="10"/>
         <v>9574</v>
       </c>
     </row>
@@ -6744,7 +6918,7 @@
         <v>63540</v>
       </c>
       <c r="D170" s="16">
-        <f>IF(B170 &gt;  0,C170-B170, 0)</f>
+        <f t="shared" si="10"/>
         <v>9588</v>
       </c>
     </row>
@@ -6759,7 +6933,7 @@
         <v>63597</v>
       </c>
       <c r="D171" s="16">
-        <f>IF(B171 &gt;  0,C171-B171, 0)</f>
+        <f t="shared" si="10"/>
         <v>9590</v>
       </c>
     </row>
@@ -6774,7 +6948,7 @@
         <v>63819</v>
       </c>
       <c r="D172" s="16">
-        <f>IF(B172 &gt;  0,C172-B172, 0)</f>
+        <f t="shared" si="10"/>
         <v>9610</v>
       </c>
     </row>
@@ -6789,7 +6963,7 @@
         <v>64047</v>
       </c>
       <c r="D173" s="16">
-        <f>IF(B173 &gt;  0,C173-B173, 0)</f>
+        <f t="shared" si="10"/>
         <v>9679</v>
       </c>
     </row>
@@ -6804,7 +6978,7 @@
         <v>64335</v>
       </c>
       <c r="D174" s="16">
-        <f>IF(B174 &gt;  0,C174-B174, 0)</f>
+        <f t="shared" si="10"/>
         <v>9684</v>
       </c>
     </row>
@@ -6819,7 +6993,7 @@
         <v>64568</v>
       </c>
       <c r="D175" s="16">
-        <f>IF(B175 &gt;  0,C175-B175, 0)</f>
+        <f t="shared" si="10"/>
         <v>9696</v>
       </c>
     </row>
@@ -6834,7 +7008,7 @@
         <v>65086</v>
       </c>
       <c r="D176" s="16">
-        <f>IF(B176 &gt;  0,C176-B176, 0)</f>
+        <f t="shared" si="10"/>
         <v>9696</v>
       </c>
       <c r="E176">
@@ -6861,7 +7035,7 @@
         <v>65479</v>
       </c>
       <c r="D178" s="16">
-        <f>IF(B178 &gt;  0,C178-B178, 0)</f>
+        <f t="shared" ref="D178:D194" si="11">IF(B178 &gt;  0,C178-B178, 0)</f>
         <v>9754</v>
       </c>
     </row>
@@ -6876,7 +7050,7 @@
         <v>66009</v>
       </c>
       <c r="D179" s="16">
-        <f>IF(B179 &gt;  0,C179-B179, 0)</f>
+        <f t="shared" si="11"/>
         <v>10051</v>
       </c>
     </row>
@@ -6891,7 +7065,7 @@
         <v>66317</v>
       </c>
       <c r="D180" s="16">
-        <f>IF(B180 &gt;  0,C180-B180, 0)</f>
+        <f t="shared" si="11"/>
         <v>10052</v>
       </c>
     </row>
@@ -6906,7 +7080,7 @@
         <v>66431</v>
       </c>
       <c r="D181" s="16">
-        <f>IF(B181 &gt;  0,C181-B181, 0)</f>
+        <f t="shared" si="11"/>
         <v>10053</v>
       </c>
     </row>
@@ -6921,7 +7095,7 @@
         <v>66483</v>
       </c>
       <c r="D182" s="16">
-        <f>IF(B182 &gt;  0,C182-B182, 0)</f>
+        <f t="shared" si="11"/>
         <v>10055</v>
       </c>
     </row>
@@ -6936,7 +7110,7 @@
         <v>66695</v>
       </c>
       <c r="D183" s="16">
-        <f>IF(B183 &gt;  0,C183-B183, 0)</f>
+        <f t="shared" si="11"/>
         <v>10055</v>
       </c>
     </row>
@@ -6951,7 +7125,7 @@
         <v>66770</v>
       </c>
       <c r="D184" s="16">
-        <f>IF(B184 &gt;  0,C184-B184, 0)</f>
+        <f t="shared" si="11"/>
         <v>10055</v>
       </c>
     </row>
@@ -6966,7 +7140,7 @@
         <v>66954</v>
       </c>
       <c r="D185" s="16">
-        <f>IF(B185 &gt;  0,C185-B185, 0)</f>
+        <f t="shared" si="11"/>
         <v>10056</v>
       </c>
     </row>
@@ -6981,7 +7155,7 @@
         <v>67039</v>
       </c>
       <c r="D186" s="16">
-        <f>IF(B186 &gt;  0,C186-B186, 0)</f>
+        <f t="shared" si="11"/>
         <v>10057</v>
       </c>
     </row>
@@ -6996,7 +7170,7 @@
         <v>67079</v>
       </c>
       <c r="D187" s="16">
-        <f>IF(B187 &gt;  0,C187-B187, 0)</f>
+        <f t="shared" si="11"/>
         <v>10059</v>
       </c>
     </row>
@@ -7011,7 +7185,7 @@
         <v>67144</v>
       </c>
       <c r="D188" s="16">
-        <f>IF(B188 &gt;  0,C188-B188, 0)</f>
+        <f t="shared" si="11"/>
         <v>10059</v>
       </c>
     </row>
@@ -7026,7 +7200,7 @@
         <v>67193</v>
       </c>
       <c r="D189" s="16">
-        <f>IF(B189 &gt;  0,C189-B189, 0)</f>
+        <f t="shared" si="11"/>
         <v>10059</v>
       </c>
     </row>
@@ -7041,7 +7215,7 @@
         <v>67293</v>
       </c>
       <c r="D190" s="16">
-        <f>IF(B190 &gt;  0,C190-B190, 0)</f>
+        <f t="shared" si="11"/>
         <v>10059</v>
       </c>
     </row>
@@ -7056,7 +7230,7 @@
         <v>67368</v>
       </c>
       <c r="D191" s="16">
-        <f>IF(B191 &gt;  0,C191-B191, 0)</f>
+        <f t="shared" si="11"/>
         <v>10059</v>
       </c>
     </row>
@@ -7071,7 +7245,7 @@
         <v>67591</v>
       </c>
       <c r="D192" s="16">
-        <f>IF(B192 &gt;  0,C192-B192, 0)</f>
+        <f t="shared" si="11"/>
         <v>10060</v>
       </c>
     </row>
@@ -7086,7 +7260,7 @@
         <v>67831</v>
       </c>
       <c r="D193" s="16">
-        <f>IF(B193 &gt;  0,C193-B193, 0)</f>
+        <f t="shared" si="11"/>
         <v>10060</v>
       </c>
     </row>
@@ -7101,7 +7275,7 @@
         <v>68349</v>
       </c>
       <c r="D194" s="16">
-        <f>IF(B194 &gt;  0,C194-B194, 0)</f>
+        <f t="shared" si="11"/>
         <v>10060</v>
       </c>
       <c r="E194">
@@ -7128,7 +7302,7 @@
         <v>69018</v>
       </c>
       <c r="D196" s="16">
-        <f>IF(B196 &gt;  0,C196-B196, 0)</f>
+        <f t="shared" ref="D196:D203" si="12">IF(B196 &gt;  0,C196-B196, 0)</f>
         <v>10396</v>
       </c>
     </row>
@@ -7143,7 +7317,7 @@
         <v>69265</v>
       </c>
       <c r="D197" s="16">
-        <f>IF(B197 &gt;  0,C197-B197, 0)</f>
+        <f t="shared" si="12"/>
         <v>10417</v>
       </c>
     </row>
@@ -7158,7 +7332,7 @@
         <v>69850</v>
       </c>
       <c r="D198" s="16">
-        <f>IF(B198 &gt;  0,C198-B198, 0)</f>
+        <f t="shared" si="12"/>
         <v>10418</v>
       </c>
     </row>
@@ -7173,7 +7347,7 @@
         <v>70031</v>
       </c>
       <c r="D199" s="16">
-        <f>IF(B199 &gt;  0,C199-B199, 0)</f>
+        <f t="shared" si="12"/>
         <v>10421</v>
       </c>
     </row>
@@ -7188,7 +7362,7 @@
         <v>70137</v>
       </c>
       <c r="D200" s="16">
-        <f>IF(B200 &gt;  0,C200-B200, 0)</f>
+        <f t="shared" si="12"/>
         <v>10421</v>
       </c>
     </row>
@@ -7203,7 +7377,7 @@
         <v>70285</v>
       </c>
       <c r="D201" s="16">
-        <f>IF(B201 &gt;  0,C201-B201, 0)</f>
+        <f t="shared" si="12"/>
         <v>10422</v>
       </c>
     </row>
@@ -7218,7 +7392,7 @@
         <v>70444</v>
       </c>
       <c r="D202" s="16">
-        <f>IF(B202 &gt;  0,C202-B202, 0)</f>
+        <f t="shared" si="12"/>
         <v>10422</v>
       </c>
     </row>
@@ -7233,7 +7407,7 @@
         <v>70962</v>
       </c>
       <c r="D203" s="16">
-        <f>IF(B203 &gt;  0,C203-B203, 0)</f>
+        <f t="shared" si="12"/>
         <v>10422</v>
       </c>
       <c r="E203">
@@ -7260,7 +7434,7 @@
         <v>71707</v>
       </c>
       <c r="D205" s="16">
-        <f>IF(B205 &gt;  0,C205-B205, 0)</f>
+        <f t="shared" ref="D205:D210" si="13">IF(B205 &gt;  0,C205-B205, 0)</f>
         <v>10798</v>
       </c>
     </row>
@@ -7275,7 +7449,7 @@
         <v>71957</v>
       </c>
       <c r="D206" s="16">
-        <f>IF(B206 &gt;  0,C206-B206, 0)</f>
+        <f t="shared" si="13"/>
         <v>10820</v>
       </c>
     </row>
@@ -7290,7 +7464,7 @@
         <v>72069</v>
       </c>
       <c r="D207" s="16">
-        <f>IF(B207 &gt;  0,C207-B207, 0)</f>
+        <f t="shared" si="13"/>
         <v>10831</v>
       </c>
     </row>
@@ -7305,7 +7479,7 @@
         <v>79905</v>
       </c>
       <c r="D208" s="16">
-        <f>IF(B208 &gt;  0,C208-B208, 0)</f>
+        <f t="shared" si="13"/>
         <v>10862</v>
       </c>
     </row>
@@ -7320,7 +7494,7 @@
         <v>80190</v>
       </c>
       <c r="D209" s="16">
-        <f>IF(B209 &gt;  0,C209-B209, 0)</f>
+        <f t="shared" si="13"/>
         <v>10881</v>
       </c>
     </row>
@@ -7335,7 +7509,7 @@
         <v>80786</v>
       </c>
       <c r="D210" s="16">
-        <f>IF(B210 &gt;  0,C210-B210, 0)</f>
+        <f t="shared" si="13"/>
         <v>10880</v>
       </c>
       <c r="E210">
@@ -7362,7 +7536,7 @@
         <v>82543</v>
       </c>
       <c r="D212" s="16">
-        <f>IF(B212 &gt;  0,C212-B212, 0)</f>
+        <f t="shared" ref="D212:D235" si="14">IF(B212 &gt;  0,C212-B212, 0)</f>
         <v>11757</v>
       </c>
     </row>
@@ -7377,7 +7551,7 @@
         <v>82799</v>
       </c>
       <c r="D213" s="16">
-        <f>IF(B213 &gt;  0,C213-B213, 0)</f>
+        <f t="shared" si="14"/>
         <v>11782</v>
       </c>
     </row>
@@ -7392,7 +7566,7 @@
         <v>83249</v>
       </c>
       <c r="D214" s="16">
-        <f>IF(B214 &gt;  0,C214-B214, 0)</f>
+        <f t="shared" si="14"/>
         <v>11782</v>
       </c>
     </row>
@@ -7407,7 +7581,7 @@
         <v>83509</v>
       </c>
       <c r="D215" s="16">
-        <f>IF(B215 &gt;  0,C215-B215, 0)</f>
+        <f t="shared" si="14"/>
         <v>11784</v>
       </c>
     </row>
@@ -7422,7 +7596,7 @@
         <v>83800</v>
       </c>
       <c r="D216" s="16">
-        <f>IF(B216 &gt;  0,C216-B216, 0)</f>
+        <f t="shared" si="14"/>
         <v>11784</v>
       </c>
     </row>
@@ -7437,7 +7611,7 @@
         <v>84128</v>
       </c>
       <c r="D217" s="16">
-        <f>IF(B217 &gt;  0,C217-B217, 0)</f>
+        <f t="shared" si="14"/>
         <v>11805</v>
       </c>
     </row>
@@ -7452,7 +7626,7 @@
         <v>84487</v>
       </c>
       <c r="D218" s="16">
-        <f>IF(B218 &gt;  0,C218-B218, 0)</f>
+        <f t="shared" si="14"/>
         <v>11822</v>
       </c>
     </row>
@@ -7467,7 +7641,7 @@
         <v>85239</v>
       </c>
       <c r="D219" s="16">
-        <f>IF(B219 &gt;  0,C219-B219, 0)</f>
+        <f t="shared" si="14"/>
         <v>11827</v>
       </c>
     </row>
@@ -7482,7 +7656,7 @@
         <v>85786</v>
       </c>
       <c r="D220" s="16">
-        <f>IF(B220 &gt;  0,C220-B220, 0)</f>
+        <f t="shared" si="14"/>
         <v>11828</v>
       </c>
     </row>
@@ -7497,7 +7671,7 @@
         <v>86590</v>
       </c>
       <c r="D221" s="16">
-        <f>IF(B221 &gt;  0,C221-B221, 0)</f>
+        <f t="shared" si="14"/>
         <v>11841</v>
       </c>
     </row>
@@ -7512,7 +7686,7 @@
         <v>86830</v>
       </c>
       <c r="D222" s="16">
-        <f>IF(B222 &gt;  0,C222-B222, 0)</f>
+        <f t="shared" si="14"/>
         <v>11848</v>
       </c>
     </row>
@@ -7527,7 +7701,7 @@
         <v>86956</v>
       </c>
       <c r="D223" s="16">
-        <f>IF(B223 &gt;  0,C223-B223, 0)</f>
+        <f t="shared" si="14"/>
         <v>11849</v>
       </c>
     </row>
@@ -7542,7 +7716,7 @@
         <v>87129</v>
       </c>
       <c r="D224" s="16">
-        <f>IF(B224 &gt;  0,C224-B224, 0)</f>
+        <f t="shared" si="14"/>
         <v>11849</v>
       </c>
     </row>
@@ -7557,7 +7731,7 @@
         <v>87443</v>
       </c>
       <c r="D225" s="16">
-        <f>IF(B225 &gt;  0,C225-B225, 0)</f>
+        <f t="shared" si="14"/>
         <v>11852</v>
       </c>
     </row>
@@ -7572,7 +7746,7 @@
         <v>87604</v>
       </c>
       <c r="D226" s="16">
-        <f>IF(B226 &gt;  0,C226-B226, 0)</f>
+        <f t="shared" si="14"/>
         <v>11863</v>
       </c>
     </row>
@@ -7587,7 +7761,7 @@
         <v>87692</v>
       </c>
       <c r="D227" s="16">
-        <f>IF(B227 &gt;  0,C227-B227, 0)</f>
+        <f t="shared" si="14"/>
         <v>11864</v>
       </c>
     </row>
@@ -7602,7 +7776,7 @@
         <v>87836</v>
       </c>
       <c r="D228" s="16">
-        <f>IF(B228 &gt;  0,C228-B228, 0)</f>
+        <f t="shared" si="14"/>
         <v>11864</v>
       </c>
     </row>
@@ -7617,7 +7791,7 @@
         <v>88091</v>
       </c>
       <c r="D229" s="16">
-        <f>IF(B229 &gt;  0,C229-B229, 0)</f>
+        <f t="shared" si="14"/>
         <v>11864</v>
       </c>
     </row>
@@ -7632,7 +7806,7 @@
         <v>88170</v>
       </c>
       <c r="D230" s="16">
-        <f>IF(B230 &gt;  0,C230-B230, 0)</f>
+        <f t="shared" si="14"/>
         <v>11864</v>
       </c>
     </row>
@@ -7647,7 +7821,7 @@
         <v>88308</v>
       </c>
       <c r="D231" s="16">
-        <f>IF(B231 &gt;  0,C231-B231, 0)</f>
+        <f t="shared" si="14"/>
         <v>11864</v>
       </c>
     </row>
@@ -7662,7 +7836,7 @@
         <v>88605</v>
       </c>
       <c r="D232" s="16">
-        <f>IF(B232 &gt;  0,C232-B232, 0)</f>
+        <f t="shared" si="14"/>
         <v>11864</v>
       </c>
     </row>
@@ -7677,7 +7851,7 @@
         <v>88946</v>
       </c>
       <c r="D233" s="16">
-        <f>IF(B233 &gt;  0,C233-B233, 0)</f>
+        <f t="shared" si="14"/>
         <v>11883</v>
       </c>
     </row>
@@ -7692,7 +7866,7 @@
         <v>89784</v>
       </c>
       <c r="D234" s="16">
-        <f>IF(B234 &gt;  0,C234-B234, 0)</f>
+        <f t="shared" si="14"/>
         <v>11918</v>
       </c>
     </row>
@@ -7707,10 +7881,10 @@
         <v>89784</v>
       </c>
       <c r="D235" s="16">
-        <f>IF(B235 &gt;  0,C235-B235, 0)</f>
+        <f t="shared" si="14"/>
         <v>11882</v>
       </c>
-      <c r="E235" s="42">
+      <c r="E235" s="36">
         <f>D235-D213</f>
         <v>100</v>
       </c>
@@ -7778,14 +7952,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -7848,14 +8022,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
@@ -8378,14 +8552,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="24" t="s">

</xml_diff>

<commit_message>
NSMB - 8-2 done.  Matches terrotim's single level 8-2 WIP desipite worse randomness with the spiders.  Uses a wall jump into the spider to initiate the bounce off it.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="242">
   <si>
     <t>1-1</t>
   </si>
@@ -743,7 +743,7 @@
     <t>Enter pipe (wall jump)</t>
   </si>
   <si>
-    <t>Hit P block</t>
+    <t>Enter Top pipe</t>
   </si>
 </sst>
 </file>
@@ -1294,8 +1294,8 @@
   <dimension ref="A1:I239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D233" sqref="D233"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F238" sqref="F238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4276,54 +4276,60 @@
         <v>29585</v>
       </c>
       <c r="F231" s="16">
-        <f t="shared" ref="F231:F235" si="10">IF(B231 &gt;  0,E231-B231, 0)</f>
+        <f t="shared" ref="F231:F232" si="10">IF(B231 &gt;  0,E231-B231, 0)</f>
         <v>480</v>
       </c>
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="16" t="s">
-        <v>241</v>
+        <v>20</v>
       </c>
       <c r="B232" s="16">
-        <v>29353</v>
+        <v>29838</v>
       </c>
       <c r="C232" s="16">
-        <v>29834</v>
+        <v>30332</v>
       </c>
       <c r="D232" s="16">
         <f t="shared" si="9"/>
-        <v>481</v>
+        <v>494</v>
       </c>
       <c r="E232" s="16">
-        <v>29834</v>
+        <v>30318</v>
       </c>
       <c r="F232" s="16">
         <f t="shared" si="10"/>
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="233" spans="1:6">
+      <c r="A233" s="16" t="s">
+        <v>239</v>
+      </c>
       <c r="B233" s="16">
-        <v>29360</v>
-      </c>
-      <c r="E233" s="16">
-        <v>29839</v>
-      </c>
-      <c r="F233" s="16">
-        <f t="shared" si="10"/>
-        <v>479</v>
+        <v>30494</v>
+      </c>
+      <c r="C233" s="16">
+        <v>30988</v>
+      </c>
+      <c r="D233" s="16">
+        <f t="shared" si="9"/>
+        <v>494</v>
       </c>
     </row>
     <row r="234" spans="1:6">
+      <c r="A234" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="B234" s="16">
-        <v>29407</v>
-      </c>
-      <c r="E234" s="16">
-        <v>29886</v>
-      </c>
-      <c r="F234" s="16">
-        <f t="shared" si="10"/>
-        <v>479</v>
+        <v>30766</v>
+      </c>
+      <c r="C234" s="16">
+        <v>31261</v>
+      </c>
+      <c r="D234" s="16">
+        <f t="shared" si="9"/>
+        <v>495</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -4331,81 +4337,73 @@
         <v>20</v>
       </c>
       <c r="B235" s="16">
-        <v>29838</v>
+        <v>31043</v>
       </c>
       <c r="C235" s="16">
-        <v>30332</v>
+        <v>31543</v>
       </c>
       <c r="D235" s="16">
         <f t="shared" si="9"/>
-        <v>494</v>
-      </c>
-      <c r="E235" s="16">
-        <v>30318</v>
-      </c>
-      <c r="F235" s="16">
-        <f t="shared" si="10"/>
-        <v>480</v>
+        <v>500</v>
       </c>
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B236" s="16">
-        <v>30494</v>
+        <v>31403</v>
       </c>
       <c r="C236" s="16">
-        <v>30988</v>
+        <v>31906</v>
       </c>
       <c r="D236" s="16">
         <f t="shared" si="9"/>
-        <v>494</v>
+        <v>503</v>
       </c>
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="16" t="s">
-        <v>20</v>
+        <v>241</v>
       </c>
       <c r="B237" s="16">
-        <v>30766</v>
-      </c>
-      <c r="C237" s="16">
-        <v>31261</v>
+        <v>31878</v>
       </c>
       <c r="D237" s="16">
-        <f t="shared" si="9"/>
-        <v>495</v>
+        <f>IF(B237 &gt;  0,E237-B237, 0)</f>
+        <v>480</v>
+      </c>
+      <c r="E237" s="16">
+        <v>32358</v>
+      </c>
+      <c r="F237" s="16">
+        <f t="shared" ref="F237:F238" si="11">IF(B237 &gt;  0,E237-B237, 0)</f>
+        <v>480</v>
       </c>
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="16" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B238" s="16">
-        <v>31043</v>
-      </c>
-      <c r="C238" s="16">
-        <v>31543</v>
+        <v>32660</v>
       </c>
       <c r="D238" s="16">
         <f t="shared" si="9"/>
-        <v>500</v>
+        <v>-32660</v>
+      </c>
+      <c r="E238" s="16">
+        <v>33140</v>
+      </c>
+      <c r="F238" s="16">
+        <f t="shared" si="11"/>
+        <v>480</v>
       </c>
     </row>
     <row r="239" spans="1:6">
-      <c r="A239" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="B239" s="16">
-        <v>31403</v>
-      </c>
-      <c r="C239" s="16">
-        <v>31906</v>
-      </c>
       <c r="D239" s="16">
         <f t="shared" si="9"/>
-        <v>503</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terrotim's 8-T WIP added to movie, has bad map movement afterwards of course.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -1291,11 +1291,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I239"/>
+  <dimension ref="A1:I241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F238" sqref="F238"/>
+      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4254,7 +4254,7 @@
         <v>29213</v>
       </c>
       <c r="D230" s="16">
-        <f t="shared" ref="D230:D239" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
+        <f t="shared" ref="D230:D241" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
         <v>480</v>
       </c>
     </row>
@@ -4404,6 +4404,18 @@
       <c r="D239" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="2:6">
+      <c r="B241" s="16">
+        <v>32981</v>
+      </c>
+      <c r="E241" s="16">
+        <v>33461</v>
+      </c>
+      <c r="F241" s="16">
+        <f t="shared" ref="F241" si="12">IF(B241 &gt;  0,E241-B241, 0)</f>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - recorded to 8-3 and then pasted 8-3 and 8-4 of the published movie (haven't attempted to improve 8-3 yet, 8-4 is at least improvable by using shell corner boosting)
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="246">
   <si>
     <t>1-1</t>
   </si>
@@ -744,6 +744,18 @@
   </si>
   <si>
     <t>Enter Top pipe</t>
+  </si>
+  <si>
+    <t>End 8-1</t>
+  </si>
+  <si>
+    <t>Enter 8-T</t>
+  </si>
+  <si>
+    <t>Enter Bowser Jr. Room</t>
+  </si>
+  <si>
+    <t>37150ish</t>
   </si>
 </sst>
 </file>
@@ -1291,11 +1303,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I241"/>
+  <dimension ref="A1:I245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4190,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" outlineLevel="1">
+    <row r="225" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A225" s="16" t="s">
         <v>204</v>
       </c>
@@ -4202,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" outlineLevel="1">
+    <row r="226" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A226" s="16" t="s">
         <v>205</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="227" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A227" s="16" t="s">
         <v>206</v>
       </c>
@@ -4230,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:6" s="31" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="228" spans="1:7" s="31" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A228" s="30"/>
       <c r="B228" s="30"/>
       <c r="C228" s="30"/>
@@ -4243,179 +4255,278 @@
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="1:6">
+    <row r="229" spans="1:7">
+      <c r="A229" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B229" s="16">
+        <v>28372</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
       <c r="A230" s="16" t="s">
         <v>129</v>
       </c>
       <c r="B230" s="16">
-        <v>28733</v>
+        <v>28731</v>
       </c>
       <c r="C230" s="16">
         <v>29213</v>
       </c>
       <c r="D230" s="16">
-        <f t="shared" ref="D230:D241" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6">
+        <f t="shared" ref="D230:D245" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
       <c r="A231" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B231" s="16">
-        <v>29105</v>
+        <v>29103</v>
       </c>
       <c r="C231" s="16">
         <v>29585</v>
       </c>
       <c r="D231" s="16">
         <f t="shared" si="9"/>
-        <v>480</v>
-      </c>
-      <c r="E231" s="16">
-        <v>29585</v>
+        <v>482</v>
       </c>
       <c r="F231" s="16">
         <f t="shared" ref="F231:F232" si="10">IF(B231 &gt;  0,E231-B231, 0)</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6">
+        <v>-29103</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
       <c r="A232" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B232" s="16">
-        <v>29838</v>
+        <v>29836</v>
       </c>
       <c r="C232" s="16">
         <v>30332</v>
       </c>
       <c r="D232" s="16">
         <f t="shared" si="9"/>
-        <v>494</v>
-      </c>
-      <c r="E232" s="16">
-        <v>30318</v>
+        <v>496</v>
       </c>
       <c r="F232" s="16">
         <f t="shared" si="10"/>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6">
+        <v>-29836</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7">
       <c r="A233" s="16" t="s">
         <v>239</v>
       </c>
       <c r="B233" s="16">
-        <v>30494</v>
+        <v>30492</v>
       </c>
       <c r="C233" s="16">
         <v>30988</v>
       </c>
       <c r="D233" s="16">
         <f t="shared" si="9"/>
-        <v>494</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7">
       <c r="A234" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B234" s="16">
-        <v>30766</v>
+        <v>30764</v>
       </c>
       <c r="C234" s="16">
         <v>31261</v>
       </c>
       <c r="D234" s="16">
         <f t="shared" si="9"/>
-        <v>495</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7">
       <c r="A235" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B235" s="16">
-        <v>31043</v>
+        <v>31041</v>
       </c>
       <c r="C235" s="16">
         <v>31543</v>
       </c>
       <c r="D235" s="16">
         <f t="shared" si="9"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
       <c r="A236" s="16" t="s">
         <v>240</v>
       </c>
       <c r="B236" s="16">
-        <v>31403</v>
+        <v>31401</v>
       </c>
       <c r="C236" s="16">
         <v>31906</v>
       </c>
       <c r="D236" s="16">
         <f t="shared" si="9"/>
-        <v>503</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
       <c r="A237" s="16" t="s">
         <v>241</v>
       </c>
       <c r="B237" s="16">
-        <v>31878</v>
+        <v>31876</v>
+      </c>
+      <c r="C237" s="16">
+        <v>32382</v>
       </c>
       <c r="D237" s="16">
-        <f>IF(B237 &gt;  0,E237-B237, 0)</f>
-        <v>480</v>
-      </c>
-      <c r="E237" s="16">
-        <v>32358</v>
+        <f t="shared" si="9"/>
+        <v>506</v>
       </c>
       <c r="F237" s="16">
         <f t="shared" ref="F237:F238" si="11">IF(B237 &gt;  0,E237-B237, 0)</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6">
+        <v>-31876</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
       <c r="A238" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B238" s="16">
-        <v>32660</v>
+        <v>32658</v>
+      </c>
+      <c r="C238" s="16">
+        <v>33164</v>
       </c>
       <c r="D238" s="16">
         <f t="shared" si="9"/>
-        <v>-32660</v>
-      </c>
-      <c r="E238" s="16">
-        <v>33140</v>
+        <v>506</v>
       </c>
       <c r="F238" s="16">
         <f t="shared" si="11"/>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6">
+        <v>-32658</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B239" s="16">
+        <v>33093</v>
+      </c>
+      <c r="C239" s="16">
+        <v>33599</v>
+      </c>
       <c r="D239" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="2:6">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="A240" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B240" s="16">
+        <v>35071</v>
+      </c>
+      <c r="C240" s="16">
+        <v>35593</v>
+      </c>
+      <c r="D240" s="16">
+        <f t="shared" si="9"/>
+        <v>522</v>
+      </c>
+      <c r="E240" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G240">
+        <v>36591</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="B241" s="16">
-        <v>32981</v>
-      </c>
-      <c r="E241" s="16">
-        <v>33461</v>
+        <v>35976</v>
+      </c>
+      <c r="C241" s="16">
+        <v>36498</v>
+      </c>
+      <c r="D241" s="16">
+        <f t="shared" si="9"/>
+        <v>522</v>
       </c>
       <c r="F241" s="16">
         <f t="shared" ref="F241" si="12">IF(B241 &gt;  0,E241-B241, 0)</f>
-        <v>480</v>
+        <v>-35976</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B242" s="16">
+        <v>36666</v>
+      </c>
+      <c r="C242" s="16">
+        <v>37222</v>
+      </c>
+      <c r="D242" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B243" s="16">
+        <v>37108</v>
+      </c>
+      <c r="C243" s="16">
+        <v>37664</v>
+      </c>
+      <c r="D243" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B244" s="16">
+        <v>41966</v>
+      </c>
+      <c r="C244" s="16">
+        <v>42521</v>
+      </c>
+      <c r="D244" s="16">
+        <f t="shared" si="9"/>
+        <v>555</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6">
+      <c r="A245" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B245" s="16">
+        <v>42394</v>
+      </c>
+      <c r="C245" s="16">
+        <v>42949</v>
+      </c>
+      <c r="D245" s="16">
+        <f t="shared" si="9"/>
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 8-4 1 frame faster than the published movie (using a shell corner boost at the beginning)
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="253">
   <si>
     <t>1-1</t>
   </si>
@@ -756,6 +756,27 @@
   </si>
   <si>
     <t>37150ish</t>
+  </si>
+  <si>
+    <t>X Camera = 206</t>
+  </si>
+  <si>
+    <t>X Camera = 548</t>
+  </si>
+  <si>
+    <t>X = 1319</t>
+  </si>
+  <si>
+    <t>X = 1611/1610</t>
+  </si>
+  <si>
+    <t>X = 1810</t>
+  </si>
+  <si>
+    <t>X=2201</t>
+  </si>
+  <si>
+    <t>X = 3192</t>
   </si>
 </sst>
 </file>
@@ -1303,11 +1324,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I245"/>
+  <dimension ref="A1:I254"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B246" sqref="B246"/>
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4274,7 +4295,7 @@
         <v>29213</v>
       </c>
       <c r="D230" s="16">
-        <f t="shared" ref="D230:D245" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
+        <f t="shared" ref="D230:D254" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
         <v>482</v>
       </c>
     </row>
@@ -4527,6 +4548,141 @@
       <c r="D245" s="16">
         <f t="shared" si="9"/>
         <v>555</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6">
+      <c r="A246" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B246" s="16">
+        <v>42729</v>
+      </c>
+      <c r="C246" s="16">
+        <v>43284</v>
+      </c>
+      <c r="D246" s="16">
+        <f t="shared" si="9"/>
+        <v>555</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6">
+      <c r="A247" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B247" s="16">
+        <v>42842</v>
+      </c>
+      <c r="C247" s="16">
+        <v>43398</v>
+      </c>
+      <c r="D247" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6">
+      <c r="A248" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B248" s="16">
+        <v>43142</v>
+      </c>
+      <c r="C248" s="16">
+        <v>43698</v>
+      </c>
+      <c r="D248" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6">
+      <c r="A249" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B249" s="16">
+        <v>43239</v>
+      </c>
+      <c r="C249" s="16">
+        <v>43795</v>
+      </c>
+      <c r="D249" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6">
+      <c r="A250" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B250" s="16">
+        <v>43305</v>
+      </c>
+      <c r="C250" s="16">
+        <v>43861</v>
+      </c>
+      <c r="D250" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6">
+      <c r="A251" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B251" s="16">
+        <v>43435</v>
+      </c>
+      <c r="C251" s="16">
+        <v>43991</v>
+      </c>
+      <c r="D251" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6">
+      <c r="A252" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B252" s="16">
+        <v>43759</v>
+      </c>
+      <c r="C252" s="16">
+        <v>44315</v>
+      </c>
+      <c r="D252" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6">
+      <c r="A253" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B253" s="16">
+        <v>44072</v>
+      </c>
+      <c r="C253" s="16">
+        <v>44628</v>
+      </c>
+      <c r="D253" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6">
+      <c r="A254" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B254" s="16">
+        <v>44590</v>
+      </c>
+      <c r="C254" s="16">
+        <v>45146</v>
+      </c>
+      <c r="D254" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8-4 ending modified for RNG manipulation (without frame loss), and the 2nd castle pasted from my published movie.
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="253">
   <si>
     <t>1-1</t>
   </si>
@@ -755,9 +755,6 @@
     <t>Enter Bowser Jr. Room</t>
   </si>
   <si>
-    <t>37150ish</t>
-  </si>
-  <si>
     <t>X Camera = 206</t>
   </si>
   <si>
@@ -777,6 +774,9 @@
   </si>
   <si>
     <t>X = 3192</t>
+  </si>
+  <si>
+    <t>Enter 8-T2</t>
   </si>
 </sst>
 </file>
@@ -1324,11 +1324,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I254"/>
+  <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C255" sqref="C255"/>
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C257" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4223,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1" outlineLevel="1">
+    <row r="225" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A225" s="16" t="s">
         <v>204</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" outlineLevel="1">
+    <row r="226" spans="1:6" hidden="1" outlineLevel="1">
       <c r="A226" s="16" t="s">
         <v>205</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="227" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A227" s="16" t="s">
         <v>206</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:7" s="31" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="228" spans="1:6" s="31" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A228" s="30"/>
       <c r="B228" s="30"/>
       <c r="C228" s="30"/>
@@ -4276,7 +4276,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:6">
       <c r="A229" s="16" t="s">
         <v>242</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>28372</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:6">
       <c r="A230" s="16" t="s">
         <v>129</v>
       </c>
@@ -4295,11 +4295,11 @@
         <v>29213</v>
       </c>
       <c r="D230" s="16">
-        <f t="shared" ref="D230:D254" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
+        <f t="shared" ref="D230:D256" si="9">IF(B230 &gt;  0,C230-B230, 0)</f>
         <v>482</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:6">
       <c r="A231" s="16" t="s">
         <v>20</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>-29103</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:6">
       <c r="A232" s="16" t="s">
         <v>20</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>-29836</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:6">
       <c r="A233" s="16" t="s">
         <v>239</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:6">
       <c r="A234" s="16" t="s">
         <v>20</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:6">
       <c r="A235" s="16" t="s">
         <v>20</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:6">
       <c r="A236" s="16" t="s">
         <v>240</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:6">
       <c r="A237" s="16" t="s">
         <v>241</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>-31876</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:6">
       <c r="A238" s="16" t="s">
         <v>83</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>-32658</v>
       </c>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:6">
       <c r="A239" s="16" t="s">
         <v>243</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:6">
       <c r="A240" s="16" t="s">
         <v>244</v>
       </c>
@@ -4464,12 +4464,6 @@
         <f t="shared" si="9"/>
         <v>522</v>
       </c>
-      <c r="E240" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="G240">
-        <v>36591</v>
-      </c>
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="16" t="s">
@@ -4552,7 +4546,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B246" s="16">
         <v>42729</v>
@@ -4567,7 +4561,7 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B247" s="16">
         <v>42842</v>
@@ -4582,7 +4576,7 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B248" s="16">
         <v>43142</v>
@@ -4597,7 +4591,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B249" s="16">
         <v>43239</v>
@@ -4612,7 +4606,7 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B250" s="16">
         <v>43305</v>
@@ -4627,7 +4621,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B251" s="16">
         <v>43435</v>
@@ -4642,7 +4636,7 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B252" s="16">
         <v>43759</v>
@@ -4681,6 +4675,36 @@
         <v>45146</v>
       </c>
       <c r="D254" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6">
+      <c r="A255" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B255" s="16">
+        <v>44968</v>
+      </c>
+      <c r="C255" s="16">
+        <v>45524</v>
+      </c>
+      <c r="D255" s="16">
+        <f t="shared" si="9"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6">
+      <c r="A256" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B256" s="16">
+        <v>48249</v>
+      </c>
+      <c r="C256" s="16">
+        <v>48805</v>
+      </c>
+      <c r="D256" s="16">
         <f t="shared" si="9"/>
         <v>556</v>
       </c>

</xml_diff>

<commit_message>
Up to World 8-Tower 1. 88 frames faster than the previous WIP. 594 frames faster than the previous run.
(Also, removing the random "a" that was added long ago to the comparison sheet.)
</commit_message>
<xml_diff>
--- a/NSMB/NSMB.xlsx
+++ b/NSMB/NSMB.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="252">
   <si>
     <t>1-1</t>
   </si>
@@ -711,9 +711,6 @@
   </si>
   <si>
     <t>Checkpoint 937</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>Note: 10154 is possible, but doesn't matter due to waiting for 465 on the timer.</t>
@@ -1324,11 +1321,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I256"/>
+  <dimension ref="A1:H256"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C257" sqref="C257"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1340,7 +1337,7 @@
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
@@ -1360,7 +1357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" ht="19.5" thickTop="1">
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
       <c r="A2" s="38" t="s">
         <v>44</v>
       </c>
@@ -1370,7 +1367,7 @@
       <c r="E2" s="38"/>
       <c r="F2" s="38"/>
     </row>
-    <row r="3" spans="1:9" outlineLevel="1">
+    <row r="3" spans="1:6" outlineLevel="1">
       <c r="A3" s="16" t="s">
         <v>48</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" outlineLevel="1">
+    <row r="4" spans="1:6" outlineLevel="1">
       <c r="A4" s="16" t="s">
         <v>49</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" outlineLevel="1">
+    <row r="5" spans="1:6" outlineLevel="1">
       <c r="A5" s="16" t="s">
         <v>50</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="18.75">
+    <row r="6" spans="1:6" s="13" customFormat="1" ht="18.75">
       <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
@@ -1445,11 +1442,8 @@
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
-      <c r="I6" s="13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" outlineLevel="1">
+    </row>
+    <row r="7" spans="1:6" outlineLevel="1">
       <c r="A7" s="20" t="s">
         <v>43</v>
       </c>
@@ -1459,7 +1453,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
     </row>
-    <row r="8" spans="1:9" outlineLevel="1">
+    <row r="8" spans="1:6" outlineLevel="1">
       <c r="A8" s="16" t="s">
         <v>51</v>
       </c>
@@ -1481,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" outlineLevel="1">
+    <row r="9" spans="1:6" outlineLevel="1">
       <c r="A9" s="16" t="s">
         <v>230</v>
       </c>
@@ -1503,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" outlineLevel="1">
+    <row r="10" spans="1:6" outlineLevel="1">
       <c r="A10" s="16" t="s">
         <v>45</v>
       </c>
@@ -1525,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" outlineLevel="1">
+    <row r="11" spans="1:6" outlineLevel="1">
       <c r="A11" s="16" t="s">
         <v>46</v>
       </c>
@@ -1547,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" outlineLevel="1">
+    <row r="12" spans="1:6" outlineLevel="1">
       <c r="A12" s="20" t="s">
         <v>80</v>
       </c>
@@ -1557,7 +1551,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:9" outlineLevel="1">
+    <row r="13" spans="1:6" outlineLevel="1">
       <c r="A13" s="16" t="s">
         <v>53</v>
       </c>
@@ -1579,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" outlineLevel="1">
+    <row r="14" spans="1:6" outlineLevel="1">
       <c r="A14" s="16" t="s">
         <v>20</v>
       </c>
@@ -1601,7 +1595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" outlineLevel="1">
+    <row r="15" spans="1:6" outlineLevel="1">
       <c r="A15" s="16" t="s">
         <v>45</v>
       </c>
@@ -1623,7 +1617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" outlineLevel="1">
+    <row r="16" spans="1:6" outlineLevel="1">
       <c r="A16" s="16" t="s">
         <v>55</v>
       </c>
@@ -1745,7 +1739,7 @@
         <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:8" outlineLevel="1">
@@ -4278,7 +4272,7 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B229" s="16">
         <v>28372</v>
@@ -4339,7 +4333,7 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B233" s="16">
         <v>30492</v>
@@ -4384,7 +4378,7 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B236" s="16">
         <v>31401</v>
@@ -4399,7 +4393,7 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B237" s="16">
         <v>31876</v>
@@ -4437,7 +4431,7 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B239" s="16">
         <v>33093</v>
@@ -4452,7 +4446,7 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B240" s="16">
         <v>35071</v>
@@ -4546,7 +4540,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B246" s="16">
         <v>42729</v>
@@ -4561,7 +4555,7 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B247" s="16">
         <v>42842</v>
@@ -4576,7 +4570,7 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B248" s="16">
         <v>43142</v>
@@ -4591,7 +4585,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B249" s="16">
         <v>43239</v>
@@ -4606,7 +4600,7 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B250" s="16">
         <v>43305</v>
@@ -4621,7 +4615,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B251" s="16">
         <v>43435</v>
@@ -4636,7 +4630,7 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B252" s="16">
         <v>43759</v>
@@ -4681,7 +4675,7 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B255" s="16">
         <v>44968</v>
@@ -4751,13 +4745,13 @@
         <v>99</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F1" s="42"/>
       <c r="G1">
@@ -4865,7 +4859,7 @@
     </row>
     <row r="10" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A10" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" s="16">
         <v>3093</v>
@@ -4880,7 +4874,7 @@
     </row>
     <row r="11" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A11" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11" s="16">
         <v>3151</v>
@@ -4895,7 +4889,7 @@
     </row>
     <row r="12" spans="1:7" hidden="1" outlineLevel="1">
       <c r="A12" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" s="16">
         <v>3712</v>
@@ -4992,7 +4986,7 @@
     </row>
     <row r="18" spans="1:9" hidden="1" outlineLevel="1">
       <c r="A18" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B18" s="16">
         <v>5296</v>

</xml_diff>